<commit_message>
Added NX-GED; Cleand Calculators;
</commit_message>
<xml_diff>
--- a/configs/test_datasets.xlsx
+++ b/configs/test_datasets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,9 @@
           <t>edge_histogram_mean</t>
         </is>
       </c>
+      <c r="N1" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -545,6 +548,304 @@
       <c r="M2" t="inlineStr">
         <is>
           <t>[2354 1004  362    1]</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="n">
+        <v>14.55840455840456</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>15.002849002849</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>{0: 0.6552706552706553, 1: 0.34472934472934474}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '2', '3', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>[   1   23    1    1    2    1    3    1    1    1    1  721  408   29
+ 3493  269  100   44   10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>[   7  436 2772 2051]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finisched Prototype and Zero Kernel
</commit_message>
<xml_diff>
--- a/configs/test_datasets.xlsx
+++ b/configs/test_datasets.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N268"/>
+  <dimension ref="A1:N338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6195,6 +6195,1488 @@
         </is>
       </c>
     </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="inlineStr"/>
+      <c r="C269" t="inlineStr"/>
+      <c r="D269" t="inlineStr"/>
+      <c r="E269" t="inlineStr"/>
+      <c r="F269" t="inlineStr"/>
+      <c r="G269" t="inlineStr"/>
+      <c r="H269" t="inlineStr"/>
+      <c r="I269" t="inlineStr"/>
+      <c r="J269" t="inlineStr"/>
+      <c r="K269" t="inlineStr"/>
+      <c r="L269" t="inlineStr"/>
+      <c r="M269" t="inlineStr"/>
+      <c r="N269" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="inlineStr"/>
+      <c r="C270" t="inlineStr"/>
+      <c r="D270" t="inlineStr"/>
+      <c r="E270" t="inlineStr"/>
+      <c r="F270" t="inlineStr"/>
+      <c r="G270" t="inlineStr"/>
+      <c r="H270" t="inlineStr"/>
+      <c r="I270" t="inlineStr"/>
+      <c r="J270" t="inlineStr"/>
+      <c r="K270" t="inlineStr"/>
+      <c r="L270" t="inlineStr"/>
+      <c r="M270" t="inlineStr"/>
+      <c r="N270" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="inlineStr"/>
+      <c r="C271" t="inlineStr"/>
+      <c r="D271" t="inlineStr"/>
+      <c r="E271" t="inlineStr"/>
+      <c r="F271" t="inlineStr"/>
+      <c r="G271" t="inlineStr"/>
+      <c r="H271" t="inlineStr"/>
+      <c r="I271" t="inlineStr"/>
+      <c r="J271" t="inlineStr"/>
+      <c r="K271" t="inlineStr"/>
+      <c r="L271" t="inlineStr"/>
+      <c r="M271" t="inlineStr"/>
+      <c r="N271" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="inlineStr"/>
+      <c r="C272" t="inlineStr"/>
+      <c r="D272" t="inlineStr"/>
+      <c r="E272" t="inlineStr"/>
+      <c r="F272" t="inlineStr"/>
+      <c r="G272" t="inlineStr"/>
+      <c r="H272" t="inlineStr"/>
+      <c r="I272" t="inlineStr"/>
+      <c r="J272" t="inlineStr"/>
+      <c r="K272" t="inlineStr"/>
+      <c r="L272" t="inlineStr"/>
+      <c r="M272" t="inlineStr"/>
+      <c r="N272" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="inlineStr"/>
+      <c r="C273" t="inlineStr"/>
+      <c r="D273" t="inlineStr"/>
+      <c r="E273" t="inlineStr"/>
+      <c r="F273" t="inlineStr"/>
+      <c r="G273" t="inlineStr"/>
+      <c r="H273" t="inlineStr"/>
+      <c r="I273" t="inlineStr"/>
+      <c r="J273" t="inlineStr"/>
+      <c r="K273" t="inlineStr"/>
+      <c r="L273" t="inlineStr"/>
+      <c r="M273" t="inlineStr"/>
+      <c r="N273" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="inlineStr"/>
+      <c r="C274" t="inlineStr"/>
+      <c r="D274" t="inlineStr"/>
+      <c r="E274" t="inlineStr"/>
+      <c r="F274" t="inlineStr"/>
+      <c r="G274" t="inlineStr"/>
+      <c r="H274" t="inlineStr"/>
+      <c r="I274" t="inlineStr"/>
+      <c r="J274" t="inlineStr"/>
+      <c r="K274" t="inlineStr"/>
+      <c r="L274" t="inlineStr"/>
+      <c r="M274" t="inlineStr"/>
+      <c r="N274" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="inlineStr"/>
+      <c r="C275" t="inlineStr"/>
+      <c r="D275" t="inlineStr"/>
+      <c r="E275" t="inlineStr"/>
+      <c r="F275" t="inlineStr"/>
+      <c r="G275" t="inlineStr"/>
+      <c r="H275" t="inlineStr"/>
+      <c r="I275" t="inlineStr"/>
+      <c r="J275" t="inlineStr"/>
+      <c r="K275" t="inlineStr"/>
+      <c r="L275" t="inlineStr"/>
+      <c r="M275" t="inlineStr"/>
+      <c r="N275" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="inlineStr"/>
+      <c r="C276" t="inlineStr"/>
+      <c r="D276" t="inlineStr"/>
+      <c r="E276" t="inlineStr"/>
+      <c r="F276" t="inlineStr"/>
+      <c r="G276" t="inlineStr"/>
+      <c r="H276" t="inlineStr"/>
+      <c r="I276" t="inlineStr"/>
+      <c r="J276" t="inlineStr"/>
+      <c r="K276" t="inlineStr"/>
+      <c r="L276" t="inlineStr"/>
+      <c r="M276" t="inlineStr"/>
+      <c r="N276" t="n">
+        <v>15.6925</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="inlineStr"/>
+      <c r="C277" t="inlineStr"/>
+      <c r="D277" t="inlineStr"/>
+      <c r="E277" t="inlineStr"/>
+      <c r="F277" t="inlineStr"/>
+      <c r="G277" t="inlineStr"/>
+      <c r="H277" t="inlineStr"/>
+      <c r="I277" t="inlineStr"/>
+      <c r="J277" t="inlineStr"/>
+      <c r="K277" t="inlineStr"/>
+      <c r="L277" t="inlineStr"/>
+      <c r="M277" t="inlineStr"/>
+      <c r="N277" t="n">
+        <v>16.195</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="inlineStr"/>
+      <c r="C278" t="inlineStr"/>
+      <c r="D278" t="inlineStr"/>
+      <c r="E278" t="inlineStr"/>
+      <c r="F278" t="inlineStr"/>
+      <c r="G278" t="inlineStr"/>
+      <c r="H278" t="inlineStr"/>
+      <c r="I278" t="inlineStr"/>
+      <c r="J278" t="inlineStr"/>
+      <c r="K278" t="inlineStr"/>
+      <c r="L278" t="inlineStr"/>
+      <c r="M278" t="inlineStr"/>
+      <c r="N278" t="inlineStr">
+        <is>
+          <t>{0: 0.2, 1: 0.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="inlineStr"/>
+      <c r="C279" t="inlineStr"/>
+      <c r="D279" t="inlineStr"/>
+      <c r="E279" t="inlineStr"/>
+      <c r="F279" t="inlineStr"/>
+      <c r="G279" t="inlineStr"/>
+      <c r="H279" t="inlineStr"/>
+      <c r="I279" t="inlineStr"/>
+      <c r="J279" t="inlineStr"/>
+      <c r="K279" t="inlineStr"/>
+      <c r="L279" t="inlineStr"/>
+      <c r="M279" t="inlineStr"/>
+      <c r="N279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">['[1.0, -1.0, 0.5, -2.3499999046325684]', '[1.0, -1.0, 1.5, -2.1500000953674316]', '[1.0, -1.0, 2.865999937057495, 0.5]', '[1.0, -1.0, 2.889400005340576, 1.0297000408172607]', '[1.0, -1.0, 3.232100009918213, 1.4329999685287476]', '[1.0, -1.0, 3.2600998878479004, -0.6739000082015991]', '[1.0, -1.0, 3.694200038909912, 0.27709999680519104]', '[1.0, -1.0, 3.7320001125335693, 1.5]', '[1.0, -1.0, 3.732100009918213, -1.4329999685287476]', '[1.0, -1.0, 4.0, 1.0]', '[1.0, -1.0, 4.232100009918213, 1.4329999685287476]', '[1.0, -1.0, 4.2600998878479, -0.6739000082015991]', '[1.0, -1.0, 4.5690999031066895, 0.27709999680519104]', '[1.0, -1.0, 4.598100185394287, -0.25]', '[1.0, -1.0, 5.464099884033203, -0.5]', '[1.0, -1.0, 5.464099884033203, -0.7842000126838684]', '[1.0, -1.0, 5.464099884033203, -1.0]', '[1.0, -1.0, 6.1905999183654785, 1.7073999643325806]', '[1.0, -1.0, 6.556700229644775, 0.34139999747276306]', '[1.0, 0.0, 0.375, 0.0]', '[1.0, 0.0, 0.5, -2.3499999046325684]', '[1.0, 0.0, 0.5, -4.349999904632568]', '[1.0, 0.0, 0.5, -6.349999904632568]', '[1.0, 0.0, 0.5, -8.350000381469727]', '[1.0, 0.0, 0.6428999900817871, -16.350000381469727]', '[1.0, 0.0, 0.666700005531311, -2.3499999046325684]', '[1.0, 0.0, 0.666700005531311, -6.349999904632568]', '[1.0, 0.0, 0.75, -20.350000381469727]', '[1.0, 0.0, 0.75, -8.350000381469727]', '[1.0, 0.0, 0.75, 0.0]', '[1.0, 0.0, 0.8999999761581421, -30.350000381469727]', '[1.0, 0.0, 1.0, -6.349999904632568]', '[1.0, 0.0, 1.25, -4.349999904632568]', '[1.0, 0.0, 1.5, -10.149999618530273]', '[1.0, 0.0, 1.5, -10.350000381469727]', '[1.0, 0.0, 1.5, -12.350000381469727]', '[1.0, 0.0, 1.5, -2.3499999046325684]', '[1.0, 0.0, 1.5, -4.150000095367432]', '[1.0, 0.0, 1.5, -4.349999904632568]', '[1.0, 0.0, 1.5, -6.150000095367432]', '[1.0, 0.0, 1.5, -8.149999618530273]', '[1.0, 0.0, 1.5, -8.350000381469727]', '[1.0, 0.0, 1.6875, -24.149999618530273]', '[1.0, 0.0, 1.6875, -26.149999618530273]', '[1.0, 0.0, 10.000699996948242, 6.783299922943115]', '[1.0, 0.0, 10.00160026550293, 8.176199913024902]', '[1.0, 0.0, 10.002900123596191, -0.43299999833106995]', '[1.0, 0.0, 10.016900062561035, 0.5907999873161316]', '[1.0, 0.0, 10.016900062561035, 1.5908000469207764]', '[1.0, 0.0, 10.0516996383667, 3.3773000240325928]', '[1.0, 0.0, 10.052800178527832, -7.656899929046631]', '[1.0, 0.0, 10.05780029296875, 6.271399974822998]', '[1.0, 0.0, 10.062199592590332, -0.16060000658035278]', '[1.0, 0.0, 10.062199592590332, -1.0]', '[1.0, 0.0, 10.062199592590332, -1.160599946975708]', '[1.0, 0.0, 10.062199592590332, -1.6739000082015991]', '[1.0, 0.0, 10.062199592590332, -1.75]', '[1.0, 0.0, 10.062199592590332, -1.910599946975708]', '[1.0, 0.0, 10.062199592590332, -2.5]', '[1.0, 0.0, 10.062199592590332, -2.75]', '[1.0, 0.0, 10.062199592590332, -3.5]', '[1.0, 0.0, 10.062199592590332, -3.6738998889923096]', '[1.0, 0.0, 10.062199592590332, 0.0]', '[1.0, 0.0, 10.062199592590332, 1.089400053024292]', '[1.0, 0.0, 10.062199592590332, 1.25]', '[1.0, 0.0, 10.062199592590332, 3.25]', '[1.0, 0.0, 10.092599868774414, 1.608199954032898]', '[1.0, 0.0, 10.100500106811523, 6.870699882507324]', '[1.0, 0.0, 10.135100364685059, -4.391600131988525]', '[1.0, 0.0, 10.136899948120117, -0.014000000432133675]', '[1.0, 0.0, 10.140000343322754, -7.939700126647949]', '[1.0, 0.0, 10.140000343322754, -8.93970012664795]', '[1.0, 0.0, 10.144399642944336, -10.459600448608398]', '[1.0, 0.0, 10.144399642944336, -11.459600448608398]', '[1.0, 0.0, 10.144399642944336, -8.089799880981445]', '[1.0, 0.0, 10.144399642944336, -9.089799880981445]', '[1.0, 0.0, 10.14490032196045, 6.62060022354126]', '[1.0, 0.0, 10.154600143432617, 4.2307000160217285]', '[1.0, 0.0, 10.160300254821777, -4.673900127410889]', '[1.0, 0.0, 10.160300254821777, 1.4514000415802002]', '[1.0, 0.0, 10.166600227355957, -0.38449999690055847]', '[1.0, 0.0, 10.1697998046875, 8.392399787902832]', '[1.0, 0.0, 10.17080020904541, 6.566999912261963]', '[1.0, 0.0, 10.185099601745605, -2.4937000274658203]', '[1.0, 0.0, 10.191800117492676, 6.886499881744385]', '[1.0, 0.0, 10.199199676513672, -1.6735999584197998]', '[1.0, 0.0, 10.215299606323242, -0.24549999833106995]', '[1.0, 0.0, 10.215299606323242, -1.2454999685287476]', '[1.0, 0.0, 10.219599723815918, 7.595300197601318]', '[1.0, 0.0, 10.226400375366211, -0.15189999341964722]', '[1.0, 0.0, 10.236100196838379, -1.3710999488830566]', '[1.0, 0.0, 10.265899658203125, -0.020899999886751175]', '[1.0, 0.0, 10.270899772644043, -0.5]', '[1.0, 0.0, 10.270899772644043, 3.6923999786376953]', '[1.0, 0.0, 10.270899772644043, 4.5584001541137695]', '[1.0, 0.0, 10.278800010681152, 2.4182000160217285]', '[1.0, 0.0, 10.28339958190918, -2.2397000789642334]', '[1.0, 0.0, 10.28339958190918, -3.2397000789642334]', '[1.0, 0.0, 10.299699783325195, 6.1006999015808105]', '[1.0, 0.0, 10.309300422668457, -5.523099899291992]', '[1.0, 0.0, 10.317500114440918, -0.4099999964237213]', '[1.0, 0.0, 10.317500114440918, -1.409999966621399]', '[1.0, 0.0, 10.317500114440918, 1.590000033378601]', '[1.0, 0.0, 10.318300247192383, 2.3649001121520996]', '[1.0, 0.0, 10.318300247192383, 2.821700096130371]', '[1.0, 0.0, 10.323699951171875, 0.7990999817848206]', '[1.0, 0.0, 10.323699951171875, 0.9036999940872192]', '[1.0, 0.0, 10.32409954071045, 8.589900016784668]', '[1.0, 0.0, 10.331100463867188, -1.2702000141143799]', '[1.0, 0.0, 10.347200393676758, 3.1205999851226807]', '[1.0, 0.0, 10.366299629211426, -2.43530011177063]', '[1.0, 0.0, 10.366299629211426, -3.43530011177063]', '[1.0, 0.0, 10.371999740600586, -0.6202999949455261]', '[1.0, 0.0, 10.371999740600586, -1.0247999429702759]', '[1.0, 0.0, 10.371999740600586, -1.620300054550171]', '[1.0, 0.0, 10.371999740600586, -2.0248000621795654]', '[1.0, 0.0, 10.371999740600586, 0.9751999974250793]', '[1.0, 0.0, 10.371999740600586, 1.379699945449829]', '[1.0, 0.0, 10.393099784851074, -4.367000102996826]', '[1.0, 0.0, 10.405400276184082, -2.2370998859405518]', '[1.0, 0.0, 10.405400276184082, 2.3268001079559326]', '[1.0, 0.0, 10.42389965057373, -5.724899768829346]', '[1.0, 0.0, 10.42389965057373, -6.724899768829346]', '[1.0, 0.0, 10.44279956817627, -2.9772000312805176]', '[1.0, 0.0, 10.444999694824219, -3.25219988822937]', '[1.0, 0.0, 10.44540023803711, -5.365600109100342]', '[1.0, 0.0, 10.446200370788574, 5.204899787902832]', '[1.0, 0.0, 10.470999717712402, -1.36489999294281]', '[1.0, 0.0, 10.470999717712402, -1.7316999435424805]', '[1.0, 0.0, 10.470999717712402, 3.9361000061035156]', '[1.0, 0.0, 10.472299575805664, -1.3495999574661255]', '[1.0, 0.0, 10.4822998046875, 2.7565999031066895]', '[1.0, 0.0, 10.485799789428711, 1.9979000091552734]', '[1.0, 0.0, 10.499300003051758, 0.7990999817848206]', '[1.0, 0.0, 10.499300003051758, 1.0082000494003296]', '[1.0, 0.0, 10.499300003051758, 1.1513999700546265]', '[1.0, 0.0, 10.499300003051758, 1.3082000017166138]', '[1.0, 0.0, 10.499300003051758, 1.6604000329971313]', '[1.0, 0.0, 10.499300003051758, 1.7127000093460083]', '[1.0, 0.0, 10.510899543762207, -1.163599967956543]', '[1.0, 0.0, 10.510899543762207, 2.5817999839782715]', '[1.0, 0.0, 10.510899543762207, 3.5817999839782715]', '[1.0, 0.0, 10.512499809265137, 0.8306000232696533]', '[1.0, 0.0, 10.532600402832031, 0.9815000295639038]', '[1.0, 0.0, 10.553299903869629, -4.129799842834473]', '[1.0, 0.0, 10.555100440979004, -3.5367000102996826]', '[1.0, 0.0, 10.561200141906738, -3.7397000789642334]', '[1.0, 0.0, 10.562199592590332, 2.134000062942505]', '[1.0, 0.0, 10.575499534606934, -4.243599891662598]', '[1.0, 0.0, 10.576499938964844, 9.305999755859375]', '[1.0, 0.0, 10.588000297546387, -7.283199787139893]', '[1.0, 0.0, 10.60319995880127, 3.4238998889923096]', '[1.0, 0.0, 10.60319995880127, 4.423900127410889]', '[1.0, 0.0, 10.60319995880127, 7.423900127410889]', '[1.0, 0.0, 10.631400108337402, 7.765399932861328]', '[1.0, 0.0, 10.632800102233887, -0.04740000143647194]', '[1.0, 0.0, 10.632800102233887, -0.15189999341964722]', '[1.0, 0.0, 10.63599967956543, -2.087399959564209]', '[1.0, 0.0, 10.636899948120117, -0.8799999952316284]', '[1.0, 0.0, 10.6427001953125, -0.04899999871850014]', '[1.0, 0.0, 10.6427001953125, -1.7319999933242798]', '[1.0, 0.0, 10.6427001953125, -2.0490000247955322]', '[1.0, 0.0, 10.6427001953125, -2.7320001125335693]', '[1.0, 0.0, 10.6427001953125, -3.0490000247955322]', '[1.0, 0.0, 10.6427001953125, 0.2680000066757202]', '[1.0, 0.0, 10.643099784851074, -0.1607999950647354]', '[1.0, 0.0, 10.649399757385254, -2.3338000774383545]', '[1.0, 0.0, 10.653599739074707, 0.9096999764442444]', '[1.0, 0.0, 10.654899597167969, 0.19179999828338623]', '[1.0, 0.0, 10.660200119018555, -0.25]', '[1.0, 0.0, 10.660200119018555, -0.3889999985694885]', '[1.0, 0.0, 10.660200119018555, -0.4106000065803528]', '[1.0, 0.0, 10.660200119018555, -0.5]', '[1.0, 0.0, 10.660200119018555, -0.6606000065803528]', '[1.0, 0.0, 10.660200119018555, -0.75]', '[1.0, 0.0, 10.660200119018555, -0.7979000210762024]', '[1.0, 0.0, 10.660200119018555, -1.0]', '[1.0, 0.0, 10.660200119018555, -1.25]', '[1.0, 0.0, 10.660200119018555, -1.3170000314712524]', '[1.0, 0.0, 10.660200119018555, -1.5]', '[1.0, 0.0, 10.660200119018555, -1.75]', '[1.0, 0.0, 10.660200119018555, -1.8170000314712524]', '[1.0, 0.0, 10.660200119018555, -2.0]', '[1.0, 0.0, 10.660200119018555, -2.316999912261963]', '[1.0, 0.0, 10.660200119018555, -2.3889999389648438]', '[1.0, 0.0, 10.660200119018555, -2.5]', '[1.0, 0.0, 10.660200119018555, -2.75]', '[1.0, 0.0, 10.660200119018555, -2.7978999614715576]', '[1.0, 0.0, 10.660200119018555, -3.0875000953674316]', '[1.0, 0.0, 10.660200119018555, -3.0]', '[1.0, 0.0, 10.660200119018555, -3.25]', '[1.0, 0.0, 10.660200119018555, -3.5]', '[1.0, 0.0, 10.660200119018555, -4.0]', '[1.0, 0.0, 10.660200119018555, 0.0]', '[1.0, 0.0, 10.660200119018555, 0.25]', '[1.0, 0.0, 10.660200119018555, 0.3393999934196472]', '[1.0, 0.0, 10.660200119018555, 0.5]', '[1.0, 0.0, 10.660200119018555, 0.6830000281333923]', '[1.0, 0.0, 10.660200119018555, 1.0]', '[1.0, 0.0, 10.660200119018555, 1.5670000314712524]', '[1.0, 0.0, 10.660200119018555, 2.0]', '[1.0, 0.0, 10.660200119018555, 3.566999912261963]', '[1.0, 0.0, 10.660200119018555, 4.482900142669678]', '[1.0, 0.0, 10.660300254821777, -0.06700000166893005]', '[1.0, 0.0, 10.660300254821777, -0.08749999850988388]', '[1.0, 0.0, 10.660300254821777, -0.25]', '[1.0, 0.0, 10.660300254821777, -0.5170999765396118]', '[1.0, 0.0, 10.660300254821777, -0.5]', '[1.0, 0.0, 10.660300254821777, -0.75]', '[1.0, 0.0, 10.660300254821777, -1.0670000314712524]', '[1.0, 0.0, 10.660300254821777, -1.0]', '[1.0, 0.0, 10.660300254821777, -1.5170999765396118]', '[1.0, 0.0, 10.660300254821777, -1.5670000314712524]', '[1.0, 0.0, 10.660300254821777, -1.5]', '[1.0, 0.0, 10.660300254821777, -1.660599946975708]', '[1.0, 0.0, 10.660300254821777, -1.75]', '[1.0, 0.0, 10.660300254821777, -2.0]', '[1.0, 0.0, 10.660300254821777, -2.25]', '[1.0, 0.0, 10.660300254821777, -2.410599946975708]', '[1.0, 0.0, 10.660300254821777, -2.5171000957489014]', '[1.0, 0.0, 10.660300254821777, -2.5]', '[1.0, 0.0, 10.660300254821777, -3.566999912261963]', '[1.0, 0.0, 10.660300254821777, -3.5]', '[1.0, 0.0, 10.660300254821777, -4.566999912261963]', '[1.0, 0.0, 10.660300254821777, 0.0]', '[1.0, 0.0, 10.660300254821777, 0.25]', '[1.0, 0.0, 10.660300254821777, 0.4828999936580658]', '[1.0, 0.0, 10.660300254821777, 0.5669999718666077]', '[1.0, 0.0, 10.660300254821777, 0.5]', '[1.0, 0.0, 10.660300254821777, 0.6830000281333923]', '[1.0, 0.0, 10.660300254821777, 0.75]', '[1.0, 0.0, 10.660300254821777, 0.9330000281333923]', '[1.0, 0.0, 10.660300254821777, 1.0]', '[1.0, 0.0, 10.660300254821777, 1.25]', '[1.0, 0.0, 10.660300254821777, 1.5670000314712524]', '[1.0, 0.0, 10.660300254821777, 1.5]', '[1.0, 0.0, 10.660300254821777, 1.9329999685287476]', '[1.0, 0.0, 10.660300254821777, 2.0]', '[1.0, 0.0, 10.660300254821777, 2.25]', '[1.0, 0.0, 10.660300254821777, 2.5]', '[1.0, 0.0, 10.660300254821777, 2.75]', '[1.0, 0.0, 10.660300254821777, 2.933000087738037]', '[1.0, 0.0, 10.660300254821777, 3.0]', '[1.0, 0.0, 10.660300254821777, 3.25]', '[1.0, 0.0, 10.660300254821777, 3.316999912261963]', '[1.0, 0.0, 10.660300254821777, 3.5]', '[1.0, 0.0, 10.660300254821777, 4.0]', '[1.0, 0.0, 10.660300254821777, 4.25]', '[1.0, 0.0, 10.660300254821777, 4.5]', '[1.0, 0.0, 10.660300254821777, 5.25]', '[1.0, 0.0, 10.660300254821777, 5.75]', '[1.0, 0.0, 10.660300254821777, 6.0]', '[1.0, 0.0, 10.660300254821777, 7.566999912261963]', '[1.0, 0.0, 10.660300254821777, 7.75]', '[1.0, 0.0, 10.6697998046875, 7.526400089263916]', '[1.0, 0.0, 10.670599937438965, -1.0717999935150146]', '[1.0, 0.0, 10.67080020904541, 7.433000087738037]', '[1.0, 0.0, 10.678799629211426, 1.5261000394821167]', '[1.0, 0.0, 10.680299758911133, 0.7990999817848206]', '[1.0, 0.0, 10.685099601745605, -0.954800009727478]', '[1.0, 0.0, 10.68970012664795, -3.135200023651123]', '[1.0, 0.0, 10.68970012664795, -3.2397000789642334]', '[1.0, 0.0, 10.689800262451172, -2.135200023651123]', '[1.0, 0.0, 10.689800262451172, -2.2397000789642334]', '[1.0, 0.0, 10.69950008392334, -5.967800140380859]', '[1.0, 0.0, 10.707799911499023, -0.801800012588501]', '[1.0, 0.0, 10.707799911499023, -0.887499988079071]', '[1.0, 0.0, 10.707799911499023, 9.08650016784668]', '[1.0, 0.0, 10.720999717712402, -2.8396999835968018]', '[1.0, 0.0, 10.721500396728516, 0.7148000001907349]', '[1.0, 0.0, 10.742400169372559, 5.039700031280518]', '[1.0, 0.0, 10.748100280761719, -5.482900142669678]', '[1.0, 0.0, 10.748900413513184, 1.8930000066757202]', '[1.0, 0.0, 10.748900413513184, 2.8929998874664307]', '[1.0, 0.0, 10.768799781799316, 0.06620000302791595]', '[1.0, 0.0, 10.770899772644043, 2.8264000415802]', '[1.0, 0.0, 10.770899772644043, 3.6923999786376953]', '[1.0, 0.0, 10.770899772644043, 4.5584001541137695]', '[1.0, 0.0, 10.770899772644043, 5.4243998527526855]', '[1.0, 0.0, 10.781200408935547, -5.253900051116943]', '[1.0, 0.0, 10.79419994354248, -0.25]', '[1.0, 0.0, 10.79419994354248, -1.25]', '[1.0, 0.0, 10.79419994354248, -3.25]', '[1.0, 0.0, 10.838800430297852, 3.3415000438690186]', '[1.0, 0.0, 10.864800453186035, 1.1887999773025513]', '[1.0, 0.0, 10.865599632263184, 0.6111999750137329]', '[1.0, 0.0, 10.866299629211426, -0.8964999914169312]', '[1.0, 0.0, 10.876899719238281, -0.10360000282526016]', '[1.0, 0.0, 10.876899719238281, -2.4110000133514404]', '[1.0, 0.0, 10.876899719238281, -2.4967000484466553]', '[1.0, 0.0, 10.876899719238281, 7.477399826049805]', '[1.0, 0.0, 10.88290023803711, 0.09080000221729279]', '[1.0, 0.0, 10.906000137329102, -1.6196000576019287]', '[1.0, 0.0, 10.906000137329102, 1.7648999691009521]', '[1.0, 0.0, 10.906000137329102, 2.012700080871582]', '[1.0, 0.0, 10.906000137329102, 2.1171998977661133]', '[1.0, 0.0, 10.906000137329102, 3.9307000637054443]', '[1.0, 0.0, 10.90839958190918, 7.652599811553955]', '[1.0, 0.0, 10.913100242614746, 8.724900245666504]', '[1.0, 0.0, 10.91569995880127, 2.4837000370025635]', '[1.0, 0.0, 10.917699813842773, 3.8773000240325928]', '[1.0, 0.0, 10.923999786376953, 1.457200050354004]', '[1.0, 0.0, 10.928199768066406, -1.5]', '[1.0, 0.0, 10.928199768066406, -1.660599946975708]', '[1.0, 0.0, 10.928199768066406, -2.0]', '[1.0, 0.0, 10.928199768066406, -2.410599946975708]', '[1.0, 0.0, 10.928199768066406, -4.0]', '[1.0, 0.0, 10.928199768066406, 0.3393999934196472]', '[1.0, 0.0, 10.928199768066406, 0.5]', '[1.0, 0.0, 10.928199768066406, 1.75]', '[1.0, 0.0, 10.928199768066406, 2.75]', '[1.0, 0.0, 10.93690013885498, 0.5066999793052673]', '[1.0, 0.0, 10.963600158691406, 3.642899990081787]', '[1.0, 0.0, 10.963899612426758, 3.2730000019073486]', '[1.0, 0.0, 10.968199729919434, 5.068699836730957]', '[1.0, 0.0, 10.969300270080566, -4.086100101470947]', '[1.0, 0.0, 10.975700378417969, -2.0806000232696533]', '[1.0, 0.0, 10.978899955749512, 0.39579999446868896]', '[1.0, 0.0, 10.978899955749512, 1.395799994468689]', '[1.0, 0.0, 11.002900123596191, -0.43299999833106995]', '[1.0, 0.0, 11.005999565124512, -10.43970012664795]', '[1.0, 0.0, 11.005999565124512, -9.43970012664795]', '[1.0, 0.0, 11.01039981842041, -10.589900016784668]', '[1.0, 0.0, 11.01039981842041, -11.959600448608398]', '[1.0, 0.0, 11.01039981842041, -12.959600448608398]', '[1.0, 0.0, 11.01039981842041, -9.589900016784668]', '[1.0, 0.0, 11.02340030670166, -0.33500000834465027]', '[1.0, 0.0, 11.02340030670166, 0.424699991941452]', '[1.0, 0.0, 11.03969955444336, 6.082200050354004]', '[1.0, 0.0, 11.077699661254883, 0.45260000228881836]', '[1.0, 0.0, 11.077699661254883, 2.1847000122070312]', '[1.0, 0.0, 11.081399917602539, -1.7454999685287476]', '[1.0, 0.0, 11.081399917602539, 0.25450000166893005]', '[1.0, 0.0, 11.0871000289917, 0.19920000433921814]', '[1.0, 0.0, 11.0871000289917, 0.9036999940872192]', '[1.0, 0.0, 11.087400436401367, -3.236599922180176]', '[1.0, 0.0, 11.097700119018555, 6.795899868011475]', '[1.0, 0.0, 11.1318998336792, 0.47909998893737793]', '[1.0, 0.0, 11.144800186157227, -0.4713999927043915]', '[1.0, 0.0, 11.149399757385254, -3.7397000789642334]', '[1.0, 0.0, 11.160300254821777, 1.4514000415802002]', '[1.0, 0.0, 11.163900375366211, -4.330100059509277]', '[1.0, 0.0, 11.170000076293945, 7.094399929046631]', '[1.0, 0.0, 11.179400444030762, -2.823699951171875]', '[1.0, 0.0, 11.183500289916992, 0.09000000357627869]', '[1.0, 0.0, 11.183500289916992, 1.090000033378601]', '[1.0, 0.0, 11.183600425720215, -3.058799982070923]', '[1.0, 0.0, 11.185099601745605, -2.4937000274658203]', '[1.0, 0.0, 11.190199851989746, 10.089799880981445]', '[1.0, 0.0, 11.190400123596191, -3.00570011138916]', '[1.0, 0.0, 11.19950008392334, 1.030500054359436]', '[1.0, 0.0, 11.206299781799316, 0.06700000166893005]', '[1.0, 0.0, 11.206299781799316, 1.0670000314712524]', '[1.0, 0.0, 11.214200019836426, -0.6956999897956848]', '[1.0, 0.0, 11.214200019836426, -1.062600016593933]', '[1.0, 0.0, 11.217499732971191, 6.701499938964844]', '[1.0, 0.0, 11.231800079345703, -3.8222999572753906]', '[1.0, 0.0, 11.236100196838379, -0.704200029373169]', '[1.0, 0.0, 11.23799991607666, -0.12030000239610672]', '[1.0, 0.0, 11.23799991607666, -0.5248000025749207]', '[1.0, 0.0, 11.23799991607666, -2.120300054550171]', '[1.0, 0.0, 11.23799991607666, -2.5248000621795654]', '[1.0, 0.0, 11.284099578857422, 3.151400089263916]', '[1.0, 0.0, 11.289899826049805, -5.224899768829346]', '[1.0, 0.0, 11.289899826049805, -7.224899768829346]', '[1.0, 0.0, 11.289899826049805, -8.224900245666504]', '[1.0, 0.0, 11.305899620056152, 1.4393999576568604]', '[1.0, 0.0, 11.312800407409668, 2.469399929046631]', '[1.0, 0.0, 11.31309986114502, 2.861799955368042]', '[1.0, 0.0, 11.321499824523926, 7.0416998863220215]', '[1.0, 0.0, 11.336400032043457, -5.8196001052856445]', '[1.0, 0.0, 11.361100196838379, -2.2493999004364014]', '[1.0, 0.0, 11.376899719238281, -1.5448999404907227]', '[1.0, 0.0, 11.376899719238281, -1.6306999921798706]', '[1.0, 0.0, 11.376899719238281, 8.343400001525879]', '[1.0, 0.0, 11.383500099182129, -2.0292000770568848]', '[1.0, 0.0, 11.383500099182129, 2.1189000606536865]', '[1.0, 0.0, 11.412199974060059, 4.946000099182129]', '[1.0, 0.0, 11.421099662780762, -3.0367000102996826]', '[1.0, 0.0, 11.422100067138672, 3.6270999908447266]', '[1.0, 0.0, 11.43690013885498, 2.3069000244140625]', '[1.0, 0.0, 11.452899932861328, 4.251100063323975]', '[1.0, 0.0, 11.453399658203125, -0.19779999554157257]', '[1.0, 0.0, 11.462300300598145, -1.5240999460220337]', '[1.0, 0.0, 11.462599754333496, 1.497499942779541]', '[1.0, 0.0, 11.464699745178223, 0.04569999873638153]', '[1.0, 0.0, 11.477800369262695, 11.190099716186523]', '[1.0, 0.0, 11.479000091552734, 8.04539966583252]', '[1.0, 0.0, 11.490599632263184, -5.356100082397461]', '[1.0, 0.0, 11.493800163269043, -2.4286000728607178]', '[1.0, 0.0, 11.493800163269043, 0.9036999940872192]', '[1.0, 0.0, 11.493800163269043, 1.2559000253677368]', '[1.0, 0.0, 11.493800163269043, 1.3082000017166138]', '[1.0, 0.0, 11.493800163269043, 1.4127000570297241]', '[1.0, 0.0, 11.493800163269043, 1.7648999691009521]', '[1.0, 0.0, 11.493800163269043, 3.1217000484466553]', '[1.0, 0.0, 11.502900123596191, 0.43299999833106995]', '[1.0, 0.0, 11.50879955291748, -0.23199999332427979]', '[1.0, 0.0, 11.50879955291748, -0.5490000247955322]', '[1.0, 0.0, 11.50879955291748, -1.2319999933242798]', '[1.0, 0.0, 11.50879955291748, -1.5490000247955322]', '[1.0, 0.0, 11.50879955291748, -3.5490000247955322]', '[1.0, 0.0, 11.50879955291748, -4.23199987411499]', '[1.0, 0.0, 11.526200294494629, -0.8889999985694885]', '[1.0, 0.0, 11.526200294494629, -2.25]', '[1.0, 0.0, 11.526200294494629, -3.25]', '[1.0, 0.0, 11.526200294494629, -4.25]', '[1.0, 0.0, 11.526200294494629, -4.75]', '[1.0, 0.0, 11.526200294494629, -5.75]', '[1.0, 0.0, 11.526300430297852, -0.06700000166893005]', '[1.0, 0.0, 11.526300430297852, -0.16060000658035278]', '[1.0, 0.0, 11.526300430297852, -0.25]', '[1.0, 0.0, 11.526300430297852, -0.31700000166893005]', '[1.0, 0.0, 11.526300430297852, -0.5669999718666077]', '[1.0, 0.0, 11.526300430297852, -0.5]', '[1.0, 0.0, 11.526300430297852, -0.75]', '[1.0, 0.0, 11.526300430297852, -0.8169999718666077]', '[1.0, 0.0, 11.526300430297852, -0.9106000065803528]', '[1.0, 0.0, 11.526300430297852, -1.0]', '[1.0, 0.0, 11.526300430297852, -1.25]', '[1.0, 0.0, 11.526300430297852, -1.2978999614715576]', '[1.0, 0.0, 11.526300430297852, -1.587499976158142]', '[1.0, 0.0, 11.526300430297852, -1.5]', '[1.0, 0.0, 11.526300430297852, -1.75]', '[1.0, 0.0, 11.526300430297852, -1.910599946975708]', '[1.0, 0.0, 11.526300430297852, -2.066999912261963]', '[1.0, 0.0, 11.526300430297852, -2.0]', '[1.0, 0.0, 11.526300430297852, -2.160599946975708]', '[1.0, 0.0, 11.526300430297852, -2.2978999614715576]', '[1.0, 0.0, 11.526300430297852, -2.5]', '[1.0, 0.0, 11.526300430297852, -3.066999912261963]', '[1.0, 0.0, 11.526300430297852, -3.0]', '[1.0, 0.0, 11.526300430297852, -3.25]', '[1.0, 0.0, 11.526300430297852, -4.0]', '[1.0, 0.0, 11.526300430297852, 0.08940000087022781]', '[1.0, 0.0, 11.526300430297852, 0.0]', '[1.0, 0.0, 11.526300430297852, 0.18299999833106995]', '[1.0, 0.0, 11.526300430297852, 0.25]', '[1.0, 0.0, 11.526300430297852, 0.43299999833106995]', '[1.0, 0.0, 11.526300430297852, 0.5]', '[1.0, 0.0, 11.526300430297852, 0.6830000281333923]', '[1.0, 0.0, 11.526300430297852, 0.75]', '[1.0, 0.0, 11.526300430297852, 0.8393999934196472]', '[1.0, 0.0, 11.526300430297852, 0.9330000281333923]', '[1.0, 0.0, 11.526300430297852, 1.0670000314712524]', '[1.0, 0.0, 11.526300430297852, 1.0]', '[1.0, 0.0, 11.526300430297852, 1.1829999685287476]', '[1.0, 0.0, 11.526300430297852, 1.25]', '[1.0, 0.0, 11.526300430297852, 1.4329999685287476]', '[1.0, 0.0, 11.526300430297852, 1.5670000314712524]', '[1.0, 0.0, 11.526300430297852, 1.5]', '[1.0, 0.0, 11.526300430297852, 1.75]', '[1.0, 0.0, 11.526300430297852, 2.066999912261963]', '[1.0, 0.0, 11.526300430297852, 2.0]', '[1.0, 0.0, 11.526300430297852, 2.183000087738037]', '[1.0, 0.0, 11.526300430297852, 2.25]', '[1.0, 0.0, 11.526300430297852, 2.5]', '[1.0, 0.0, 11.526300430297852, 2.75]', '[1.0, 0.0, 11.526300430297852, 2.9828999042510986]', '[1.0, 0.0, 11.526300430297852, 3.066999912261963]', '[1.0, 0.0, 11.526300430297852, 3.0]', '[1.0, 0.0, 11.526300430297852, 3.433000087738037]', '[1.0, 0.0, 11.526300430297852, 3.5]', '[1.0, 0.0, 11.526300430297852, 3.75]', '[1.0, 0.0, 11.526300430297852, 3.9828999042510986]', '[1.0, 0.0, 11.526300430297852, 4.066999912261963]', '[1.0, 0.0, 11.526300430297852, 4.5]', '[1.0, 0.0, 11.526300430297852, 5.066999912261963]', '[1.0, 0.0, 11.526300430297852, 5.5]', '[1.0, 0.0, 11.526300430297852, 5.75]', '[1.0, 0.0, 11.526300430297852, 6.066999912261963]', '[1.0, 0.0, 11.526300430297852, 6.0]', '[1.0, 0.0, 11.526300430297852, 6.25]', '[1.0, 0.0, 11.526300430297852, 7.066999912261963]', '[1.0, 0.0, 11.526300430297852, 7.0]', '[1.0, 0.0, 11.526300430297852, 7.25]', '[1.0, 0.0, 11.526300430297852, 8.75]', '[1.0, 0.0, 11.526399612426758, 9.75]', '[1.0, 0.0, 11.555800437927246, -3.635200023651123]', '[1.0, 0.0, 11.555800437927246, -3.7397000789642334]', '[1.0, 0.0, 11.566900253295898, -0.5435000061988831]', '[1.0, 0.0, 11.571900367736816, 1.895900011062622]', '[1.0, 0.0, 11.5871000289917, -1.3396999835968018]', '[1.0, 0.0, 11.5871000289917, -4.339700222015381]', '[1.0, 0.0, 11.590299606323242, -2.672600030899048]', '[1.0, 0.0, 11.591099739074707, -2.5302999019622803]', '[1.0, 0.0, 11.592300415039062, 1.1194000244140625]', '[1.0, 0.0, 11.611200332641602, 2.706399917602539]', '[1.0, 0.0, 11.611300468444824, -0.20800000429153442]', '[1.0, 0.0, 11.611300468444824, -1.8260999917984009]', '[1.0, 0.0, 11.636899948120117, -0.8799999952316284]', '[1.0, 0.0, 11.644200325012207, 4.845600128173828]', '[1.0, 0.0, 11.644800186157227, -1.337499976158142]', '[1.0, 0.0, 11.64490032196045, -5.97629976272583]', '[1.0, 0.0, 11.660200119018555, -1.75]', '[1.0, 0.0, 11.660300254821777, 0.25]', '[1.0, 0.0, 11.660300254821777, 0.5]', '[1.0, 0.0, 11.660300254821777, 1.5]', '[1.0, 0.0, 11.66100025177002, 7.622200012207031]', '[1.0, 0.0, 11.670999526977539, 0.6341000199317932]', '[1.0, 0.0, 11.670999526977539, 2.5659000873565674]', '[1.0, 0.0, 11.670999526977539, 3.98009991645813]', '[1.0, 0.0, 11.67490005493164, 0.9036999940872192]', '[1.0, 0.0, 11.692500114440918, 1.1678999662399292]', '[1.0, 0.0, 11.69260025024414, -1.0781999826431274]', '[1.0, 0.0, 11.717499732971191, 8.240400314331055]', '[1.0, 0.0, 11.717499732971191, 9.240400314331055]', '[1.0, 0.0, 11.743599891662598, 3.8131000995635986]', '[1.0, 0.0, 11.74370002746582, -3.723400115966797]', '[1.0, 0.0, 11.748100280761719, 2.2604000568389893]', '[1.0, 0.0, 11.770899772644043, 2.8264000415802]', '[1.0, 0.0, 11.770899772644043, 3.6923999786376953]', '[1.0, 0.0, 11.770899772644043, 4.5584001541137695]', '[1.0, 0.0, 11.770899772644043, 5.4243998527526855]', '[1.0, 0.0, 11.772899627685547, -3.3027000427246094]', '[1.0, 0.0, 11.783699989318848, 5.377299785614014]', '[1.0, 0.0, 11.79419994354248, -0.16060000658035278]', '[1.0, 0.0, 11.79419994354248, -0.9106000065803528]', '[1.0, 0.0, 11.79419994354248, -1.0]', '[1.0, 0.0, 11.79419994354248, -1.160599946975708]', '[1.0, 0.0, 11.79419994354248, -1.910599946975708]', '[1.0, 0.0, 11.79419994354248, -2.5]', '[1.0, 0.0, 11.79419994354248, -3.5]', '[1.0, 0.0, 11.79419994354248, 0.0]', '[1.0, 0.0, 11.79419994354248, 0.8393999934196472]', '[1.0, 0.0, 11.79419994354248, 2.0]', '[1.0, 0.0, 11.79419994354248, 3.0]', '[1.0, 0.0, 11.844900131225586, -0.10419999808073044]', '[1.0, 0.0, 11.844900131225586, 1.895799994468689]', '[1.0, 0.0, 11.876500129699707, -13.459600448608398]', '[1.0, 0.0, 11.876500129699707, -14.459600448608398]', '[1.0, 0.0, 11.888199806213379, 6.3719000816345215]', '[1.0, 0.0, 11.90060043334961, 1.6604000329971313]', '[1.0, 0.0, 11.90060043334961, 2.1171998977661133]', '[1.0, 0.0, 11.920299530029297, -2.777100086212158]', '[1.0, 0.0, 11.920299530029297, -4.395199775695801]', '[1.0, 0.0, 11.929800033569336, 1.600000023841858]', '[1.0, 0.0, 11.939000129699707, 12.911399841308594]', '[1.0, 0.0, 11.947400093078613, -0.24549999833106995]', '[1.0, 0.0, 11.947400093078613, -1.2454999685287476]', '[1.0, 0.0, 11.947400093078613, 0.7544999718666077]', '[1.0, 0.0, 11.953200340270996, 3.8945999145507812]', '[1.0, 0.0, 11.953399658203125, -1.7366000413894653]', '[1.0, 0.0, 11.953399658203125, -4.736599922180176]', '[1.0, 0.0, 11.954000473022461, -5.025199890136719]', '[1.0, 0.0, 11.977800369262695, 10.32409954071045]', '[1.0, 0.0, 12.010899543762207, 0.028599999845027924]', '[1.0, 0.0, 12.031700134277344, 6.1006999015808105]', '[1.0, 0.0, 12.05270004272461, -2.77239990234375]', '[1.0, 0.0, 12.05270004272461, 2.8620998859405518]', '[1.0, 0.0, 12.05620002746582, 8.589799880981445]', '[1.0, 0.0, 12.07229995727539, -0.43299999833106995]', '[1.0, 0.0, 12.07229995727539, 1.5670000314712524]', '[1.0, 0.0, 12.077699661254883, 0.45260000228881836]', '[1.0, 0.0, 12.081600189208984, 0.44690001010894775]', '[1.0, 0.0, 12.081600189208984, 0.9559000134468079]', '[1.0, 0.0, 12.081600189208984, 1.0082000494003296]', '[1.0, 0.0, 12.0871000289917, 0.19920000433921814]', '[1.0, 0.0, 12.104100227355957, -0.6202999949455261]', '[1.0, 0.0, 12.104100227355957, -1.0247999429702759]', '[1.0, 0.0, 12.104100227355957, -1.620300054550171]', '[1.0, 0.0, 12.104100227355957, -2.0248000621795654]', '[1.0, 0.0, 12.12279987335205, -4.276299953460693]', '[1.0, 0.0, 12.12279987335205, 1.523800015449524]', '[1.0, 0.0, 12.126399993896484, -2.1565001010894775]', '[1.0, 0.0, 12.136300086975098, 5.106100082397461]', '[1.0, 0.0, 12.136899948120117, -1.7460999488830566]', '[1.0, 0.0, 12.155900001525879, -8.724900245666504]', '[1.0, 0.0, 12.159700393676758, -4.6128997802734375]', '[1.0, 0.0, 12.165200233459473, -1.004699945449829]', '[1.0, 0.0, 12.165200233459473, -1.3716000318527222]', '[1.0, 0.0, 12.165200233459473, 4.296199798583984]', '[1.0, 0.0, 12.175100326538086, -5.275000095367432]', '[1.0, 0.0, 12.177000045776367, -1.0428999662399292]', '[1.0, 0.0, 12.180000305175781, 1.6376999616622925]', '[1.0, 0.0, 12.19909954071045, -1.0169999599456787]', '[1.0, 0.0, 12.2298002243042, 1.0566999912261963]', '[1.0, 0.0, 12.253100395202637, 6.728499889373779]', '[1.0, 0.0, 12.258299827575684, -3.25]', '[1.0, 0.0, 12.26259994506836, 0.09459999948740005]', '[1.0, 0.0, 12.270899772644043, 3.6923999786376953]', '[1.0, 0.0, 12.270899772644043, 4.5584001541137695]', '[1.0, 0.0, 12.278200149536133, -1.1217000484466553]', '[1.0, 0.0, 12.288700103759766, -1.277400016784668]', '[1.0, 0.0, 12.330699920654297, 0.5457000136375427]', '[1.0, 0.0, 12.354100227355957, -2.027100086212158]', '[1.0, 0.0, 12.35569953918457, -2.14490008354187]', '[1.0, 0.0, 12.360300064086914, 0.06530000269412994]', '[1.0, 0.0, 12.363200187683105, -1.957900047302246]', '[1.0, 0.0, 12.374799728393555, -0.04899999871850014]', '[1.0, 0.0, 12.374799728393555, -1.7319999933242798]', '[1.0, 0.0, 12.374799728393555, -2.0490000247955322]', '[1.0, 0.0, 12.374799728393555, -3.0490000247955322]', '[1.0, 0.0, 12.378100395202637, 3.2730000019073486]', '[1.0, 0.0, 12.392200469970703, -4.75]', '[1.0, 0.0, 12.392200469970703, -5.75]', '[1.0, 0.0, 12.39229965209961, -0.25]', '[1.0, 0.0, 12.39229965209961, -0.4106000065803528]', '[1.0, 0.0, 12.39229965209961, -0.5669999718666077]', '[1.0, 0.0, 12.39229965209961, -0.5]', '[1.0, 0.0, 12.39229965209961, -0.6606000065803528]', '[1.0, 0.0, 12.39229965209961, -0.75]', '[1.0, 0.0, 12.39229965209961, -0.8169999718666077]', '[1.0, 0.0, 12.39229965209961, -1.0]', '[1.0, 0.0, 12.39229965209961, -1.25]', '[1.0, 0.0, 12.39229965209961, -1.5]', '[1.0, 0.0, 12.39229965209961, -1.660599946975708]', '[1.0, 0.0, 12.39229965209961, -1.75]', '[1.0, 0.0, 12.39229965209961, -2.0]', '[1.0, 0.0, 12.39229965209961, -2.3889999389648438]', '[1.0, 0.0, 12.39229965209961, -2.410599946975708]', '[1.0, 0.0, 12.39229965209961, -2.5]', '[1.0, 0.0, 12.39229965209961, -2.75]', '[1.0, 0.0, 12.39229965209961, -4.25]', '[1.0, 0.0, 12.39229965209961, -5.25]', '[1.0, 0.0, 12.39229965209961, -6.25]', '[1.0, 0.0, 12.39229965209961, 0.0]', '[1.0, 0.0, 12.39229965209961, 0.25]', '[1.0, 0.0, 12.39229965209961, 0.5893999934196472]', '[1.0, 0.0, 12.39229965209961, 0.5]', '[1.0, 0.0, 12.39229965209961, 0.6830000281333923]', '[1.0, 0.0, 12.39229965209961, 0.75]', '[1.0, 0.0, 12.39229965209961, 1.0]', '[1.0, 0.0, 12.39229965209961, 1.1829999685287476]', '[1.0, 0.0, 12.39229965209961, 1.25]', '[1.0, 0.0, 12.39229965209961, 1.339400053024292]', '[1.0, 0.0, 12.39229965209961, 1.4329999685287476]', '[1.0, 0.0, 12.39229965209961, 1.5670000314712524]', '[1.0, 0.0, 12.39229965209961, 1.5]', '[1.0, 0.0, 12.39229965209961, 1.75]', '[1.0, 0.0, 12.39229965209961, 1.9329999685287476]', '[1.0, 0.0, 12.39229965209961, 2.0]', '[1.0, 0.0, 12.39229965209961, 2.25]', '[1.0, 0.0, 12.39229965209961, 2.316999912261963]', '[1.0, 0.0, 12.39229965209961, 2.4830000400543213]', '[1.0, 0.0, 12.39229965209961, 2.566999912261963]', '[1.0, 0.0, 12.39229965209961, 2.5]', '[1.0, 0.0, 12.39229965209961, 2.683000087738037]', '[1.0, 0.0, 12.39229965209961, 2.75]', '[1.0, 0.0, 12.39229965209961, 2.933000087738037]', '[1.0, 0.0, 12.39229965209961, 3.0]', '[1.0, 0.0, 12.39229965209961, 3.316999912261963]', '[1.0, 0.0, 12.39229965209961, 3.5]', '[1.0, 0.0, 12.39229965209961, 4.25]', '[1.0, 0.0, 12.392399787902832, 10.25]', '[1.0, 0.0, 12.392399787902832, 4.25]', '[1.0, 0.0, 12.392399787902832, 5.25]', '[1.0, 0.0, 12.392399787902832, 8.25]', '[1.0, 0.0, 12.396100044250488, -0.7519000172615051]', '[1.0, 0.0, 12.401599884033203, -3.389899969100952]', '[1.0, 0.0, 12.412799835205078, -4.466599941253662]', '[1.0, 0.0, 12.412799835205078, 4.556300163269043]', '[1.0, 0.0, 12.426300048828125, 6.599299907684326]', '[1.0, 0.0, 12.445199966430664, -1.2336000204086304]', '[1.0, 0.0, 12.453100204467773, -2.8396999835968018]', '[1.0, 0.0, 12.453100204467773, -3.8396999835968018]', '[1.0, 0.0, </t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="inlineStr"/>
+      <c r="C280" t="inlineStr"/>
+      <c r="D280" t="inlineStr"/>
+      <c r="E280" t="inlineStr"/>
+      <c r="F280" t="inlineStr"/>
+      <c r="G280" t="inlineStr"/>
+      <c r="H280" t="inlineStr"/>
+      <c r="I280" t="inlineStr"/>
+      <c r="J280" t="inlineStr"/>
+      <c r="K280" t="inlineStr"/>
+      <c r="L280" t="inlineStr"/>
+      <c r="M280" t="inlineStr"/>
+      <c r="N280" t="inlineStr">
+        <is>
+          <t>['0', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="inlineStr"/>
+      <c r="C281" t="inlineStr"/>
+      <c r="D281" t="inlineStr"/>
+      <c r="E281" t="inlineStr"/>
+      <c r="F281" t="inlineStr"/>
+      <c r="G281" t="inlineStr"/>
+      <c r="H281" t="inlineStr"/>
+      <c r="I281" t="inlineStr"/>
+      <c r="J281" t="inlineStr"/>
+      <c r="K281" t="inlineStr"/>
+      <c r="L281" t="inlineStr"/>
+      <c r="M281" t="inlineStr"/>
+      <c r="N281" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="inlineStr"/>
+      <c r="C282" t="inlineStr"/>
+      <c r="D282" t="inlineStr"/>
+      <c r="E282" t="inlineStr"/>
+      <c r="F282" t="inlineStr"/>
+      <c r="G282" t="inlineStr"/>
+      <c r="H282" t="inlineStr"/>
+      <c r="I282" t="inlineStr"/>
+      <c r="J282" t="inlineStr"/>
+      <c r="K282" t="inlineStr"/>
+      <c r="L282" t="inlineStr"/>
+      <c r="M282" t="inlineStr"/>
+      <c r="N282" t="inlineStr">
+        <is>
+          <t>[23835  8375   180]</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="inlineStr"/>
+      <c r="C283" t="inlineStr"/>
+      <c r="D283" t="inlineStr"/>
+      <c r="E283" t="inlineStr"/>
+      <c r="F283" t="inlineStr"/>
+      <c r="G283" t="inlineStr"/>
+      <c r="H283" t="inlineStr"/>
+      <c r="I283" t="inlineStr"/>
+      <c r="J283" t="inlineStr"/>
+      <c r="K283" t="inlineStr"/>
+      <c r="L283" t="inlineStr"/>
+      <c r="M283" t="inlineStr"/>
+      <c r="N283" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="inlineStr"/>
+      <c r="C284" t="inlineStr"/>
+      <c r="D284" t="inlineStr"/>
+      <c r="E284" t="inlineStr"/>
+      <c r="F284" t="inlineStr"/>
+      <c r="G284" t="inlineStr"/>
+      <c r="H284" t="inlineStr"/>
+      <c r="I284" t="inlineStr"/>
+      <c r="J284" t="inlineStr"/>
+      <c r="K284" t="inlineStr"/>
+      <c r="L284" t="inlineStr"/>
+      <c r="M284" t="inlineStr"/>
+      <c r="N284" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="inlineStr"/>
+      <c r="C285" t="inlineStr"/>
+      <c r="D285" t="inlineStr"/>
+      <c r="E285" t="inlineStr"/>
+      <c r="F285" t="inlineStr"/>
+      <c r="G285" t="inlineStr"/>
+      <c r="H285" t="inlineStr"/>
+      <c r="I285" t="inlineStr"/>
+      <c r="J285" t="inlineStr"/>
+      <c r="K285" t="inlineStr"/>
+      <c r="L285" t="inlineStr"/>
+      <c r="M285" t="inlineStr"/>
+      <c r="N285" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="inlineStr"/>
+      <c r="C286" t="inlineStr"/>
+      <c r="D286" t="inlineStr"/>
+      <c r="E286" t="inlineStr"/>
+      <c r="F286" t="inlineStr"/>
+      <c r="G286" t="inlineStr"/>
+      <c r="H286" t="inlineStr"/>
+      <c r="I286" t="inlineStr"/>
+      <c r="J286" t="inlineStr"/>
+      <c r="K286" t="inlineStr"/>
+      <c r="L286" t="inlineStr"/>
+      <c r="M286" t="inlineStr"/>
+      <c r="N286" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="B287" t="inlineStr"/>
+      <c r="C287" t="inlineStr"/>
+      <c r="D287" t="inlineStr"/>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="inlineStr"/>
+      <c r="G287" t="inlineStr"/>
+      <c r="H287" t="inlineStr"/>
+      <c r="I287" t="inlineStr"/>
+      <c r="J287" t="inlineStr"/>
+      <c r="K287" t="inlineStr"/>
+      <c r="L287" t="inlineStr"/>
+      <c r="M287" t="inlineStr"/>
+      <c r="N287" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="inlineStr"/>
+      <c r="C288" t="inlineStr"/>
+      <c r="D288" t="inlineStr"/>
+      <c r="E288" t="inlineStr"/>
+      <c r="F288" t="inlineStr"/>
+      <c r="G288" t="inlineStr"/>
+      <c r="H288" t="inlineStr"/>
+      <c r="I288" t="inlineStr"/>
+      <c r="J288" t="inlineStr"/>
+      <c r="K288" t="inlineStr"/>
+      <c r="L288" t="inlineStr"/>
+      <c r="M288" t="inlineStr"/>
+      <c r="N288" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="inlineStr"/>
+      <c r="C289" t="inlineStr"/>
+      <c r="D289" t="inlineStr"/>
+      <c r="E289" t="inlineStr"/>
+      <c r="F289" t="inlineStr"/>
+      <c r="G289" t="inlineStr"/>
+      <c r="H289" t="inlineStr"/>
+      <c r="I289" t="inlineStr"/>
+      <c r="J289" t="inlineStr"/>
+      <c r="K289" t="inlineStr"/>
+      <c r="L289" t="inlineStr"/>
+      <c r="M289" t="inlineStr"/>
+      <c r="N289" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="inlineStr"/>
+      <c r="C290" t="inlineStr"/>
+      <c r="D290" t="inlineStr"/>
+      <c r="E290" t="inlineStr"/>
+      <c r="F290" t="inlineStr"/>
+      <c r="G290" t="inlineStr"/>
+      <c r="H290" t="inlineStr"/>
+      <c r="I290" t="inlineStr"/>
+      <c r="J290" t="inlineStr"/>
+      <c r="K290" t="inlineStr"/>
+      <c r="L290" t="inlineStr"/>
+      <c r="M290" t="inlineStr"/>
+      <c r="N290" t="n">
+        <v>14.55840455840456</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="inlineStr"/>
+      <c r="C291" t="inlineStr"/>
+      <c r="D291" t="inlineStr"/>
+      <c r="E291" t="inlineStr"/>
+      <c r="F291" t="inlineStr"/>
+      <c r="G291" t="inlineStr"/>
+      <c r="H291" t="inlineStr"/>
+      <c r="I291" t="inlineStr"/>
+      <c r="J291" t="inlineStr"/>
+      <c r="K291" t="inlineStr"/>
+      <c r="L291" t="inlineStr"/>
+      <c r="M291" t="inlineStr"/>
+      <c r="N291" t="n">
+        <v>15.002849002849</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="inlineStr"/>
+      <c r="C292" t="inlineStr"/>
+      <c r="D292" t="inlineStr"/>
+      <c r="E292" t="inlineStr"/>
+      <c r="F292" t="inlineStr"/>
+      <c r="G292" t="inlineStr"/>
+      <c r="H292" t="inlineStr"/>
+      <c r="I292" t="inlineStr"/>
+      <c r="J292" t="inlineStr"/>
+      <c r="K292" t="inlineStr"/>
+      <c r="L292" t="inlineStr"/>
+      <c r="M292" t="inlineStr"/>
+      <c r="N292" t="inlineStr">
+        <is>
+          <t>{0: 0.6552706552706553, 1: 0.34472934472934474}</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="inlineStr"/>
+      <c r="C293" t="inlineStr"/>
+      <c r="D293" t="inlineStr"/>
+      <c r="E293" t="inlineStr"/>
+      <c r="F293" t="inlineStr"/>
+      <c r="G293" t="inlineStr"/>
+      <c r="H293" t="inlineStr"/>
+      <c r="I293" t="inlineStr"/>
+      <c r="J293" t="inlineStr"/>
+      <c r="K293" t="inlineStr"/>
+      <c r="L293" t="inlineStr"/>
+      <c r="M293" t="inlineStr"/>
+      <c r="N293" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '2', '3', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="inlineStr"/>
+      <c r="C294" t="inlineStr"/>
+      <c r="D294" t="inlineStr"/>
+      <c r="E294" t="inlineStr"/>
+      <c r="F294" t="inlineStr"/>
+      <c r="G294" t="inlineStr"/>
+      <c r="H294" t="inlineStr"/>
+      <c r="I294" t="inlineStr"/>
+      <c r="J294" t="inlineStr"/>
+      <c r="K294" t="inlineStr"/>
+      <c r="L294" t="inlineStr"/>
+      <c r="M294" t="inlineStr"/>
+      <c r="N294" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="inlineStr"/>
+      <c r="C295" t="inlineStr"/>
+      <c r="D295" t="inlineStr"/>
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="inlineStr"/>
+      <c r="G295" t="inlineStr"/>
+      <c r="H295" t="inlineStr"/>
+      <c r="I295" t="inlineStr"/>
+      <c r="J295" t="inlineStr"/>
+      <c r="K295" t="inlineStr"/>
+      <c r="L295" t="inlineStr"/>
+      <c r="M295" t="inlineStr"/>
+      <c r="N295" t="inlineStr">
+        <is>
+          <t>[   1   23    1    1    2    1    3    1    1    1    1  721  408   29
+ 3493  269  100   44   10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="inlineStr"/>
+      <c r="C296" t="inlineStr"/>
+      <c r="D296" t="inlineStr"/>
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="inlineStr"/>
+      <c r="G296" t="inlineStr"/>
+      <c r="H296" t="inlineStr"/>
+      <c r="I296" t="inlineStr"/>
+      <c r="J296" t="inlineStr"/>
+      <c r="K296" t="inlineStr"/>
+      <c r="L296" t="inlineStr"/>
+      <c r="M296" t="inlineStr"/>
+      <c r="N296" t="inlineStr">
+        <is>
+          <t>[   7  436 2772 2051]</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr"/>
+      <c r="C297" t="inlineStr"/>
+      <c r="D297" t="inlineStr"/>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+      <c r="G297" t="inlineStr"/>
+      <c r="H297" t="inlineStr"/>
+      <c r="I297" t="inlineStr"/>
+      <c r="J297" t="inlineStr"/>
+      <c r="K297" t="inlineStr"/>
+      <c r="L297" t="inlineStr"/>
+      <c r="M297" t="inlineStr"/>
+      <c r="N297" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="inlineStr"/>
+      <c r="C298" t="inlineStr"/>
+      <c r="D298" t="inlineStr"/>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+      <c r="G298" t="inlineStr"/>
+      <c r="H298" t="inlineStr"/>
+      <c r="I298" t="inlineStr"/>
+      <c r="J298" t="inlineStr"/>
+      <c r="K298" t="inlineStr"/>
+      <c r="L298" t="inlineStr"/>
+      <c r="M298" t="inlineStr"/>
+      <c r="N298" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr"/>
+      <c r="C299" t="inlineStr"/>
+      <c r="D299" t="inlineStr"/>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+      <c r="G299" t="inlineStr"/>
+      <c r="H299" t="inlineStr"/>
+      <c r="I299" t="inlineStr"/>
+      <c r="J299" t="inlineStr"/>
+      <c r="K299" t="inlineStr"/>
+      <c r="L299" t="inlineStr"/>
+      <c r="M299" t="inlineStr"/>
+      <c r="N299" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="inlineStr"/>
+      <c r="C300" t="inlineStr"/>
+      <c r="D300" t="inlineStr"/>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+      <c r="G300" t="inlineStr"/>
+      <c r="H300" t="inlineStr"/>
+      <c r="I300" t="inlineStr"/>
+      <c r="J300" t="inlineStr"/>
+      <c r="K300" t="inlineStr"/>
+      <c r="L300" t="inlineStr"/>
+      <c r="M300" t="inlineStr"/>
+      <c r="N300" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="inlineStr"/>
+      <c r="C301" t="inlineStr"/>
+      <c r="D301" t="inlineStr"/>
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+      <c r="G301" t="inlineStr"/>
+      <c r="H301" t="inlineStr"/>
+      <c r="I301" t="inlineStr"/>
+      <c r="J301" t="inlineStr"/>
+      <c r="K301" t="inlineStr"/>
+      <c r="L301" t="inlineStr"/>
+      <c r="M301" t="inlineStr"/>
+      <c r="N301" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="inlineStr"/>
+      <c r="C302" t="inlineStr"/>
+      <c r="D302" t="inlineStr"/>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+      <c r="G302" t="inlineStr"/>
+      <c r="H302" t="inlineStr"/>
+      <c r="I302" t="inlineStr"/>
+      <c r="J302" t="inlineStr"/>
+      <c r="K302" t="inlineStr"/>
+      <c r="L302" t="inlineStr"/>
+      <c r="M302" t="inlineStr"/>
+      <c r="N302" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="inlineStr"/>
+      <c r="C303" t="inlineStr"/>
+      <c r="D303" t="inlineStr"/>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+      <c r="G303" t="inlineStr"/>
+      <c r="H303" t="inlineStr"/>
+      <c r="I303" t="inlineStr"/>
+      <c r="J303" t="inlineStr"/>
+      <c r="K303" t="inlineStr"/>
+      <c r="L303" t="inlineStr"/>
+      <c r="M303" t="inlineStr"/>
+      <c r="N303" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="inlineStr"/>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="inlineStr"/>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+      <c r="G304" t="inlineStr"/>
+      <c r="H304" t="inlineStr"/>
+      <c r="I304" t="inlineStr"/>
+      <c r="J304" t="inlineStr"/>
+      <c r="K304" t="inlineStr"/>
+      <c r="L304" t="inlineStr"/>
+      <c r="M304" t="inlineStr"/>
+      <c r="N304" t="n">
+        <v>14.55840455840456</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="inlineStr"/>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+      <c r="G305" t="inlineStr"/>
+      <c r="H305" t="inlineStr"/>
+      <c r="I305" t="inlineStr"/>
+      <c r="J305" t="inlineStr"/>
+      <c r="K305" t="inlineStr"/>
+      <c r="L305" t="inlineStr"/>
+      <c r="M305" t="inlineStr"/>
+      <c r="N305" t="n">
+        <v>15.002849002849</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="inlineStr"/>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="inlineStr"/>
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
+      <c r="G306" t="inlineStr"/>
+      <c r="H306" t="inlineStr"/>
+      <c r="I306" t="inlineStr"/>
+      <c r="J306" t="inlineStr"/>
+      <c r="K306" t="inlineStr"/>
+      <c r="L306" t="inlineStr"/>
+      <c r="M306" t="inlineStr"/>
+      <c r="N306" t="inlineStr">
+        <is>
+          <t>{0: 0.6552706552706553, 1: 0.34472934472934474}</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="inlineStr"/>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="inlineStr"/>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+      <c r="G307" t="inlineStr"/>
+      <c r="H307" t="inlineStr"/>
+      <c r="I307" t="inlineStr"/>
+      <c r="J307" t="inlineStr"/>
+      <c r="K307" t="inlineStr"/>
+      <c r="L307" t="inlineStr"/>
+      <c r="M307" t="inlineStr"/>
+      <c r="N307" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '2', '3', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="inlineStr"/>
+      <c r="C308" t="inlineStr"/>
+      <c r="D308" t="inlineStr"/>
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+      <c r="G308" t="inlineStr"/>
+      <c r="H308" t="inlineStr"/>
+      <c r="I308" t="inlineStr"/>
+      <c r="J308" t="inlineStr"/>
+      <c r="K308" t="inlineStr"/>
+      <c r="L308" t="inlineStr"/>
+      <c r="M308" t="inlineStr"/>
+      <c r="N308" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="inlineStr"/>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="inlineStr"/>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+      <c r="G309" t="inlineStr"/>
+      <c r="H309" t="inlineStr"/>
+      <c r="I309" t="inlineStr"/>
+      <c r="J309" t="inlineStr"/>
+      <c r="K309" t="inlineStr"/>
+      <c r="L309" t="inlineStr"/>
+      <c r="M309" t="inlineStr"/>
+      <c r="N309" t="inlineStr">
+        <is>
+          <t>[   1   23    1    1    2    1    3    1    1    1    1  721  408   29
+ 3493  269  100   44   10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="inlineStr"/>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="inlineStr"/>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+      <c r="G310" t="inlineStr"/>
+      <c r="H310" t="inlineStr"/>
+      <c r="I310" t="inlineStr"/>
+      <c r="J310" t="inlineStr"/>
+      <c r="K310" t="inlineStr"/>
+      <c r="L310" t="inlineStr"/>
+      <c r="M310" t="inlineStr"/>
+      <c r="N310" t="inlineStr">
+        <is>
+          <t>[   7  436 2772 2051]</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="inlineStr"/>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="inlineStr"/>
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+      <c r="G311" t="inlineStr"/>
+      <c r="H311" t="inlineStr"/>
+      <c r="I311" t="inlineStr"/>
+      <c r="J311" t="inlineStr"/>
+      <c r="K311" t="inlineStr"/>
+      <c r="L311" t="inlineStr"/>
+      <c r="M311" t="inlineStr"/>
+      <c r="N311" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="inlineStr"/>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="inlineStr"/>
+      <c r="E312" t="inlineStr"/>
+      <c r="F312" t="inlineStr"/>
+      <c r="G312" t="inlineStr"/>
+      <c r="H312" t="inlineStr"/>
+      <c r="I312" t="inlineStr"/>
+      <c r="J312" t="inlineStr"/>
+      <c r="K312" t="inlineStr"/>
+      <c r="L312" t="inlineStr"/>
+      <c r="M312" t="inlineStr"/>
+      <c r="N312" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="inlineStr"/>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="inlineStr"/>
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+      <c r="G313" t="inlineStr"/>
+      <c r="H313" t="inlineStr"/>
+      <c r="I313" t="inlineStr"/>
+      <c r="J313" t="inlineStr"/>
+      <c r="K313" t="inlineStr"/>
+      <c r="L313" t="inlineStr"/>
+      <c r="M313" t="inlineStr"/>
+      <c r="N313" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="inlineStr"/>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="inlineStr"/>
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+      <c r="G314" t="inlineStr"/>
+      <c r="H314" t="inlineStr"/>
+      <c r="I314" t="inlineStr"/>
+      <c r="J314" t="inlineStr"/>
+      <c r="K314" t="inlineStr"/>
+      <c r="L314" t="inlineStr"/>
+      <c r="M314" t="inlineStr"/>
+      <c r="N314" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="inlineStr"/>
+      <c r="C315" t="inlineStr"/>
+      <c r="D315" t="inlineStr"/>
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="inlineStr"/>
+      <c r="G315" t="inlineStr"/>
+      <c r="H315" t="inlineStr"/>
+      <c r="I315" t="inlineStr"/>
+      <c r="J315" t="inlineStr"/>
+      <c r="K315" t="inlineStr"/>
+      <c r="L315" t="inlineStr"/>
+      <c r="M315" t="inlineStr"/>
+      <c r="N315" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="inlineStr"/>
+      <c r="C316" t="inlineStr"/>
+      <c r="D316" t="inlineStr"/>
+      <c r="E316" t="inlineStr"/>
+      <c r="F316" t="inlineStr"/>
+      <c r="G316" t="inlineStr"/>
+      <c r="H316" t="inlineStr"/>
+      <c r="I316" t="inlineStr"/>
+      <c r="J316" t="inlineStr"/>
+      <c r="K316" t="inlineStr"/>
+      <c r="L316" t="inlineStr"/>
+      <c r="M316" t="inlineStr"/>
+      <c r="N316" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="B317" t="inlineStr"/>
+      <c r="C317" t="inlineStr"/>
+      <c r="D317" t="inlineStr"/>
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="inlineStr"/>
+      <c r="G317" t="inlineStr"/>
+      <c r="H317" t="inlineStr"/>
+      <c r="I317" t="inlineStr"/>
+      <c r="J317" t="inlineStr"/>
+      <c r="K317" t="inlineStr"/>
+      <c r="L317" t="inlineStr"/>
+      <c r="M317" t="inlineStr"/>
+      <c r="N317" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="B318" t="inlineStr"/>
+      <c r="C318" t="inlineStr"/>
+      <c r="D318" t="inlineStr"/>
+      <c r="E318" t="inlineStr"/>
+      <c r="F318" t="inlineStr"/>
+      <c r="G318" t="inlineStr"/>
+      <c r="H318" t="inlineStr"/>
+      <c r="I318" t="inlineStr"/>
+      <c r="J318" t="inlineStr"/>
+      <c r="K318" t="inlineStr"/>
+      <c r="L318" t="inlineStr"/>
+      <c r="M318" t="inlineStr"/>
+      <c r="N318" t="n">
+        <v>32.63333333333333</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="B319" t="inlineStr"/>
+      <c r="C319" t="inlineStr"/>
+      <c r="D319" t="inlineStr"/>
+      <c r="E319" t="inlineStr"/>
+      <c r="F319" t="inlineStr"/>
+      <c r="G319" t="inlineStr"/>
+      <c r="H319" t="inlineStr"/>
+      <c r="I319" t="inlineStr"/>
+      <c r="J319" t="inlineStr"/>
+      <c r="K319" t="inlineStr"/>
+      <c r="L319" t="inlineStr"/>
+      <c r="M319" t="inlineStr"/>
+      <c r="N319" t="n">
+        <v>62.13666666666666</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="B320" t="inlineStr"/>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="inlineStr"/>
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="inlineStr"/>
+      <c r="G320" t="inlineStr"/>
+      <c r="H320" t="inlineStr"/>
+      <c r="I320" t="inlineStr"/>
+      <c r="J320" t="inlineStr"/>
+      <c r="K320" t="inlineStr"/>
+      <c r="L320" t="inlineStr"/>
+      <c r="M320" t="inlineStr"/>
+      <c r="N320" t="inlineStr">
+        <is>
+          <t>{0: 0.8333333333333334, 1: 0.16666666666666666}</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="B321" t="inlineStr"/>
+      <c r="C321" t="inlineStr"/>
+      <c r="D321" t="inlineStr"/>
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="inlineStr"/>
+      <c r="G321" t="inlineStr"/>
+      <c r="H321" t="inlineStr"/>
+      <c r="I321" t="inlineStr"/>
+      <c r="J321" t="inlineStr"/>
+      <c r="K321" t="inlineStr"/>
+      <c r="L321" t="inlineStr"/>
+      <c r="M321" t="inlineStr"/>
+      <c r="N321" t="inlineStr">
+        <is>
+          <t>['[-149.0, 6.973113, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.9733, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.973318, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.973461, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.973644, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011002, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011396, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011633, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011736, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.012369, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-5.0, 11.366548, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[-5.0, 11.423346, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[-5.0, 11.429201, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[-5.0, 11.477434, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[1.0, 0.0, 0.0, -0.8, 0.0, 9.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0]', '[1.0, 0.0, 1.6, -0.97, 0.062, 9.2, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0]', '[1.0, 0.0, 3.95, -1.1, 0.18, 10.5, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0]', '[1.0, 0.0, 4.0, 1.81, 0.186, 5.2, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0]', '[10.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 0.0, 22.05, -1.77, 0.988, 84.1, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 0.0, 23.84, 0.53, 1.089, 78.8, 6.0, 2.0, 2.0, 1.0, 5.0, 4.0, 4.0, 5.0, 1.0, 6.0, 2.0, 2.0]', '[10.0, 0.0, 25.5, 3.68, 1.166, 73.0, 4.0, 6.0, 0.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 3.0, 7.0, 0.0]', '[10.0, 0.0, 29.13, -0.5, 1.313, 85.2, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 0.0, 29.3, -1.99, 1.314, 83.4, 6.0, 2.0, 2.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 6.0, 2.0, 2.0]', '[10.0, 0.0, 29.52, 0.61, 1.322, 87.1, 5.0, 3.0, 2.0, 3.0, 5.0, 2.0, 3.0, 4.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 0.0, 29.53, 1.43, 1.344, 81.3, 5.0, 4.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 5.0, 1.0]', '[10.0, 0.0, 30.88, -0.53, 1.367, 87.5, 4.0, 5.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 5.0, 1.0]', '[10.0, 0.0, 31.2, -2.9, 1.413, 88.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 0.0, 31.2, 7.29, 1.464, 66.8, 2.0, 6.0, 2.0, 1.0, 2.0, 7.0, 7.0, 2.0, 1.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 31.23, -2.02, 1.403, 94.7, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 32.71, 2.58, 1.518, 75.4, 4.0, 4.0, 2.0, 1.0, 5.0, 4.0, 5.0, 3.0, 2.0, 3.0, 5.0, 2.0]', '[10.0, 0.0, 33.19, 4.2, 1.559, 70.7, 4.0, 3.0, 3.0, 0.0, 5.0, 5.0, 6.0, 3.0, 1.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 33.29, 3.11, 1.541, 78.1, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 33.61, -0.17, 1.535, 83.2, 4.0, 4.0, 2.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 5.0, 2.0]', '[10.0, 0.0, 33.97, -1.74, 1.525, 87.4, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 0.0, 34.72, 2.93, 1.601, 75.9, 4.0, 5.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 2.0, 7.0, 1.0]', '[10.0, 0.0, 35.54, 0.13, 1.618, 86.5, 2.0, 5.0, 3.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 2.0, 5.0, 3.0]', '[10.0, 0.0, 36.07, -0.53, 1.652, 87.3, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0, 3.0, 4.0, 3.0, 4.0, 2.0, 4.0]', '[10.0, 0.0, 36.19, -2.3, 1.609, 94.7, 2.0, 6.0, 2.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 36.7, -2.99, 1.67, 94.0, 3.0, 6.0, 1.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 2.0, 7.0, 1.0]', '[10.0, 0.0, 36.73, 0.24, 1.643, 86.7, 2.0, 5.0, 3.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 2.0, 5.0, 3.0]', '[10.0, 0.0, 36.74, -1.34, 1.687, 92.4, 4.0, 2.0, 4.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0]', '[10.0, 0.0, 37.12, 2.48, 1.694, 87.5, 2.0, 5.0, 3.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 0.0, 37.53, 1.45, 1.765, 78.7, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 37.77, 0.58, 1.714, 87.6, 2.0, 6.0, 2.0, 5.0, 2.0, 3.0, 3.0, 2.0, 5.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 38.67, -2.74, 1.719, 93.8, 3.0, 4.0, 3.0, 5.0, 4.0, 1.0, 2.0, 3.0, 5.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 39.22, 5.58, 1.789, 73.2, 1.0, 7.0, 2.0, 3.0, 0.0, 7.0, 7.0, 0.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 0.0, 39.35, 4.07, 1.812, 74.5, 1.0, 7.0, 2.0, 3.0, 1.0, 6.0, 6.0, 1.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 0.0, 39.91, -1.04, 1.788, 87.7, 2.0, 6.0, 2.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 41.3, 1.02, 1.938, 81.9, 2.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 2.0, 4.0, 4.0]', '[10.0, 0.0, 43.36, 4.45, 2.042, 77.7, 1.0, 5.0, 4.0, 3.0, 2.0, 5.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 0.0, 44.68, -0.39, 2.062, 90.5, 2.0, 3.0, 5.0, 4.0, 4.0, 2.0, 3.0, 2.0, 5.0, 2.0, 3.0, 5.0]', '[10.0, 0.0, 45.79, -1.29, 2.115, 94.1, 1.0, 3.0, 6.0, 6.0, 2.0, 2.0, 3.0, 1.0, 6.0, 1.0, 3.0, 6.0]', '[10.0, 0.0, 47.26, 5.56, 2.292, 76.7, 1.0, 3.0, 6.0, 2.0, 3.0, 5.0, 5.0, 1.0, 4.0, 1.0, 3.0, 6.0]', '[10.0, 0.0, 53.73, 7.47, 2.59, 73.9, 0.0, 3.0, 7.0, 2.0, 3.0, 5.0, 6.0, 0.0, 4.0, 0.0, 3.0, 7.0]', '[10.0, 0.0, 55.62, 7.01, 2.694, 73.9, 0.0, 2.0, 8.0, 2.0, 3.0, 5.0, 6.0, 0.0, 4.0, 0.0, 2.0, 8.0]', '[10.0, 12.231122, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 12.602876, 32.51, -1.03, 1.49, 85.4, 5.0, 2.0, 3.0, 2.0, 5.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 12.636695, 32.51, -1.03, 1.49, 85.4, 5.0, 2.0, 3.0, 2.0, 5.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 12.825064, 32.09, -2.33, 1.434, 86.8, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 12.831107, 21.16, -0.3, 0.922, 84.9, 6.0, 4.0, 0.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 6.0, 4.0, 0.0]', '[10.0, 12.833985, 21.16, -0.3, 0.922, 84.9, 6.0, 4.0, 0.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 6.0, 4.0, 0.0]', '[10.0, 12.862465, 25.38, -2.42, 1.079, 84.3, 8.0, 2.0, 0.0, 1.0, 7.0, 2.0, 2.0, 7.0, 1.0, 8.0, 2.0, 0.0]', '[10.0, 12.866284, 41.67, -1.3, 1.889, 93.7, 1.0, 5.0, 4.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 1.0, 5.0, 4.0]', '[10.0, 12.875708, 33.53, 4.6, 1.539, 75.9, 4.0, 4.0, 2.0, 1.0, 4.0, 5.0, 5.0, 3.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 12.894289, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.002887, 35.55, -0.88, 1.588, 84.9, 3.0, 6.0, 1.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.003345, 35.55, -0.88, 1.588, 84.9, 3.0, 6.0, 1.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.011763, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.076318, 25.61, -2.15, 1.16, 86.8, 6.0, 3.0, 1.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 6.0, 3.0, 1.0]', '[10.0, 13.165224, 32.09, -2.33, 1.434, 86.8, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 13.2302, 41.41, 4.77, 1.924, 67.3, 3.0, 4.0, 3.0, 1.0, 4.0, 5.0, 6.0, 3.0, 1.0, 2.0, 5.0, 3.0]', '[10.0, 13.2564, 22.05, -1.77, 0.988, 84.1, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.256543, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.300899, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.301272, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.301789, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.301918, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.30215, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.422756, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 13.427407, 22.05, -1.77, 0.988, 84.1, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.432258, 39.3, 1.68, 1.794, 87.0, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.48406, 39.3, 1.68, 1.794, 87.0, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.509898, 45.5, -2.5, 2.061, 100.7, 2.0, 2.0, 6.0, 7.0, 2.0, 1.0, 2.0, 1.0, 7.0, 2.0, 2.0, 6.0]', '[10.0, 13.523679, 28.45, -3.28, 1.28, 90.4, 7.0, 2.0, 1.0, 3.0, 6.0, 1.0, 1.0, 6.0, 3.0, 4.0, 5.0, 1.0]', '[10.0, 13.536176, 40.66, 0.61, 1.843, 89.0, 1.0, 5.0, 4.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 1.0, 5.0, 4.0]', '[10.0, 13.544919, 31.67, 2.27, 1.459, 77.3, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.554057, 35.82, -4.45, 1.568, 99.4, 4.0, 4.0, 2.0, 5.0, 3.0, 2.0, 2.0, 2.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.573598, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.625075, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.635057, 34.84, -1.07, 1.602, 88.6, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 13.635601, 33.39, -5.98, 1.453, 101.9, 4.0, 4.0, 2.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.636476, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.641503, 33.12, -0.96, 1.517, 88.7, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 13.656127, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.656542, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.667926, 39.33, -4.2, 1.754, 98.2, 2.0, 5.0, 3.0, 6.0, 3.0, 1.0, 2.0, 2.0, 6.0, 2.0, 5.0, 3.0]', '[10.0, 13.674337, 33.59, 1.6, 1.535, 85.8, 3.0, 5.0, 2.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.679361, 40.32, -3.73, 1.842, 98.6, 4.0, 1.0, 5.0, 6.0, 4.0, 0.0, 1.0, 3.0, 6.0, 3.0, 2.0, 5.0]', '[10.0, 13.691627, 34.25, 1.48, 1.52, 82.6, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 13.696875, 35.26, -3.31, 1.58, 96.1, 4.0, 4.0, 2.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.705323, 34.84, -1.07, 1.602, 88.6, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 13.709828, 21.11, -1.54, 0.965, 85.9, 5.0, 5.0, 0.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 6.0, 0.0]', '[10.0, 13.711534, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.718501, 44.37, 1.27, 2.036, 84.9, 2.0, 3.0, 5.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.721821, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.728899, 31.2, -2.9, 1.413, 88.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.729721, 34.13, 2.27, 1.546, 78.6, 3.0, 6.0, 1.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 7.0, 1.0]', '[10.0, 13.74546, 33.39, -5.98, 1.453, 101.9, 4.0, 4.0, 2.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.747208, 33.12, -2.62, 1.505, 89.1, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 13.764486, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.783585, 34.13, 2.27, 1.546, 78.6, 3.0, 6.0, 1.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 7.0, 1.0]', '[10.0, 13.79329, 31.2, -2.9, 1.413, 88.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.796657, 38.4, -1.71, 1.793, 89.2, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 13.809725, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.835076, 38.19, 4.14, 1.803, 79.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 3.0, 3.0, 4.0]', '[10.0, 13.840067, 39.61, 0.22, 1.803, 88.4, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.848726, 23.99, -0.22, 1.087, 87.3, 5.0, 4.0, 1.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 4.0, 1.0]', '[10.0, 13.849965, 38.19, 4.14, 1.803, 79.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 3.0, 3.0, 4.0]', '[10.0, 13.85373, 37.04, 5.76, 1.709, 75.9, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 13.864258, 21.11, -1.54, 0.965, 85.9, 5.0, 5.0, 0.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 6.0, 0.0]', '[10.0, 13.865242, 39.62, -3.15, 1.812, 94.1, 3.0, 4.0, 3.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 2.0, 5.0, 3.0]', '[10.0, 13.866588, 40.62, 1.81, 1.908, 82.9, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.868733, 29.89, 3.33, 1.4, 72.4, 6.0, 3.0, 1.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 13.870766, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.871456, 33.91, 0.1, 1.511, 85.7, 4.0, 5.0, 1.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.87348, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.878806, 38.65, 4.6, 1.869, 72.7, 3.0, 3.0, 4.0, 3.0, 1.0, 6.0, 7.0, 0.0, 3.0, 0.0, 6.0, 4.0]', '[10.0, 13.898501, 32.2, 0.64, 1.482, 81.3, 5.0, 3.0, 2.0, 2.0, 4.0, 4.0, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 13.899586, 32.95, -2.66, 1.476, 90.9, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 13.903127, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.913788, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.923096, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 13.923403, 29.89, 3.33, 1.4, 72.4, 6.0, 3.0, 1.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 13.928315, 37.18, 1.61, 1.733, 79.1, 2.0, 3.0, 4.0, 4.0, 2.0, 3.0, 3.0, 1.0, 5.0, 2.0, 3.0, 4.0]', '[10.0, 13.944123, 33.87, 3.87, 1.587, 78.6, 2.0, 5.0, 3.0, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0, 2.0, 5.0, 3.0]', '[10.0, 13.944978, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 13.946486, 40.62, 1.81, 1.908, 82.9, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.949725, 34.25, 1.48, 1.52, 82.6, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 13.952652, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 13.952741, 39.61, 0.22, 1.803, 88.4, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.959268, 28.5, -5.52, 1.22, 97.1, 6.0, 2.0, 2.0, 4.0, 5.0, 1.0, 1.0, 5.0, 4.0, 6.0, 2.0, 2.0]', '[10.0, 13.965471, 41.12, 0.63, 1.828, 94.7, 1.0, 5.0, 4.0, 6.0, 1.0, 3.0, 4.0, 0.0, 6.0, 1.0, 5.0, 4.0]', '[10.0, 13.966332, 45.61, 1.22, 2.12, 86.1, 2.0, 3.0, 5.0, 4.0, 4.0, 2.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.968701, 18.28, -1.94, 0.803, 88.0, 7.0, 3.0, 0.0, 2.0, 7.0, 1.0, 1.0, 7.0, 2.0, 6.0, 4.0, 0.0]', '[10.0, 13.968908, 36.63, 3.8, 1.736, 74.7, 3.0, 4.0, 3.0, 2.0, 4.0, 4.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.969321, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.971485, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.973165, 29.89, 3.33, 1.4, 72.4, 6.0, 3.0, 1.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 13.97335, 35.03, 1.28, 1.57, 85.4, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.98024, 31.67, 2.27, 1.459, 77.3, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.981382, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 13.991016, 40.65, 4.39, 1.918, 77.8, 2.0, 4.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 4.0, 4.0]', '[10.0, 13.993335, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 13.996099, 25.91, 1.81, 1.184, 79.2, 5.0, 4.0, 1.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.998617, 41.82, 2.7, 1.942, 82.8, 1.0, 5.0, 4.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 13.99883, 32.81, 0.28, 1.497, 86.7, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.000609, 37.04, 5.76, 1.709, 75.9, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 14.000667, 36.47, 1.28, 1.637, 84.8, 2.0, 6.0, 2.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 2.0, 6.0, 2.0]', '[10.0, 14.001177, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 14.003231, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.004918, 38.4, -1.71, 1.793, 89.2, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 14.006487, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.009073, 30.07, 3.06, 1.397, 76.8, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.009584, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.010435, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 14.019653, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.020818, 27.42, -1.31, 1.213, 89.7, 6.0, 2.0, 2.0, 3.0, 5.0, 2.0, 2.0, 5.0, 3.0, 6.0, 2.0, 2.0]', '[10.0, 14.024644, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.025478, 34.0, 2.5, 1.552, 81.4, 4.0, 4.0, 2.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 5.0, 2.0]', '[10.0, 14.028098, 23.4, 0.91, 1.06, 78.2, 4.0, 5.0, 0.0, 3.0, 4.0, 2.0, 2.0, 4.0, 3.0, 3.0, 6.0, 0.0]', '[10.0, 14.030268, 32.81, 0.28, 1.497, 86.7, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.030828, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.031948, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 14.032445, 30.63, 3.1, 1.411, 75.6, 3.0, 6.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 2.0, 7.0, 1.0]', '[10.0, 14.037899, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.038204, 39.54, 0.18, 1.809, 87.5, 3.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0]', '[10.0, 14.0384, 23.4, 0.91, 1.06, 78.2, 4.0, 5.0, 0.0, 3.0, 4.0, 2.0, 2.0, 4.0, 3.0, 3.0, 6.0, 0.0]', '[10.0, 14.038975, 34.79, 0.74, 1.638, 87.9, 2.0, 5.0, 3.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 1.0, 6.0, 3.0]', '[10.0, 14.041416, 44.9, 3.87, 2.079, 80.0, 1.0, 6.0, 3.0, 4.0, 1.0, 5.0, 6.0, 0.0, 4.0, 1.0, 6.0, 3.0]', '[10.0, 14.042293, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.043569, 35.3, 4.32, 1.704, 74.8, 4.0, 3.0, 3.0, 1.0, 5.0, 4.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.046, 39.62, -3.15, 1.812, 94.1, 3.0, 4.0, 3.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 2.0, 5.0, 3.0]', '[10.0, 14.049706, 38.59, 1.46, 1.761, 82.4, 1.0, 7.0, 2.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 7.0, 2.0]', '[10.0, 14.049902, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.055429, 36.58, -2.36, 1.676, 94.8, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0]', '[10.0, 14.057396, 32.98, -2.03, 1.493, 87.4, 4.0, 5.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.059718, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.068825, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.069587, 34.71, 1.25, 1.579, 87.4, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.069694, 34.02, 0.58, 1.604, 84.1, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 14.069977, 42.87, -2.32, 2.014, 95.3, 1.0, 4.0, 5.0, 6.0, 2.0, 2.0, 2.0, 1.0, 7.0, 1.0, 4.0, 5.0]', '[10.0, 14.071734, 34.02, 0.58, 1.604, 84.1, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 14.073797, 38.29, 3.96, 1.739, 79.0, 2.0, 6.0, 2.0, 3.0, 3.0, 4.0, 5.0, 2.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 14.074481, 33.12, -2.62, 1.505, 89.1, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 14.079386, 34.02, 0.58, 1.604, 84.1, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 14.082984, 38.59, 1.46, 1.761, 82.4, 1.0, 7.0, 2.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 7.0, 2.0]', '[10.0, 14.093163, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.093235, 33.09, 1.89, 1.541, 77.8, 4.0, 3.0, 3.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.095173, 39.54, 0.18, 1.809, 87.5, 3.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0]', '[10.0, 14.099388, 37.54, 1.8, 1.729, 81.8, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 14.103475, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.105171, 30.07, 3.06, 1.397, 76.8, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.106567, 35.03, 1.28, 1.57, 85.4, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 14.107534, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.1079, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.108442, 46.62, -0.26, 2.135, 88.6, 0.0, 6.0, 4.0, 6.0, 1.0, 3.0, 4.0, 0.0, 6.0, 0.0, 6.0, 4.0]', '[10.0, 14.109158, 40.77, 1.29, 1.85, 85.5, 0.0, 8.0, 2.0, 5.0, 1.0, 4.0, 5.0, 0.0, 5.0, 0.0, 8.0, 2.0]', '[10.0, 14.109771, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.110333, 41.82, 2.7, 1.942, 82.8, 1.0, 5.0, 4.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 14.113433, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.114399, 32.78, -1.19, 1.501, 85.2, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 14.114652, 41.82, 2.7, 1.942, 82.8, 1.0, 5.0, 4.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 14.119208, 31.67, 2.27, 1.459, 77.3, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.121864, 40.32, -3.73, 1.842, 98.6, 4.0, 1.0, 5.0, 6.0, 4.0, 0.0, 1.0, 3.0, 6.0, 3.0, 2.0, 5.0]', '[10.0, 14.129521, 33.12, -2.62, 1.505, 89.1, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 14.133211, 37.54, 1.8, 1.729, 81.8, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 14.136464, 38.4, -1.71, 1.793, 89.2, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 14.136483, 34.27, -1.09, 1.564, 90.6, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 14.137226, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.137248, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.139355, 13.76, -2.79, 0.566, 49.0, 3.0, 2.0, 0.0, 2.0, 2.0, 1.0, 1.0, 2.0, 2.0, 3.0, 2.0, 0.0]', '[10.0, 14.139792, 32.78, -1.19, 1.501, 85.2, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 14.140756, 42.87, -2.32, 2.014, 95.3, 1.0, 4.0, 5.0, 6.0, 2.0, 2.0, 2.0, 1.0, 7.0, 1.0, 4.0, 5.0]', '[10.0, 14.143339, 31.67, -3.01, 1.423, 89.1, 4.0, 5.0, 1.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.145168, 33.06, 0.57, 1.512, 84.8, 3.0, 5.0, 2.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 14.1461, 30.07, 3.06, 1.397, 76.8, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.146968, 32.92, 2.55, 1.504, 74.7, 3.0, 6.0, 1.0, 2.0, 4.0, 4.0, 5.0, 3.0, 2.0, 2.0, 7.0, 1.0]', '[10.0, 14.148196, 42.15, -1.86, 1.903, 88.6, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 2.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 14.148559, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.150026, 37.01, -0.09, 1.66, 88.2, 3.0, 5.0, 2.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 3.0, 5.0, 2.0]', '[10.0, 14.152457, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.152708, 34.69, 5.44, 1.639, 71.9, 3.0, 4.0, 3.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.152807, 34.69, 5.44, 1.639, 71.9, 3.0, 4.0, 3.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.15318, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.157504, 38.98, 2.84, 1.793, 83.1, 3.0, 5.0, 2.0, 4.0, 1.0, 5.0, 5.0, 1.0, 4.0, 2.0, 6.0, 2.0]', '[10.0, 14.159579, 36.58, -2.36, 1.676, 94.8, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0]', '[10.0, 14.159942, 32.58, -4.17, 1.49, 89.6, 5.0, 1.0, 3.0, 4.0, 4.0, 1.0, 1.0, 3.0, 5.0, 5.0, 1.0, 3.0]', '[10.0, 14.163594, 37.04, 5.76, 1.709, 75.9, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 14.165008, 30.36, -1.56, 1.368, 88.7, 4.0, 5.0, 1.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.168352, 31.41, 1.75, 1.422, 81.8, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 14.170017, 36.93, 3.16, 1.68, 78.5, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 5.0, 2.0, 3.0, 3.0, 5.0, 2.0]', '[10.0, 14.171338, 39.54, 0.18, 1.809, 87.5, 3.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0]', '[10.0, 14.171887, 36.67, 1.21, 1.688, 86.7, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.176259, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 14.179652, 28.08, -0.39, 1.263, 82.8, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 14.179842, 43.6, 0.63, 1.987, 88.6, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 4.0, 1.0, 5.0, 1.0, 4.0, 5.0]', '[10.0, 14.180959, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.182482, 40.62, 1.81, 1.908, 82.9, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 14.184709, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.186073, 34.71, 1.25, 1.579, 87.4, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.187119, 36.53, -0.63, 1.641, 90.3, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0, 3.0, 3.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.18831, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.19365, 32.56, -1.43, 1.448, 90.1, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 2.0, 7.0, 1.0]', '[10.0, 14.194487, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.196987, 43.55, 2.8, 1.986, 77.4, 3.0, 4.0, 3.0, 2.0, 5.0, 3.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.201266, 25.59, 0.76, 1.162, 78.6, 6.0, 3.0, 1.0, 1.0, 5.0, 4.0, 4.0, 5.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 14.201822, 13.76, -2.79, 0.566, 49.0, 3.0, 2.0, 0.0, 2.0, 2.0, 1.0, 1.0, 2.0, 2.0, 3.0, 2.0, 0.0]', '[10.0, 14.203003, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.203758, 38.65, 4.6, 1.869, 72.7, 3.0, 3.0, 4.0, 3.0, 1.0, 6.0, 7.0, 0.0, 3.0, 0.0, 6.0, 4.0]', '[10.0, 14.205182, 28.08, -0.39, 1.263, 82.8, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 14.205329, 32.54, 0.73, 1.511, 75.0, 3.0, 4.0, 2.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 4.0, 2.0]', '[10.0, 14.205691, 38.44, -1.2, 1.647, 95.3, 4.0, 4.0, 2.0, 5.0, 3.0, 2.0, 4.0, 1.0, 5.0, 4.0, 4.0, 2.0]', '[10.0, 14.205761, 32.65, -3.89, 1.463, 91.9, 3.0, 6.0, 1.0, 5.0, 4.0, 1.0, 2.0, 3.0, 5.0, 3.0, 6.0, 1.0]', '[10.0, 14.206644, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.20914, 29.6, -1.33, 1.371, 90.0, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.21102, 31.71, 1.02, 1.471, 78.5, 4.0, 3.0, 3.0, 1.0, 6.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0]', '[10.0, 14.211214, 40.65, 4.39, 1.918, 77.8, 2.0, 4.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 4.0, 4.0]', '[10.0, 14.21542, 34.69, 5.44, 1.639, 71.9, 3.0, 4.0, 3.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.216608, 32.47, -0.0, 1.458, 84.4, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 14.216707, 35.93, -1.62, 1.628, 92.1, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 2.0, 5.0, 4.0, 3.0, 3.0]', '[10.0, 14.220979, 36.53, -0.63, 1.641, 90.3, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0, 3.0, 3.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.223986, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.226548, 33.09, 1.89, 1.541, 77.8, 4.0, 3.0, 3.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.232534, 46.62, -0.26, 2.135, 88.6, 0.0, 6.0, 4.0, 6.0, 1.0, 3.0, 4.0, 0.0, 6.0, 0.0, 6.0, 4.0]', '[10.0, 14.233028, 21.36, -1.59, 0.96, 87.1, 8.0, 1.0, 1.0, 1.0, 8.0, 1.0, 1.0, 7.0, 2.0, 7.0, 2.0, 1.0]', '[10.0, 14.233681, 37.71, -1.24, 1.706, 96.9, 4.0, 4.0, 2.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 3.0, 5.0, 2.0]', '[10.0, 14.233716, 33.07, 1.42, 1.552, 74.8, 5.0, 2.0, 3.0, 1.0, 6.0, 3.0, 4.0, 5.0, 1.0, 3.0, 4.0, 3.0]', '[10.0, 14.233938, 37.54, 1.8, 1.729, 81.8, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 14.23473, 43.85, -2.39, 2.021, 91.3, 2.0, 4.0, 4.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 2.0, 4.0, 4.0]', '[10.0, 14.235544, 28.08, -0.39, 1.263, 82.8, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 14.237524, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 14.24404, 38.29, 3.96, 1.739, 79.0, 2.0, 6.0, 2.0, 3.0, 3.0, 4.0, 5.0, 2.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 14.244555, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.244813, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.245194, 38.51, 2.37, 1.815, 80.5, 3.0, 2.0, 5.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 1.0, 4.0, 5.0]', '[10.0, 14.245522, 39.54, 2.97, 1.84, 86.8, 2.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 1.0, 5.0, 4.0]', '[10.0, 14.245532, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.246739, 39.54, 2.97, 1.84, 86.8, 2.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 1.0, 5.0, 4.0]', '[10.0, 14.248511, 30.77, 2.54, 1.389, 79.0, 6.0, 3.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.253366, 40.11, -0.56, 1.888, 87.8, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0, 4.0, 1.0, 5.0, 1.0, 4.0, 5.0]', '[10.0, 14.253503, 37.27, 0.59, 1.7, 88.0, 3.0, 4.0, 3.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 3.0, 4.0, 3.0]', '[10.0, 14.25433, 44.9, 3.87, 2.079, 80.0, 1.0, 6.0, 3.0, 4.0, 1.0, 5.0, 6.0, 0.0, 4.0, 1.0, 6.0, 3.0]', '[10.0, 14.254751, 35.71, 0.98, 1.599, 86.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 4.0, 4.0, 2.0]', '[10.0, 14.25688, 31.41, 1.75, 1.422, 81.8, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 14.257303, 29.6, -1.33, 1.371, 90.0, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.259783, 27.32, 1.1, 1.241, 83.3, 4.0, 4.0, 2.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 14.26067, 39.73, 4.97, 1.891, 74.8, 3.0, 3.0, 4.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 2.0, 4.0, 4.0]', '[10.0, 14.260986, 33.73, -1.1, 1.563, 78.0, 4.0, 2.0, 3.0, 3.0, 4.0, 2.0, 2.0, 4.0, 3.0, 4.0, 2.0, 3.0]', '[10.0, 14.264573, 36.66, 1.45, 1.733, 82.9, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 1.0, 6.0, 3.0]', '[10.0, 14.265572, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 14.266937, 43.6, 1.93, 1.971, 86.9, 3.0, 3.0, 4.0, 5.0, 1.0, 4.0, 5.0, 0.0, 5.0, 3.0, 3.0, 4.0]', '[10.0, 14.270904, 49.33, 2.01, 2.267, 88.3, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0, 5.0, 0.0, 5.0, 2.0, 3.0, 5.0]', '[10.0, 14.27145, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 14.271929, 38.66, 0.58, 1.782, 87.4, 2.0, 5.0, 3.0, 4.0, 3.0, 3.0, 3.0, 2.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 14.274005, 38.66, 0.58, 1.782, 87.4, 2.0, 5.0, 3.0, 4.0, 3.0, 3.0, 3.0, 2.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 14.275044, 40.97, -0.12, 1.877, 89.7, 1.0, 6.0, 3.0, 6.0, 0.0, 4.0, 4.0, 0.0, 6.0, 0.0, 7.0, 3.0]', '[10.0, 14.276442, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.2767, 27.28, 0.02, 1.25, 72.8, 4.0, 3.0, 2.0, 1.0, 6.0, 2.0, 3.0, 4.0, 2.0, 4.0, 3.0, 2.0]', '[10.0, 14.28106, 33.38, 1.22, 1.564, 75.9, 5.0, 1.0, 4.0, 1.0, 6.0, 3.0, 4.0, 5.0, 1.0, 4.0, 2.0, 4.0]', '[10.0, 14.281342, 38.66, 0.58, 1.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B322" t="inlineStr"/>
+      <c r="C322" t="inlineStr"/>
+      <c r="D322" t="inlineStr"/>
+      <c r="E322" t="inlineStr"/>
+      <c r="F322" t="inlineStr"/>
+      <c r="G322" t="inlineStr"/>
+      <c r="H322" t="inlineStr"/>
+      <c r="I322" t="inlineStr"/>
+      <c r="J322" t="inlineStr"/>
+      <c r="K322" t="inlineStr"/>
+      <c r="L322" t="inlineStr"/>
+      <c r="M322" t="inlineStr"/>
+      <c r="N322" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B323" t="inlineStr"/>
+      <c r="C323" t="inlineStr"/>
+      <c r="D323" t="inlineStr"/>
+      <c r="E323" t="inlineStr"/>
+      <c r="F323" t="inlineStr"/>
+      <c r="G323" t="inlineStr"/>
+      <c r="H323" t="inlineStr"/>
+      <c r="I323" t="inlineStr"/>
+      <c r="J323" t="inlineStr"/>
+      <c r="K323" t="inlineStr"/>
+      <c r="L323" t="inlineStr"/>
+      <c r="M323" t="inlineStr"/>
+      <c r="N323" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="B324" t="inlineStr"/>
+      <c r="C324" t="inlineStr"/>
+      <c r="D324" t="inlineStr"/>
+      <c r="E324" t="inlineStr"/>
+      <c r="F324" t="inlineStr"/>
+      <c r="G324" t="inlineStr"/>
+      <c r="H324" t="inlineStr"/>
+      <c r="I324" t="inlineStr"/>
+      <c r="J324" t="inlineStr"/>
+      <c r="K324" t="inlineStr"/>
+      <c r="L324" t="inlineStr"/>
+      <c r="M324" t="inlineStr"/>
+      <c r="N324" t="inlineStr">
+        <is>
+          <t>[37282]</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="B325" t="inlineStr"/>
+      <c r="C325" t="inlineStr"/>
+      <c r="D325" t="inlineStr"/>
+      <c r="E325" t="inlineStr"/>
+      <c r="F325" t="inlineStr"/>
+      <c r="G325" t="inlineStr"/>
+      <c r="H325" t="inlineStr"/>
+      <c r="I325" t="inlineStr"/>
+      <c r="J325" t="inlineStr"/>
+      <c r="K325" t="inlineStr"/>
+      <c r="L325" t="inlineStr"/>
+      <c r="M325" t="inlineStr"/>
+      <c r="N325" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="B326" t="inlineStr"/>
+      <c r="C326" t="inlineStr"/>
+      <c r="D326" t="inlineStr"/>
+      <c r="E326" t="inlineStr"/>
+      <c r="F326" t="inlineStr"/>
+      <c r="G326" t="inlineStr"/>
+      <c r="H326" t="inlineStr"/>
+      <c r="I326" t="inlineStr"/>
+      <c r="J326" t="inlineStr"/>
+      <c r="K326" t="inlineStr"/>
+      <c r="L326" t="inlineStr"/>
+      <c r="M326" t="inlineStr"/>
+      <c r="N326" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="B327" t="inlineStr"/>
+      <c r="C327" t="inlineStr"/>
+      <c r="D327" t="inlineStr"/>
+      <c r="E327" t="inlineStr"/>
+      <c r="F327" t="inlineStr"/>
+      <c r="G327" t="inlineStr"/>
+      <c r="H327" t="inlineStr"/>
+      <c r="I327" t="inlineStr"/>
+      <c r="J327" t="inlineStr"/>
+      <c r="K327" t="inlineStr"/>
+      <c r="L327" t="inlineStr"/>
+      <c r="M327" t="inlineStr"/>
+      <c r="N327" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="B328" t="inlineStr"/>
+      <c r="C328" t="inlineStr"/>
+      <c r="D328" t="inlineStr"/>
+      <c r="E328" t="inlineStr"/>
+      <c r="F328" t="inlineStr"/>
+      <c r="G328" t="inlineStr"/>
+      <c r="H328" t="inlineStr"/>
+      <c r="I328" t="inlineStr"/>
+      <c r="J328" t="inlineStr"/>
+      <c r="K328" t="inlineStr"/>
+      <c r="L328" t="inlineStr"/>
+      <c r="M328" t="inlineStr"/>
+      <c r="N328" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="B329" t="inlineStr"/>
+      <c r="C329" t="inlineStr"/>
+      <c r="D329" t="inlineStr"/>
+      <c r="E329" t="inlineStr"/>
+      <c r="F329" t="inlineStr"/>
+      <c r="G329" t="inlineStr"/>
+      <c r="H329" t="inlineStr"/>
+      <c r="I329" t="inlineStr"/>
+      <c r="J329" t="inlineStr"/>
+      <c r="K329" t="inlineStr"/>
+      <c r="L329" t="inlineStr"/>
+      <c r="M329" t="inlineStr"/>
+      <c r="N329" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="B330" t="inlineStr"/>
+      <c r="C330" t="inlineStr"/>
+      <c r="D330" t="inlineStr"/>
+      <c r="E330" t="inlineStr"/>
+      <c r="F330" t="inlineStr"/>
+      <c r="G330" t="inlineStr"/>
+      <c r="H330" t="inlineStr"/>
+      <c r="I330" t="inlineStr"/>
+      <c r="J330" t="inlineStr"/>
+      <c r="K330" t="inlineStr"/>
+      <c r="L330" t="inlineStr"/>
+      <c r="M330" t="inlineStr"/>
+      <c r="N330" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>329</v>
+      </c>
+      <c r="B331" t="inlineStr"/>
+      <c r="C331" t="inlineStr"/>
+      <c r="D331" t="inlineStr"/>
+      <c r="E331" t="inlineStr"/>
+      <c r="F331" t="inlineStr"/>
+      <c r="G331" t="inlineStr"/>
+      <c r="H331" t="inlineStr"/>
+      <c r="I331" t="inlineStr"/>
+      <c r="J331" t="inlineStr"/>
+      <c r="K331" t="inlineStr"/>
+      <c r="L331" t="inlineStr"/>
+      <c r="M331" t="inlineStr"/>
+      <c r="N331" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>330</v>
+      </c>
+      <c r="B332" t="inlineStr"/>
+      <c r="C332" t="inlineStr"/>
+      <c r="D332" t="inlineStr"/>
+      <c r="E332" t="inlineStr"/>
+      <c r="F332" t="inlineStr"/>
+      <c r="G332" t="inlineStr"/>
+      <c r="H332" t="inlineStr"/>
+      <c r="I332" t="inlineStr"/>
+      <c r="J332" t="inlineStr"/>
+      <c r="K332" t="inlineStr"/>
+      <c r="L332" t="inlineStr"/>
+      <c r="M332" t="inlineStr"/>
+      <c r="N332" t="n">
+        <v>32.63333333333333</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="B333" t="inlineStr"/>
+      <c r="C333" t="inlineStr"/>
+      <c r="D333" t="inlineStr"/>
+      <c r="E333" t="inlineStr"/>
+      <c r="F333" t="inlineStr"/>
+      <c r="G333" t="inlineStr"/>
+      <c r="H333" t="inlineStr"/>
+      <c r="I333" t="inlineStr"/>
+      <c r="J333" t="inlineStr"/>
+      <c r="K333" t="inlineStr"/>
+      <c r="L333" t="inlineStr"/>
+      <c r="M333" t="inlineStr"/>
+      <c r="N333" t="n">
+        <v>62.13666666666666</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="n">
+        <v>332</v>
+      </c>
+      <c r="B334" t="inlineStr"/>
+      <c r="C334" t="inlineStr"/>
+      <c r="D334" t="inlineStr"/>
+      <c r="E334" t="inlineStr"/>
+      <c r="F334" t="inlineStr"/>
+      <c r="G334" t="inlineStr"/>
+      <c r="H334" t="inlineStr"/>
+      <c r="I334" t="inlineStr"/>
+      <c r="J334" t="inlineStr"/>
+      <c r="K334" t="inlineStr"/>
+      <c r="L334" t="inlineStr"/>
+      <c r="M334" t="inlineStr"/>
+      <c r="N334" t="inlineStr">
+        <is>
+          <t>{0: 0.8333333333333334, 1: 0.16666666666666666}</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="B335" t="inlineStr"/>
+      <c r="C335" t="inlineStr"/>
+      <c r="D335" t="inlineStr"/>
+      <c r="E335" t="inlineStr"/>
+      <c r="F335" t="inlineStr"/>
+      <c r="G335" t="inlineStr"/>
+      <c r="H335" t="inlineStr"/>
+      <c r="I335" t="inlineStr"/>
+      <c r="J335" t="inlineStr"/>
+      <c r="K335" t="inlineStr"/>
+      <c r="L335" t="inlineStr"/>
+      <c r="M335" t="inlineStr"/>
+      <c r="N335" t="inlineStr">
+        <is>
+          <t>['[-149.0, 6.973113, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.9733, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.973318, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.973461, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-149.0, 6.973644, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011002, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011396, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011633, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.011736, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-213.0, 5.012369, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[-5.0, 11.366548, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[-5.0, 11.423346, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[-5.0, 11.429201, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[-5.0, 11.477434, 101.8, -1.02, 4.612, 312.9, 18.0, 13.0, 6.0, 9.0, 16.0, 12.0, 13.0, 14.0, 10.0, 16.0, 15.0, 6.0]', '[1.0, 0.0, 0.0, -0.8, 0.0, 9.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0]', '[1.0, 0.0, 1.6, -0.97, 0.062, 9.2, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0]', '[1.0, 0.0, 3.95, -1.1, 0.18, 10.5, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0]', '[1.0, 0.0, 4.0, 1.81, 0.186, 5.2, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0]', '[10.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 0.0, 22.05, -1.77, 0.988, 84.1, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 0.0, 23.84, 0.53, 1.089, 78.8, 6.0, 2.0, 2.0, 1.0, 5.0, 4.0, 4.0, 5.0, 1.0, 6.0, 2.0, 2.0]', '[10.0, 0.0, 25.5, 3.68, 1.166, 73.0, 4.0, 6.0, 0.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 3.0, 7.0, 0.0]', '[10.0, 0.0, 29.13, -0.5, 1.313, 85.2, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 0.0, 29.3, -1.99, 1.314, 83.4, 6.0, 2.0, 2.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 6.0, 2.0, 2.0]', '[10.0, 0.0, 29.52, 0.61, 1.322, 87.1, 5.0, 3.0, 2.0, 3.0, 5.0, 2.0, 3.0, 4.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 0.0, 29.53, 1.43, 1.344, 81.3, 5.0, 4.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 5.0, 1.0]', '[10.0, 0.0, 30.88, -0.53, 1.367, 87.5, 4.0, 5.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 5.0, 1.0]', '[10.0, 0.0, 31.2, -2.9, 1.413, 88.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 0.0, 31.2, 7.29, 1.464, 66.8, 2.0, 6.0, 2.0, 1.0, 2.0, 7.0, 7.0, 2.0, 1.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 31.23, -2.02, 1.403, 94.7, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 32.71, 2.58, 1.518, 75.4, 4.0, 4.0, 2.0, 1.0, 5.0, 4.0, 5.0, 3.0, 2.0, 3.0, 5.0, 2.0]', '[10.0, 0.0, 33.19, 4.2, 1.559, 70.7, 4.0, 3.0, 3.0, 0.0, 5.0, 5.0, 6.0, 3.0, 1.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 33.29, 3.11, 1.541, 78.1, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 33.61, -0.17, 1.535, 83.2, 4.0, 4.0, 2.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 5.0, 2.0]', '[10.0, 0.0, 33.97, -1.74, 1.525, 87.4, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 0.0, 34.72, 2.93, 1.601, 75.9, 4.0, 5.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 2.0, 7.0, 1.0]', '[10.0, 0.0, 35.54, 0.13, 1.618, 86.5, 2.0, 5.0, 3.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 2.0, 5.0, 3.0]', '[10.0, 0.0, 36.07, -0.53, 1.652, 87.3, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0, 3.0, 4.0, 3.0, 4.0, 2.0, 4.0]', '[10.0, 0.0, 36.19, -2.3, 1.609, 94.7, 2.0, 6.0, 2.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 36.7, -2.99, 1.67, 94.0, 3.0, 6.0, 1.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 2.0, 7.0, 1.0]', '[10.0, 0.0, 36.73, 0.24, 1.643, 86.7, 2.0, 5.0, 3.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 2.0, 5.0, 3.0]', '[10.0, 0.0, 36.74, -1.34, 1.687, 92.4, 4.0, 2.0, 4.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0]', '[10.0, 0.0, 37.12, 2.48, 1.694, 87.5, 2.0, 5.0, 3.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 0.0, 37.53, 1.45, 1.765, 78.7, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 37.77, 0.58, 1.714, 87.6, 2.0, 6.0, 2.0, 5.0, 2.0, 3.0, 3.0, 2.0, 5.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 38.67, -2.74, 1.719, 93.8, 3.0, 4.0, 3.0, 5.0, 4.0, 1.0, 2.0, 3.0, 5.0, 3.0, 4.0, 3.0]', '[10.0, 0.0, 39.22, 5.58, 1.789, 73.2, 1.0, 7.0, 2.0, 3.0, 0.0, 7.0, 7.0, 0.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 0.0, 39.35, 4.07, 1.812, 74.5, 1.0, 7.0, 2.0, 3.0, 1.0, 6.0, 6.0, 1.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 0.0, 39.91, -1.04, 1.788, 87.7, 2.0, 6.0, 2.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 6.0, 2.0]', '[10.0, 0.0, 41.3, 1.02, 1.938, 81.9, 2.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 2.0, 4.0, 4.0]', '[10.0, 0.0, 43.36, 4.45, 2.042, 77.7, 1.0, 5.0, 4.0, 3.0, 2.0, 5.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 0.0, 44.68, -0.39, 2.062, 90.5, 2.0, 3.0, 5.0, 4.0, 4.0, 2.0, 3.0, 2.0, 5.0, 2.0, 3.0, 5.0]', '[10.0, 0.0, 45.79, -1.29, 2.115, 94.1, 1.0, 3.0, 6.0, 6.0, 2.0, 2.0, 3.0, 1.0, 6.0, 1.0, 3.0, 6.0]', '[10.0, 0.0, 47.26, 5.56, 2.292, 76.7, 1.0, 3.0, 6.0, 2.0, 3.0, 5.0, 5.0, 1.0, 4.0, 1.0, 3.0, 6.0]', '[10.0, 0.0, 53.73, 7.47, 2.59, 73.9, 0.0, 3.0, 7.0, 2.0, 3.0, 5.0, 6.0, 0.0, 4.0, 0.0, 3.0, 7.0]', '[10.0, 0.0, 55.62, 7.01, 2.694, 73.9, 0.0, 2.0, 8.0, 2.0, 3.0, 5.0, 6.0, 0.0, 4.0, 0.0, 2.0, 8.0]', '[10.0, 12.231122, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 12.602876, 32.51, -1.03, 1.49, 85.4, 5.0, 2.0, 3.0, 2.0, 5.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 12.636695, 32.51, -1.03, 1.49, 85.4, 5.0, 2.0, 3.0, 2.0, 5.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 12.825064, 32.09, -2.33, 1.434, 86.8, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 12.831107, 21.16, -0.3, 0.922, 84.9, 6.0, 4.0, 0.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 6.0, 4.0, 0.0]', '[10.0, 12.833985, 21.16, -0.3, 0.922, 84.9, 6.0, 4.0, 0.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 6.0, 4.0, 0.0]', '[10.0, 12.862465, 25.38, -2.42, 1.079, 84.3, 8.0, 2.0, 0.0, 1.0, 7.0, 2.0, 2.0, 7.0, 1.0, 8.0, 2.0, 0.0]', '[10.0, 12.866284, 41.67, -1.3, 1.889, 93.7, 1.0, 5.0, 4.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 1.0, 5.0, 4.0]', '[10.0, 12.875708, 33.53, 4.6, 1.539, 75.9, 4.0, 4.0, 2.0, 1.0, 4.0, 5.0, 5.0, 3.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 12.894289, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.002887, 35.55, -0.88, 1.588, 84.9, 3.0, 6.0, 1.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.003345, 35.55, -0.88, 1.588, 84.9, 3.0, 6.0, 1.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.011763, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.076318, 25.61, -2.15, 1.16, 86.8, 6.0, 3.0, 1.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 6.0, 3.0, 1.0]', '[10.0, 13.165224, 32.09, -2.33, 1.434, 86.8, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 13.2302, 41.41, 4.77, 1.924, 67.3, 3.0, 4.0, 3.0, 1.0, 4.0, 5.0, 6.0, 3.0, 1.0, 2.0, 5.0, 3.0]', '[10.0, 13.2564, 22.05, -1.77, 0.988, 84.1, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.256543, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.300899, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.301272, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.301789, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.301918, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.30215, 31.51, 4.05, 1.493, 76.1, 4.0, 3.0, 3.0, 0.0, 7.0, 3.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.422756, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 13.427407, 22.05, -1.77, 0.988, 84.1, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.432258, 39.3, 1.68, 1.794, 87.0, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.48406, 39.3, 1.68, 1.794, 87.0, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.509898, 45.5, -2.5, 2.061, 100.7, 2.0, 2.0, 6.0, 7.0, 2.0, 1.0, 2.0, 1.0, 7.0, 2.0, 2.0, 6.0]', '[10.0, 13.523679, 28.45, -3.28, 1.28, 90.4, 7.0, 2.0, 1.0, 3.0, 6.0, 1.0, 1.0, 6.0, 3.0, 4.0, 5.0, 1.0]', '[10.0, 13.536176, 40.66, 0.61, 1.843, 89.0, 1.0, 5.0, 4.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 1.0, 5.0, 4.0]', '[10.0, 13.544919, 31.67, 2.27, 1.459, 77.3, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.554057, 35.82, -4.45, 1.568, 99.4, 4.0, 4.0, 2.0, 5.0, 3.0, 2.0, 2.0, 2.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.573598, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.625075, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.635057, 34.84, -1.07, 1.602, 88.6, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 13.635601, 33.39, -5.98, 1.453, 101.9, 4.0, 4.0, 2.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.636476, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.641503, 33.12, -0.96, 1.517, 88.7, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 13.656127, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.656542, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.667926, 39.33, -4.2, 1.754, 98.2, 2.0, 5.0, 3.0, 6.0, 3.0, 1.0, 2.0, 2.0, 6.0, 2.0, 5.0, 3.0]', '[10.0, 13.674337, 33.59, 1.6, 1.535, 85.8, 3.0, 5.0, 2.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.679361, 40.32, -3.73, 1.842, 98.6, 4.0, 1.0, 5.0, 6.0, 4.0, 0.0, 1.0, 3.0, 6.0, 3.0, 2.0, 5.0]', '[10.0, 13.691627, 34.25, 1.48, 1.52, 82.6, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 13.696875, 35.26, -3.31, 1.58, 96.1, 4.0, 4.0, 2.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.705323, 34.84, -1.07, 1.602, 88.6, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 13.709828, 21.11, -1.54, 0.965, 85.9, 5.0, 5.0, 0.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 6.0, 0.0]', '[10.0, 13.711534, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.718501, 44.37, 1.27, 2.036, 84.9, 2.0, 3.0, 5.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.721821, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.728899, 31.2, -2.9, 1.413, 88.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.729721, 34.13, 2.27, 1.546, 78.6, 3.0, 6.0, 1.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 7.0, 1.0]', '[10.0, 13.74546, 33.39, -5.98, 1.453, 101.9, 4.0, 4.0, 2.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 4.0, 4.0, 2.0]', '[10.0, 13.747208, 33.12, -2.62, 1.505, 89.1, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 13.764486, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.783585, 34.13, 2.27, 1.546, 78.6, 3.0, 6.0, 1.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 7.0, 1.0]', '[10.0, 13.79329, 31.2, -2.9, 1.413, 88.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.796657, 38.4, -1.71, 1.793, 89.2, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 13.809725, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.835076, 38.19, 4.14, 1.803, 79.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 3.0, 3.0, 4.0]', '[10.0, 13.840067, 39.61, 0.22, 1.803, 88.4, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.848726, 23.99, -0.22, 1.087, 87.3, 5.0, 4.0, 1.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 4.0, 1.0]', '[10.0, 13.849965, 38.19, 4.14, 1.803, 79.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 3.0, 3.0, 4.0]', '[10.0, 13.85373, 37.04, 5.76, 1.709, 75.9, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 13.864258, 21.11, -1.54, 0.965, 85.9, 5.0, 5.0, 0.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 6.0, 0.0]', '[10.0, 13.865242, 39.62, -3.15, 1.812, 94.1, 3.0, 4.0, 3.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 2.0, 5.0, 3.0]', '[10.0, 13.866588, 40.62, 1.81, 1.908, 82.9, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.868733, 29.89, 3.33, 1.4, 72.4, 6.0, 3.0, 1.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 13.870766, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 13.871456, 33.91, 0.1, 1.511, 85.7, 4.0, 5.0, 1.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.87348, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.878806, 38.65, 4.6, 1.869, 72.7, 3.0, 3.0, 4.0, 3.0, 1.0, 6.0, 7.0, 0.0, 3.0, 0.0, 6.0, 4.0]', '[10.0, 13.898501, 32.2, 0.64, 1.482, 81.3, 5.0, 3.0, 2.0, 2.0, 4.0, 4.0, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 13.899586, 32.95, -2.66, 1.476, 90.9, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 13.903127, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.913788, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 13.923096, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 13.923403, 29.89, 3.33, 1.4, 72.4, 6.0, 3.0, 1.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 13.928315, 37.18, 1.61, 1.733, 79.1, 2.0, 3.0, 4.0, 4.0, 2.0, 3.0, 3.0, 1.0, 5.0, 2.0, 3.0, 4.0]', '[10.0, 13.944123, 33.87, 3.87, 1.587, 78.6, 2.0, 5.0, 3.0, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0, 2.0, 5.0, 3.0]', '[10.0, 13.944978, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 13.946486, 40.62, 1.81, 1.908, 82.9, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.949725, 34.25, 1.48, 1.52, 82.6, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 13.952652, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 13.952741, 39.61, 0.22, 1.803, 88.4, 2.0, 5.0, 3.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 13.959268, 28.5, -5.52, 1.22, 97.1, 6.0, 2.0, 2.0, 4.0, 5.0, 1.0, 1.0, 5.0, 4.0, 6.0, 2.0, 2.0]', '[10.0, 13.965471, 41.12, 0.63, 1.828, 94.7, 1.0, 5.0, 4.0, 6.0, 1.0, 3.0, 4.0, 0.0, 6.0, 1.0, 5.0, 4.0]', '[10.0, 13.966332, 45.61, 1.22, 2.12, 86.1, 2.0, 3.0, 5.0, 4.0, 4.0, 2.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 13.968701, 18.28, -1.94, 0.803, 88.0, 7.0, 3.0, 0.0, 2.0, 7.0, 1.0, 1.0, 7.0, 2.0, 6.0, 4.0, 0.0]', '[10.0, 13.968908, 36.63, 3.8, 1.736, 74.7, 3.0, 4.0, 3.0, 2.0, 4.0, 4.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 13.969321, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 13.971485, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.973165, 29.89, 3.33, 1.4, 72.4, 6.0, 3.0, 1.0, 1.0, 4.0, 5.0, 5.0, 4.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 13.97335, 35.03, 1.28, 1.57, 85.4, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 13.98024, 31.67, 2.27, 1.459, 77.3, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.981382, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 13.991016, 40.65, 4.39, 1.918, 77.8, 2.0, 4.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 4.0, 4.0]', '[10.0, 13.993335, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 13.996099, 25.91, 1.81, 1.184, 79.2, 5.0, 4.0, 1.0, 2.0, 5.0, 3.0, 3.0, 5.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 13.998617, 41.82, 2.7, 1.942, 82.8, 1.0, 5.0, 4.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 13.99883, 32.81, 0.28, 1.497, 86.7, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.000609, 37.04, 5.76, 1.709, 75.9, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 14.000667, 36.47, 1.28, 1.637, 84.8, 2.0, 6.0, 2.0, 4.0, 2.0, 4.0, 4.0, 2.0, 4.0, 2.0, 6.0, 2.0]', '[10.0, 14.001177, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 14.003231, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.004918, 38.4, -1.71, 1.793, 89.2, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 14.006487, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.009073, 30.07, 3.06, 1.397, 76.8, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.009584, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.010435, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 14.019653, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.020818, 27.42, -1.31, 1.213, 89.7, 6.0, 2.0, 2.0, 3.0, 5.0, 2.0, 2.0, 5.0, 3.0, 6.0, 2.0, 2.0]', '[10.0, 14.024644, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.025478, 34.0, 2.5, 1.552, 81.4, 4.0, 4.0, 2.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 5.0, 2.0]', '[10.0, 14.028098, 23.4, 0.91, 1.06, 78.2, 4.0, 5.0, 0.0, 3.0, 4.0, 2.0, 2.0, 4.0, 3.0, 3.0, 6.0, 0.0]', '[10.0, 14.030268, 32.81, 0.28, 1.497, 86.7, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.030828, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.031948, 20.28, -2.45, 0.897, 85.6, 6.0, 4.0, 0.0, 2.0, 6.0, 2.0, 2.0, 6.0, 2.0, 5.0, 5.0, 0.0]', '[10.0, 14.032445, 30.63, 3.1, 1.411, 75.6, 3.0, 6.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 2.0, 7.0, 1.0]', '[10.0, 14.037899, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.038204, 39.54, 0.18, 1.809, 87.5, 3.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0]', '[10.0, 14.0384, 23.4, 0.91, 1.06, 78.2, 4.0, 5.0, 0.0, 3.0, 4.0, 2.0, 2.0, 4.0, 3.0, 3.0, 6.0, 0.0]', '[10.0, 14.038975, 34.79, 0.74, 1.638, 87.9, 2.0, 5.0, 3.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 1.0, 6.0, 3.0]', '[10.0, 14.041416, 44.9, 3.87, 2.079, 80.0, 1.0, 6.0, 3.0, 4.0, 1.0, 5.0, 6.0, 0.0, 4.0, 1.0, 6.0, 3.0]', '[10.0, 14.042293, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.043569, 35.3, 4.32, 1.704, 74.8, 4.0, 3.0, 3.0, 1.0, 5.0, 4.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.046, 39.62, -3.15, 1.812, 94.1, 3.0, 4.0, 3.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 2.0, 5.0, 3.0]', '[10.0, 14.049706, 38.59, 1.46, 1.761, 82.4, 1.0, 7.0, 2.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 7.0, 2.0]', '[10.0, 14.049902, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.055429, 36.58, -2.36, 1.676, 94.8, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0]', '[10.0, 14.057396, 32.98, -2.03, 1.493, 87.4, 4.0, 5.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.059718, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.068825, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.069587, 34.71, 1.25, 1.579, 87.4, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.069694, 34.02, 0.58, 1.604, 84.1, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 14.069977, 42.87, -2.32, 2.014, 95.3, 1.0, 4.0, 5.0, 6.0, 2.0, 2.0, 2.0, 1.0, 7.0, 1.0, 4.0, 5.0]', '[10.0, 14.071734, 34.02, 0.58, 1.604, 84.1, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 14.073797, 38.29, 3.96, 1.739, 79.0, 2.0, 6.0, 2.0, 3.0, 3.0, 4.0, 5.0, 2.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 14.074481, 33.12, -2.62, 1.505, 89.1, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 14.079386, 34.02, 0.58, 1.604, 84.1, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0]', '[10.0, 14.082984, 38.59, 1.46, 1.761, 82.4, 1.0, 7.0, 2.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 7.0, 2.0]', '[10.0, 14.093163, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.093235, 33.09, 1.89, 1.541, 77.8, 4.0, 3.0, 3.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.095173, 39.54, 0.18, 1.809, 87.5, 3.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0]', '[10.0, 14.099388, 37.54, 1.8, 1.729, 81.8, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 14.103475, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.105171, 30.07, 3.06, 1.397, 76.8, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.106567, 35.03, 1.28, 1.57, 85.4, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 14.107534, 39.42, 0.77, 1.788, 86.6, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.1079, 38.59, 1.14, 1.771, 85.9, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.108442, 46.62, -0.26, 2.135, 88.6, 0.0, 6.0, 4.0, 6.0, 1.0, 3.0, 4.0, 0.0, 6.0, 0.0, 6.0, 4.0]', '[10.0, 14.109158, 40.77, 1.29, 1.85, 85.5, 0.0, 8.0, 2.0, 5.0, 1.0, 4.0, 5.0, 0.0, 5.0, 0.0, 8.0, 2.0]', '[10.0, 14.109771, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.110333, 41.82, 2.7, 1.942, 82.8, 1.0, 5.0, 4.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 14.113433, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.114399, 32.78, -1.19, 1.501, 85.2, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 14.114652, 41.82, 2.7, 1.942, 82.8, 1.0, 5.0, 4.0, 4.0, 2.0, 4.0, 5.0, 1.0, 4.0, 1.0, 5.0, 4.0]', '[10.0, 14.119208, 31.67, 2.27, 1.459, 77.3, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.121864, 40.32, -3.73, 1.842, 98.6, 4.0, 1.0, 5.0, 6.0, 4.0, 0.0, 1.0, 3.0, 6.0, 3.0, 2.0, 5.0]', '[10.0, 14.129521, 33.12, -2.62, 1.505, 89.1, 3.0, 6.0, 1.0, 5.0, 3.0, 2.0, 2.0, 3.0, 5.0, 2.0, 7.0, 1.0]', '[10.0, 14.133211, 37.54, 1.8, 1.729, 81.8, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 14.136464, 38.4, -1.71, 1.793, 89.2, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 14.136483, 34.27, -1.09, 1.564, 90.6, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0]', '[10.0, 14.137226, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.137248, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.139355, 13.76, -2.79, 0.566, 49.0, 3.0, 2.0, 0.0, 2.0, 2.0, 1.0, 1.0, 2.0, 2.0, 3.0, 2.0, 0.0]', '[10.0, 14.139792, 32.78, -1.19, 1.501, 85.2, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 14.140756, 42.87, -2.32, 2.014, 95.3, 1.0, 4.0, 5.0, 6.0, 2.0, 2.0, 2.0, 1.0, 7.0, 1.0, 4.0, 5.0]', '[10.0, 14.143339, 31.67, -3.01, 1.423, 89.1, 4.0, 5.0, 1.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.145168, 33.06, 0.57, 1.512, 84.8, 3.0, 5.0, 2.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 5.0, 2.0]', '[10.0, 14.1461, 30.07, 3.06, 1.397, 76.8, 6.0, 3.0, 1.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.146968, 32.92, 2.55, 1.504, 74.7, 3.0, 6.0, 1.0, 2.0, 4.0, 4.0, 5.0, 3.0, 2.0, 2.0, 7.0, 1.0]', '[10.0, 14.148196, 42.15, -1.86, 1.903, 88.6, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 2.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 14.148559, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.150026, 37.01, -0.09, 1.66, 88.2, 3.0, 5.0, 2.0, 5.0, 1.0, 4.0, 4.0, 1.0, 5.0, 3.0, 5.0, 2.0]', '[10.0, 14.152457, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.152708, 34.69, 5.44, 1.639, 71.9, 3.0, 4.0, 3.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.152807, 34.69, 5.44, 1.639, 71.9, 3.0, 4.0, 3.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.15318, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.157504, 38.98, 2.84, 1.793, 83.1, 3.0, 5.0, 2.0, 4.0, 1.0, 5.0, 5.0, 1.0, 4.0, 2.0, 6.0, 2.0]', '[10.0, 14.159579, 36.58, -2.36, 1.676, 94.8, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0]', '[10.0, 14.159942, 32.58, -4.17, 1.49, 89.6, 5.0, 1.0, 3.0, 4.0, 4.0, 1.0, 1.0, 3.0, 5.0, 5.0, 1.0, 3.0]', '[10.0, 14.163594, 37.04, 5.76, 1.709, 75.9, 2.0, 6.0, 2.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 6.0, 2.0]', '[10.0, 14.165008, 30.36, -1.56, 1.368, 88.7, 4.0, 5.0, 1.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.168352, 31.41, 1.75, 1.422, 81.8, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 14.170017, 36.93, 3.16, 1.68, 78.5, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 5.0, 2.0, 3.0, 3.0, 5.0, 2.0]', '[10.0, 14.171338, 39.54, 0.18, 1.809, 87.5, 3.0, 2.0, 5.0, 3.0, 5.0, 2.0, 3.0, 3.0, 4.0, 3.0, 2.0, 5.0]', '[10.0, 14.171887, 36.67, 1.21, 1.688, 86.7, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.176259, 39.7, -5.68, 1.773, 99.0, 3.0, 4.0, 3.0, 6.0, 3.0, 1.0, 1.0, 3.0, 6.0, 3.0, 4.0, 3.0]', '[10.0, 14.179652, 28.08, -0.39, 1.263, 82.8, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 14.179842, 43.6, 0.63, 1.987, 88.6, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 4.0, 1.0, 5.0, 1.0, 4.0, 5.0]', '[10.0, 14.180959, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.182482, 40.62, 1.81, 1.908, 82.9, 2.0, 3.0, 5.0, 3.0, 3.0, 4.0, 4.0, 2.0, 4.0, 2.0, 3.0, 5.0]', '[10.0, 14.184709, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.186073, 34.71, 1.25, 1.579, 87.4, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.187119, 36.53, -0.63, 1.641, 90.3, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0, 3.0, 3.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.18831, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.19365, 32.56, -1.43, 1.448, 90.1, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 2.0, 7.0, 1.0]', '[10.0, 14.194487, 31.95, -2.07, 1.432, 87.4, 3.0, 6.0, 1.0, 4.0, 3.0, 3.0, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0]', '[10.0, 14.196987, 43.55, 2.8, 1.986, 77.4, 3.0, 4.0, 3.0, 2.0, 5.0, 3.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.201266, 25.59, 0.76, 1.162, 78.6, 6.0, 3.0, 1.0, 1.0, 5.0, 4.0, 4.0, 5.0, 1.0, 5.0, 4.0, 1.0]', '[10.0, 14.201822, 13.76, -2.79, 0.566, 49.0, 3.0, 2.0, 0.0, 2.0, 2.0, 1.0, 1.0, 2.0, 2.0, 3.0, 2.0, 0.0]', '[10.0, 14.203003, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.203758, 38.65, 4.6, 1.869, 72.7, 3.0, 3.0, 4.0, 3.0, 1.0, 6.0, 7.0, 0.0, 3.0, 0.0, 6.0, 4.0]', '[10.0, 14.205182, 28.08, -0.39, 1.263, 82.8, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 14.205329, 32.54, 0.73, 1.511, 75.0, 3.0, 4.0, 2.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 4.0, 2.0]', '[10.0, 14.205691, 38.44, -1.2, 1.647, 95.3, 4.0, 4.0, 2.0, 5.0, 3.0, 2.0, 4.0, 1.0, 5.0, 4.0, 4.0, 2.0]', '[10.0, 14.205761, 32.65, -3.89, 1.463, 91.9, 3.0, 6.0, 1.0, 5.0, 4.0, 1.0, 2.0, 3.0, 5.0, 3.0, 6.0, 1.0]', '[10.0, 14.206644, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.20914, 29.6, -1.33, 1.371, 90.0, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.21102, 31.71, 1.02, 1.471, 78.5, 4.0, 3.0, 3.0, 1.0, 6.0, 3.0, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0]', '[10.0, 14.211214, 40.65, 4.39, 1.918, 77.8, 2.0, 4.0, 4.0, 3.0, 2.0, 5.0, 5.0, 2.0, 3.0, 2.0, 4.0, 4.0]', '[10.0, 14.21542, 34.69, 5.44, 1.639, 71.9, 3.0, 4.0, 3.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.216608, 32.47, -0.0, 1.458, 84.4, 5.0, 3.0, 2.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 5.0, 3.0, 2.0]', '[10.0, 14.216707, 35.93, -1.62, 1.628, 92.1, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 2.0, 5.0, 4.0, 3.0, 3.0]', '[10.0, 14.220979, 36.53, -0.63, 1.641, 90.3, 3.0, 3.0, 4.0, 3.0, 6.0, 1.0, 3.0, 3.0, 4.0, 3.0, 3.0, 4.0]', '[10.0, 14.223986, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.226548, 33.09, 1.89, 1.541, 77.8, 4.0, 3.0, 3.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 3.0, 4.0, 3.0]', '[10.0, 14.232534, 46.62, -0.26, 2.135, 88.6, 0.0, 6.0, 4.0, 6.0, 1.0, 3.0, 4.0, 0.0, 6.0, 0.0, 6.0, 4.0]', '[10.0, 14.233028, 21.36, -1.59, 0.96, 87.1, 8.0, 1.0, 1.0, 1.0, 8.0, 1.0, 1.0, 7.0, 2.0, 7.0, 2.0, 1.0]', '[10.0, 14.233681, 37.71, -1.24, 1.706, 96.9, 4.0, 4.0, 2.0, 6.0, 1.0, 3.0, 3.0, 1.0, 6.0, 3.0, 5.0, 2.0]', '[10.0, 14.233716, 33.07, 1.42, 1.552, 74.8, 5.0, 2.0, 3.0, 1.0, 6.0, 3.0, 4.0, 5.0, 1.0, 3.0, 4.0, 3.0]', '[10.0, 14.233938, 37.54, 1.8, 1.729, 81.8, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 3.0]', '[10.0, 14.23473, 43.85, -2.39, 2.021, 91.3, 2.0, 4.0, 4.0, 6.0, 2.0, 2.0, 2.0, 2.0, 6.0, 2.0, 4.0, 4.0]', '[10.0, 14.235544, 28.08, -0.39, 1.263, 82.8, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 2.0]', '[10.0, 14.237524, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 14.24404, 38.29, 3.96, 1.739, 79.0, 2.0, 6.0, 2.0, 3.0, 3.0, 4.0, 5.0, 2.0, 3.0, 1.0, 7.0, 2.0]', '[10.0, 14.244555, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.244813, 28.05, 1.53, 1.258, 79.9, 5.0, 4.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.245194, 38.51, 2.37, 1.815, 80.5, 3.0, 2.0, 5.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 1.0, 4.0, 5.0]', '[10.0, 14.245522, 39.54, 2.97, 1.84, 86.8, 2.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 1.0, 5.0, 4.0]', '[10.0, 14.245532, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.246739, 39.54, 2.97, 1.84, 86.8, 2.0, 4.0, 4.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 1.0, 5.0, 4.0]', '[10.0, 14.248511, 30.77, 2.54, 1.389, 79.0, 6.0, 3.0, 1.0, 2.0, 4.0, 4.0, 4.0, 4.0, 2.0, 5.0, 4.0, 1.0]', '[10.0, 14.253366, 40.11, -0.56, 1.888, 87.8, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0, 4.0, 1.0, 5.0, 1.0, 4.0, 5.0]', '[10.0, 14.253503, 37.27, 0.59, 1.7, 88.0, 3.0, 4.0, 3.0, 4.0, 2.0, 4.0, 4.0, 1.0, 5.0, 3.0, 4.0, 3.0]', '[10.0, 14.25433, 44.9, 3.87, 2.079, 80.0, 1.0, 6.0, 3.0, 4.0, 1.0, 5.0, 6.0, 0.0, 4.0, 1.0, 6.0, 3.0]', '[10.0, 14.254751, 35.71, 0.98, 1.599, 86.6, 4.0, 4.0, 2.0, 4.0, 3.0, 3.0, 4.0, 2.0, 4.0, 4.0, 4.0, 2.0]', '[10.0, 14.25688, 31.41, 1.75, 1.422, 81.8, 4.0, 5.0, 1.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 3.0, 6.0, 1.0]', '[10.0, 14.257303, 29.6, -1.33, 1.371, 90.0, 5.0, 2.0, 3.0, 4.0, 4.0, 2.0, 2.0, 4.0, 4.0, 3.0, 4.0, 3.0]', '[10.0, 14.259783, 27.32, 1.1, 1.241, 83.3, 4.0, 4.0, 2.0, 3.0, 3.0, 4.0, 4.0, 3.0, 3.0, 4.0, 4.0, 2.0]', '[10.0, 14.26067, 39.73, 4.97, 1.891, 74.8, 3.0, 3.0, 4.0, 2.0, 3.0, 5.0, 5.0, 3.0, 2.0, 2.0, 4.0, 4.0]', '[10.0, 14.260986, 33.73, -1.1, 1.563, 78.0, 4.0, 2.0, 3.0, 3.0, 4.0, 2.0, 2.0, 4.0, 3.0, 4.0, 2.0, 3.0]', '[10.0, 14.264573, 36.66, 1.45, 1.733, 82.9, 3.0, 4.0, 3.0, 3.0, 4.0, 3.0, 3.0, 3.0, 4.0, 1.0, 6.0, 3.0]', '[10.0, 14.265572, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 14.266937, 43.6, 1.93, 1.971, 86.9, 3.0, 3.0, 4.0, 5.0, 1.0, 4.0, 5.0, 0.0, 5.0, 3.0, 3.0, 4.0]', '[10.0, 14.270904, 49.33, 2.01, 2.267, 88.3, 2.0, 3.0, 5.0, 5.0, 2.0, 3.0, 5.0, 0.0, 5.0, 2.0, 3.0, 5.0]', '[10.0, 14.27145, 41.67, -1.67, 1.89, 94.3, 0.0, 8.0, 2.0, 7.0, 0.0, 3.0, 3.0, 0.0, 7.0, 0.0, 8.0, 2.0]', '[10.0, 14.271929, 38.66, 0.58, 1.782, 87.4, 2.0, 5.0, 3.0, 4.0, 3.0, 3.0, 3.0, 2.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 14.274005, 38.66, 0.58, 1.782, 87.4, 2.0, 5.0, 3.0, 4.0, 3.0, 3.0, 3.0, 2.0, 5.0, 2.0, 5.0, 3.0]', '[10.0, 14.275044, 40.97, -0.12, 1.877, 89.7, 1.0, 6.0, 3.0, 6.0, 0.0, 4.0, 4.0, 0.0, 6.0, 0.0, 7.0, 3.0]', '[10.0, 14.276442, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0]', '[10.0, 14.2767, 27.28, 0.02, 1.25, 72.8, 4.0, 3.0, 2.0, 1.0, 6.0, 2.0, 3.0, 4.0, 2.0, 4.0, 3.0, 2.0]', '[10.0, 14.28106, 33.38, 1.22, 1.564, 75.9, 5.0, 1.0, 4.0, 1.0, 6.0, 3.0, 4.0, 5.0, 1.0, 4.0, 2.0, 4.0]', '[10.0, 14.281342, 38.66, 0.58, 1.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B336" t="inlineStr"/>
+      <c r="C336" t="inlineStr"/>
+      <c r="D336" t="inlineStr"/>
+      <c r="E336" t="inlineStr"/>
+      <c r="F336" t="inlineStr"/>
+      <c r="G336" t="inlineStr"/>
+      <c r="H336" t="inlineStr"/>
+      <c r="I336" t="inlineStr"/>
+      <c r="J336" t="inlineStr"/>
+      <c r="K336" t="inlineStr"/>
+      <c r="L336" t="inlineStr"/>
+      <c r="M336" t="inlineStr"/>
+      <c r="N336" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="n">
+        <v>335</v>
+      </c>
+      <c r="B337" t="inlineStr"/>
+      <c r="C337" t="inlineStr"/>
+      <c r="D337" t="inlineStr"/>
+      <c r="E337" t="inlineStr"/>
+      <c r="F337" t="inlineStr"/>
+      <c r="G337" t="inlineStr"/>
+      <c r="H337" t="inlineStr"/>
+      <c r="I337" t="inlineStr"/>
+      <c r="J337" t="inlineStr"/>
+      <c r="K337" t="inlineStr"/>
+      <c r="L337" t="inlineStr"/>
+      <c r="M337" t="inlineStr"/>
+      <c r="N337" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="B338" t="inlineStr"/>
+      <c r="C338" t="inlineStr"/>
+      <c r="D338" t="inlineStr"/>
+      <c r="E338" t="inlineStr"/>
+      <c r="F338" t="inlineStr"/>
+      <c r="G338" t="inlineStr"/>
+      <c r="H338" t="inlineStr"/>
+      <c r="I338" t="inlineStr"/>
+      <c r="J338" t="inlineStr"/>
+      <c r="K338" t="inlineStr"/>
+      <c r="L338" t="inlineStr"/>
+      <c r="M338" t="inlineStr"/>
+      <c r="N338" t="inlineStr">
+        <is>
+          <t>[37282]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chancges for Dataset Loading
</commit_message>
<xml_diff>
--- a/configs/test_datasets.xlsx
+++ b/configs/test_datasets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N338"/>
+  <dimension ref="A1:N422"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7677,6 +7677,1783 @@
         </is>
       </c>
     </row>
+    <row r="339">
+      <c r="A339" s="1" t="n">
+        <v>337</v>
+      </c>
+      <c r="B339" t="inlineStr"/>
+      <c r="C339" t="inlineStr"/>
+      <c r="D339" t="inlineStr"/>
+      <c r="E339" t="inlineStr"/>
+      <c r="F339" t="inlineStr"/>
+      <c r="G339" t="inlineStr"/>
+      <c r="H339" t="inlineStr"/>
+      <c r="I339" t="inlineStr"/>
+      <c r="J339" t="inlineStr"/>
+      <c r="K339" t="inlineStr"/>
+      <c r="L339" t="inlineStr"/>
+      <c r="M339" t="inlineStr"/>
+      <c r="N339" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="B340" t="inlineStr"/>
+      <c r="C340" t="inlineStr"/>
+      <c r="D340" t="inlineStr"/>
+      <c r="E340" t="inlineStr"/>
+      <c r="F340" t="inlineStr"/>
+      <c r="G340" t="inlineStr"/>
+      <c r="H340" t="inlineStr"/>
+      <c r="I340" t="inlineStr"/>
+      <c r="J340" t="inlineStr"/>
+      <c r="K340" t="inlineStr"/>
+      <c r="L340" t="inlineStr"/>
+      <c r="M340" t="inlineStr"/>
+      <c r="N340" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="B341" t="inlineStr"/>
+      <c r="C341" t="inlineStr"/>
+      <c r="D341" t="inlineStr"/>
+      <c r="E341" t="inlineStr"/>
+      <c r="F341" t="inlineStr"/>
+      <c r="G341" t="inlineStr"/>
+      <c r="H341" t="inlineStr"/>
+      <c r="I341" t="inlineStr"/>
+      <c r="J341" t="inlineStr"/>
+      <c r="K341" t="inlineStr"/>
+      <c r="L341" t="inlineStr"/>
+      <c r="M341" t="inlineStr"/>
+      <c r="N341" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="B342" t="inlineStr"/>
+      <c r="C342" t="inlineStr"/>
+      <c r="D342" t="inlineStr"/>
+      <c r="E342" t="inlineStr"/>
+      <c r="F342" t="inlineStr"/>
+      <c r="G342" t="inlineStr"/>
+      <c r="H342" t="inlineStr"/>
+      <c r="I342" t="inlineStr"/>
+      <c r="J342" t="inlineStr"/>
+      <c r="K342" t="inlineStr"/>
+      <c r="L342" t="inlineStr"/>
+      <c r="M342" t="inlineStr"/>
+      <c r="N342" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="B343" t="inlineStr"/>
+      <c r="C343" t="inlineStr"/>
+      <c r="D343" t="inlineStr"/>
+      <c r="E343" t="inlineStr"/>
+      <c r="F343" t="inlineStr"/>
+      <c r="G343" t="inlineStr"/>
+      <c r="H343" t="inlineStr"/>
+      <c r="I343" t="inlineStr"/>
+      <c r="J343" t="inlineStr"/>
+      <c r="K343" t="inlineStr"/>
+      <c r="L343" t="inlineStr"/>
+      <c r="M343" t="inlineStr"/>
+      <c r="N343" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B344" t="inlineStr"/>
+      <c r="C344" t="inlineStr"/>
+      <c r="D344" t="inlineStr"/>
+      <c r="E344" t="inlineStr"/>
+      <c r="F344" t="inlineStr"/>
+      <c r="G344" t="inlineStr"/>
+      <c r="H344" t="inlineStr"/>
+      <c r="I344" t="inlineStr"/>
+      <c r="J344" t="inlineStr"/>
+      <c r="K344" t="inlineStr"/>
+      <c r="L344" t="inlineStr"/>
+      <c r="M344" t="inlineStr"/>
+      <c r="N344" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="B345" t="inlineStr"/>
+      <c r="C345" t="inlineStr"/>
+      <c r="D345" t="inlineStr"/>
+      <c r="E345" t="inlineStr"/>
+      <c r="F345" t="inlineStr"/>
+      <c r="G345" t="inlineStr"/>
+      <c r="H345" t="inlineStr"/>
+      <c r="I345" t="inlineStr"/>
+      <c r="J345" t="inlineStr"/>
+      <c r="K345" t="inlineStr"/>
+      <c r="L345" t="inlineStr"/>
+      <c r="M345" t="inlineStr"/>
+      <c r="N345" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B346" t="inlineStr"/>
+      <c r="C346" t="inlineStr"/>
+      <c r="D346" t="inlineStr"/>
+      <c r="E346" t="inlineStr"/>
+      <c r="F346" t="inlineStr"/>
+      <c r="G346" t="inlineStr"/>
+      <c r="H346" t="inlineStr"/>
+      <c r="I346" t="inlineStr"/>
+      <c r="J346" t="inlineStr"/>
+      <c r="K346" t="inlineStr"/>
+      <c r="L346" t="inlineStr"/>
+      <c r="M346" t="inlineStr"/>
+      <c r="N346" t="n">
+        <v>15.6925</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="B347" t="inlineStr"/>
+      <c r="C347" t="inlineStr"/>
+      <c r="D347" t="inlineStr"/>
+      <c r="E347" t="inlineStr"/>
+      <c r="F347" t="inlineStr"/>
+      <c r="G347" t="inlineStr"/>
+      <c r="H347" t="inlineStr"/>
+      <c r="I347" t="inlineStr"/>
+      <c r="J347" t="inlineStr"/>
+      <c r="K347" t="inlineStr"/>
+      <c r="L347" t="inlineStr"/>
+      <c r="M347" t="inlineStr"/>
+      <c r="N347" t="n">
+        <v>16.195</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="B348" t="inlineStr"/>
+      <c r="C348" t="inlineStr"/>
+      <c r="D348" t="inlineStr"/>
+      <c r="E348" t="inlineStr"/>
+      <c r="F348" t="inlineStr"/>
+      <c r="G348" t="inlineStr"/>
+      <c r="H348" t="inlineStr"/>
+      <c r="I348" t="inlineStr"/>
+      <c r="J348" t="inlineStr"/>
+      <c r="K348" t="inlineStr"/>
+      <c r="L348" t="inlineStr"/>
+      <c r="M348" t="inlineStr"/>
+      <c r="N348" t="inlineStr">
+        <is>
+          <t>{0: 0.2, 1: 0.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="n">
+        <v>347</v>
+      </c>
+      <c r="B349" t="inlineStr"/>
+      <c r="C349" t="inlineStr"/>
+      <c r="D349" t="inlineStr"/>
+      <c r="E349" t="inlineStr"/>
+      <c r="F349" t="inlineStr"/>
+      <c r="G349" t="inlineStr"/>
+      <c r="H349" t="inlineStr"/>
+      <c r="I349" t="inlineStr"/>
+      <c r="J349" t="inlineStr"/>
+      <c r="K349" t="inlineStr"/>
+      <c r="L349" t="inlineStr"/>
+      <c r="M349" t="inlineStr"/>
+      <c r="N349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">['[1.0, -1.0, 0.5, -2.3499999046325684]', '[1.0, -1.0, 1.5, -2.1500000953674316]', '[1.0, -1.0, 2.865999937057495, 0.5]', '[1.0, -1.0, 2.889400005340576, 1.0297000408172607]', '[1.0, -1.0, 3.232100009918213, 1.4329999685287476]', '[1.0, -1.0, 3.2600998878479004, -0.6739000082015991]', '[1.0, -1.0, 3.694200038909912, 0.27709999680519104]', '[1.0, -1.0, 3.7320001125335693, 1.5]', '[1.0, -1.0, 3.732100009918213, -1.4329999685287476]', '[1.0, -1.0, 4.0, 1.0]', '[1.0, -1.0, 4.232100009918213, 1.4329999685287476]', '[1.0, -1.0, 4.2600998878479, -0.6739000082015991]', '[1.0, -1.0, 4.5690999031066895, 0.27709999680519104]', '[1.0, -1.0, 4.598100185394287, -0.25]', '[1.0, -1.0, 5.464099884033203, -0.5]', '[1.0, -1.0, 5.464099884033203, -0.7842000126838684]', '[1.0, -1.0, 5.464099884033203, -1.0]', '[1.0, -1.0, 6.1905999183654785, 1.7073999643325806]', '[1.0, -1.0, 6.556700229644775, 0.34139999747276306]', '[1.0, 0.0, 0.375, 0.0]', '[1.0, 0.0, 0.5, -2.3499999046325684]', '[1.0, 0.0, 0.5, -4.349999904632568]', '[1.0, 0.0, 0.5, -6.349999904632568]', '[1.0, 0.0, 0.5, -8.350000381469727]', '[1.0, 0.0, 0.6428999900817871, -16.350000381469727]', '[1.0, 0.0, 0.666700005531311, -2.3499999046325684]', '[1.0, 0.0, 0.666700005531311, -6.349999904632568]', '[1.0, 0.0, 0.75, -20.350000381469727]', '[1.0, 0.0, 0.75, -8.350000381469727]', '[1.0, 0.0, 0.75, 0.0]', '[1.0, 0.0, 0.8999999761581421, -30.350000381469727]', '[1.0, 0.0, 1.0, -6.349999904632568]', '[1.0, 0.0, 1.25, -4.349999904632568]', '[1.0, 0.0, 1.5, -10.149999618530273]', '[1.0, 0.0, 1.5, -10.350000381469727]', '[1.0, 0.0, 1.5, -12.350000381469727]', '[1.0, 0.0, 1.5, -2.3499999046325684]', '[1.0, 0.0, 1.5, -4.150000095367432]', '[1.0, 0.0, 1.5, -4.349999904632568]', '[1.0, 0.0, 1.5, -6.150000095367432]', '[1.0, 0.0, 1.5, -8.149999618530273]', '[1.0, 0.0, 1.5, -8.350000381469727]', '[1.0, 0.0, 1.6875, -24.149999618530273]', '[1.0, 0.0, 1.6875, -26.149999618530273]', '[1.0, 0.0, 10.000699996948242, 6.783299922943115]', '[1.0, 0.0, 10.00160026550293, 8.176199913024902]', '[1.0, 0.0, 10.002900123596191, -0.43299999833106995]', '[1.0, 0.0, 10.016900062561035, 0.5907999873161316]', '[1.0, 0.0, 10.016900062561035, 1.5908000469207764]', '[1.0, 0.0, 10.0516996383667, 3.3773000240325928]', '[1.0, 0.0, 10.052800178527832, -7.656899929046631]', '[1.0, 0.0, 10.05780029296875, 6.271399974822998]', '[1.0, 0.0, 10.062199592590332, -0.16060000658035278]', '[1.0, 0.0, 10.062199592590332, -1.0]', '[1.0, 0.0, 10.062199592590332, -1.160599946975708]', '[1.0, 0.0, 10.062199592590332, -1.6739000082015991]', '[1.0, 0.0, 10.062199592590332, -1.75]', '[1.0, 0.0, 10.062199592590332, -1.910599946975708]', '[1.0, 0.0, 10.062199592590332, -2.5]', '[1.0, 0.0, 10.062199592590332, -2.75]', '[1.0, 0.0, 10.062199592590332, -3.5]', '[1.0, 0.0, 10.062199592590332, -3.6738998889923096]', '[1.0, 0.0, 10.062199592590332, 0.0]', '[1.0, 0.0, 10.062199592590332, 1.089400053024292]', '[1.0, 0.0, 10.062199592590332, 1.25]', '[1.0, 0.0, 10.062199592590332, 3.25]', '[1.0, 0.0, 10.092599868774414, 1.608199954032898]', '[1.0, 0.0, 10.100500106811523, 6.870699882507324]', '[1.0, 0.0, 10.135100364685059, -4.391600131988525]', '[1.0, 0.0, 10.136899948120117, -0.014000000432133675]', '[1.0, 0.0, 10.140000343322754, -7.939700126647949]', '[1.0, 0.0, 10.140000343322754, -8.93970012664795]', '[1.0, 0.0, 10.144399642944336, -10.459600448608398]', '[1.0, 0.0, 10.144399642944336, -11.459600448608398]', '[1.0, 0.0, 10.144399642944336, -8.089799880981445]', '[1.0, 0.0, 10.144399642944336, -9.089799880981445]', '[1.0, 0.0, 10.14490032196045, 6.62060022354126]', '[1.0, 0.0, 10.154600143432617, 4.2307000160217285]', '[1.0, 0.0, 10.160300254821777, -4.673900127410889]', '[1.0, 0.0, 10.160300254821777, 1.4514000415802002]', '[1.0, 0.0, 10.166600227355957, -0.38449999690055847]', '[1.0, 0.0, 10.1697998046875, 8.392399787902832]', '[1.0, 0.0, 10.17080020904541, 6.566999912261963]', '[1.0, 0.0, 10.185099601745605, -2.4937000274658203]', '[1.0, 0.0, 10.191800117492676, 6.886499881744385]', '[1.0, 0.0, 10.199199676513672, -1.6735999584197998]', '[1.0, 0.0, 10.215299606323242, -0.24549999833106995]', '[1.0, 0.0, 10.215299606323242, -1.2454999685287476]', '[1.0, 0.0, 10.219599723815918, 7.595300197601318]', '[1.0, 0.0, 10.226400375366211, -0.15189999341964722]', '[1.0, 0.0, 10.236100196838379, -1.3710999488830566]', '[1.0, 0.0, 10.265899658203125, -0.020899999886751175]', '[1.0, 0.0, 10.270899772644043, -0.5]', '[1.0, 0.0, 10.270899772644043, 3.6923999786376953]', '[1.0, 0.0, 10.270899772644043, 4.5584001541137695]', '[1.0, 0.0, 10.278800010681152, 2.4182000160217285]', '[1.0, 0.0, 10.28339958190918, -2.2397000789642334]', '[1.0, 0.0, 10.28339958190918, -3.2397000789642334]', '[1.0, 0.0, 10.299699783325195, 6.1006999015808105]', '[1.0, 0.0, 10.309300422668457, -5.523099899291992]', '[1.0, 0.0, 10.317500114440918, -0.4099999964237213]', '[1.0, 0.0, 10.317500114440918, -1.409999966621399]', '[1.0, 0.0, 10.317500114440918, 1.590000033378601]', '[1.0, 0.0, 10.318300247192383, 2.3649001121520996]', '[1.0, 0.0, 10.318300247192383, 2.821700096130371]', '[1.0, 0.0, 10.323699951171875, 0.7990999817848206]', '[1.0, 0.0, 10.323699951171875, 0.9036999940872192]', '[1.0, 0.0, 10.32409954071045, 8.589900016784668]', '[1.0, 0.0, 10.331100463867188, -1.2702000141143799]', '[1.0, 0.0, 10.347200393676758, 3.1205999851226807]', '[1.0, 0.0, 10.366299629211426, -2.43530011177063]', '[1.0, 0.0, 10.366299629211426, -3.43530011177063]', '[1.0, 0.0, 10.371999740600586, -0.6202999949455261]', '[1.0, 0.0, 10.371999740600586, -1.0247999429702759]', '[1.0, 0.0, 10.371999740600586, -1.620300054550171]', '[1.0, 0.0, 10.371999740600586, -2.0248000621795654]', '[1.0, 0.0, 10.371999740600586, 0.9751999974250793]', '[1.0, 0.0, 10.371999740600586, 1.379699945449829]', '[1.0, 0.0, 10.393099784851074, -4.367000102996826]', '[1.0, 0.0, 10.405400276184082, -2.2370998859405518]', '[1.0, 0.0, 10.405400276184082, 2.3268001079559326]', '[1.0, 0.0, 10.42389965057373, -5.724899768829346]', '[1.0, 0.0, 10.42389965057373, -6.724899768829346]', '[1.0, 0.0, 10.44279956817627, -2.9772000312805176]', '[1.0, 0.0, 10.444999694824219, -3.25219988822937]', '[1.0, 0.0, 10.44540023803711, -5.365600109100342]', '[1.0, 0.0, 10.446200370788574, 5.204899787902832]', '[1.0, 0.0, 10.470999717712402, -1.36489999294281]', '[1.0, 0.0, 10.470999717712402, -1.7316999435424805]', '[1.0, 0.0, 10.470999717712402, 3.9361000061035156]', '[1.0, 0.0, 10.472299575805664, -1.3495999574661255]', '[1.0, 0.0, 10.4822998046875, 2.7565999031066895]', '[1.0, 0.0, 10.485799789428711, 1.9979000091552734]', '[1.0, 0.0, 10.499300003051758, 0.7990999817848206]', '[1.0, 0.0, 10.499300003051758, 1.0082000494003296]', '[1.0, 0.0, 10.499300003051758, 1.1513999700546265]', '[1.0, 0.0, 10.499300003051758, 1.3082000017166138]', '[1.0, 0.0, 10.499300003051758, 1.6604000329971313]', '[1.0, 0.0, 10.499300003051758, 1.7127000093460083]', '[1.0, 0.0, 10.510899543762207, -1.163599967956543]', '[1.0, 0.0, 10.510899543762207, 2.5817999839782715]', '[1.0, 0.0, 10.510899543762207, 3.5817999839782715]', '[1.0, 0.0, 10.512499809265137, 0.8306000232696533]', '[1.0, 0.0, 10.532600402832031, 0.9815000295639038]', '[1.0, 0.0, 10.553299903869629, -4.129799842834473]', '[1.0, 0.0, 10.555100440979004, -3.5367000102996826]', '[1.0, 0.0, 10.561200141906738, -3.7397000789642334]', '[1.0, 0.0, 10.562199592590332, 2.134000062942505]', '[1.0, 0.0, 10.575499534606934, -4.243599891662598]', '[1.0, 0.0, 10.576499938964844, 9.305999755859375]', '[1.0, 0.0, 10.588000297546387, -7.283199787139893]', '[1.0, 0.0, 10.60319995880127, 3.4238998889923096]', '[1.0, 0.0, 10.60319995880127, 4.423900127410889]', '[1.0, 0.0, 10.60319995880127, 7.423900127410889]', '[1.0, 0.0, 10.631400108337402, 7.765399932861328]', '[1.0, 0.0, 10.632800102233887, -0.04740000143647194]', '[1.0, 0.0, 10.632800102233887, -0.15189999341964722]', '[1.0, 0.0, 10.63599967956543, -2.087399959564209]', '[1.0, 0.0, 10.636899948120117, -0.8799999952316284]', '[1.0, 0.0, 10.6427001953125, -0.04899999871850014]', '[1.0, 0.0, 10.6427001953125, -1.7319999933242798]', '[1.0, 0.0, 10.6427001953125, -2.0490000247955322]', '[1.0, 0.0, 10.6427001953125, -2.7320001125335693]', '[1.0, 0.0, 10.6427001953125, -3.0490000247955322]', '[1.0, 0.0, 10.6427001953125, 0.2680000066757202]', '[1.0, 0.0, 10.643099784851074, -0.1607999950647354]', '[1.0, 0.0, 10.649399757385254, -2.3338000774383545]', '[1.0, 0.0, 10.653599739074707, 0.9096999764442444]', '[1.0, 0.0, 10.654899597167969, 0.19179999828338623]', '[1.0, 0.0, 10.660200119018555, -0.25]', '[1.0, 0.0, 10.660200119018555, -0.3889999985694885]', '[1.0, 0.0, 10.660200119018555, -0.4106000065803528]', '[1.0, 0.0, 10.660200119018555, -0.5]', '[1.0, 0.0, 10.660200119018555, -0.6606000065803528]', '[1.0, 0.0, 10.660200119018555, -0.75]', '[1.0, 0.0, 10.660200119018555, -0.7979000210762024]', '[1.0, 0.0, 10.660200119018555, -1.0]', '[1.0, 0.0, 10.660200119018555, -1.25]', '[1.0, 0.0, 10.660200119018555, -1.3170000314712524]', '[1.0, 0.0, 10.660200119018555, -1.5]', '[1.0, 0.0, 10.660200119018555, -1.75]', '[1.0, 0.0, 10.660200119018555, -1.8170000314712524]', '[1.0, 0.0, 10.660200119018555, -2.0]', '[1.0, 0.0, 10.660200119018555, -2.316999912261963]', '[1.0, 0.0, 10.660200119018555, -2.3889999389648438]', '[1.0, 0.0, 10.660200119018555, -2.5]', '[1.0, 0.0, 10.660200119018555, -2.75]', '[1.0, 0.0, 10.660200119018555, -2.7978999614715576]', '[1.0, 0.0, 10.660200119018555, -3.0875000953674316]', '[1.0, 0.0, 10.660200119018555, -3.0]', '[1.0, 0.0, 10.660200119018555, -3.25]', '[1.0, 0.0, 10.660200119018555, -3.5]', '[1.0, 0.0, 10.660200119018555, -4.0]', '[1.0, 0.0, 10.660200119018555, 0.0]', '[1.0, 0.0, 10.660200119018555, 0.25]', '[1.0, 0.0, 10.660200119018555, 0.3393999934196472]', '[1.0, 0.0, 10.660200119018555, 0.5]', '[1.0, 0.0, 10.660200119018555, 0.6830000281333923]', '[1.0, 0.0, 10.660200119018555, 1.0]', '[1.0, 0.0, 10.660200119018555, 1.5670000314712524]', '[1.0, 0.0, 10.660200119018555, 2.0]', '[1.0, 0.0, 10.660200119018555, 3.566999912261963]', '[1.0, 0.0, 10.660200119018555, 4.482900142669678]', '[1.0, 0.0, 10.660300254821777, -0.06700000166893005]', '[1.0, 0.0, 10.660300254821777, -0.08749999850988388]', '[1.0, 0.0, 10.660300254821777, -0.25]', '[1.0, 0.0, 10.660300254821777, -0.5170999765396118]', '[1.0, 0.0, 10.660300254821777, -0.5]', '[1.0, 0.0, 10.660300254821777, -0.75]', '[1.0, 0.0, 10.660300254821777, -1.0670000314712524]', '[1.0, 0.0, 10.660300254821777, -1.0]', '[1.0, 0.0, 10.660300254821777, -1.5170999765396118]', '[1.0, 0.0, 10.660300254821777, -1.5670000314712524]', '[1.0, 0.0, 10.660300254821777, -1.5]', '[1.0, 0.0, 10.660300254821777, -1.660599946975708]', '[1.0, 0.0, 10.660300254821777, -1.75]', '[1.0, 0.0, 10.660300254821777, -2.0]', '[1.0, 0.0, 10.660300254821777, -2.25]', '[1.0, 0.0, 10.660300254821777, -2.410599946975708]', '[1.0, 0.0, 10.660300254821777, -2.5171000957489014]', '[1.0, 0.0, 10.660300254821777, -2.5]', '[1.0, 0.0, 10.660300254821777, -3.566999912261963]', '[1.0, 0.0, 10.660300254821777, -3.5]', '[1.0, 0.0, 10.660300254821777, -4.566999912261963]', '[1.0, 0.0, 10.660300254821777, 0.0]', '[1.0, 0.0, 10.660300254821777, 0.25]', '[1.0, 0.0, 10.660300254821777, 0.4828999936580658]', '[1.0, 0.0, 10.660300254821777, 0.5669999718666077]', '[1.0, 0.0, 10.660300254821777, 0.5]', '[1.0, 0.0, 10.660300254821777, 0.6830000281333923]', '[1.0, 0.0, 10.660300254821777, 0.75]', '[1.0, 0.0, 10.660300254821777, 0.9330000281333923]', '[1.0, 0.0, 10.660300254821777, 1.0]', '[1.0, 0.0, 10.660300254821777, 1.25]', '[1.0, 0.0, 10.660300254821777, 1.5670000314712524]', '[1.0, 0.0, 10.660300254821777, 1.5]', '[1.0, 0.0, 10.660300254821777, 1.9329999685287476]', '[1.0, 0.0, 10.660300254821777, 2.0]', '[1.0, 0.0, 10.660300254821777, 2.25]', '[1.0, 0.0, 10.660300254821777, 2.5]', '[1.0, 0.0, 10.660300254821777, 2.75]', '[1.0, 0.0, 10.660300254821777, 2.933000087738037]', '[1.0, 0.0, 10.660300254821777, 3.0]', '[1.0, 0.0, 10.660300254821777, 3.25]', '[1.0, 0.0, 10.660300254821777, 3.316999912261963]', '[1.0, 0.0, 10.660300254821777, 3.5]', '[1.0, 0.0, 10.660300254821777, 4.0]', '[1.0, 0.0, 10.660300254821777, 4.25]', '[1.0, 0.0, 10.660300254821777, 4.5]', '[1.0, 0.0, 10.660300254821777, 5.25]', '[1.0, 0.0, 10.660300254821777, 5.75]', '[1.0, 0.0, 10.660300254821777, 6.0]', '[1.0, 0.0, 10.660300254821777, 7.566999912261963]', '[1.0, 0.0, 10.660300254821777, 7.75]', '[1.0, 0.0, 10.6697998046875, 7.526400089263916]', '[1.0, 0.0, 10.670599937438965, -1.0717999935150146]', '[1.0, 0.0, 10.67080020904541, 7.433000087738037]', '[1.0, 0.0, 10.678799629211426, 1.5261000394821167]', '[1.0, 0.0, 10.680299758911133, 0.7990999817848206]', '[1.0, 0.0, 10.685099601745605, -0.954800009727478]', '[1.0, 0.0, 10.68970012664795, -3.135200023651123]', '[1.0, 0.0, 10.68970012664795, -3.2397000789642334]', '[1.0, 0.0, 10.689800262451172, -2.135200023651123]', '[1.0, 0.0, 10.689800262451172, -2.2397000789642334]', '[1.0, 0.0, 10.69950008392334, -5.967800140380859]', '[1.0, 0.0, 10.707799911499023, -0.801800012588501]', '[1.0, 0.0, 10.707799911499023, -0.887499988079071]', '[1.0, 0.0, 10.707799911499023, 9.08650016784668]', '[1.0, 0.0, 10.720999717712402, -2.8396999835968018]', '[1.0, 0.0, 10.721500396728516, 0.7148000001907349]', '[1.0, 0.0, 10.742400169372559, 5.039700031280518]', '[1.0, 0.0, 10.748100280761719, -5.482900142669678]', '[1.0, 0.0, 10.748900413513184, 1.8930000066757202]', '[1.0, 0.0, 10.748900413513184, 2.8929998874664307]', '[1.0, 0.0, 10.768799781799316, 0.06620000302791595]', '[1.0, 0.0, 10.770899772644043, 2.8264000415802]', '[1.0, 0.0, 10.770899772644043, 3.6923999786376953]', '[1.0, 0.0, 10.770899772644043, 4.5584001541137695]', '[1.0, 0.0, 10.770899772644043, 5.4243998527526855]', '[1.0, 0.0, 10.781200408935547, -5.253900051116943]', '[1.0, 0.0, 10.79419994354248, -0.25]', '[1.0, 0.0, 10.79419994354248, -1.25]', '[1.0, 0.0, 10.79419994354248, -3.25]', '[1.0, 0.0, 10.838800430297852, 3.3415000438690186]', '[1.0, 0.0, 10.864800453186035, 1.1887999773025513]', '[1.0, 0.0, 10.865599632263184, 0.6111999750137329]', '[1.0, 0.0, 10.866299629211426, -0.8964999914169312]', '[1.0, 0.0, 10.876899719238281, -0.10360000282526016]', '[1.0, 0.0, 10.876899719238281, -2.4110000133514404]', '[1.0, 0.0, 10.876899719238281, -2.4967000484466553]', '[1.0, 0.0, 10.876899719238281, 7.477399826049805]', '[1.0, 0.0, 10.88290023803711, 0.09080000221729279]', '[1.0, 0.0, 10.906000137329102, -1.6196000576019287]', '[1.0, 0.0, 10.906000137329102, 1.7648999691009521]', '[1.0, 0.0, 10.906000137329102, 2.012700080871582]', '[1.0, 0.0, 10.906000137329102, 2.1171998977661133]', '[1.0, 0.0, 10.906000137329102, 3.9307000637054443]', '[1.0, 0.0, 10.90839958190918, 7.652599811553955]', '[1.0, 0.0, 10.913100242614746, 8.724900245666504]', '[1.0, 0.0, 10.91569995880127, 2.4837000370025635]', '[1.0, 0.0, 10.917699813842773, 3.8773000240325928]', '[1.0, 0.0, 10.923999786376953, 1.457200050354004]', '[1.0, 0.0, 10.928199768066406, -1.5]', '[1.0, 0.0, 10.928199768066406, -1.660599946975708]', '[1.0, 0.0, 10.928199768066406, -2.0]', '[1.0, 0.0, 10.928199768066406, -2.410599946975708]', '[1.0, 0.0, 10.928199768066406, -4.0]', '[1.0, 0.0, 10.928199768066406, 0.3393999934196472]', '[1.0, 0.0, 10.928199768066406, 0.5]', '[1.0, 0.0, 10.928199768066406, 1.75]', '[1.0, 0.0, 10.928199768066406, 2.75]', '[1.0, 0.0, 10.93690013885498, 0.5066999793052673]', '[1.0, 0.0, 10.963600158691406, 3.642899990081787]', '[1.0, 0.0, 10.963899612426758, 3.2730000019073486]', '[1.0, 0.0, 10.968199729919434, 5.068699836730957]', '[1.0, 0.0, 10.969300270080566, -4.086100101470947]', '[1.0, 0.0, 10.975700378417969, -2.0806000232696533]', '[1.0, 0.0, 10.978899955749512, 0.39579999446868896]', '[1.0, 0.0, 10.978899955749512, 1.395799994468689]', '[1.0, 0.0, 11.002900123596191, -0.43299999833106995]', '[1.0, 0.0, 11.005999565124512, -10.43970012664795]', '[1.0, 0.0, 11.005999565124512, -9.43970012664795]', '[1.0, 0.0, 11.01039981842041, -10.589900016784668]', '[1.0, 0.0, 11.01039981842041, -11.959600448608398]', '[1.0, 0.0, 11.01039981842041, -12.959600448608398]', '[1.0, 0.0, 11.01039981842041, -9.589900016784668]', '[1.0, 0.0, 11.02340030670166, -0.33500000834465027]', '[1.0, 0.0, 11.02340030670166, 0.424699991941452]', '[1.0, 0.0, 11.03969955444336, 6.082200050354004]', '[1.0, 0.0, 11.077699661254883, 0.45260000228881836]', '[1.0, 0.0, 11.077699661254883, 2.1847000122070312]', '[1.0, 0.0, 11.081399917602539, -1.7454999685287476]', '[1.0, 0.0, 11.081399917602539, 0.25450000166893005]', '[1.0, 0.0, 11.0871000289917, 0.19920000433921814]', '[1.0, 0.0, 11.0871000289917, 0.9036999940872192]', '[1.0, 0.0, 11.087400436401367, -3.236599922180176]', '[1.0, 0.0, 11.097700119018555, 6.795899868011475]', '[1.0, 0.0, 11.1318998336792, 0.47909998893737793]', '[1.0, 0.0, 11.144800186157227, -0.4713999927043915]', '[1.0, 0.0, 11.149399757385254, -3.7397000789642334]', '[1.0, 0.0, 11.160300254821777, 1.4514000415802002]', '[1.0, 0.0, 11.163900375366211, -4.330100059509277]', '[1.0, 0.0, 11.170000076293945, 7.094399929046631]', '[1.0, 0.0, 11.179400444030762, -2.823699951171875]', '[1.0, 0.0, 11.183500289916992, 0.09000000357627869]', '[1.0, 0.0, 11.183500289916992, 1.090000033378601]', '[1.0, 0.0, 11.183600425720215, -3.058799982070923]', '[1.0, 0.0, 11.185099601745605, -2.4937000274658203]', '[1.0, 0.0, 11.190199851989746, 10.089799880981445]', '[1.0, 0.0, 11.190400123596191, -3.00570011138916]', '[1.0, 0.0, 11.19950008392334, 1.030500054359436]', '[1.0, 0.0, 11.206299781799316, 0.06700000166893005]', '[1.0, 0.0, 11.206299781799316, 1.0670000314712524]', '[1.0, 0.0, 11.214200019836426, -0.6956999897956848]', '[1.0, 0.0, 11.214200019836426, -1.062600016593933]', '[1.0, 0.0, 11.217499732971191, 6.701499938964844]', '[1.0, 0.0, 11.231800079345703, -3.8222999572753906]', '[1.0, 0.0, 11.236100196838379, -0.704200029373169]', '[1.0, 0.0, 11.23799991607666, -0.12030000239610672]', '[1.0, 0.0, 11.23799991607666, -0.5248000025749207]', '[1.0, 0.0, 11.23799991607666, -2.120300054550171]', '[1.0, 0.0, 11.23799991607666, -2.5248000621795654]', '[1.0, 0.0, 11.284099578857422, 3.151400089263916]', '[1.0, 0.0, 11.289899826049805, -5.224899768829346]', '[1.0, 0.0, 11.289899826049805, -7.224899768829346]', '[1.0, 0.0, 11.289899826049805, -8.224900245666504]', '[1.0, 0.0, 11.305899620056152, 1.4393999576568604]', '[1.0, 0.0, 11.312800407409668, 2.469399929046631]', '[1.0, 0.0, 11.31309986114502, 2.861799955368042]', '[1.0, 0.0, 11.321499824523926, 7.0416998863220215]', '[1.0, 0.0, 11.336400032043457, -5.8196001052856445]', '[1.0, 0.0, 11.361100196838379, -2.2493999004364014]', '[1.0, 0.0, 11.376899719238281, -1.5448999404907227]', '[1.0, 0.0, 11.376899719238281, -1.6306999921798706]', '[1.0, 0.0, 11.376899719238281, 8.343400001525879]', '[1.0, 0.0, 11.383500099182129, -2.0292000770568848]', '[1.0, 0.0, 11.383500099182129, 2.1189000606536865]', '[1.0, 0.0, 11.412199974060059, 4.946000099182129]', '[1.0, 0.0, 11.421099662780762, -3.0367000102996826]', '[1.0, 0.0, 11.422100067138672, 3.6270999908447266]', '[1.0, 0.0, 11.43690013885498, 2.3069000244140625]', '[1.0, 0.0, 11.452899932861328, 4.251100063323975]', '[1.0, 0.0, 11.453399658203125, -0.19779999554157257]', '[1.0, 0.0, 11.462300300598145, -1.5240999460220337]', '[1.0, 0.0, 11.462599754333496, 1.497499942779541]', '[1.0, 0.0, 11.464699745178223, 0.04569999873638153]', '[1.0, 0.0, 11.477800369262695, 11.190099716186523]', '[1.0, 0.0, 11.479000091552734, 8.04539966583252]', '[1.0, 0.0, 11.490599632263184, -5.356100082397461]', '[1.0, 0.0, 11.493800163269043, -2.4286000728607178]', '[1.0, 0.0, 11.493800163269043, 0.9036999940872192]', '[1.0, 0.0, 11.493800163269043, 1.2559000253677368]', '[1.0, 0.0, 11.493800163269043, 1.3082000017166138]', '[1.0, 0.0, 11.493800163269043, 1.4127000570297241]', '[1.0, 0.0, 11.493800163269043, 1.7648999691009521]', '[1.0, 0.0, 11.493800163269043, 3.1217000484466553]', '[1.0, 0.0, 11.502900123596191, 0.43299999833106995]', '[1.0, 0.0, 11.50879955291748, -0.23199999332427979]', '[1.0, 0.0, 11.50879955291748, -0.5490000247955322]', '[1.0, 0.0, 11.50879955291748, -1.2319999933242798]', '[1.0, 0.0, 11.50879955291748, -1.5490000247955322]', '[1.0, 0.0, 11.50879955291748, -3.5490000247955322]', '[1.0, 0.0, 11.50879955291748, -4.23199987411499]', '[1.0, 0.0, 11.526200294494629, -0.8889999985694885]', '[1.0, 0.0, 11.526200294494629, -2.25]', '[1.0, 0.0, 11.526200294494629, -3.25]', '[1.0, 0.0, 11.526200294494629, -4.25]', '[1.0, 0.0, 11.526200294494629, -4.75]', '[1.0, 0.0, 11.526200294494629, -5.75]', '[1.0, 0.0, 11.526300430297852, -0.06700000166893005]', '[1.0, 0.0, 11.526300430297852, -0.16060000658035278]', '[1.0, 0.0, 11.526300430297852, -0.25]', '[1.0, 0.0, 11.526300430297852, -0.31700000166893005]', '[1.0, 0.0, 11.526300430297852, -0.5669999718666077]', '[1.0, 0.0, 11.526300430297852, -0.5]', '[1.0, 0.0, 11.526300430297852, -0.75]', '[1.0, 0.0, 11.526300430297852, -0.8169999718666077]', '[1.0, 0.0, 11.526300430297852, -0.9106000065803528]', '[1.0, 0.0, 11.526300430297852, -1.0]', '[1.0, 0.0, 11.526300430297852, -1.25]', '[1.0, 0.0, 11.526300430297852, -1.2978999614715576]', '[1.0, 0.0, 11.526300430297852, -1.587499976158142]', '[1.0, 0.0, 11.526300430297852, -1.5]', '[1.0, 0.0, 11.526300430297852, -1.75]', '[1.0, 0.0, 11.526300430297852, -1.910599946975708]', '[1.0, 0.0, 11.526300430297852, -2.066999912261963]', '[1.0, 0.0, 11.526300430297852, -2.0]', '[1.0, 0.0, 11.526300430297852, -2.160599946975708]', '[1.0, 0.0, 11.526300430297852, -2.2978999614715576]', '[1.0, 0.0, 11.526300430297852, -2.5]', '[1.0, 0.0, 11.526300430297852, -3.066999912261963]', '[1.0, 0.0, 11.526300430297852, -3.0]', '[1.0, 0.0, 11.526300430297852, -3.25]', '[1.0, 0.0, 11.526300430297852, -4.0]', '[1.0, 0.0, 11.526300430297852, 0.08940000087022781]', '[1.0, 0.0, 11.526300430297852, 0.0]', '[1.0, 0.0, 11.526300430297852, 0.18299999833106995]', '[1.0, 0.0, 11.526300430297852, 0.25]', '[1.0, 0.0, 11.526300430297852, 0.43299999833106995]', '[1.0, 0.0, 11.526300430297852, 0.5]', '[1.0, 0.0, 11.526300430297852, 0.6830000281333923]', '[1.0, 0.0, 11.526300430297852, 0.75]', '[1.0, 0.0, 11.526300430297852, 0.8393999934196472]', '[1.0, 0.0, 11.526300430297852, 0.9330000281333923]', '[1.0, 0.0, 11.526300430297852, 1.0670000314712524]', '[1.0, 0.0, 11.526300430297852, 1.0]', '[1.0, 0.0, 11.526300430297852, 1.1829999685287476]', '[1.0, 0.0, 11.526300430297852, 1.25]', '[1.0, 0.0, 11.526300430297852, 1.4329999685287476]', '[1.0, 0.0, 11.526300430297852, 1.5670000314712524]', '[1.0, 0.0, 11.526300430297852, 1.5]', '[1.0, 0.0, 11.526300430297852, 1.75]', '[1.0, 0.0, 11.526300430297852, 2.066999912261963]', '[1.0, 0.0, 11.526300430297852, 2.0]', '[1.0, 0.0, 11.526300430297852, 2.183000087738037]', '[1.0, 0.0, 11.526300430297852, 2.25]', '[1.0, 0.0, 11.526300430297852, 2.5]', '[1.0, 0.0, 11.526300430297852, 2.75]', '[1.0, 0.0, 11.526300430297852, 2.9828999042510986]', '[1.0, 0.0, 11.526300430297852, 3.066999912261963]', '[1.0, 0.0, 11.526300430297852, 3.0]', '[1.0, 0.0, 11.526300430297852, 3.433000087738037]', '[1.0, 0.0, 11.526300430297852, 3.5]', '[1.0, 0.0, 11.526300430297852, 3.75]', '[1.0, 0.0, 11.526300430297852, 3.9828999042510986]', '[1.0, 0.0, 11.526300430297852, 4.066999912261963]', '[1.0, 0.0, 11.526300430297852, 4.5]', '[1.0, 0.0, 11.526300430297852, 5.066999912261963]', '[1.0, 0.0, 11.526300430297852, 5.5]', '[1.0, 0.0, 11.526300430297852, 5.75]', '[1.0, 0.0, 11.526300430297852, 6.066999912261963]', '[1.0, 0.0, 11.526300430297852, 6.0]', '[1.0, 0.0, 11.526300430297852, 6.25]', '[1.0, 0.0, 11.526300430297852, 7.066999912261963]', '[1.0, 0.0, 11.526300430297852, 7.0]', '[1.0, 0.0, 11.526300430297852, 7.25]', '[1.0, 0.0, 11.526300430297852, 8.75]', '[1.0, 0.0, 11.526399612426758, 9.75]', '[1.0, 0.0, 11.555800437927246, -3.635200023651123]', '[1.0, 0.0, 11.555800437927246, -3.7397000789642334]', '[1.0, 0.0, 11.566900253295898, -0.5435000061988831]', '[1.0, 0.0, 11.571900367736816, 1.895900011062622]', '[1.0, 0.0, 11.5871000289917, -1.3396999835968018]', '[1.0, 0.0, 11.5871000289917, -4.339700222015381]', '[1.0, 0.0, 11.590299606323242, -2.672600030899048]', '[1.0, 0.0, 11.591099739074707, -2.5302999019622803]', '[1.0, 0.0, 11.592300415039062, 1.1194000244140625]', '[1.0, 0.0, 11.611200332641602, 2.706399917602539]', '[1.0, 0.0, 11.611300468444824, -0.20800000429153442]', '[1.0, 0.0, 11.611300468444824, -1.8260999917984009]', '[1.0, 0.0, 11.636899948120117, -0.8799999952316284]', '[1.0, 0.0, 11.644200325012207, 4.845600128173828]', '[1.0, 0.0, 11.644800186157227, -1.337499976158142]', '[1.0, 0.0, 11.64490032196045, -5.97629976272583]', '[1.0, 0.0, 11.660200119018555, -1.75]', '[1.0, 0.0, 11.660300254821777, 0.25]', '[1.0, 0.0, 11.660300254821777, 0.5]', '[1.0, 0.0, 11.660300254821777, 1.5]', '[1.0, 0.0, 11.66100025177002, 7.622200012207031]', '[1.0, 0.0, 11.670999526977539, 0.6341000199317932]', '[1.0, 0.0, 11.670999526977539, 2.5659000873565674]', '[1.0, 0.0, 11.670999526977539, 3.98009991645813]', '[1.0, 0.0, 11.67490005493164, 0.9036999940872192]', '[1.0, 0.0, 11.692500114440918, 1.1678999662399292]', '[1.0, 0.0, 11.69260025024414, -1.0781999826431274]', '[1.0, 0.0, 11.717499732971191, 8.240400314331055]', '[1.0, 0.0, 11.717499732971191, 9.240400314331055]', '[1.0, 0.0, 11.743599891662598, 3.8131000995635986]', '[1.0, 0.0, 11.74370002746582, -3.723400115966797]', '[1.0, 0.0, 11.748100280761719, 2.2604000568389893]', '[1.0, 0.0, 11.770899772644043, 2.8264000415802]', '[1.0, 0.0, 11.770899772644043, 3.6923999786376953]', '[1.0, 0.0, 11.770899772644043, 4.5584001541137695]', '[1.0, 0.0, 11.770899772644043, 5.4243998527526855]', '[1.0, 0.0, 11.772899627685547, -3.3027000427246094]', '[1.0, 0.0, 11.783699989318848, 5.377299785614014]', '[1.0, 0.0, 11.79419994354248, -0.16060000658035278]', '[1.0, 0.0, 11.79419994354248, -0.9106000065803528]', '[1.0, 0.0, 11.79419994354248, -1.0]', '[1.0, 0.0, 11.79419994354248, -1.160599946975708]', '[1.0, 0.0, 11.79419994354248, -1.910599946975708]', '[1.0, 0.0, 11.79419994354248, -2.5]', '[1.0, 0.0, 11.79419994354248, -3.5]', '[1.0, 0.0, 11.79419994354248, 0.0]', '[1.0, 0.0, 11.79419994354248, 0.8393999934196472]', '[1.0, 0.0, 11.79419994354248, 2.0]', '[1.0, 0.0, 11.79419994354248, 3.0]', '[1.0, 0.0, 11.844900131225586, -0.10419999808073044]', '[1.0, 0.0, 11.844900131225586, 1.895799994468689]', '[1.0, 0.0, 11.876500129699707, -13.459600448608398]', '[1.0, 0.0, 11.876500129699707, -14.459600448608398]', '[1.0, 0.0, 11.888199806213379, 6.3719000816345215]', '[1.0, 0.0, 11.90060043334961, 1.6604000329971313]', '[1.0, 0.0, 11.90060043334961, 2.1171998977661133]', '[1.0, 0.0, 11.920299530029297, -2.777100086212158]', '[1.0, 0.0, 11.920299530029297, -4.395199775695801]', '[1.0, 0.0, 11.929800033569336, 1.600000023841858]', '[1.0, 0.0, 11.939000129699707, 12.911399841308594]', '[1.0, 0.0, 11.947400093078613, -0.24549999833106995]', '[1.0, 0.0, 11.947400093078613, -1.2454999685287476]', '[1.0, 0.0, 11.947400093078613, 0.7544999718666077]', '[1.0, 0.0, 11.953200340270996, 3.8945999145507812]', '[1.0, 0.0, 11.953399658203125, -1.7366000413894653]', '[1.0, 0.0, 11.953399658203125, -4.736599922180176]', '[1.0, 0.0, 11.954000473022461, -5.025199890136719]', '[1.0, 0.0, 11.977800369262695, 10.32409954071045]', '[1.0, 0.0, 12.010899543762207, 0.028599999845027924]', '[1.0, 0.0, 12.031700134277344, 6.1006999015808105]', '[1.0, 0.0, 12.05270004272461, -2.77239990234375]', '[1.0, 0.0, 12.05270004272461, 2.8620998859405518]', '[1.0, 0.0, 12.05620002746582, 8.589799880981445]', '[1.0, 0.0, 12.07229995727539, -0.43299999833106995]', '[1.0, 0.0, 12.07229995727539, 1.5670000314712524]', '[1.0, 0.0, 12.077699661254883, 0.45260000228881836]', '[1.0, 0.0, 12.081600189208984, 0.44690001010894775]', '[1.0, 0.0, 12.081600189208984, 0.9559000134468079]', '[1.0, 0.0, 12.081600189208984, 1.0082000494003296]', '[1.0, 0.0, 12.0871000289917, 0.19920000433921814]', '[1.0, 0.0, 12.104100227355957, -0.6202999949455261]', '[1.0, 0.0, 12.104100227355957, -1.0247999429702759]', '[1.0, 0.0, 12.104100227355957, -1.620300054550171]', '[1.0, 0.0, 12.104100227355957, -2.0248000621795654]', '[1.0, 0.0, 12.12279987335205, -4.276299953460693]', '[1.0, 0.0, 12.12279987335205, 1.523800015449524]', '[1.0, 0.0, 12.126399993896484, -2.1565001010894775]', '[1.0, 0.0, 12.136300086975098, 5.106100082397461]', '[1.0, 0.0, 12.136899948120117, -1.7460999488830566]', '[1.0, 0.0, 12.155900001525879, -8.724900245666504]', '[1.0, 0.0, 12.159700393676758, -4.6128997802734375]', '[1.0, 0.0, 12.165200233459473, -1.004699945449829]', '[1.0, 0.0, 12.165200233459473, -1.3716000318527222]', '[1.0, 0.0, 12.165200233459473, 4.296199798583984]', '[1.0, 0.0, 12.175100326538086, -5.275000095367432]', '[1.0, 0.0, 12.177000045776367, -1.0428999662399292]', '[1.0, 0.0, 12.180000305175781, 1.6376999616622925]', '[1.0, 0.0, 12.19909954071045, -1.0169999599456787]', '[1.0, 0.0, 12.2298002243042, 1.0566999912261963]', '[1.0, 0.0, 12.253100395202637, 6.728499889373779]', '[1.0, 0.0, 12.258299827575684, -3.25]', '[1.0, 0.0, 12.26259994506836, 0.09459999948740005]', '[1.0, 0.0, 12.270899772644043, 3.6923999786376953]', '[1.0, 0.0, 12.270899772644043, 4.5584001541137695]', '[1.0, 0.0, 12.278200149536133, -1.1217000484466553]', '[1.0, 0.0, 12.288700103759766, -1.277400016784668]', '[1.0, 0.0, 12.330699920654297, 0.5457000136375427]', '[1.0, 0.0, 12.354100227355957, -2.027100086212158]', '[1.0, 0.0, 12.35569953918457, -2.14490008354187]', '[1.0, 0.0, 12.360300064086914, 0.06530000269412994]', '[1.0, 0.0, 12.363200187683105, -1.957900047302246]', '[1.0, 0.0, 12.374799728393555, -0.04899999871850014]', '[1.0, 0.0, 12.374799728393555, -1.7319999933242798]', '[1.0, 0.0, 12.374799728393555, -2.0490000247955322]', '[1.0, 0.0, 12.374799728393555, -3.0490000247955322]', '[1.0, 0.0, 12.378100395202637, 3.2730000019073486]', '[1.0, 0.0, 12.392200469970703, -4.75]', '[1.0, 0.0, 12.392200469970703, -5.75]', '[1.0, 0.0, 12.39229965209961, -0.25]', '[1.0, 0.0, 12.39229965209961, -0.4106000065803528]', '[1.0, 0.0, 12.39229965209961, -0.5669999718666077]', '[1.0, 0.0, 12.39229965209961, -0.5]', '[1.0, 0.0, 12.39229965209961, -0.6606000065803528]', '[1.0, 0.0, 12.39229965209961, -0.75]', '[1.0, 0.0, 12.39229965209961, -0.8169999718666077]', '[1.0, 0.0, 12.39229965209961, -1.0]', '[1.0, 0.0, 12.39229965209961, -1.25]', '[1.0, 0.0, 12.39229965209961, -1.5]', '[1.0, 0.0, 12.39229965209961, -1.660599946975708]', '[1.0, 0.0, 12.39229965209961, -1.75]', '[1.0, 0.0, 12.39229965209961, -2.0]', '[1.0, 0.0, 12.39229965209961, -2.3889999389648438]', '[1.0, 0.0, 12.39229965209961, -2.410599946975708]', '[1.0, 0.0, 12.39229965209961, -2.5]', '[1.0, 0.0, 12.39229965209961, -2.75]', '[1.0, 0.0, 12.39229965209961, -4.25]', '[1.0, 0.0, 12.39229965209961, -5.25]', '[1.0, 0.0, 12.39229965209961, -6.25]', '[1.0, 0.0, 12.39229965209961, 0.0]', '[1.0, 0.0, 12.39229965209961, 0.25]', '[1.0, 0.0, 12.39229965209961, 0.5893999934196472]', '[1.0, 0.0, 12.39229965209961, 0.5]', '[1.0, 0.0, 12.39229965209961, 0.6830000281333923]', '[1.0, 0.0, 12.39229965209961, 0.75]', '[1.0, 0.0, 12.39229965209961, 1.0]', '[1.0, 0.0, 12.39229965209961, 1.1829999685287476]', '[1.0, 0.0, 12.39229965209961, 1.25]', '[1.0, 0.0, 12.39229965209961, 1.339400053024292]', '[1.0, 0.0, 12.39229965209961, 1.4329999685287476]', '[1.0, 0.0, 12.39229965209961, 1.5670000314712524]', '[1.0, 0.0, 12.39229965209961, 1.5]', '[1.0, 0.0, 12.39229965209961, 1.75]', '[1.0, 0.0, 12.39229965209961, 1.9329999685287476]', '[1.0, 0.0, 12.39229965209961, 2.0]', '[1.0, 0.0, 12.39229965209961, 2.25]', '[1.0, 0.0, 12.39229965209961, 2.316999912261963]', '[1.0, 0.0, 12.39229965209961, 2.4830000400543213]', '[1.0, 0.0, 12.39229965209961, 2.566999912261963]', '[1.0, 0.0, 12.39229965209961, 2.5]', '[1.0, 0.0, 12.39229965209961, 2.683000087738037]', '[1.0, 0.0, 12.39229965209961, 2.75]', '[1.0, 0.0, 12.39229965209961, 2.933000087738037]', '[1.0, 0.0, 12.39229965209961, 3.0]', '[1.0, 0.0, 12.39229965209961, 3.316999912261963]', '[1.0, 0.0, 12.39229965209961, 3.5]', '[1.0, 0.0, 12.39229965209961, 4.25]', '[1.0, 0.0, 12.392399787902832, 10.25]', '[1.0, 0.0, 12.392399787902832, 4.25]', '[1.0, 0.0, 12.392399787902832, 5.25]', '[1.0, 0.0, 12.392399787902832, 8.25]', '[1.0, 0.0, 12.396100044250488, -0.7519000172615051]', '[1.0, 0.0, 12.401599884033203, -3.389899969100952]', '[1.0, 0.0, 12.412799835205078, -4.466599941253662]', '[1.0, 0.0, 12.412799835205078, 4.556300163269043]', '[1.0, 0.0, 12.426300048828125, 6.599299907684326]', '[1.0, 0.0, 12.445199966430664, -1.2336000204086304]', '[1.0, 0.0, 12.453100204467773, -2.8396999835968018]', '[1.0, 0.0, 12.453100204467773, -3.8396999835968018]', '[1.0, 0.0, </t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="B350" t="inlineStr"/>
+      <c r="C350" t="inlineStr"/>
+      <c r="D350" t="inlineStr"/>
+      <c r="E350" t="inlineStr"/>
+      <c r="F350" t="inlineStr"/>
+      <c r="G350" t="inlineStr"/>
+      <c r="H350" t="inlineStr"/>
+      <c r="I350" t="inlineStr"/>
+      <c r="J350" t="inlineStr"/>
+      <c r="K350" t="inlineStr"/>
+      <c r="L350" t="inlineStr"/>
+      <c r="M350" t="inlineStr"/>
+      <c r="N350" t="inlineStr">
+        <is>
+          <t>['0', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="B351" t="inlineStr"/>
+      <c r="C351" t="inlineStr"/>
+      <c r="D351" t="inlineStr"/>
+      <c r="E351" t="inlineStr"/>
+      <c r="F351" t="inlineStr"/>
+      <c r="G351" t="inlineStr"/>
+      <c r="H351" t="inlineStr"/>
+      <c r="I351" t="inlineStr"/>
+      <c r="J351" t="inlineStr"/>
+      <c r="K351" t="inlineStr"/>
+      <c r="L351" t="inlineStr"/>
+      <c r="M351" t="inlineStr"/>
+      <c r="N351" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B352" t="inlineStr"/>
+      <c r="C352" t="inlineStr"/>
+      <c r="D352" t="inlineStr"/>
+      <c r="E352" t="inlineStr"/>
+      <c r="F352" t="inlineStr"/>
+      <c r="G352" t="inlineStr"/>
+      <c r="H352" t="inlineStr"/>
+      <c r="I352" t="inlineStr"/>
+      <c r="J352" t="inlineStr"/>
+      <c r="K352" t="inlineStr"/>
+      <c r="L352" t="inlineStr"/>
+      <c r="M352" t="inlineStr"/>
+      <c r="N352" t="inlineStr">
+        <is>
+          <t>[23835  8375   180]</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B353" t="inlineStr"/>
+      <c r="C353" t="inlineStr"/>
+      <c r="D353" t="inlineStr"/>
+      <c r="E353" t="inlineStr"/>
+      <c r="F353" t="inlineStr"/>
+      <c r="G353" t="inlineStr"/>
+      <c r="H353" t="inlineStr"/>
+      <c r="I353" t="inlineStr"/>
+      <c r="J353" t="inlineStr"/>
+      <c r="K353" t="inlineStr"/>
+      <c r="L353" t="inlineStr"/>
+      <c r="M353" t="inlineStr"/>
+      <c r="N353" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="B354" t="inlineStr"/>
+      <c r="C354" t="inlineStr"/>
+      <c r="D354" t="inlineStr"/>
+      <c r="E354" t="inlineStr"/>
+      <c r="F354" t="inlineStr"/>
+      <c r="G354" t="inlineStr"/>
+      <c r="H354" t="inlineStr"/>
+      <c r="I354" t="inlineStr"/>
+      <c r="J354" t="inlineStr"/>
+      <c r="K354" t="inlineStr"/>
+      <c r="L354" t="inlineStr"/>
+      <c r="M354" t="inlineStr"/>
+      <c r="N354" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="B355" t="inlineStr"/>
+      <c r="C355" t="inlineStr"/>
+      <c r="D355" t="inlineStr"/>
+      <c r="E355" t="inlineStr"/>
+      <c r="F355" t="inlineStr"/>
+      <c r="G355" t="inlineStr"/>
+      <c r="H355" t="inlineStr"/>
+      <c r="I355" t="inlineStr"/>
+      <c r="J355" t="inlineStr"/>
+      <c r="K355" t="inlineStr"/>
+      <c r="L355" t="inlineStr"/>
+      <c r="M355" t="inlineStr"/>
+      <c r="N355" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B356" t="inlineStr"/>
+      <c r="C356" t="inlineStr"/>
+      <c r="D356" t="inlineStr"/>
+      <c r="E356" t="inlineStr"/>
+      <c r="F356" t="inlineStr"/>
+      <c r="G356" t="inlineStr"/>
+      <c r="H356" t="inlineStr"/>
+      <c r="I356" t="inlineStr"/>
+      <c r="J356" t="inlineStr"/>
+      <c r="K356" t="inlineStr"/>
+      <c r="L356" t="inlineStr"/>
+      <c r="M356" t="inlineStr"/>
+      <c r="N356" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="B357" t="inlineStr"/>
+      <c r="C357" t="inlineStr"/>
+      <c r="D357" t="inlineStr"/>
+      <c r="E357" t="inlineStr"/>
+      <c r="F357" t="inlineStr"/>
+      <c r="G357" t="inlineStr"/>
+      <c r="H357" t="inlineStr"/>
+      <c r="I357" t="inlineStr"/>
+      <c r="J357" t="inlineStr"/>
+      <c r="K357" t="inlineStr"/>
+      <c r="L357" t="inlineStr"/>
+      <c r="M357" t="inlineStr"/>
+      <c r="N357" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="B358" t="inlineStr"/>
+      <c r="C358" t="inlineStr"/>
+      <c r="D358" t="inlineStr"/>
+      <c r="E358" t="inlineStr"/>
+      <c r="F358" t="inlineStr"/>
+      <c r="G358" t="inlineStr"/>
+      <c r="H358" t="inlineStr"/>
+      <c r="I358" t="inlineStr"/>
+      <c r="J358" t="inlineStr"/>
+      <c r="K358" t="inlineStr"/>
+      <c r="L358" t="inlineStr"/>
+      <c r="M358" t="inlineStr"/>
+      <c r="N358" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B359" t="inlineStr"/>
+      <c r="C359" t="inlineStr"/>
+      <c r="D359" t="inlineStr"/>
+      <c r="E359" t="inlineStr"/>
+      <c r="F359" t="inlineStr"/>
+      <c r="G359" t="inlineStr"/>
+      <c r="H359" t="inlineStr"/>
+      <c r="I359" t="inlineStr"/>
+      <c r="J359" t="inlineStr"/>
+      <c r="K359" t="inlineStr"/>
+      <c r="L359" t="inlineStr"/>
+      <c r="M359" t="inlineStr"/>
+      <c r="N359" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="B360" t="inlineStr"/>
+      <c r="C360" t="inlineStr"/>
+      <c r="D360" t="inlineStr"/>
+      <c r="E360" t="inlineStr"/>
+      <c r="F360" t="inlineStr"/>
+      <c r="G360" t="inlineStr"/>
+      <c r="H360" t="inlineStr"/>
+      <c r="I360" t="inlineStr"/>
+      <c r="J360" t="inlineStr"/>
+      <c r="K360" t="inlineStr"/>
+      <c r="L360" t="inlineStr"/>
+      <c r="M360" t="inlineStr"/>
+      <c r="N360" t="n">
+        <v>14.55840455840456</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="B361" t="inlineStr"/>
+      <c r="C361" t="inlineStr"/>
+      <c r="D361" t="inlineStr"/>
+      <c r="E361" t="inlineStr"/>
+      <c r="F361" t="inlineStr"/>
+      <c r="G361" t="inlineStr"/>
+      <c r="H361" t="inlineStr"/>
+      <c r="I361" t="inlineStr"/>
+      <c r="J361" t="inlineStr"/>
+      <c r="K361" t="inlineStr"/>
+      <c r="L361" t="inlineStr"/>
+      <c r="M361" t="inlineStr"/>
+      <c r="N361" t="n">
+        <v>15.002849002849</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B362" t="inlineStr"/>
+      <c r="C362" t="inlineStr"/>
+      <c r="D362" t="inlineStr"/>
+      <c r="E362" t="inlineStr"/>
+      <c r="F362" t="inlineStr"/>
+      <c r="G362" t="inlineStr"/>
+      <c r="H362" t="inlineStr"/>
+      <c r="I362" t="inlineStr"/>
+      <c r="J362" t="inlineStr"/>
+      <c r="K362" t="inlineStr"/>
+      <c r="L362" t="inlineStr"/>
+      <c r="M362" t="inlineStr"/>
+      <c r="N362" t="inlineStr">
+        <is>
+          <t>{0: 0.6552706552706553, 1: 0.34472934472934474}</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="n">
+        <v>361</v>
+      </c>
+      <c r="B363" t="inlineStr"/>
+      <c r="C363" t="inlineStr"/>
+      <c r="D363" t="inlineStr"/>
+      <c r="E363" t="inlineStr"/>
+      <c r="F363" t="inlineStr"/>
+      <c r="G363" t="inlineStr"/>
+      <c r="H363" t="inlineStr"/>
+      <c r="I363" t="inlineStr"/>
+      <c r="J363" t="inlineStr"/>
+      <c r="K363" t="inlineStr"/>
+      <c r="L363" t="inlineStr"/>
+      <c r="M363" t="inlineStr"/>
+      <c r="N363" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '2', '3', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="n">
+        <v>362</v>
+      </c>
+      <c r="B364" t="inlineStr"/>
+      <c r="C364" t="inlineStr"/>
+      <c r="D364" t="inlineStr"/>
+      <c r="E364" t="inlineStr"/>
+      <c r="F364" t="inlineStr"/>
+      <c r="G364" t="inlineStr"/>
+      <c r="H364" t="inlineStr"/>
+      <c r="I364" t="inlineStr"/>
+      <c r="J364" t="inlineStr"/>
+      <c r="K364" t="inlineStr"/>
+      <c r="L364" t="inlineStr"/>
+      <c r="M364" t="inlineStr"/>
+      <c r="N364" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="n">
+        <v>363</v>
+      </c>
+      <c r="B365" t="inlineStr"/>
+      <c r="C365" t="inlineStr"/>
+      <c r="D365" t="inlineStr"/>
+      <c r="E365" t="inlineStr"/>
+      <c r="F365" t="inlineStr"/>
+      <c r="G365" t="inlineStr"/>
+      <c r="H365" t="inlineStr"/>
+      <c r="I365" t="inlineStr"/>
+      <c r="J365" t="inlineStr"/>
+      <c r="K365" t="inlineStr"/>
+      <c r="L365" t="inlineStr"/>
+      <c r="M365" t="inlineStr"/>
+      <c r="N365" t="inlineStr">
+        <is>
+          <t>[   1   23    1    1    2    1    3    1    1    1    1  721  408   29
+ 3493  269  100   44   10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="n">
+        <v>364</v>
+      </c>
+      <c r="B366" t="inlineStr"/>
+      <c r="C366" t="inlineStr"/>
+      <c r="D366" t="inlineStr"/>
+      <c r="E366" t="inlineStr"/>
+      <c r="F366" t="inlineStr"/>
+      <c r="G366" t="inlineStr"/>
+      <c r="H366" t="inlineStr"/>
+      <c r="I366" t="inlineStr"/>
+      <c r="J366" t="inlineStr"/>
+      <c r="K366" t="inlineStr"/>
+      <c r="L366" t="inlineStr"/>
+      <c r="M366" t="inlineStr"/>
+      <c r="N366" t="inlineStr">
+        <is>
+          <t>[   7  436 2772 2051]</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="n">
+        <v>365</v>
+      </c>
+      <c r="B367" t="inlineStr"/>
+      <c r="C367" t="inlineStr"/>
+      <c r="D367" t="inlineStr"/>
+      <c r="E367" t="inlineStr"/>
+      <c r="F367" t="inlineStr"/>
+      <c r="G367" t="inlineStr"/>
+      <c r="H367" t="inlineStr"/>
+      <c r="I367" t="inlineStr"/>
+      <c r="J367" t="inlineStr"/>
+      <c r="K367" t="inlineStr"/>
+      <c r="L367" t="inlineStr"/>
+      <c r="M367" t="inlineStr"/>
+      <c r="N367" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="B368" t="inlineStr"/>
+      <c r="C368" t="inlineStr"/>
+      <c r="D368" t="inlineStr"/>
+      <c r="E368" t="inlineStr"/>
+      <c r="F368" t="inlineStr"/>
+      <c r="G368" t="inlineStr"/>
+      <c r="H368" t="inlineStr"/>
+      <c r="I368" t="inlineStr"/>
+      <c r="J368" t="inlineStr"/>
+      <c r="K368" t="inlineStr"/>
+      <c r="L368" t="inlineStr"/>
+      <c r="M368" t="inlineStr"/>
+      <c r="N368" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="B369" t="inlineStr"/>
+      <c r="C369" t="inlineStr"/>
+      <c r="D369" t="inlineStr"/>
+      <c r="E369" t="inlineStr"/>
+      <c r="F369" t="inlineStr"/>
+      <c r="G369" t="inlineStr"/>
+      <c r="H369" t="inlineStr"/>
+      <c r="I369" t="inlineStr"/>
+      <c r="J369" t="inlineStr"/>
+      <c r="K369" t="inlineStr"/>
+      <c r="L369" t="inlineStr"/>
+      <c r="M369" t="inlineStr"/>
+      <c r="N369" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="B370" t="inlineStr"/>
+      <c r="C370" t="inlineStr"/>
+      <c r="D370" t="inlineStr"/>
+      <c r="E370" t="inlineStr"/>
+      <c r="F370" t="inlineStr"/>
+      <c r="G370" t="inlineStr"/>
+      <c r="H370" t="inlineStr"/>
+      <c r="I370" t="inlineStr"/>
+      <c r="J370" t="inlineStr"/>
+      <c r="K370" t="inlineStr"/>
+      <c r="L370" t="inlineStr"/>
+      <c r="M370" t="inlineStr"/>
+      <c r="N370" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="B371" t="inlineStr"/>
+      <c r="C371" t="inlineStr"/>
+      <c r="D371" t="inlineStr"/>
+      <c r="E371" t="inlineStr"/>
+      <c r="F371" t="inlineStr"/>
+      <c r="G371" t="inlineStr"/>
+      <c r="H371" t="inlineStr"/>
+      <c r="I371" t="inlineStr"/>
+      <c r="J371" t="inlineStr"/>
+      <c r="K371" t="inlineStr"/>
+      <c r="L371" t="inlineStr"/>
+      <c r="M371" t="inlineStr"/>
+      <c r="N371" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="B372" t="inlineStr"/>
+      <c r="C372" t="inlineStr"/>
+      <c r="D372" t="inlineStr"/>
+      <c r="E372" t="inlineStr"/>
+      <c r="F372" t="inlineStr"/>
+      <c r="G372" t="inlineStr"/>
+      <c r="H372" t="inlineStr"/>
+      <c r="I372" t="inlineStr"/>
+      <c r="J372" t="inlineStr"/>
+      <c r="K372" t="inlineStr"/>
+      <c r="L372" t="inlineStr"/>
+      <c r="M372" t="inlineStr"/>
+      <c r="N372" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="n">
+        <v>371</v>
+      </c>
+      <c r="B373" t="inlineStr"/>
+      <c r="C373" t="inlineStr"/>
+      <c r="D373" t="inlineStr"/>
+      <c r="E373" t="inlineStr"/>
+      <c r="F373" t="inlineStr"/>
+      <c r="G373" t="inlineStr"/>
+      <c r="H373" t="inlineStr"/>
+      <c r="I373" t="inlineStr"/>
+      <c r="J373" t="inlineStr"/>
+      <c r="K373" t="inlineStr"/>
+      <c r="L373" t="inlineStr"/>
+      <c r="M373" t="inlineStr"/>
+      <c r="N373" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="n">
+        <v>372</v>
+      </c>
+      <c r="B374" t="inlineStr"/>
+      <c r="C374" t="inlineStr"/>
+      <c r="D374" t="inlineStr"/>
+      <c r="E374" t="inlineStr"/>
+      <c r="F374" t="inlineStr"/>
+      <c r="G374" t="inlineStr"/>
+      <c r="H374" t="inlineStr"/>
+      <c r="I374" t="inlineStr"/>
+      <c r="J374" t="inlineStr"/>
+      <c r="K374" t="inlineStr"/>
+      <c r="L374" t="inlineStr"/>
+      <c r="M374" t="inlineStr"/>
+      <c r="N374" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="B375" t="inlineStr"/>
+      <c r="C375" t="inlineStr"/>
+      <c r="D375" t="inlineStr"/>
+      <c r="E375" t="inlineStr"/>
+      <c r="F375" t="inlineStr"/>
+      <c r="G375" t="inlineStr"/>
+      <c r="H375" t="inlineStr"/>
+      <c r="I375" t="inlineStr"/>
+      <c r="J375" t="inlineStr"/>
+      <c r="K375" t="inlineStr"/>
+      <c r="L375" t="inlineStr"/>
+      <c r="M375" t="inlineStr"/>
+      <c r="N375" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="B376" t="inlineStr"/>
+      <c r="C376" t="inlineStr"/>
+      <c r="D376" t="inlineStr"/>
+      <c r="E376" t="inlineStr"/>
+      <c r="F376" t="inlineStr"/>
+      <c r="G376" t="inlineStr"/>
+      <c r="H376" t="inlineStr"/>
+      <c r="I376" t="inlineStr"/>
+      <c r="J376" t="inlineStr"/>
+      <c r="K376" t="inlineStr"/>
+      <c r="L376" t="inlineStr"/>
+      <c r="M376" t="inlineStr"/>
+      <c r="N376" t="inlineStr">
+        <is>
+          <t>{0: 0.9333333333333333, 1: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="B377" t="inlineStr"/>
+      <c r="C377" t="inlineStr"/>
+      <c r="D377" t="inlineStr"/>
+      <c r="E377" t="inlineStr"/>
+      <c r="F377" t="inlineStr"/>
+      <c r="G377" t="inlineStr"/>
+      <c r="H377" t="inlineStr"/>
+      <c r="I377" t="inlineStr"/>
+      <c r="J377" t="inlineStr"/>
+      <c r="K377" t="inlineStr"/>
+      <c r="L377" t="inlineStr"/>
+      <c r="M377" t="inlineStr"/>
+      <c r="N377" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="n">
+        <v>376</v>
+      </c>
+      <c r="B378" t="inlineStr"/>
+      <c r="C378" t="inlineStr"/>
+      <c r="D378" t="inlineStr"/>
+      <c r="E378" t="inlineStr"/>
+      <c r="F378" t="inlineStr"/>
+      <c r="G378" t="inlineStr"/>
+      <c r="H378" t="inlineStr"/>
+      <c r="I378" t="inlineStr"/>
+      <c r="J378" t="inlineStr"/>
+      <c r="K378" t="inlineStr"/>
+      <c r="L378" t="inlineStr"/>
+      <c r="M378" t="inlineStr"/>
+      <c r="N378" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="n">
+        <v>377</v>
+      </c>
+      <c r="B379" t="inlineStr"/>
+      <c r="C379" t="inlineStr"/>
+      <c r="D379" t="inlineStr"/>
+      <c r="E379" t="inlineStr"/>
+      <c r="F379" t="inlineStr"/>
+      <c r="G379" t="inlineStr"/>
+      <c r="H379" t="inlineStr"/>
+      <c r="I379" t="inlineStr"/>
+      <c r="J379" t="inlineStr"/>
+      <c r="K379" t="inlineStr"/>
+      <c r="L379" t="inlineStr"/>
+      <c r="M379" t="inlineStr"/>
+      <c r="N379" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="n">
+        <v>378</v>
+      </c>
+      <c r="B380" t="inlineStr"/>
+      <c r="C380" t="inlineStr"/>
+      <c r="D380" t="inlineStr"/>
+      <c r="E380" t="inlineStr"/>
+      <c r="F380" t="inlineStr"/>
+      <c r="G380" t="inlineStr"/>
+      <c r="H380" t="inlineStr"/>
+      <c r="I380" t="inlineStr"/>
+      <c r="J380" t="inlineStr"/>
+      <c r="K380" t="inlineStr"/>
+      <c r="L380" t="inlineStr"/>
+      <c r="M380" t="inlineStr"/>
+      <c r="N380" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="n">
+        <v>379</v>
+      </c>
+      <c r="B381" t="inlineStr"/>
+      <c r="C381" t="inlineStr"/>
+      <c r="D381" t="inlineStr"/>
+      <c r="E381" t="inlineStr"/>
+      <c r="F381" t="inlineStr"/>
+      <c r="G381" t="inlineStr"/>
+      <c r="H381" t="inlineStr"/>
+      <c r="I381" t="inlineStr"/>
+      <c r="J381" t="inlineStr"/>
+      <c r="K381" t="inlineStr"/>
+      <c r="L381" t="inlineStr"/>
+      <c r="M381" t="inlineStr"/>
+      <c r="N381" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="B382" t="inlineStr"/>
+      <c r="C382" t="inlineStr"/>
+      <c r="D382" t="inlineStr"/>
+      <c r="E382" t="inlineStr"/>
+      <c r="F382" t="inlineStr"/>
+      <c r="G382" t="inlineStr"/>
+      <c r="H382" t="inlineStr"/>
+      <c r="I382" t="inlineStr"/>
+      <c r="J382" t="inlineStr"/>
+      <c r="K382" t="inlineStr"/>
+      <c r="L382" t="inlineStr"/>
+      <c r="M382" t="inlineStr"/>
+      <c r="N382" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1" t="n">
+        <v>381</v>
+      </c>
+      <c r="B383" t="inlineStr"/>
+      <c r="C383" t="inlineStr"/>
+      <c r="D383" t="inlineStr"/>
+      <c r="E383" t="inlineStr"/>
+      <c r="F383" t="inlineStr"/>
+      <c r="G383" t="inlineStr"/>
+      <c r="H383" t="inlineStr"/>
+      <c r="I383" t="inlineStr"/>
+      <c r="J383" t="inlineStr"/>
+      <c r="K383" t="inlineStr"/>
+      <c r="L383" t="inlineStr"/>
+      <c r="M383" t="inlineStr"/>
+      <c r="N383" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="n">
+        <v>382</v>
+      </c>
+      <c r="B384" t="inlineStr"/>
+      <c r="C384" t="inlineStr"/>
+      <c r="D384" t="inlineStr"/>
+      <c r="E384" t="inlineStr"/>
+      <c r="F384" t="inlineStr"/>
+      <c r="G384" t="inlineStr"/>
+      <c r="H384" t="inlineStr"/>
+      <c r="I384" t="inlineStr"/>
+      <c r="J384" t="inlineStr"/>
+      <c r="K384" t="inlineStr"/>
+      <c r="L384" t="inlineStr"/>
+      <c r="M384" t="inlineStr"/>
+      <c r="N384" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1" t="n">
+        <v>383</v>
+      </c>
+      <c r="B385" t="inlineStr"/>
+      <c r="C385" t="inlineStr"/>
+      <c r="D385" t="inlineStr"/>
+      <c r="E385" t="inlineStr"/>
+      <c r="F385" t="inlineStr"/>
+      <c r="G385" t="inlineStr"/>
+      <c r="H385" t="inlineStr"/>
+      <c r="I385" t="inlineStr"/>
+      <c r="J385" t="inlineStr"/>
+      <c r="K385" t="inlineStr"/>
+      <c r="L385" t="inlineStr"/>
+      <c r="M385" t="inlineStr"/>
+      <c r="N385" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="n">
+        <v>384</v>
+      </c>
+      <c r="B386" t="inlineStr"/>
+      <c r="C386" t="inlineStr"/>
+      <c r="D386" t="inlineStr"/>
+      <c r="E386" t="inlineStr"/>
+      <c r="F386" t="inlineStr"/>
+      <c r="G386" t="inlineStr"/>
+      <c r="H386" t="inlineStr"/>
+      <c r="I386" t="inlineStr"/>
+      <c r="J386" t="inlineStr"/>
+      <c r="K386" t="inlineStr"/>
+      <c r="L386" t="inlineStr"/>
+      <c r="M386" t="inlineStr"/>
+      <c r="N386" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="B387" t="inlineStr"/>
+      <c r="C387" t="inlineStr"/>
+      <c r="D387" t="inlineStr"/>
+      <c r="E387" t="inlineStr"/>
+      <c r="F387" t="inlineStr"/>
+      <c r="G387" t="inlineStr"/>
+      <c r="H387" t="inlineStr"/>
+      <c r="I387" t="inlineStr"/>
+      <c r="J387" t="inlineStr"/>
+      <c r="K387" t="inlineStr"/>
+      <c r="L387" t="inlineStr"/>
+      <c r="M387" t="inlineStr"/>
+      <c r="N387" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1" t="n">
+        <v>386</v>
+      </c>
+      <c r="B388" t="inlineStr"/>
+      <c r="C388" t="inlineStr"/>
+      <c r="D388" t="inlineStr"/>
+      <c r="E388" t="inlineStr"/>
+      <c r="F388" t="inlineStr"/>
+      <c r="G388" t="inlineStr"/>
+      <c r="H388" t="inlineStr"/>
+      <c r="I388" t="inlineStr"/>
+      <c r="J388" t="inlineStr"/>
+      <c r="K388" t="inlineStr"/>
+      <c r="L388" t="inlineStr"/>
+      <c r="M388" t="inlineStr"/>
+      <c r="N388" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1" t="n">
+        <v>387</v>
+      </c>
+      <c r="B389" t="inlineStr"/>
+      <c r="C389" t="inlineStr"/>
+      <c r="D389" t="inlineStr"/>
+      <c r="E389" t="inlineStr"/>
+      <c r="F389" t="inlineStr"/>
+      <c r="G389" t="inlineStr"/>
+      <c r="H389" t="inlineStr"/>
+      <c r="I389" t="inlineStr"/>
+      <c r="J389" t="inlineStr"/>
+      <c r="K389" t="inlineStr"/>
+      <c r="L389" t="inlineStr"/>
+      <c r="M389" t="inlineStr"/>
+      <c r="N389" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1" t="n">
+        <v>388</v>
+      </c>
+      <c r="B390" t="inlineStr"/>
+      <c r="C390" t="inlineStr"/>
+      <c r="D390" t="inlineStr"/>
+      <c r="E390" t="inlineStr"/>
+      <c r="F390" t="inlineStr"/>
+      <c r="G390" t="inlineStr"/>
+      <c r="H390" t="inlineStr"/>
+      <c r="I390" t="inlineStr"/>
+      <c r="J390" t="inlineStr"/>
+      <c r="K390" t="inlineStr"/>
+      <c r="L390" t="inlineStr"/>
+      <c r="M390" t="inlineStr"/>
+      <c r="N390" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1" t="n">
+        <v>389</v>
+      </c>
+      <c r="B391" t="inlineStr"/>
+      <c r="C391" t="inlineStr"/>
+      <c r="D391" t="inlineStr"/>
+      <c r="E391" t="inlineStr"/>
+      <c r="F391" t="inlineStr"/>
+      <c r="G391" t="inlineStr"/>
+      <c r="H391" t="inlineStr"/>
+      <c r="I391" t="inlineStr"/>
+      <c r="J391" t="inlineStr"/>
+      <c r="K391" t="inlineStr"/>
+      <c r="L391" t="inlineStr"/>
+      <c r="M391" t="inlineStr"/>
+      <c r="N391" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1" t="n">
+        <v>390</v>
+      </c>
+      <c r="B392" t="inlineStr"/>
+      <c r="C392" t="inlineStr"/>
+      <c r="D392" t="inlineStr"/>
+      <c r="E392" t="inlineStr"/>
+      <c r="F392" t="inlineStr"/>
+      <c r="G392" t="inlineStr"/>
+      <c r="H392" t="inlineStr"/>
+      <c r="I392" t="inlineStr"/>
+      <c r="J392" t="inlineStr"/>
+      <c r="K392" t="inlineStr"/>
+      <c r="L392" t="inlineStr"/>
+      <c r="M392" t="inlineStr"/>
+      <c r="N392" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1" t="n">
+        <v>391</v>
+      </c>
+      <c r="B393" t="inlineStr"/>
+      <c r="C393" t="inlineStr"/>
+      <c r="D393" t="inlineStr"/>
+      <c r="E393" t="inlineStr"/>
+      <c r="F393" t="inlineStr"/>
+      <c r="G393" t="inlineStr"/>
+      <c r="H393" t="inlineStr"/>
+      <c r="I393" t="inlineStr"/>
+      <c r="J393" t="inlineStr"/>
+      <c r="K393" t="inlineStr"/>
+      <c r="L393" t="inlineStr"/>
+      <c r="M393" t="inlineStr"/>
+      <c r="N393" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1" t="n">
+        <v>392</v>
+      </c>
+      <c r="B394" t="inlineStr"/>
+      <c r="C394" t="inlineStr"/>
+      <c r="D394" t="inlineStr"/>
+      <c r="E394" t="inlineStr"/>
+      <c r="F394" t="inlineStr"/>
+      <c r="G394" t="inlineStr"/>
+      <c r="H394" t="inlineStr"/>
+      <c r="I394" t="inlineStr"/>
+      <c r="J394" t="inlineStr"/>
+      <c r="K394" t="inlineStr"/>
+      <c r="L394" t="inlineStr"/>
+      <c r="M394" t="inlineStr"/>
+      <c r="N394" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1" t="n">
+        <v>393</v>
+      </c>
+      <c r="B395" t="inlineStr"/>
+      <c r="C395" t="inlineStr"/>
+      <c r="D395" t="inlineStr"/>
+      <c r="E395" t="inlineStr"/>
+      <c r="F395" t="inlineStr"/>
+      <c r="G395" t="inlineStr"/>
+      <c r="H395" t="inlineStr"/>
+      <c r="I395" t="inlineStr"/>
+      <c r="J395" t="inlineStr"/>
+      <c r="K395" t="inlineStr"/>
+      <c r="L395" t="inlineStr"/>
+      <c r="M395" t="inlineStr"/>
+      <c r="N395" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="1" t="n">
+        <v>394</v>
+      </c>
+      <c r="B396" t="inlineStr"/>
+      <c r="C396" t="inlineStr"/>
+      <c r="D396" t="inlineStr"/>
+      <c r="E396" t="inlineStr"/>
+      <c r="F396" t="inlineStr"/>
+      <c r="G396" t="inlineStr"/>
+      <c r="H396" t="inlineStr"/>
+      <c r="I396" t="inlineStr"/>
+      <c r="J396" t="inlineStr"/>
+      <c r="K396" t="inlineStr"/>
+      <c r="L396" t="inlineStr"/>
+      <c r="M396" t="inlineStr"/>
+      <c r="N396" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1" t="n">
+        <v>395</v>
+      </c>
+      <c r="B397" t="inlineStr"/>
+      <c r="C397" t="inlineStr"/>
+      <c r="D397" t="inlineStr"/>
+      <c r="E397" t="inlineStr"/>
+      <c r="F397" t="inlineStr"/>
+      <c r="G397" t="inlineStr"/>
+      <c r="H397" t="inlineStr"/>
+      <c r="I397" t="inlineStr"/>
+      <c r="J397" t="inlineStr"/>
+      <c r="K397" t="inlineStr"/>
+      <c r="L397" t="inlineStr"/>
+      <c r="M397" t="inlineStr"/>
+      <c r="N397" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1" t="n">
+        <v>396</v>
+      </c>
+      <c r="B398" t="inlineStr"/>
+      <c r="C398" t="inlineStr"/>
+      <c r="D398" t="inlineStr"/>
+      <c r="E398" t="inlineStr"/>
+      <c r="F398" t="inlineStr"/>
+      <c r="G398" t="inlineStr"/>
+      <c r="H398" t="inlineStr"/>
+      <c r="I398" t="inlineStr"/>
+      <c r="J398" t="inlineStr"/>
+      <c r="K398" t="inlineStr"/>
+      <c r="L398" t="inlineStr"/>
+      <c r="M398" t="inlineStr"/>
+      <c r="N398" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="1" t="n">
+        <v>397</v>
+      </c>
+      <c r="B399" t="inlineStr"/>
+      <c r="C399" t="inlineStr"/>
+      <c r="D399" t="inlineStr"/>
+      <c r="E399" t="inlineStr"/>
+      <c r="F399" t="inlineStr"/>
+      <c r="G399" t="inlineStr"/>
+      <c r="H399" t="inlineStr"/>
+      <c r="I399" t="inlineStr"/>
+      <c r="J399" t="inlineStr"/>
+      <c r="K399" t="inlineStr"/>
+      <c r="L399" t="inlineStr"/>
+      <c r="M399" t="inlineStr"/>
+      <c r="N399" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="B400" t="inlineStr"/>
+      <c r="C400" t="inlineStr"/>
+      <c r="D400" t="inlineStr"/>
+      <c r="E400" t="inlineStr"/>
+      <c r="F400" t="inlineStr"/>
+      <c r="G400" t="inlineStr"/>
+      <c r="H400" t="inlineStr"/>
+      <c r="I400" t="inlineStr"/>
+      <c r="J400" t="inlineStr"/>
+      <c r="K400" t="inlineStr"/>
+      <c r="L400" t="inlineStr"/>
+      <c r="M400" t="inlineStr"/>
+      <c r="N400" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="n">
+        <v>399</v>
+      </c>
+      <c r="B401" t="inlineStr"/>
+      <c r="C401" t="inlineStr"/>
+      <c r="D401" t="inlineStr"/>
+      <c r="E401" t="inlineStr"/>
+      <c r="F401" t="inlineStr"/>
+      <c r="G401" t="inlineStr"/>
+      <c r="H401" t="inlineStr"/>
+      <c r="I401" t="inlineStr"/>
+      <c r="J401" t="inlineStr"/>
+      <c r="K401" t="inlineStr"/>
+      <c r="L401" t="inlineStr"/>
+      <c r="M401" t="inlineStr"/>
+      <c r="N401" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="B402" t="inlineStr"/>
+      <c r="C402" t="inlineStr"/>
+      <c r="D402" t="inlineStr"/>
+      <c r="E402" t="inlineStr"/>
+      <c r="F402" t="inlineStr"/>
+      <c r="G402" t="inlineStr"/>
+      <c r="H402" t="inlineStr"/>
+      <c r="I402" t="inlineStr"/>
+      <c r="J402" t="inlineStr"/>
+      <c r="K402" t="inlineStr"/>
+      <c r="L402" t="inlineStr"/>
+      <c r="M402" t="inlineStr"/>
+      <c r="N402" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="n">
+        <v>401</v>
+      </c>
+      <c r="B403" t="inlineStr"/>
+      <c r="C403" t="inlineStr"/>
+      <c r="D403" t="inlineStr"/>
+      <c r="E403" t="inlineStr"/>
+      <c r="F403" t="inlineStr"/>
+      <c r="G403" t="inlineStr"/>
+      <c r="H403" t="inlineStr"/>
+      <c r="I403" t="inlineStr"/>
+      <c r="J403" t="inlineStr"/>
+      <c r="K403" t="inlineStr"/>
+      <c r="L403" t="inlineStr"/>
+      <c r="M403" t="inlineStr"/>
+      <c r="N403" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="1" t="n">
+        <v>402</v>
+      </c>
+      <c r="B404" t="inlineStr"/>
+      <c r="C404" t="inlineStr"/>
+      <c r="D404" t="inlineStr"/>
+      <c r="E404" t="inlineStr"/>
+      <c r="F404" t="inlineStr"/>
+      <c r="G404" t="inlineStr"/>
+      <c r="H404" t="inlineStr"/>
+      <c r="I404" t="inlineStr"/>
+      <c r="J404" t="inlineStr"/>
+      <c r="K404" t="inlineStr"/>
+      <c r="L404" t="inlineStr"/>
+      <c r="M404" t="inlineStr"/>
+      <c r="N404" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="1" t="n">
+        <v>403</v>
+      </c>
+      <c r="B405" t="inlineStr"/>
+      <c r="C405" t="inlineStr"/>
+      <c r="D405" t="inlineStr"/>
+      <c r="E405" t="inlineStr"/>
+      <c r="F405" t="inlineStr"/>
+      <c r="G405" t="inlineStr"/>
+      <c r="H405" t="inlineStr"/>
+      <c r="I405" t="inlineStr"/>
+      <c r="J405" t="inlineStr"/>
+      <c r="K405" t="inlineStr"/>
+      <c r="L405" t="inlineStr"/>
+      <c r="M405" t="inlineStr"/>
+      <c r="N405" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="1" t="n">
+        <v>404</v>
+      </c>
+      <c r="B406" t="inlineStr"/>
+      <c r="C406" t="inlineStr"/>
+      <c r="D406" t="inlineStr"/>
+      <c r="E406" t="inlineStr"/>
+      <c r="F406" t="inlineStr"/>
+      <c r="G406" t="inlineStr"/>
+      <c r="H406" t="inlineStr"/>
+      <c r="I406" t="inlineStr"/>
+      <c r="J406" t="inlineStr"/>
+      <c r="K406" t="inlineStr"/>
+      <c r="L406" t="inlineStr"/>
+      <c r="M406" t="inlineStr"/>
+      <c r="N406" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="1" t="n">
+        <v>405</v>
+      </c>
+      <c r="B407" t="inlineStr"/>
+      <c r="C407" t="inlineStr"/>
+      <c r="D407" t="inlineStr"/>
+      <c r="E407" t="inlineStr"/>
+      <c r="F407" t="inlineStr"/>
+      <c r="G407" t="inlineStr"/>
+      <c r="H407" t="inlineStr"/>
+      <c r="I407" t="inlineStr"/>
+      <c r="J407" t="inlineStr"/>
+      <c r="K407" t="inlineStr"/>
+      <c r="L407" t="inlineStr"/>
+      <c r="M407" t="inlineStr"/>
+      <c r="N407" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="1" t="n">
+        <v>406</v>
+      </c>
+      <c r="B408" t="inlineStr"/>
+      <c r="C408" t="inlineStr"/>
+      <c r="D408" t="inlineStr"/>
+      <c r="E408" t="inlineStr"/>
+      <c r="F408" t="inlineStr"/>
+      <c r="G408" t="inlineStr"/>
+      <c r="H408" t="inlineStr"/>
+      <c r="I408" t="inlineStr"/>
+      <c r="J408" t="inlineStr"/>
+      <c r="K408" t="inlineStr"/>
+      <c r="L408" t="inlineStr"/>
+      <c r="M408" t="inlineStr"/>
+      <c r="N408" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="1" t="n">
+        <v>407</v>
+      </c>
+      <c r="B409" t="inlineStr"/>
+      <c r="C409" t="inlineStr"/>
+      <c r="D409" t="inlineStr"/>
+      <c r="E409" t="inlineStr"/>
+      <c r="F409" t="inlineStr"/>
+      <c r="G409" t="inlineStr"/>
+      <c r="H409" t="inlineStr"/>
+      <c r="I409" t="inlineStr"/>
+      <c r="J409" t="inlineStr"/>
+      <c r="K409" t="inlineStr"/>
+      <c r="L409" t="inlineStr"/>
+      <c r="M409" t="inlineStr"/>
+      <c r="N409" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="B410" t="inlineStr"/>
+      <c r="C410" t="inlineStr"/>
+      <c r="D410" t="inlineStr"/>
+      <c r="E410" t="inlineStr"/>
+      <c r="F410" t="inlineStr"/>
+      <c r="G410" t="inlineStr"/>
+      <c r="H410" t="inlineStr"/>
+      <c r="I410" t="inlineStr"/>
+      <c r="J410" t="inlineStr"/>
+      <c r="K410" t="inlineStr"/>
+      <c r="L410" t="inlineStr"/>
+      <c r="M410" t="inlineStr"/>
+      <c r="N410" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="1" t="n">
+        <v>409</v>
+      </c>
+      <c r="B411" t="inlineStr"/>
+      <c r="C411" t="inlineStr"/>
+      <c r="D411" t="inlineStr"/>
+      <c r="E411" t="inlineStr"/>
+      <c r="F411" t="inlineStr"/>
+      <c r="G411" t="inlineStr"/>
+      <c r="H411" t="inlineStr"/>
+      <c r="I411" t="inlineStr"/>
+      <c r="J411" t="inlineStr"/>
+      <c r="K411" t="inlineStr"/>
+      <c r="L411" t="inlineStr"/>
+      <c r="M411" t="inlineStr"/>
+      <c r="N411" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="1" t="n">
+        <v>410</v>
+      </c>
+      <c r="B412" t="inlineStr"/>
+      <c r="C412" t="inlineStr"/>
+      <c r="D412" t="inlineStr"/>
+      <c r="E412" t="inlineStr"/>
+      <c r="F412" t="inlineStr"/>
+      <c r="G412" t="inlineStr"/>
+      <c r="H412" t="inlineStr"/>
+      <c r="I412" t="inlineStr"/>
+      <c r="J412" t="inlineStr"/>
+      <c r="K412" t="inlineStr"/>
+      <c r="L412" t="inlineStr"/>
+      <c r="M412" t="inlineStr"/>
+      <c r="N412" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="1" t="n">
+        <v>411</v>
+      </c>
+      <c r="B413" t="inlineStr"/>
+      <c r="C413" t="inlineStr"/>
+      <c r="D413" t="inlineStr"/>
+      <c r="E413" t="inlineStr"/>
+      <c r="F413" t="inlineStr"/>
+      <c r="G413" t="inlineStr"/>
+      <c r="H413" t="inlineStr"/>
+      <c r="I413" t="inlineStr"/>
+      <c r="J413" t="inlineStr"/>
+      <c r="K413" t="inlineStr"/>
+      <c r="L413" t="inlineStr"/>
+      <c r="M413" t="inlineStr"/>
+      <c r="N413" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="1" t="n">
+        <v>412</v>
+      </c>
+      <c r="B414" t="inlineStr"/>
+      <c r="C414" t="inlineStr"/>
+      <c r="D414" t="inlineStr"/>
+      <c r="E414" t="inlineStr"/>
+      <c r="F414" t="inlineStr"/>
+      <c r="G414" t="inlineStr"/>
+      <c r="H414" t="inlineStr"/>
+      <c r="I414" t="inlineStr"/>
+      <c r="J414" t="inlineStr"/>
+      <c r="K414" t="inlineStr"/>
+      <c r="L414" t="inlineStr"/>
+      <c r="M414" t="inlineStr"/>
+      <c r="N414" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="1" t="n">
+        <v>413</v>
+      </c>
+      <c r="B415" t="inlineStr"/>
+      <c r="C415" t="inlineStr"/>
+      <c r="D415" t="inlineStr"/>
+      <c r="E415" t="inlineStr"/>
+      <c r="F415" t="inlineStr"/>
+      <c r="G415" t="inlineStr"/>
+      <c r="H415" t="inlineStr"/>
+      <c r="I415" t="inlineStr"/>
+      <c r="J415" t="inlineStr"/>
+      <c r="K415" t="inlineStr"/>
+      <c r="L415" t="inlineStr"/>
+      <c r="M415" t="inlineStr"/>
+      <c r="N415" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="1" t="n">
+        <v>414</v>
+      </c>
+      <c r="B416" t="inlineStr"/>
+      <c r="C416" t="inlineStr"/>
+      <c r="D416" t="inlineStr"/>
+      <c r="E416" t="inlineStr"/>
+      <c r="F416" t="inlineStr"/>
+      <c r="G416" t="inlineStr"/>
+      <c r="H416" t="inlineStr"/>
+      <c r="I416" t="inlineStr"/>
+      <c r="J416" t="inlineStr"/>
+      <c r="K416" t="inlineStr"/>
+      <c r="L416" t="inlineStr"/>
+      <c r="M416" t="inlineStr"/>
+      <c r="N416" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="1" t="n">
+        <v>415</v>
+      </c>
+      <c r="B417" t="inlineStr"/>
+      <c r="C417" t="inlineStr"/>
+      <c r="D417" t="inlineStr"/>
+      <c r="E417" t="inlineStr"/>
+      <c r="F417" t="inlineStr"/>
+      <c r="G417" t="inlineStr"/>
+      <c r="H417" t="inlineStr"/>
+      <c r="I417" t="inlineStr"/>
+      <c r="J417" t="inlineStr"/>
+      <c r="K417" t="inlineStr"/>
+      <c r="L417" t="inlineStr"/>
+      <c r="M417" t="inlineStr"/>
+      <c r="N417" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="1" t="n">
+        <v>416</v>
+      </c>
+      <c r="B418" t="inlineStr"/>
+      <c r="C418" t="inlineStr"/>
+      <c r="D418" t="inlineStr"/>
+      <c r="E418" t="inlineStr"/>
+      <c r="F418" t="inlineStr"/>
+      <c r="G418" t="inlineStr"/>
+      <c r="H418" t="inlineStr"/>
+      <c r="I418" t="inlineStr"/>
+      <c r="J418" t="inlineStr"/>
+      <c r="K418" t="inlineStr"/>
+      <c r="L418" t="inlineStr"/>
+      <c r="M418" t="inlineStr"/>
+      <c r="N418" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="1" t="n">
+        <v>417</v>
+      </c>
+      <c r="B419" t="inlineStr"/>
+      <c r="C419" t="inlineStr"/>
+      <c r="D419" t="inlineStr"/>
+      <c r="E419" t="inlineStr"/>
+      <c r="F419" t="inlineStr"/>
+      <c r="G419" t="inlineStr"/>
+      <c r="H419" t="inlineStr"/>
+      <c r="I419" t="inlineStr"/>
+      <c r="J419" t="inlineStr"/>
+      <c r="K419" t="inlineStr"/>
+      <c r="L419" t="inlineStr"/>
+      <c r="M419" t="inlineStr"/>
+      <c r="N419" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="1" t="n">
+        <v>418</v>
+      </c>
+      <c r="B420" t="inlineStr"/>
+      <c r="C420" t="inlineStr"/>
+      <c r="D420" t="inlineStr"/>
+      <c r="E420" t="inlineStr"/>
+      <c r="F420" t="inlineStr"/>
+      <c r="G420" t="inlineStr"/>
+      <c r="H420" t="inlineStr"/>
+      <c r="I420" t="inlineStr"/>
+      <c r="J420" t="inlineStr"/>
+      <c r="K420" t="inlineStr"/>
+      <c r="L420" t="inlineStr"/>
+      <c r="M420" t="inlineStr"/>
+      <c r="N420" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="1" t="n">
+        <v>419</v>
+      </c>
+      <c r="B421" t="inlineStr"/>
+      <c r="C421" t="inlineStr"/>
+      <c r="D421" t="inlineStr"/>
+      <c r="E421" t="inlineStr"/>
+      <c r="F421" t="inlineStr"/>
+      <c r="G421" t="inlineStr"/>
+      <c r="H421" t="inlineStr"/>
+      <c r="I421" t="inlineStr"/>
+      <c r="J421" t="inlineStr"/>
+      <c r="K421" t="inlineStr"/>
+      <c r="L421" t="inlineStr"/>
+      <c r="M421" t="inlineStr"/>
+      <c r="N421" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="B422" t="inlineStr"/>
+      <c r="C422" t="inlineStr"/>
+      <c r="D422" t="inlineStr"/>
+      <c r="E422" t="inlineStr"/>
+      <c r="F422" t="inlineStr"/>
+      <c r="G422" t="inlineStr"/>
+      <c r="H422" t="inlineStr"/>
+      <c r="I422" t="inlineStr"/>
+      <c r="J422" t="inlineStr"/>
+      <c r="K422" t="inlineStr"/>
+      <c r="L422" t="inlineStr"/>
+      <c r="M422" t="inlineStr"/>
+      <c r="N422" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updating files, to be ready to go to SSH
</commit_message>
<xml_diff>
--- a/configs/test_datasets.xlsx
+++ b/configs/test_datasets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N422"/>
+  <dimension ref="A1:N534"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9454,6 +9454,2542 @@
         </is>
       </c>
     </row>
+    <row r="423">
+      <c r="A423" s="1" t="n">
+        <v>421</v>
+      </c>
+      <c r="B423" t="inlineStr"/>
+      <c r="C423" t="inlineStr"/>
+      <c r="D423" t="inlineStr"/>
+      <c r="E423" t="inlineStr"/>
+      <c r="F423" t="inlineStr"/>
+      <c r="G423" t="inlineStr"/>
+      <c r="H423" t="inlineStr"/>
+      <c r="I423" t="inlineStr"/>
+      <c r="J423" t="inlineStr"/>
+      <c r="K423" t="inlineStr"/>
+      <c r="L423" t="inlineStr"/>
+      <c r="M423" t="inlineStr"/>
+      <c r="N423" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="1" t="n">
+        <v>422</v>
+      </c>
+      <c r="B424" t="inlineStr"/>
+      <c r="C424" t="inlineStr"/>
+      <c r="D424" t="inlineStr"/>
+      <c r="E424" t="inlineStr"/>
+      <c r="F424" t="inlineStr"/>
+      <c r="G424" t="inlineStr"/>
+      <c r="H424" t="inlineStr"/>
+      <c r="I424" t="inlineStr"/>
+      <c r="J424" t="inlineStr"/>
+      <c r="K424" t="inlineStr"/>
+      <c r="L424" t="inlineStr"/>
+      <c r="M424" t="inlineStr"/>
+      <c r="N424" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="1" t="n">
+        <v>423</v>
+      </c>
+      <c r="B425" t="inlineStr"/>
+      <c r="C425" t="inlineStr"/>
+      <c r="D425" t="inlineStr"/>
+      <c r="E425" t="inlineStr"/>
+      <c r="F425" t="inlineStr"/>
+      <c r="G425" t="inlineStr"/>
+      <c r="H425" t="inlineStr"/>
+      <c r="I425" t="inlineStr"/>
+      <c r="J425" t="inlineStr"/>
+      <c r="K425" t="inlineStr"/>
+      <c r="L425" t="inlineStr"/>
+      <c r="M425" t="inlineStr"/>
+      <c r="N425" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="1" t="n">
+        <v>424</v>
+      </c>
+      <c r="B426" t="inlineStr"/>
+      <c r="C426" t="inlineStr"/>
+      <c r="D426" t="inlineStr"/>
+      <c r="E426" t="inlineStr"/>
+      <c r="F426" t="inlineStr"/>
+      <c r="G426" t="inlineStr"/>
+      <c r="H426" t="inlineStr"/>
+      <c r="I426" t="inlineStr"/>
+      <c r="J426" t="inlineStr"/>
+      <c r="K426" t="inlineStr"/>
+      <c r="L426" t="inlineStr"/>
+      <c r="M426" t="inlineStr"/>
+      <c r="N426" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="1" t="n">
+        <v>425</v>
+      </c>
+      <c r="B427" t="inlineStr"/>
+      <c r="C427" t="inlineStr"/>
+      <c r="D427" t="inlineStr"/>
+      <c r="E427" t="inlineStr"/>
+      <c r="F427" t="inlineStr"/>
+      <c r="G427" t="inlineStr"/>
+      <c r="H427" t="inlineStr"/>
+      <c r="I427" t="inlineStr"/>
+      <c r="J427" t="inlineStr"/>
+      <c r="K427" t="inlineStr"/>
+      <c r="L427" t="inlineStr"/>
+      <c r="M427" t="inlineStr"/>
+      <c r="N427" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="1" t="n">
+        <v>426</v>
+      </c>
+      <c r="B428" t="inlineStr"/>
+      <c r="C428" t="inlineStr"/>
+      <c r="D428" t="inlineStr"/>
+      <c r="E428" t="inlineStr"/>
+      <c r="F428" t="inlineStr"/>
+      <c r="G428" t="inlineStr"/>
+      <c r="H428" t="inlineStr"/>
+      <c r="I428" t="inlineStr"/>
+      <c r="J428" t="inlineStr"/>
+      <c r="K428" t="inlineStr"/>
+      <c r="L428" t="inlineStr"/>
+      <c r="M428" t="inlineStr"/>
+      <c r="N428" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="B429" t="inlineStr"/>
+      <c r="C429" t="inlineStr"/>
+      <c r="D429" t="inlineStr"/>
+      <c r="E429" t="inlineStr"/>
+      <c r="F429" t="inlineStr"/>
+      <c r="G429" t="inlineStr"/>
+      <c r="H429" t="inlineStr"/>
+      <c r="I429" t="inlineStr"/>
+      <c r="J429" t="inlineStr"/>
+      <c r="K429" t="inlineStr"/>
+      <c r="L429" t="inlineStr"/>
+      <c r="M429" t="inlineStr"/>
+      <c r="N429" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="1" t="n">
+        <v>428</v>
+      </c>
+      <c r="B430" t="inlineStr"/>
+      <c r="C430" t="inlineStr"/>
+      <c r="D430" t="inlineStr"/>
+      <c r="E430" t="inlineStr"/>
+      <c r="F430" t="inlineStr"/>
+      <c r="G430" t="inlineStr"/>
+      <c r="H430" t="inlineStr"/>
+      <c r="I430" t="inlineStr"/>
+      <c r="J430" t="inlineStr"/>
+      <c r="K430" t="inlineStr"/>
+      <c r="L430" t="inlineStr"/>
+      <c r="M430" t="inlineStr"/>
+      <c r="N430" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="1" t="n">
+        <v>429</v>
+      </c>
+      <c r="B431" t="inlineStr"/>
+      <c r="C431" t="inlineStr"/>
+      <c r="D431" t="inlineStr"/>
+      <c r="E431" t="inlineStr"/>
+      <c r="F431" t="inlineStr"/>
+      <c r="G431" t="inlineStr"/>
+      <c r="H431" t="inlineStr"/>
+      <c r="I431" t="inlineStr"/>
+      <c r="J431" t="inlineStr"/>
+      <c r="K431" t="inlineStr"/>
+      <c r="L431" t="inlineStr"/>
+      <c r="M431" t="inlineStr"/>
+      <c r="N431" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="1" t="n">
+        <v>430</v>
+      </c>
+      <c r="B432" t="inlineStr"/>
+      <c r="C432" t="inlineStr"/>
+      <c r="D432" t="inlineStr"/>
+      <c r="E432" t="inlineStr"/>
+      <c r="F432" t="inlineStr"/>
+      <c r="G432" t="inlineStr"/>
+      <c r="H432" t="inlineStr"/>
+      <c r="I432" t="inlineStr"/>
+      <c r="J432" t="inlineStr"/>
+      <c r="K432" t="inlineStr"/>
+      <c r="L432" t="inlineStr"/>
+      <c r="M432" t="inlineStr"/>
+      <c r="N432" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="1" t="n">
+        <v>431</v>
+      </c>
+      <c r="B433" t="inlineStr"/>
+      <c r="C433" t="inlineStr"/>
+      <c r="D433" t="inlineStr"/>
+      <c r="E433" t="inlineStr"/>
+      <c r="F433" t="inlineStr"/>
+      <c r="G433" t="inlineStr"/>
+      <c r="H433" t="inlineStr"/>
+      <c r="I433" t="inlineStr"/>
+      <c r="J433" t="inlineStr"/>
+      <c r="K433" t="inlineStr"/>
+      <c r="L433" t="inlineStr"/>
+      <c r="M433" t="inlineStr"/>
+      <c r="N433" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="1" t="n">
+        <v>432</v>
+      </c>
+      <c r="B434" t="inlineStr"/>
+      <c r="C434" t="inlineStr"/>
+      <c r="D434" t="inlineStr"/>
+      <c r="E434" t="inlineStr"/>
+      <c r="F434" t="inlineStr"/>
+      <c r="G434" t="inlineStr"/>
+      <c r="H434" t="inlineStr"/>
+      <c r="I434" t="inlineStr"/>
+      <c r="J434" t="inlineStr"/>
+      <c r="K434" t="inlineStr"/>
+      <c r="L434" t="inlineStr"/>
+      <c r="M434" t="inlineStr"/>
+      <c r="N434" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="1" t="n">
+        <v>433</v>
+      </c>
+      <c r="B435" t="inlineStr"/>
+      <c r="C435" t="inlineStr"/>
+      <c r="D435" t="inlineStr"/>
+      <c r="E435" t="inlineStr"/>
+      <c r="F435" t="inlineStr"/>
+      <c r="G435" t="inlineStr"/>
+      <c r="H435" t="inlineStr"/>
+      <c r="I435" t="inlineStr"/>
+      <c r="J435" t="inlineStr"/>
+      <c r="K435" t="inlineStr"/>
+      <c r="L435" t="inlineStr"/>
+      <c r="M435" t="inlineStr"/>
+      <c r="N435" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="1" t="n">
+        <v>434</v>
+      </c>
+      <c r="B436" t="inlineStr"/>
+      <c r="C436" t="inlineStr"/>
+      <c r="D436" t="inlineStr"/>
+      <c r="E436" t="inlineStr"/>
+      <c r="F436" t="inlineStr"/>
+      <c r="G436" t="inlineStr"/>
+      <c r="H436" t="inlineStr"/>
+      <c r="I436" t="inlineStr"/>
+      <c r="J436" t="inlineStr"/>
+      <c r="K436" t="inlineStr"/>
+      <c r="L436" t="inlineStr"/>
+      <c r="M436" t="inlineStr"/>
+      <c r="N436" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="1" t="n">
+        <v>435</v>
+      </c>
+      <c r="B437" t="inlineStr"/>
+      <c r="C437" t="inlineStr"/>
+      <c r="D437" t="inlineStr"/>
+      <c r="E437" t="inlineStr"/>
+      <c r="F437" t="inlineStr"/>
+      <c r="G437" t="inlineStr"/>
+      <c r="H437" t="inlineStr"/>
+      <c r="I437" t="inlineStr"/>
+      <c r="J437" t="inlineStr"/>
+      <c r="K437" t="inlineStr"/>
+      <c r="L437" t="inlineStr"/>
+      <c r="M437" t="inlineStr"/>
+      <c r="N437" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="1" t="n">
+        <v>436</v>
+      </c>
+      <c r="B438" t="inlineStr"/>
+      <c r="C438" t="inlineStr"/>
+      <c r="D438" t="inlineStr"/>
+      <c r="E438" t="inlineStr"/>
+      <c r="F438" t="inlineStr"/>
+      <c r="G438" t="inlineStr"/>
+      <c r="H438" t="inlineStr"/>
+      <c r="I438" t="inlineStr"/>
+      <c r="J438" t="inlineStr"/>
+      <c r="K438" t="inlineStr"/>
+      <c r="L438" t="inlineStr"/>
+      <c r="M438" t="inlineStr"/>
+      <c r="N438" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="1" t="n">
+        <v>437</v>
+      </c>
+      <c r="B439" t="inlineStr"/>
+      <c r="C439" t="inlineStr"/>
+      <c r="D439" t="inlineStr"/>
+      <c r="E439" t="inlineStr"/>
+      <c r="F439" t="inlineStr"/>
+      <c r="G439" t="inlineStr"/>
+      <c r="H439" t="inlineStr"/>
+      <c r="I439" t="inlineStr"/>
+      <c r="J439" t="inlineStr"/>
+      <c r="K439" t="inlineStr"/>
+      <c r="L439" t="inlineStr"/>
+      <c r="M439" t="inlineStr"/>
+      <c r="N439" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="1" t="n">
+        <v>438</v>
+      </c>
+      <c r="B440" t="inlineStr"/>
+      <c r="C440" t="inlineStr"/>
+      <c r="D440" t="inlineStr"/>
+      <c r="E440" t="inlineStr"/>
+      <c r="F440" t="inlineStr"/>
+      <c r="G440" t="inlineStr"/>
+      <c r="H440" t="inlineStr"/>
+      <c r="I440" t="inlineStr"/>
+      <c r="J440" t="inlineStr"/>
+      <c r="K440" t="inlineStr"/>
+      <c r="L440" t="inlineStr"/>
+      <c r="M440" t="inlineStr"/>
+      <c r="N440" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="1" t="n">
+        <v>439</v>
+      </c>
+      <c r="B441" t="inlineStr"/>
+      <c r="C441" t="inlineStr"/>
+      <c r="D441" t="inlineStr"/>
+      <c r="E441" t="inlineStr"/>
+      <c r="F441" t="inlineStr"/>
+      <c r="G441" t="inlineStr"/>
+      <c r="H441" t="inlineStr"/>
+      <c r="I441" t="inlineStr"/>
+      <c r="J441" t="inlineStr"/>
+      <c r="K441" t="inlineStr"/>
+      <c r="L441" t="inlineStr"/>
+      <c r="M441" t="inlineStr"/>
+      <c r="N441" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="1" t="n">
+        <v>440</v>
+      </c>
+      <c r="B442" t="inlineStr"/>
+      <c r="C442" t="inlineStr"/>
+      <c r="D442" t="inlineStr"/>
+      <c r="E442" t="inlineStr"/>
+      <c r="F442" t="inlineStr"/>
+      <c r="G442" t="inlineStr"/>
+      <c r="H442" t="inlineStr"/>
+      <c r="I442" t="inlineStr"/>
+      <c r="J442" t="inlineStr"/>
+      <c r="K442" t="inlineStr"/>
+      <c r="L442" t="inlineStr"/>
+      <c r="M442" t="inlineStr"/>
+      <c r="N442" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="1" t="n">
+        <v>441</v>
+      </c>
+      <c r="B443" t="inlineStr"/>
+      <c r="C443" t="inlineStr"/>
+      <c r="D443" t="inlineStr"/>
+      <c r="E443" t="inlineStr"/>
+      <c r="F443" t="inlineStr"/>
+      <c r="G443" t="inlineStr"/>
+      <c r="H443" t="inlineStr"/>
+      <c r="I443" t="inlineStr"/>
+      <c r="J443" t="inlineStr"/>
+      <c r="K443" t="inlineStr"/>
+      <c r="L443" t="inlineStr"/>
+      <c r="M443" t="inlineStr"/>
+      <c r="N443" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="1" t="n">
+        <v>442</v>
+      </c>
+      <c r="B444" t="inlineStr"/>
+      <c r="C444" t="inlineStr"/>
+      <c r="D444" t="inlineStr"/>
+      <c r="E444" t="inlineStr"/>
+      <c r="F444" t="inlineStr"/>
+      <c r="G444" t="inlineStr"/>
+      <c r="H444" t="inlineStr"/>
+      <c r="I444" t="inlineStr"/>
+      <c r="J444" t="inlineStr"/>
+      <c r="K444" t="inlineStr"/>
+      <c r="L444" t="inlineStr"/>
+      <c r="M444" t="inlineStr"/>
+      <c r="N444" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="B445" t="inlineStr"/>
+      <c r="C445" t="inlineStr"/>
+      <c r="D445" t="inlineStr"/>
+      <c r="E445" t="inlineStr"/>
+      <c r="F445" t="inlineStr"/>
+      <c r="G445" t="inlineStr"/>
+      <c r="H445" t="inlineStr"/>
+      <c r="I445" t="inlineStr"/>
+      <c r="J445" t="inlineStr"/>
+      <c r="K445" t="inlineStr"/>
+      <c r="L445" t="inlineStr"/>
+      <c r="M445" t="inlineStr"/>
+      <c r="N445" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="1" t="n">
+        <v>444</v>
+      </c>
+      <c r="B446" t="inlineStr"/>
+      <c r="C446" t="inlineStr"/>
+      <c r="D446" t="inlineStr"/>
+      <c r="E446" t="inlineStr"/>
+      <c r="F446" t="inlineStr"/>
+      <c r="G446" t="inlineStr"/>
+      <c r="H446" t="inlineStr"/>
+      <c r="I446" t="inlineStr"/>
+      <c r="J446" t="inlineStr"/>
+      <c r="K446" t="inlineStr"/>
+      <c r="L446" t="inlineStr"/>
+      <c r="M446" t="inlineStr"/>
+      <c r="N446" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="1" t="n">
+        <v>445</v>
+      </c>
+      <c r="B447" t="inlineStr"/>
+      <c r="C447" t="inlineStr"/>
+      <c r="D447" t="inlineStr"/>
+      <c r="E447" t="inlineStr"/>
+      <c r="F447" t="inlineStr"/>
+      <c r="G447" t="inlineStr"/>
+      <c r="H447" t="inlineStr"/>
+      <c r="I447" t="inlineStr"/>
+      <c r="J447" t="inlineStr"/>
+      <c r="K447" t="inlineStr"/>
+      <c r="L447" t="inlineStr"/>
+      <c r="M447" t="inlineStr"/>
+      <c r="N447" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="1" t="n">
+        <v>446</v>
+      </c>
+      <c r="B448" t="inlineStr"/>
+      <c r="C448" t="inlineStr"/>
+      <c r="D448" t="inlineStr"/>
+      <c r="E448" t="inlineStr"/>
+      <c r="F448" t="inlineStr"/>
+      <c r="G448" t="inlineStr"/>
+      <c r="H448" t="inlineStr"/>
+      <c r="I448" t="inlineStr"/>
+      <c r="J448" t="inlineStr"/>
+      <c r="K448" t="inlineStr"/>
+      <c r="L448" t="inlineStr"/>
+      <c r="M448" t="inlineStr"/>
+      <c r="N448" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="1" t="n">
+        <v>447</v>
+      </c>
+      <c r="B449" t="inlineStr"/>
+      <c r="C449" t="inlineStr"/>
+      <c r="D449" t="inlineStr"/>
+      <c r="E449" t="inlineStr"/>
+      <c r="F449" t="inlineStr"/>
+      <c r="G449" t="inlineStr"/>
+      <c r="H449" t="inlineStr"/>
+      <c r="I449" t="inlineStr"/>
+      <c r="J449" t="inlineStr"/>
+      <c r="K449" t="inlineStr"/>
+      <c r="L449" t="inlineStr"/>
+      <c r="M449" t="inlineStr"/>
+      <c r="N449" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="1" t="n">
+        <v>448</v>
+      </c>
+      <c r="B450" t="inlineStr"/>
+      <c r="C450" t="inlineStr"/>
+      <c r="D450" t="inlineStr"/>
+      <c r="E450" t="inlineStr"/>
+      <c r="F450" t="inlineStr"/>
+      <c r="G450" t="inlineStr"/>
+      <c r="H450" t="inlineStr"/>
+      <c r="I450" t="inlineStr"/>
+      <c r="J450" t="inlineStr"/>
+      <c r="K450" t="inlineStr"/>
+      <c r="L450" t="inlineStr"/>
+      <c r="M450" t="inlineStr"/>
+      <c r="N450" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr"/>
+      <c r="C451" t="inlineStr"/>
+      <c r="D451" t="inlineStr"/>
+      <c r="E451" t="inlineStr"/>
+      <c r="F451" t="inlineStr"/>
+      <c r="G451" t="inlineStr"/>
+      <c r="H451" t="inlineStr"/>
+      <c r="I451" t="inlineStr"/>
+      <c r="J451" t="inlineStr"/>
+      <c r="K451" t="inlineStr"/>
+      <c r="L451" t="inlineStr"/>
+      <c r="M451" t="inlineStr"/>
+      <c r="N451" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr"/>
+      <c r="C452" t="inlineStr"/>
+      <c r="D452" t="inlineStr"/>
+      <c r="E452" t="inlineStr"/>
+      <c r="F452" t="inlineStr"/>
+      <c r="G452" t="inlineStr"/>
+      <c r="H452" t="inlineStr"/>
+      <c r="I452" t="inlineStr"/>
+      <c r="J452" t="inlineStr"/>
+      <c r="K452" t="inlineStr"/>
+      <c r="L452" t="inlineStr"/>
+      <c r="M452" t="inlineStr"/>
+      <c r="N452" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr"/>
+      <c r="C453" t="inlineStr"/>
+      <c r="D453" t="inlineStr"/>
+      <c r="E453" t="inlineStr"/>
+      <c r="F453" t="inlineStr"/>
+      <c r="G453" t="inlineStr"/>
+      <c r="H453" t="inlineStr"/>
+      <c r="I453" t="inlineStr"/>
+      <c r="J453" t="inlineStr"/>
+      <c r="K453" t="inlineStr"/>
+      <c r="L453" t="inlineStr"/>
+      <c r="M453" t="inlineStr"/>
+      <c r="N453" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr"/>
+      <c r="C454" t="inlineStr"/>
+      <c r="D454" t="inlineStr"/>
+      <c r="E454" t="inlineStr"/>
+      <c r="F454" t="inlineStr"/>
+      <c r="G454" t="inlineStr"/>
+      <c r="H454" t="inlineStr"/>
+      <c r="I454" t="inlineStr"/>
+      <c r="J454" t="inlineStr"/>
+      <c r="K454" t="inlineStr"/>
+      <c r="L454" t="inlineStr"/>
+      <c r="M454" t="inlineStr"/>
+      <c r="N454" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr"/>
+      <c r="C455" t="inlineStr"/>
+      <c r="D455" t="inlineStr"/>
+      <c r="E455" t="inlineStr"/>
+      <c r="F455" t="inlineStr"/>
+      <c r="G455" t="inlineStr"/>
+      <c r="H455" t="inlineStr"/>
+      <c r="I455" t="inlineStr"/>
+      <c r="J455" t="inlineStr"/>
+      <c r="K455" t="inlineStr"/>
+      <c r="L455" t="inlineStr"/>
+      <c r="M455" t="inlineStr"/>
+      <c r="N455" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr"/>
+      <c r="C456" t="inlineStr"/>
+      <c r="D456" t="inlineStr"/>
+      <c r="E456" t="inlineStr"/>
+      <c r="F456" t="inlineStr"/>
+      <c r="G456" t="inlineStr"/>
+      <c r="H456" t="inlineStr"/>
+      <c r="I456" t="inlineStr"/>
+      <c r="J456" t="inlineStr"/>
+      <c r="K456" t="inlineStr"/>
+      <c r="L456" t="inlineStr"/>
+      <c r="M456" t="inlineStr"/>
+      <c r="N456" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr"/>
+      <c r="C457" t="inlineStr"/>
+      <c r="D457" t="inlineStr"/>
+      <c r="E457" t="inlineStr"/>
+      <c r="F457" t="inlineStr"/>
+      <c r="G457" t="inlineStr"/>
+      <c r="H457" t="inlineStr"/>
+      <c r="I457" t="inlineStr"/>
+      <c r="J457" t="inlineStr"/>
+      <c r="K457" t="inlineStr"/>
+      <c r="L457" t="inlineStr"/>
+      <c r="M457" t="inlineStr"/>
+      <c r="N457" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr"/>
+      <c r="C458" t="inlineStr"/>
+      <c r="D458" t="inlineStr"/>
+      <c r="E458" t="inlineStr"/>
+      <c r="F458" t="inlineStr"/>
+      <c r="G458" t="inlineStr"/>
+      <c r="H458" t="inlineStr"/>
+      <c r="I458" t="inlineStr"/>
+      <c r="J458" t="inlineStr"/>
+      <c r="K458" t="inlineStr"/>
+      <c r="L458" t="inlineStr"/>
+      <c r="M458" t="inlineStr"/>
+      <c r="N458" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr"/>
+      <c r="C459" t="inlineStr"/>
+      <c r="D459" t="inlineStr"/>
+      <c r="E459" t="inlineStr"/>
+      <c r="F459" t="inlineStr"/>
+      <c r="G459" t="inlineStr"/>
+      <c r="H459" t="inlineStr"/>
+      <c r="I459" t="inlineStr"/>
+      <c r="J459" t="inlineStr"/>
+      <c r="K459" t="inlineStr"/>
+      <c r="L459" t="inlineStr"/>
+      <c r="M459" t="inlineStr"/>
+      <c r="N459" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr"/>
+      <c r="C460" t="inlineStr"/>
+      <c r="D460" t="inlineStr"/>
+      <c r="E460" t="inlineStr"/>
+      <c r="F460" t="inlineStr"/>
+      <c r="G460" t="inlineStr"/>
+      <c r="H460" t="inlineStr"/>
+      <c r="I460" t="inlineStr"/>
+      <c r="J460" t="inlineStr"/>
+      <c r="K460" t="inlineStr"/>
+      <c r="L460" t="inlineStr"/>
+      <c r="M460" t="inlineStr"/>
+      <c r="N460" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr"/>
+      <c r="C461" t="inlineStr"/>
+      <c r="D461" t="inlineStr"/>
+      <c r="E461" t="inlineStr"/>
+      <c r="F461" t="inlineStr"/>
+      <c r="G461" t="inlineStr"/>
+      <c r="H461" t="inlineStr"/>
+      <c r="I461" t="inlineStr"/>
+      <c r="J461" t="inlineStr"/>
+      <c r="K461" t="inlineStr"/>
+      <c r="L461" t="inlineStr"/>
+      <c r="M461" t="inlineStr"/>
+      <c r="N461" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr"/>
+      <c r="C462" t="inlineStr"/>
+      <c r="D462" t="inlineStr"/>
+      <c r="E462" t="inlineStr"/>
+      <c r="F462" t="inlineStr"/>
+      <c r="G462" t="inlineStr"/>
+      <c r="H462" t="inlineStr"/>
+      <c r="I462" t="inlineStr"/>
+      <c r="J462" t="inlineStr"/>
+      <c r="K462" t="inlineStr"/>
+      <c r="L462" t="inlineStr"/>
+      <c r="M462" t="inlineStr"/>
+      <c r="N462" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr"/>
+      <c r="C463" t="inlineStr"/>
+      <c r="D463" t="inlineStr"/>
+      <c r="E463" t="inlineStr"/>
+      <c r="F463" t="inlineStr"/>
+      <c r="G463" t="inlineStr"/>
+      <c r="H463" t="inlineStr"/>
+      <c r="I463" t="inlineStr"/>
+      <c r="J463" t="inlineStr"/>
+      <c r="K463" t="inlineStr"/>
+      <c r="L463" t="inlineStr"/>
+      <c r="M463" t="inlineStr"/>
+      <c r="N463" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr"/>
+      <c r="C464" t="inlineStr"/>
+      <c r="D464" t="inlineStr"/>
+      <c r="E464" t="inlineStr"/>
+      <c r="F464" t="inlineStr"/>
+      <c r="G464" t="inlineStr"/>
+      <c r="H464" t="inlineStr"/>
+      <c r="I464" t="inlineStr"/>
+      <c r="J464" t="inlineStr"/>
+      <c r="K464" t="inlineStr"/>
+      <c r="L464" t="inlineStr"/>
+      <c r="M464" t="inlineStr"/>
+      <c r="N464" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr"/>
+      <c r="C465" t="inlineStr"/>
+      <c r="D465" t="inlineStr"/>
+      <c r="E465" t="inlineStr"/>
+      <c r="F465" t="inlineStr"/>
+      <c r="G465" t="inlineStr"/>
+      <c r="H465" t="inlineStr"/>
+      <c r="I465" t="inlineStr"/>
+      <c r="J465" t="inlineStr"/>
+      <c r="K465" t="inlineStr"/>
+      <c r="L465" t="inlineStr"/>
+      <c r="M465" t="inlineStr"/>
+      <c r="N465" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr"/>
+      <c r="C466" t="inlineStr"/>
+      <c r="D466" t="inlineStr"/>
+      <c r="E466" t="inlineStr"/>
+      <c r="F466" t="inlineStr"/>
+      <c r="G466" t="inlineStr"/>
+      <c r="H466" t="inlineStr"/>
+      <c r="I466" t="inlineStr"/>
+      <c r="J466" t="inlineStr"/>
+      <c r="K466" t="inlineStr"/>
+      <c r="L466" t="inlineStr"/>
+      <c r="M466" t="inlineStr"/>
+      <c r="N466" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr"/>
+      <c r="C467" t="inlineStr"/>
+      <c r="D467" t="inlineStr"/>
+      <c r="E467" t="inlineStr"/>
+      <c r="F467" t="inlineStr"/>
+      <c r="G467" t="inlineStr"/>
+      <c r="H467" t="inlineStr"/>
+      <c r="I467" t="inlineStr"/>
+      <c r="J467" t="inlineStr"/>
+      <c r="K467" t="inlineStr"/>
+      <c r="L467" t="inlineStr"/>
+      <c r="M467" t="inlineStr"/>
+      <c r="N467" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr"/>
+      <c r="C468" t="inlineStr"/>
+      <c r="D468" t="inlineStr"/>
+      <c r="E468" t="inlineStr"/>
+      <c r="F468" t="inlineStr"/>
+      <c r="G468" t="inlineStr"/>
+      <c r="H468" t="inlineStr"/>
+      <c r="I468" t="inlineStr"/>
+      <c r="J468" t="inlineStr"/>
+      <c r="K468" t="inlineStr"/>
+      <c r="L468" t="inlineStr"/>
+      <c r="M468" t="inlineStr"/>
+      <c r="N468" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr"/>
+      <c r="C469" t="inlineStr"/>
+      <c r="D469" t="inlineStr"/>
+      <c r="E469" t="inlineStr"/>
+      <c r="F469" t="inlineStr"/>
+      <c r="G469" t="inlineStr"/>
+      <c r="H469" t="inlineStr"/>
+      <c r="I469" t="inlineStr"/>
+      <c r="J469" t="inlineStr"/>
+      <c r="K469" t="inlineStr"/>
+      <c r="L469" t="inlineStr"/>
+      <c r="M469" t="inlineStr"/>
+      <c r="N469" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr"/>
+      <c r="C470" t="inlineStr"/>
+      <c r="D470" t="inlineStr"/>
+      <c r="E470" t="inlineStr"/>
+      <c r="F470" t="inlineStr"/>
+      <c r="G470" t="inlineStr"/>
+      <c r="H470" t="inlineStr"/>
+      <c r="I470" t="inlineStr"/>
+      <c r="J470" t="inlineStr"/>
+      <c r="K470" t="inlineStr"/>
+      <c r="L470" t="inlineStr"/>
+      <c r="M470" t="inlineStr"/>
+      <c r="N470" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr"/>
+      <c r="C471" t="inlineStr"/>
+      <c r="D471" t="inlineStr"/>
+      <c r="E471" t="inlineStr"/>
+      <c r="F471" t="inlineStr"/>
+      <c r="G471" t="inlineStr"/>
+      <c r="H471" t="inlineStr"/>
+      <c r="I471" t="inlineStr"/>
+      <c r="J471" t="inlineStr"/>
+      <c r="K471" t="inlineStr"/>
+      <c r="L471" t="inlineStr"/>
+      <c r="M471" t="inlineStr"/>
+      <c r="N471" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr"/>
+      <c r="C472" t="inlineStr"/>
+      <c r="D472" t="inlineStr"/>
+      <c r="E472" t="inlineStr"/>
+      <c r="F472" t="inlineStr"/>
+      <c r="G472" t="inlineStr"/>
+      <c r="H472" t="inlineStr"/>
+      <c r="I472" t="inlineStr"/>
+      <c r="J472" t="inlineStr"/>
+      <c r="K472" t="inlineStr"/>
+      <c r="L472" t="inlineStr"/>
+      <c r="M472" t="inlineStr"/>
+      <c r="N472" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr"/>
+      <c r="C473" t="inlineStr"/>
+      <c r="D473" t="inlineStr"/>
+      <c r="E473" t="inlineStr"/>
+      <c r="F473" t="inlineStr"/>
+      <c r="G473" t="inlineStr"/>
+      <c r="H473" t="inlineStr"/>
+      <c r="I473" t="inlineStr"/>
+      <c r="J473" t="inlineStr"/>
+      <c r="K473" t="inlineStr"/>
+      <c r="L473" t="inlineStr"/>
+      <c r="M473" t="inlineStr"/>
+      <c r="N473" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr"/>
+      <c r="C474" t="inlineStr"/>
+      <c r="D474" t="inlineStr"/>
+      <c r="E474" t="inlineStr"/>
+      <c r="F474" t="inlineStr"/>
+      <c r="G474" t="inlineStr"/>
+      <c r="H474" t="inlineStr"/>
+      <c r="I474" t="inlineStr"/>
+      <c r="J474" t="inlineStr"/>
+      <c r="K474" t="inlineStr"/>
+      <c r="L474" t="inlineStr"/>
+      <c r="M474" t="inlineStr"/>
+      <c r="N474" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr"/>
+      <c r="C475" t="inlineStr"/>
+      <c r="D475" t="inlineStr"/>
+      <c r="E475" t="inlineStr"/>
+      <c r="F475" t="inlineStr"/>
+      <c r="G475" t="inlineStr"/>
+      <c r="H475" t="inlineStr"/>
+      <c r="I475" t="inlineStr"/>
+      <c r="J475" t="inlineStr"/>
+      <c r="K475" t="inlineStr"/>
+      <c r="L475" t="inlineStr"/>
+      <c r="M475" t="inlineStr"/>
+      <c r="N475" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr"/>
+      <c r="C476" t="inlineStr"/>
+      <c r="D476" t="inlineStr"/>
+      <c r="E476" t="inlineStr"/>
+      <c r="F476" t="inlineStr"/>
+      <c r="G476" t="inlineStr"/>
+      <c r="H476" t="inlineStr"/>
+      <c r="I476" t="inlineStr"/>
+      <c r="J476" t="inlineStr"/>
+      <c r="K476" t="inlineStr"/>
+      <c r="L476" t="inlineStr"/>
+      <c r="M476" t="inlineStr"/>
+      <c r="N476" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr"/>
+      <c r="C477" t="inlineStr"/>
+      <c r="D477" t="inlineStr"/>
+      <c r="E477" t="inlineStr"/>
+      <c r="F477" t="inlineStr"/>
+      <c r="G477" t="inlineStr"/>
+      <c r="H477" t="inlineStr"/>
+      <c r="I477" t="inlineStr"/>
+      <c r="J477" t="inlineStr"/>
+      <c r="K477" t="inlineStr"/>
+      <c r="L477" t="inlineStr"/>
+      <c r="M477" t="inlineStr"/>
+      <c r="N477" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr"/>
+      <c r="C478" t="inlineStr"/>
+      <c r="D478" t="inlineStr"/>
+      <c r="E478" t="inlineStr"/>
+      <c r="F478" t="inlineStr"/>
+      <c r="G478" t="inlineStr"/>
+      <c r="H478" t="inlineStr"/>
+      <c r="I478" t="inlineStr"/>
+      <c r="J478" t="inlineStr"/>
+      <c r="K478" t="inlineStr"/>
+      <c r="L478" t="inlineStr"/>
+      <c r="M478" t="inlineStr"/>
+      <c r="N478" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr"/>
+      <c r="C479" t="inlineStr"/>
+      <c r="D479" t="inlineStr"/>
+      <c r="E479" t="inlineStr"/>
+      <c r="F479" t="inlineStr"/>
+      <c r="G479" t="inlineStr"/>
+      <c r="H479" t="inlineStr"/>
+      <c r="I479" t="inlineStr"/>
+      <c r="J479" t="inlineStr"/>
+      <c r="K479" t="inlineStr"/>
+      <c r="L479" t="inlineStr"/>
+      <c r="M479" t="inlineStr"/>
+      <c r="N479" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr"/>
+      <c r="C480" t="inlineStr"/>
+      <c r="D480" t="inlineStr"/>
+      <c r="E480" t="inlineStr"/>
+      <c r="F480" t="inlineStr"/>
+      <c r="G480" t="inlineStr"/>
+      <c r="H480" t="inlineStr"/>
+      <c r="I480" t="inlineStr"/>
+      <c r="J480" t="inlineStr"/>
+      <c r="K480" t="inlineStr"/>
+      <c r="L480" t="inlineStr"/>
+      <c r="M480" t="inlineStr"/>
+      <c r="N480" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr"/>
+      <c r="C481" t="inlineStr"/>
+      <c r="D481" t="inlineStr"/>
+      <c r="E481" t="inlineStr"/>
+      <c r="F481" t="inlineStr"/>
+      <c r="G481" t="inlineStr"/>
+      <c r="H481" t="inlineStr"/>
+      <c r="I481" t="inlineStr"/>
+      <c r="J481" t="inlineStr"/>
+      <c r="K481" t="inlineStr"/>
+      <c r="L481" t="inlineStr"/>
+      <c r="M481" t="inlineStr"/>
+      <c r="N481" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr"/>
+      <c r="C482" t="inlineStr"/>
+      <c r="D482" t="inlineStr"/>
+      <c r="E482" t="inlineStr"/>
+      <c r="F482" t="inlineStr"/>
+      <c r="G482" t="inlineStr"/>
+      <c r="H482" t="inlineStr"/>
+      <c r="I482" t="inlineStr"/>
+      <c r="J482" t="inlineStr"/>
+      <c r="K482" t="inlineStr"/>
+      <c r="L482" t="inlineStr"/>
+      <c r="M482" t="inlineStr"/>
+      <c r="N482" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr"/>
+      <c r="C483" t="inlineStr"/>
+      <c r="D483" t="inlineStr"/>
+      <c r="E483" t="inlineStr"/>
+      <c r="F483" t="inlineStr"/>
+      <c r="G483" t="inlineStr"/>
+      <c r="H483" t="inlineStr"/>
+      <c r="I483" t="inlineStr"/>
+      <c r="J483" t="inlineStr"/>
+      <c r="K483" t="inlineStr"/>
+      <c r="L483" t="inlineStr"/>
+      <c r="M483" t="inlineStr"/>
+      <c r="N483" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr"/>
+      <c r="C484" t="inlineStr"/>
+      <c r="D484" t="inlineStr"/>
+      <c r="E484" t="inlineStr"/>
+      <c r="F484" t="inlineStr"/>
+      <c r="G484" t="inlineStr"/>
+      <c r="H484" t="inlineStr"/>
+      <c r="I484" t="inlineStr"/>
+      <c r="J484" t="inlineStr"/>
+      <c r="K484" t="inlineStr"/>
+      <c r="L484" t="inlineStr"/>
+      <c r="M484" t="inlineStr"/>
+      <c r="N484" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr"/>
+      <c r="C485" t="inlineStr"/>
+      <c r="D485" t="inlineStr"/>
+      <c r="E485" t="inlineStr"/>
+      <c r="F485" t="inlineStr"/>
+      <c r="G485" t="inlineStr"/>
+      <c r="H485" t="inlineStr"/>
+      <c r="I485" t="inlineStr"/>
+      <c r="J485" t="inlineStr"/>
+      <c r="K485" t="inlineStr"/>
+      <c r="L485" t="inlineStr"/>
+      <c r="M485" t="inlineStr"/>
+      <c r="N485" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr"/>
+      <c r="C486" t="inlineStr"/>
+      <c r="D486" t="inlineStr"/>
+      <c r="E486" t="inlineStr"/>
+      <c r="F486" t="inlineStr"/>
+      <c r="G486" t="inlineStr"/>
+      <c r="H486" t="inlineStr"/>
+      <c r="I486" t="inlineStr"/>
+      <c r="J486" t="inlineStr"/>
+      <c r="K486" t="inlineStr"/>
+      <c r="L486" t="inlineStr"/>
+      <c r="M486" t="inlineStr"/>
+      <c r="N486" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr"/>
+      <c r="C487" t="inlineStr"/>
+      <c r="D487" t="inlineStr"/>
+      <c r="E487" t="inlineStr"/>
+      <c r="F487" t="inlineStr"/>
+      <c r="G487" t="inlineStr"/>
+      <c r="H487" t="inlineStr"/>
+      <c r="I487" t="inlineStr"/>
+      <c r="J487" t="inlineStr"/>
+      <c r="K487" t="inlineStr"/>
+      <c r="L487" t="inlineStr"/>
+      <c r="M487" t="inlineStr"/>
+      <c r="N487" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr"/>
+      <c r="C488" t="inlineStr"/>
+      <c r="D488" t="inlineStr"/>
+      <c r="E488" t="inlineStr"/>
+      <c r="F488" t="inlineStr"/>
+      <c r="G488" t="inlineStr"/>
+      <c r="H488" t="inlineStr"/>
+      <c r="I488" t="inlineStr"/>
+      <c r="J488" t="inlineStr"/>
+      <c r="K488" t="inlineStr"/>
+      <c r="L488" t="inlineStr"/>
+      <c r="M488" t="inlineStr"/>
+      <c r="N488" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr"/>
+      <c r="C489" t="inlineStr"/>
+      <c r="D489" t="inlineStr"/>
+      <c r="E489" t="inlineStr"/>
+      <c r="F489" t="inlineStr"/>
+      <c r="G489" t="inlineStr"/>
+      <c r="H489" t="inlineStr"/>
+      <c r="I489" t="inlineStr"/>
+      <c r="J489" t="inlineStr"/>
+      <c r="K489" t="inlineStr"/>
+      <c r="L489" t="inlineStr"/>
+      <c r="M489" t="inlineStr"/>
+      <c r="N489" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr"/>
+      <c r="C490" t="inlineStr"/>
+      <c r="D490" t="inlineStr"/>
+      <c r="E490" t="inlineStr"/>
+      <c r="F490" t="inlineStr"/>
+      <c r="G490" t="inlineStr"/>
+      <c r="H490" t="inlineStr"/>
+      <c r="I490" t="inlineStr"/>
+      <c r="J490" t="inlineStr"/>
+      <c r="K490" t="inlineStr"/>
+      <c r="L490" t="inlineStr"/>
+      <c r="M490" t="inlineStr"/>
+      <c r="N490" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr"/>
+      <c r="C491" t="inlineStr"/>
+      <c r="D491" t="inlineStr"/>
+      <c r="E491" t="inlineStr"/>
+      <c r="F491" t="inlineStr"/>
+      <c r="G491" t="inlineStr"/>
+      <c r="H491" t="inlineStr"/>
+      <c r="I491" t="inlineStr"/>
+      <c r="J491" t="inlineStr"/>
+      <c r="K491" t="inlineStr"/>
+      <c r="L491" t="inlineStr"/>
+      <c r="M491" t="inlineStr"/>
+      <c r="N491" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr"/>
+      <c r="C492" t="inlineStr"/>
+      <c r="D492" t="inlineStr"/>
+      <c r="E492" t="inlineStr"/>
+      <c r="F492" t="inlineStr"/>
+      <c r="G492" t="inlineStr"/>
+      <c r="H492" t="inlineStr"/>
+      <c r="I492" t="inlineStr"/>
+      <c r="J492" t="inlineStr"/>
+      <c r="K492" t="inlineStr"/>
+      <c r="L492" t="inlineStr"/>
+      <c r="M492" t="inlineStr"/>
+      <c r="N492" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr"/>
+      <c r="C493" t="inlineStr"/>
+      <c r="D493" t="inlineStr"/>
+      <c r="E493" t="inlineStr"/>
+      <c r="F493" t="inlineStr"/>
+      <c r="G493" t="inlineStr"/>
+      <c r="H493" t="inlineStr"/>
+      <c r="I493" t="inlineStr"/>
+      <c r="J493" t="inlineStr"/>
+      <c r="K493" t="inlineStr"/>
+      <c r="L493" t="inlineStr"/>
+      <c r="M493" t="inlineStr"/>
+      <c r="N493" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr"/>
+      <c r="C494" t="inlineStr"/>
+      <c r="D494" t="inlineStr"/>
+      <c r="E494" t="inlineStr"/>
+      <c r="F494" t="inlineStr"/>
+      <c r="G494" t="inlineStr"/>
+      <c r="H494" t="inlineStr"/>
+      <c r="I494" t="inlineStr"/>
+      <c r="J494" t="inlineStr"/>
+      <c r="K494" t="inlineStr"/>
+      <c r="L494" t="inlineStr"/>
+      <c r="M494" t="inlineStr"/>
+      <c r="N494" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr"/>
+      <c r="C495" t="inlineStr"/>
+      <c r="D495" t="inlineStr"/>
+      <c r="E495" t="inlineStr"/>
+      <c r="F495" t="inlineStr"/>
+      <c r="G495" t="inlineStr"/>
+      <c r="H495" t="inlineStr"/>
+      <c r="I495" t="inlineStr"/>
+      <c r="J495" t="inlineStr"/>
+      <c r="K495" t="inlineStr"/>
+      <c r="L495" t="inlineStr"/>
+      <c r="M495" t="inlineStr"/>
+      <c r="N495" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr"/>
+      <c r="C496" t="inlineStr"/>
+      <c r="D496" t="inlineStr"/>
+      <c r="E496" t="inlineStr"/>
+      <c r="F496" t="inlineStr"/>
+      <c r="G496" t="inlineStr"/>
+      <c r="H496" t="inlineStr"/>
+      <c r="I496" t="inlineStr"/>
+      <c r="J496" t="inlineStr"/>
+      <c r="K496" t="inlineStr"/>
+      <c r="L496" t="inlineStr"/>
+      <c r="M496" t="inlineStr"/>
+      <c r="N496" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr"/>
+      <c r="C497" t="inlineStr"/>
+      <c r="D497" t="inlineStr"/>
+      <c r="E497" t="inlineStr"/>
+      <c r="F497" t="inlineStr"/>
+      <c r="G497" t="inlineStr"/>
+      <c r="H497" t="inlineStr"/>
+      <c r="I497" t="inlineStr"/>
+      <c r="J497" t="inlineStr"/>
+      <c r="K497" t="inlineStr"/>
+      <c r="L497" t="inlineStr"/>
+      <c r="M497" t="inlineStr"/>
+      <c r="N497" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr"/>
+      <c r="C498" t="inlineStr"/>
+      <c r="D498" t="inlineStr"/>
+      <c r="E498" t="inlineStr"/>
+      <c r="F498" t="inlineStr"/>
+      <c r="G498" t="inlineStr"/>
+      <c r="H498" t="inlineStr"/>
+      <c r="I498" t="inlineStr"/>
+      <c r="J498" t="inlineStr"/>
+      <c r="K498" t="inlineStr"/>
+      <c r="L498" t="inlineStr"/>
+      <c r="M498" t="inlineStr"/>
+      <c r="N498" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr"/>
+      <c r="C499" t="inlineStr"/>
+      <c r="D499" t="inlineStr"/>
+      <c r="E499" t="inlineStr"/>
+      <c r="F499" t="inlineStr"/>
+      <c r="G499" t="inlineStr"/>
+      <c r="H499" t="inlineStr"/>
+      <c r="I499" t="inlineStr"/>
+      <c r="J499" t="inlineStr"/>
+      <c r="K499" t="inlineStr"/>
+      <c r="L499" t="inlineStr"/>
+      <c r="M499" t="inlineStr"/>
+      <c r="N499" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr"/>
+      <c r="C500" t="inlineStr"/>
+      <c r="D500" t="inlineStr"/>
+      <c r="E500" t="inlineStr"/>
+      <c r="F500" t="inlineStr"/>
+      <c r="G500" t="inlineStr"/>
+      <c r="H500" t="inlineStr"/>
+      <c r="I500" t="inlineStr"/>
+      <c r="J500" t="inlineStr"/>
+      <c r="K500" t="inlineStr"/>
+      <c r="L500" t="inlineStr"/>
+      <c r="M500" t="inlineStr"/>
+      <c r="N500" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr"/>
+      <c r="C501" t="inlineStr"/>
+      <c r="D501" t="inlineStr"/>
+      <c r="E501" t="inlineStr"/>
+      <c r="F501" t="inlineStr"/>
+      <c r="G501" t="inlineStr"/>
+      <c r="H501" t="inlineStr"/>
+      <c r="I501" t="inlineStr"/>
+      <c r="J501" t="inlineStr"/>
+      <c r="K501" t="inlineStr"/>
+      <c r="L501" t="inlineStr"/>
+      <c r="M501" t="inlineStr"/>
+      <c r="N501" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr"/>
+      <c r="C502" t="inlineStr"/>
+      <c r="D502" t="inlineStr"/>
+      <c r="E502" t="inlineStr"/>
+      <c r="F502" t="inlineStr"/>
+      <c r="G502" t="inlineStr"/>
+      <c r="H502" t="inlineStr"/>
+      <c r="I502" t="inlineStr"/>
+      <c r="J502" t="inlineStr"/>
+      <c r="K502" t="inlineStr"/>
+      <c r="L502" t="inlineStr"/>
+      <c r="M502" t="inlineStr"/>
+      <c r="N502" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr"/>
+      <c r="C503" t="inlineStr"/>
+      <c r="D503" t="inlineStr"/>
+      <c r="E503" t="inlineStr"/>
+      <c r="F503" t="inlineStr"/>
+      <c r="G503" t="inlineStr"/>
+      <c r="H503" t="inlineStr"/>
+      <c r="I503" t="inlineStr"/>
+      <c r="J503" t="inlineStr"/>
+      <c r="K503" t="inlineStr"/>
+      <c r="L503" t="inlineStr"/>
+      <c r="M503" t="inlineStr"/>
+      <c r="N503" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr"/>
+      <c r="C504" t="inlineStr"/>
+      <c r="D504" t="inlineStr"/>
+      <c r="E504" t="inlineStr"/>
+      <c r="F504" t="inlineStr"/>
+      <c r="G504" t="inlineStr"/>
+      <c r="H504" t="inlineStr"/>
+      <c r="I504" t="inlineStr"/>
+      <c r="J504" t="inlineStr"/>
+      <c r="K504" t="inlineStr"/>
+      <c r="L504" t="inlineStr"/>
+      <c r="M504" t="inlineStr"/>
+      <c r="N504" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr"/>
+      <c r="C505" t="inlineStr"/>
+      <c r="D505" t="inlineStr"/>
+      <c r="E505" t="inlineStr"/>
+      <c r="F505" t="inlineStr"/>
+      <c r="G505" t="inlineStr"/>
+      <c r="H505" t="inlineStr"/>
+      <c r="I505" t="inlineStr"/>
+      <c r="J505" t="inlineStr"/>
+      <c r="K505" t="inlineStr"/>
+      <c r="L505" t="inlineStr"/>
+      <c r="M505" t="inlineStr"/>
+      <c r="N505" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr"/>
+      <c r="C506" t="inlineStr"/>
+      <c r="D506" t="inlineStr"/>
+      <c r="E506" t="inlineStr"/>
+      <c r="F506" t="inlineStr"/>
+      <c r="G506" t="inlineStr"/>
+      <c r="H506" t="inlineStr"/>
+      <c r="I506" t="inlineStr"/>
+      <c r="J506" t="inlineStr"/>
+      <c r="K506" t="inlineStr"/>
+      <c r="L506" t="inlineStr"/>
+      <c r="M506" t="inlineStr"/>
+      <c r="N506" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr"/>
+      <c r="C507" t="inlineStr"/>
+      <c r="D507" t="inlineStr"/>
+      <c r="E507" t="inlineStr"/>
+      <c r="F507" t="inlineStr"/>
+      <c r="G507" t="inlineStr"/>
+      <c r="H507" t="inlineStr"/>
+      <c r="I507" t="inlineStr"/>
+      <c r="J507" t="inlineStr"/>
+      <c r="K507" t="inlineStr"/>
+      <c r="L507" t="inlineStr"/>
+      <c r="M507" t="inlineStr"/>
+      <c r="N507" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr"/>
+      <c r="C508" t="inlineStr"/>
+      <c r="D508" t="inlineStr"/>
+      <c r="E508" t="inlineStr"/>
+      <c r="F508" t="inlineStr"/>
+      <c r="G508" t="inlineStr"/>
+      <c r="H508" t="inlineStr"/>
+      <c r="I508" t="inlineStr"/>
+      <c r="J508" t="inlineStr"/>
+      <c r="K508" t="inlineStr"/>
+      <c r="L508" t="inlineStr"/>
+      <c r="M508" t="inlineStr"/>
+      <c r="N508" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr"/>
+      <c r="C509" t="inlineStr"/>
+      <c r="D509" t="inlineStr"/>
+      <c r="E509" t="inlineStr"/>
+      <c r="F509" t="inlineStr"/>
+      <c r="G509" t="inlineStr"/>
+      <c r="H509" t="inlineStr"/>
+      <c r="I509" t="inlineStr"/>
+      <c r="J509" t="inlineStr"/>
+      <c r="K509" t="inlineStr"/>
+      <c r="L509" t="inlineStr"/>
+      <c r="M509" t="inlineStr"/>
+      <c r="N509" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr"/>
+      <c r="C510" t="inlineStr"/>
+      <c r="D510" t="inlineStr"/>
+      <c r="E510" t="inlineStr"/>
+      <c r="F510" t="inlineStr"/>
+      <c r="G510" t="inlineStr"/>
+      <c r="H510" t="inlineStr"/>
+      <c r="I510" t="inlineStr"/>
+      <c r="J510" t="inlineStr"/>
+      <c r="K510" t="inlineStr"/>
+      <c r="L510" t="inlineStr"/>
+      <c r="M510" t="inlineStr"/>
+      <c r="N510" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr"/>
+      <c r="C511" t="inlineStr"/>
+      <c r="D511" t="inlineStr"/>
+      <c r="E511" t="inlineStr"/>
+      <c r="F511" t="inlineStr"/>
+      <c r="G511" t="inlineStr"/>
+      <c r="H511" t="inlineStr"/>
+      <c r="I511" t="inlineStr"/>
+      <c r="J511" t="inlineStr"/>
+      <c r="K511" t="inlineStr"/>
+      <c r="L511" t="inlineStr"/>
+      <c r="M511" t="inlineStr"/>
+      <c r="N511" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr"/>
+      <c r="C512" t="inlineStr"/>
+      <c r="D512" t="inlineStr"/>
+      <c r="E512" t="inlineStr"/>
+      <c r="F512" t="inlineStr"/>
+      <c r="G512" t="inlineStr"/>
+      <c r="H512" t="inlineStr"/>
+      <c r="I512" t="inlineStr"/>
+      <c r="J512" t="inlineStr"/>
+      <c r="K512" t="inlineStr"/>
+      <c r="L512" t="inlineStr"/>
+      <c r="M512" t="inlineStr"/>
+      <c r="N512" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr"/>
+      <c r="C513" t="inlineStr"/>
+      <c r="D513" t="inlineStr"/>
+      <c r="E513" t="inlineStr"/>
+      <c r="F513" t="inlineStr"/>
+      <c r="G513" t="inlineStr"/>
+      <c r="H513" t="inlineStr"/>
+      <c r="I513" t="inlineStr"/>
+      <c r="J513" t="inlineStr"/>
+      <c r="K513" t="inlineStr"/>
+      <c r="L513" t="inlineStr"/>
+      <c r="M513" t="inlineStr"/>
+      <c r="N513" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr"/>
+      <c r="C514" t="inlineStr"/>
+      <c r="D514" t="inlineStr"/>
+      <c r="E514" t="inlineStr"/>
+      <c r="F514" t="inlineStr"/>
+      <c r="G514" t="inlineStr"/>
+      <c r="H514" t="inlineStr"/>
+      <c r="I514" t="inlineStr"/>
+      <c r="J514" t="inlineStr"/>
+      <c r="K514" t="inlineStr"/>
+      <c r="L514" t="inlineStr"/>
+      <c r="M514" t="inlineStr"/>
+      <c r="N514" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr"/>
+      <c r="C515" t="inlineStr"/>
+      <c r="D515" t="inlineStr"/>
+      <c r="E515" t="inlineStr"/>
+      <c r="F515" t="inlineStr"/>
+      <c r="G515" t="inlineStr"/>
+      <c r="H515" t="inlineStr"/>
+      <c r="I515" t="inlineStr"/>
+      <c r="J515" t="inlineStr"/>
+      <c r="K515" t="inlineStr"/>
+      <c r="L515" t="inlineStr"/>
+      <c r="M515" t="inlineStr"/>
+      <c r="N515" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr"/>
+      <c r="C516" t="inlineStr"/>
+      <c r="D516" t="inlineStr"/>
+      <c r="E516" t="inlineStr"/>
+      <c r="F516" t="inlineStr"/>
+      <c r="G516" t="inlineStr"/>
+      <c r="H516" t="inlineStr"/>
+      <c r="I516" t="inlineStr"/>
+      <c r="J516" t="inlineStr"/>
+      <c r="K516" t="inlineStr"/>
+      <c r="L516" t="inlineStr"/>
+      <c r="M516" t="inlineStr"/>
+      <c r="N516" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr"/>
+      <c r="C517" t="inlineStr"/>
+      <c r="D517" t="inlineStr"/>
+      <c r="E517" t="inlineStr"/>
+      <c r="F517" t="inlineStr"/>
+      <c r="G517" t="inlineStr"/>
+      <c r="H517" t="inlineStr"/>
+      <c r="I517" t="inlineStr"/>
+      <c r="J517" t="inlineStr"/>
+      <c r="K517" t="inlineStr"/>
+      <c r="L517" t="inlineStr"/>
+      <c r="M517" t="inlineStr"/>
+      <c r="N517" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr"/>
+      <c r="C518" t="inlineStr"/>
+      <c r="D518" t="inlineStr"/>
+      <c r="E518" t="inlineStr"/>
+      <c r="F518" t="inlineStr"/>
+      <c r="G518" t="inlineStr"/>
+      <c r="H518" t="inlineStr"/>
+      <c r="I518" t="inlineStr"/>
+      <c r="J518" t="inlineStr"/>
+      <c r="K518" t="inlineStr"/>
+      <c r="L518" t="inlineStr"/>
+      <c r="M518" t="inlineStr"/>
+      <c r="N518" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr"/>
+      <c r="C519" t="inlineStr"/>
+      <c r="D519" t="inlineStr"/>
+      <c r="E519" t="inlineStr"/>
+      <c r="F519" t="inlineStr"/>
+      <c r="G519" t="inlineStr"/>
+      <c r="H519" t="inlineStr"/>
+      <c r="I519" t="inlineStr"/>
+      <c r="J519" t="inlineStr"/>
+      <c r="K519" t="inlineStr"/>
+      <c r="L519" t="inlineStr"/>
+      <c r="M519" t="inlineStr"/>
+      <c r="N519" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr"/>
+      <c r="C520" t="inlineStr"/>
+      <c r="D520" t="inlineStr"/>
+      <c r="E520" t="inlineStr"/>
+      <c r="F520" t="inlineStr"/>
+      <c r="G520" t="inlineStr"/>
+      <c r="H520" t="inlineStr"/>
+      <c r="I520" t="inlineStr"/>
+      <c r="J520" t="inlineStr"/>
+      <c r="K520" t="inlineStr"/>
+      <c r="L520" t="inlineStr"/>
+      <c r="M520" t="inlineStr"/>
+      <c r="N520" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr"/>
+      <c r="C521" t="inlineStr"/>
+      <c r="D521" t="inlineStr"/>
+      <c r="E521" t="inlineStr"/>
+      <c r="F521" t="inlineStr"/>
+      <c r="G521" t="inlineStr"/>
+      <c r="H521" t="inlineStr"/>
+      <c r="I521" t="inlineStr"/>
+      <c r="J521" t="inlineStr"/>
+      <c r="K521" t="inlineStr"/>
+      <c r="L521" t="inlineStr"/>
+      <c r="M521" t="inlineStr"/>
+      <c r="N521" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr"/>
+      <c r="C522" t="inlineStr"/>
+      <c r="D522" t="inlineStr"/>
+      <c r="E522" t="inlineStr"/>
+      <c r="F522" t="inlineStr"/>
+      <c r="G522" t="inlineStr"/>
+      <c r="H522" t="inlineStr"/>
+      <c r="I522" t="inlineStr"/>
+      <c r="J522" t="inlineStr"/>
+      <c r="K522" t="inlineStr"/>
+      <c r="L522" t="inlineStr"/>
+      <c r="M522" t="inlineStr"/>
+      <c r="N522" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr"/>
+      <c r="C523" t="inlineStr"/>
+      <c r="D523" t="inlineStr"/>
+      <c r="E523" t="inlineStr"/>
+      <c r="F523" t="inlineStr"/>
+      <c r="G523" t="inlineStr"/>
+      <c r="H523" t="inlineStr"/>
+      <c r="I523" t="inlineStr"/>
+      <c r="J523" t="inlineStr"/>
+      <c r="K523" t="inlineStr"/>
+      <c r="L523" t="inlineStr"/>
+      <c r="M523" t="inlineStr"/>
+      <c r="N523" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr"/>
+      <c r="C524" t="inlineStr"/>
+      <c r="D524" t="inlineStr"/>
+      <c r="E524" t="inlineStr"/>
+      <c r="F524" t="inlineStr"/>
+      <c r="G524" t="inlineStr"/>
+      <c r="H524" t="inlineStr"/>
+      <c r="I524" t="inlineStr"/>
+      <c r="J524" t="inlineStr"/>
+      <c r="K524" t="inlineStr"/>
+      <c r="L524" t="inlineStr"/>
+      <c r="M524" t="inlineStr"/>
+      <c r="N524" t="n">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr"/>
+      <c r="C525" t="inlineStr"/>
+      <c r="D525" t="inlineStr"/>
+      <c r="E525" t="inlineStr"/>
+      <c r="F525" t="inlineStr"/>
+      <c r="G525" t="inlineStr"/>
+      <c r="H525" t="inlineStr"/>
+      <c r="I525" t="inlineStr"/>
+      <c r="J525" t="inlineStr"/>
+      <c r="K525" t="inlineStr"/>
+      <c r="L525" t="inlineStr"/>
+      <c r="M525" t="inlineStr"/>
+      <c r="N525" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr"/>
+      <c r="C526" t="inlineStr"/>
+      <c r="D526" t="inlineStr"/>
+      <c r="E526" t="inlineStr"/>
+      <c r="F526" t="inlineStr"/>
+      <c r="G526" t="inlineStr"/>
+      <c r="H526" t="inlineStr"/>
+      <c r="I526" t="inlineStr"/>
+      <c r="J526" t="inlineStr"/>
+      <c r="K526" t="inlineStr"/>
+      <c r="L526" t="inlineStr"/>
+      <c r="M526" t="inlineStr"/>
+      <c r="N526" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr"/>
+      <c r="C527" t="inlineStr"/>
+      <c r="D527" t="inlineStr"/>
+      <c r="E527" t="inlineStr"/>
+      <c r="F527" t="inlineStr"/>
+      <c r="G527" t="inlineStr"/>
+      <c r="H527" t="inlineStr"/>
+      <c r="I527" t="inlineStr"/>
+      <c r="J527" t="inlineStr"/>
+      <c r="K527" t="inlineStr"/>
+      <c r="L527" t="inlineStr"/>
+      <c r="M527" t="inlineStr"/>
+      <c r="N527" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr"/>
+      <c r="C528" t="inlineStr"/>
+      <c r="D528" t="inlineStr"/>
+      <c r="E528" t="inlineStr"/>
+      <c r="F528" t="inlineStr"/>
+      <c r="G528" t="inlineStr"/>
+      <c r="H528" t="inlineStr"/>
+      <c r="I528" t="inlineStr"/>
+      <c r="J528" t="inlineStr"/>
+      <c r="K528" t="inlineStr"/>
+      <c r="L528" t="inlineStr"/>
+      <c r="M528" t="inlineStr"/>
+      <c r="N528" t="n">
+        <v>4.669777777777778</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr"/>
+      <c r="C529" t="inlineStr"/>
+      <c r="D529" t="inlineStr"/>
+      <c r="E529" t="inlineStr"/>
+      <c r="F529" t="inlineStr"/>
+      <c r="G529" t="inlineStr"/>
+      <c r="H529" t="inlineStr"/>
+      <c r="I529" t="inlineStr"/>
+      <c r="J529" t="inlineStr"/>
+      <c r="K529" t="inlineStr"/>
+      <c r="L529" t="inlineStr"/>
+      <c r="M529" t="inlineStr"/>
+      <c r="N529" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr"/>
+      <c r="C530" t="inlineStr"/>
+      <c r="D530" t="inlineStr"/>
+      <c r="E530" t="inlineStr"/>
+      <c r="F530" t="inlineStr"/>
+      <c r="G530" t="inlineStr"/>
+      <c r="H530" t="inlineStr"/>
+      <c r="I530" t="inlineStr"/>
+      <c r="J530" t="inlineStr"/>
+      <c r="K530" t="inlineStr"/>
+      <c r="L530" t="inlineStr"/>
+      <c r="M530" t="inlineStr"/>
+      <c r="N530" t="inlineStr">
+        <is>
+          <t>{0: 0.06666666666666667, 1: 0.06666666666666667, 2: 0.06666666666666667, 3: 0.06666666666666667, 4: 0.06666666666666667, 5: 0.06666666666666667, 6: 0.06666666666666667, 7: 0.06666666666666667, 8: 0.06666666666666667, 9: 0.06666666666666667, 10: 0.06666666666666667, 11: 0.06666666666666667, 12: 0.06666666666666667, 13: 0.06666666666666667, 14: 0.06666666666666667}</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr"/>
+      <c r="C531" t="inlineStr"/>
+      <c r="D531" t="inlineStr"/>
+      <c r="E531" t="inlineStr"/>
+      <c r="F531" t="inlineStr"/>
+      <c r="G531" t="inlineStr"/>
+      <c r="H531" t="inlineStr"/>
+      <c r="I531" t="inlineStr"/>
+      <c r="J531" t="inlineStr"/>
+      <c r="K531" t="inlineStr"/>
+      <c r="L531" t="inlineStr"/>
+      <c r="M531" t="inlineStr"/>
+      <c r="N531" t="inlineStr">
+        <is>
+          <t>['[-0.0009776350343599916, 2.520699977874756]', '[-0.0012633800506591797, 2.0419600009918213]', '[-0.0025883899070322514, 2.808150053024292]', '[-0.0045527801848948, 0.45742499828338623]', '[-0.006321670021861792, 1.3289899826049805]', '[-0.007083420176059008, 2.0637400150299072]', '[-0.007362130098044872, 2.7051899433135986]', '[-0.00818943977355957, 0.4245370030403137]', '[-0.012052999809384346, 0.9471909999847412]', '[-0.013943299651145935, 0.20943599939346313]', '[-0.014347399584949017, 3.025860071182251]', '[-0.015203399583697319, 2.5843300819396973]', '[-0.017614800482988358, 3.3935599327087402]', '[-0.02017419971525669, 0.9521859884262085]', '[-0.021791499108076096, 2.712239980697632]', '[-0.022242499515414238, 0.2983810007572174]', '[-0.026512300595641136, 1.5236599445343018]', '[-0.02670760080218315, 3.432760000228882]', '[-0.02803869917988777, 3.0]', '[-0.029058199375867844, 2.347369909286499]', '[-0.029064200818538666, 2.100529909133911]', '[-0.029380399733781815, 0.3312169909477234]', '[-0.033528298139572144, 0.47436100244522095]', '[-0.036360401660203934, 1.3271299600601196]', '[-0.03657050058245659, 3.2184898853302]', '[-0.03897939994931221, 1.7664899826049805]', '[-0.03923200070858002, 3.3294899463653564]', '[-0.03964250162243843, 1.6664400100708008]', '[-0.041360799223184586, 3.544480085372925]', '[-0.04163390025496483, 0.7761669754981995]', '[-0.04344389960169792, 1.8447799682617188]', '[-0.04487530142068863, 2.6537399291992188]', '[-0.044893600046634674, 2.882240056991577]', '[-0.04597700014710426, 2.597830057144165]', '[-0.0491551011800766, 0.8076500296592712]', '[-0.05169830098748207, 0.3074930012226105]', '[-0.05233730003237724, 2.6529600620269775]', '[-0.053155601024627686, 0.9211879968643188]', '[-0.05385600030422211, 2.7053699493408203]', '[-0.05563569813966751, 2.8615100383758545]', '[-0.05675220116972923, 1.0783900022506714]', '[-0.05872099846601486, 0.3208889961242676]', '[-0.06141730025410652, 0.221110999584198]', '[-0.061974700540304184, 2.4560599327087402]', '[-0.06349419802427292, 1.3456900119781494]', '[-0.06351300328969955, 0.08961399644613266]', '[-0.06355930119752884, 2.69638991355896]', '[-0.066982202231884, 2.743769884109497]', '[-0.06877110153436661, 0.6093249917030334]', '[-0.06988160312175751, 0.11686400324106216]', '[-0.07278440147638321, 3.1892199516296387]', '[-0.07363729923963547, 2.7940099239349365]', '[-0.07796479761600494, 2.681649923324585]', '[-0.0786907970905304, 1.2066899538040161]', '[-0.07917500287294388, 2.6620500087738037]', '[-0.08223550021648407, 1.7528599500656128]', '[-0.08419360220432281, 1.9230999946594238]', '[-0.08734049648046494, 2.6550700664520264]', '[-0.0888959988951683, 2.6646900177001953]', '[-0.09145980328321457, 0.8206549882888794]', '[-0.09306669980287552, 2.8389599323272705]', '[-0.09315220266580582, 3.287329912185669]', '[-0.10025300085544586, 1.4390900135040283]', '[-0.10026799887418747, 0.7405380010604858]', '[-0.10134399682283401, 3.524060010910034]', '[-0.10218799859285355, 0.5567119717597961]', '[-0.10523100197315216, 3.3036398887634277]', '[-0.10663600265979767, 3.2089600563049316]', '[-0.10946699976921082, 0.5695199966430664]', '[-0.11165600270032883, 3.0868799686431885]', '[-0.11243999749422073, 1.9580600261688232]', '[-0.11321400105953217, 3.230710029602051]', '[-0.11342199891805649, 0.3952710032463074]', '[-0.11577799916267395, 2.7018399238586426]', '[-0.12934699654579163, 0.5144919753074646]', '[-0.1295669972896576, 3.0848801136016846]', '[-0.12978899478912354, 3.073580026626587]', '[-0.13062399625778198, 2.8397998809814453]', '[-0.14531099796295166, 0.29065099358558655]', '[-0.14608199894428253, 3.1735100746154785]', '[-0.14622700214385986, 2.7958600521087646]', '[-0.16269700229167938, 2.3758299350738525]', '[-0.16563299298286438, 2.5047199726104736]', '[-0.17705200612545013, 0.3678649961948395]', '[-0.18442000448703766, 2.9986000061035156]', '[-0.1894419938325882, 1.6455700397491455]', '[-0.1970289945602417, 0.5033289790153503]', '[-0.19869300723075867, 3.3459999561309814]', '[-0.23119400441646576, 2.583750009536743]', '[-0.2345300018787384, 0.8940349817276001]', '[-0.2496740072965622, 0.5864930152893066]', '[-0.2528719902038574, 2.626310110092163]', '[-0.2915840148925781, 0.17844200134277344]', '[-0.3021169900894165, 1.8686100244522095]', '[-0.359811007976532, 2.9359099864959717]', '[0.0008771420107223094, 1.4219499826431274]', '[0.0020502801053225994, 2.8222100734710693]', '[0.0021669899579137564, 1.643779993057251]', '[0.0029406200628727674, 0.7672119736671448]', '[0.0030243999790400267, 1.716770052909851]', '[0.00563073018565774, 3.237989902496338]', '[0.006859899964183569, 2.1709399223327637]', '[0.006951000075787306, 0.05224649980664253]', '[0.007422389928251505, 3.059760093688965]', '[0.007739370223134756, 0.2300969958305359]', '[0.007815360091626644, 2.980340003967285]', '[0.008600950241088867, 3.439970016479492]', '[0.009095069952309132, 2.603879928588867]', '[0.01153970044106245, 1.8023300170898438]', '[0.012676199898123741, 1.242650032043457]', '[0.012943900190293789, 1.7260700464248657]', '[0.013201399706304073, 0.7930960059165955]', '[0.013485699892044067, 3.528059959411621]', '[0.014512299560010433, 2.9839000701904297]', '[0.015212999656796455, 1.1079399585723877]', '[0.01580129936337471, 1.3472299575805664]', '[0.016393499448895454, 3.4384500980377197]', '[0.016449199989438057, 2.8159101009368896]', '[0.018940599635243416, 2.863379955291748]', '[0.01925629936158657, 0.4666140079498291]', '[0.02088649943470955, -0.10123699903488159]', '[0.021726500242948532, 2.3071401119232178]', '[0.022097699344158173, 0.4407849907875061]', '[0.02229510061442852, 1.0489000082015991]', '[0.022367099300026894, 1.8845200538635254]', '[0.023792199790477753, 2.9987199306488037]', '[0.024684300646185875, 2.765660047531128]', '[0.025316700339317322, 3.1442298889160156]', '[0.02671780064702034, 2.8396100997924805]', '[0.02687850035727024, 0.0024925998877733946]', '[0.02694310061633587, 0.7786989808082581]', '[0.0274656992405653, 1.9266200065612793]', '[0.029196299612522125, 0.5538110136985779]', '[0.030670199543237686, 0.7858089804649353]', '[0.0314394012093544, 3.1038599014282227]', '[0.03263520076870918, 1.2319200038909912]', '[0.0330796018242836, 2.5304999351501465]', '[0.034361500293016434, 2.8786299228668213]', '[0.035384099930524826, 2.779409885406494]', '[0.035733699798583984, 3.215939998626709]', '[0.03653259947896004, 2.988100051879883]', '[0.03682209923863411, 3.6463301181793213]', '[0.03776809945702553, 2.919189929962158]', '[0.03795519843697548, 2.9462199211120605]', '[0.038596898317337036, 0.5440559983253479]', '[0.03904670104384422, 2.9110400676727295]', '[0.04022129997611046, 3.093590021133423]', '[0.04040930047631264, 0.8390309810638428]', '[0.04290499910712242, 2.7498199939727783]', '[0.043901801109313965, 2.0228800773620605]', '[0.04404409974813461, 2.0069100856781006]', '[0.04720370098948479, 0.7449989914894104]', '[0.04805989935994148, 0.1718049943447113]', '[0.048487599939107895, 0.3873260021209717]', '[0.048890601843595505, 2.781450033187866]', '[0.05207369849085808, -0.2416979968547821]', '[0.052163999527692795, 2.1010000705718994]', '[0.053748201578855515, 0.6357510089874268]', '[0.053881898522377014, 0.38201001286506653]', '[0.054447900503873825, 1.7524399757385254]', '[0.05471380054950714, 2.673569917678833]', '[0.05564559996128082, 0.8794419765472412]', '[0.05591059848666191, 2.9075000286102295]', '[0.05837329849600792, 1.0551999807357788]', '[0.05886689946055412, 0.7529879808425903]', '[0.058977801352739334, 3.511579990386963]', '[0.060908399522304535, 1.5287699699401855]', '[0.06214990094304085, 2.733880043029785]', '[0.06345699727535248, 1.235990047454834]', '[0.06364669650793076, 3.0224499702453613]', '[0.06689529865980148, 0.8248739838600159]', '[0.06810220330953598, 1.1833699941635132]', '[0.06854840368032455, 1.2028000354766846]', '[0.07020069658756256, 0.823108971118927]', '[0.07054729759693146, 0.30217400193214417]', '[0.07155189663171768, 0.9149540066719055]', '[0.0732956975698471, 2.8837199211120605]', '[0.07383269816637039, 2.950239896774292]', '[0.07385729998350143, 1.7306499481201172]', '[0.0755767971277237, 1.7403000593185425]', '[0.07581479847431183, 2.805340051651001]', '[0.07590849697589874, 2.9230799674987793]', '[0.07659299671649933, 3.281369924545288]', '[0.07716730237007141, 3.4435200691223145]', '[0.07804369926452637, 0.4326860010623932]', '[0.07850690186023712, 0.7311019897460938]', '[0.07896210253238678, 1.3075499534606934]', '[0.08006910234689713, 1.3375400304794312]', '[0.08072470128536224, 2.876230001449585]', '[0.08105859905481339, 2.8584399223327637]', '[0.08161280304193497, 2.9649300575256348]', '[0.0831070989370346, 2.5530500411987305]', '[0.08330260217189789, 2.4401800632476807]', '[0.08387040346860886, 1.3134900331497192]', '[0.08485320210456848, 2.6361100673675537]', '[0.08610700070858002, 2.791110038757324]', '[0.08873060345649719, 0.46615201234817505]', '[0.08889850229024887, 2.3440001010894775]', '[0.08999810367822647, 0.5516219735145569]', '[0.0906601995229721, 2.3483099937438965]', '[0.09393390268087387, 1.1810200214385986]', '[0.09399110078811646, 0.8634939789772034]', '[0.09404739737510681, 0.0822812020778656]', '[0.0941300019621849, -0.18387700617313385]', '[0.0944266989827156, 0.6545370221138]', '[0.09517130255699158, 3.0890800952911377]', '[0.09695280343294144, 3.1605799198150635]', '[0.09704519808292389, 0.21639899909496307]', '[0.09727679938077927, 3.07069993019104]', '[0.09764649718999863, 2.5141100883483887]', '[0.09878040105104446, 1.2646199464797974]', '[0.09887400269508362, 0.5979070067405701]', '[0.09965880215167999, 0.569661021232605]', '[0.10077299922704697, 3.006999969482422]', '[0.10134299844503403, 3.238229990005493]', '[0.10233200341463089, 0.37714800238609314]', '[0.10244099795818329, 3.382110118865967]', '[0.10373400151729584, 0.5543460249900818]', '[0.10482600331306458, 1.5056099891662598]', '[0.10528799891471863, 1.5161800384521484]', '[0.10590100288391113, 1.746559977531433]', '[0.10678300261497498, 2.955319881439209]', '[0.10704199969768524, 2.4604198932647705]', '[0.10774999856948853, 1.730720043182373]', '[0.10878100246191025, 2.3489298820495605]', '[0.10881400108337402, 2.3312599658966064]', '[0.1091570034623146, 2.8630099296569824]', '[0.11053799837827682, 3.195499897003174]', '[0.11083400249481201, 0.49000000953674316]', '[0.11124099791049957, 0.44751501083374023]', '[0.11274600028991699, 2.9396400451660156]', '[0.11332300305366516, 2.244110107421875]', '[0.11336900293827057, 0.4550360143184662]', '[0.11363500356674194, 3.2443199157714844]', '[0.11545299738645554, 2.636899948120117]', '[0.11560799926519394, 0.4825649857521057]', '[0.11803899705410004, 1.1008000373840332]', '[0.11834000051021576, 2.5886600017547607]', '[0.11865200102329254, 3.1060099601745605]', '[0.11929299682378769, 3.3195900917053223]', '[0.1203640028834343, 1.2825000286102295]', '[0.1204650029540062, 2.3504300117492676]', '[0.12298599630594254, 1.0341500043869019]', '[0.12306500226259232, 2.5200700759887695]', '[0.12309399992227554, 2.911530017852783]', '[0.12345100194215775, 3.0537800788879395]', '[0.12372200191020966, 3.396359920501709]', '[0.12381300330162048, 0.14071400463581085]', '[0.12409999966621399, 3.335930109024048]', '[0.12578999996185303, 2.079770088195801]', '[0.1259630024433136, 3.324399948120117]', '[0.12747499346733093, 2.6949501037597656]', '[0.12799899280071259, 2.721060037612915]', '[0.12928199768066406, 2.3022100925445557]', '[0.1295669972896576, 0.8986309766769409]', '[0.13060100376605988, 2.8552699089050293]', '[0.13105499744415283, 2.024600028991699]', '[0.1310579925775528, 0.3499720096588135]', '[0.13120600581169128, 1.0012999773025513]', '[0.1326490044593811, 2.97625994682312]', '[0.13441599905490875, 3.574310064315796]', '[0.1349180042743683, 1.0995099544525146]', '[0.13503800332546234, 2.9830400943756104]', '[0.1350499987602234, -0.06172189861536026]', '[0.13536499440670013, 2.809109926223755]', '[0.135452002286911, 2.689379930496216]', '[0.1364080011844635, 0.4970569908618927]', '[0.13698799908161163, 2.866179943084717]', '[0.14031000435352325, 3.4372200965881348]', '[0.14032700657844543, 2.755500078201294]', '[0.14067499339580536, 1.0010099411010742]', '[0.1407250016927719, 1.4371399879455566]', '[0.14124399423599243, 0.8826850056648254]', '[0.14256399869918823, 2.647249937057495]', '[0.14260299503803253, 0.1435140073299408]', '[0.14385199546813965, 2.946510076522827]', '[0.14421799778938293, -0.02722020074725151]', '[0.14462600648403168, 2.6231400966644287]', '[0.14495499432086945, 2.4281399250030518]', '[0.14523200690746307, 2.535799980163574]', '[0.1454869955778122, 2.63385009765625]', '[0.14582400023937225, 2.0397799015045166]', '[0.14631199836730957, 3.0251801013946533]', '[0.1463869959115982, 0.19641800224781036]', '[0.14680500328540802, 2.604290008544922]', '[0.14704200625419617, 2.358059883117676]', '[0.1471879929304123, 0.6644629836082458]', '[0.14734899997711182, 2.082089900970459]', '[0.14906099438667297, 2.8975400924682617]', '[0.1499200016260147, 3.5100998878479004]', '[0.15183000266551971, 3.0257999897003174]', '[0.15220899879932404, 2.0034101009368896]', '[0.15363000333309174, 0.19139400124549866]', '[0.15459799766540527, 1.0424799919128418]', '[0.15569999814033508, 0.6208119988441467]', '[0.15726099908351898, 0.5595880150794983]', '[0.15794700384140015, 0.6395480036735535]', '[0.15838399529457092, 1.7662800550460815]', '[0.1586180031299591, 2.348560094833374]', '[0.1590069979429245, 0.7552610039710999]', '[0.1596740037202835, 1.0744199752807617]', '[0.15987500548362732, 0.4047369956970215]', '[0.1609880030155182, 1.8621799945831299]', '[0.1622450053691864, 2.8833398818969727]', '[0.16264399886131287, 2.295599937438965]', '[0.1629440039396286, 2.725559949874878]', '[0.16306500136852264, 2.248339891433716]', '[0.1638460010290146, 3.2626900672912598]', '[0.16401000320911407, 1.3493000268936157]', '[0.1641779989004135, 2.979449987411499]', '[0.16423800587654114, 0.41895899176597595]', '[0.16458000242710114, 1.8814799785614014]', '[0.1653210073709488, 1.8069599866867065]', '[0.1668429970741272, 1.839020013809204]', '[0.16714799404144287, 2.6528100967407227]', '[0.16745999455451965, 0.4250420033931732]', '[0.16748900711536407, 3.490609884262085]', '[0.1689240038394928, 1.0509899854660034]', '[0.16970199346542358, 3.03971004486084]', '[0.1715490072965622, 3.063159942626953]', '[0.17180900275707245, 3.1900599002838135]', '[0.17183800041675568, 3.128999948501587]', '[0.17231500148773193, 1.5455900430679321]', '[0.17302100360393524, 1.9638899564743042]', '[0.17339099943637848, 2.714329957962036]', '[0.17346200346946716, 0.8287960290908813]', '[0.17439599335193634, 3.4499199390411377]', '[0.17471100389957428, 0.9002150297164917]', '[0.17476099729537964, -0.11082500219345093]', '[0.17502599954605103, 1.9865599870681763]', '[0.17621800303459167, 2.700969934463501]', '[0.17657600343227386, 2.487370014190674]', '[0.17691299319267273, 1.4029200077056885]', '[0.17692600190639496, 1.7047200202941895]', '[0.17693400382995605, 2.805840015411377]', '[0.1770700067281723, 0.949741005897522]', '[0.17757900059223175, 0.5590459704399109]', '[0.17774300277233124, 1.3673800230026245]', '[0.17782999575138092, 2.6366701126098633]', '[0.17788000404834747, 2.8457000255584717]', '[0.17843300104141235, 3.044100046157837]', '[0.1787630021572113, 2.6336700916290283]', '[0.1803860068321228, 3.279409885406494]', '[0.18062500655651093, 0.707843005657196]', '[0.18107299506664276, 3.256890058517456]', '[0.18110999464988708, 2.675220012664795]', '[0.18210400640964508, 1.3541500568389893]', '[0.18315500020980835, 0.2841559946537018]', '[0.18372799456119537, 1.3496700525283813]', '[0.1838580071926117, 0.5196449756622314]', '[0.1838890016078949, 2.794919967651367]', '[0.18461699783802032, 2.8184499740600586]', '[0.18539200723171234, 2.9773800373077393]', '[0.18595099449157715, 3.189300060272217]', '[0.18628400564193726, 3.0501999855041504]', '[0.18643300235271454, 0.5928900241851807]', '[0.18665499985218048, 2.624300003051758]', '[0.1868620067834854, 0.714136004447937]', '[0.18807299435138702, 0.6904540061950684]', '[0.18951000273227692, 3.5419199466705322]', '[0.18997199833393097, 1.2466000318527222]', '[0.19155199825763702, 0.19674600660800934]', '[0.19188599288463593, 0.2958660125732422]', '[0.19225700199604034, -0.010019400157034397]', '[0.19248299300670624, 0.009403419680893421]', '[0.1934249997138977, 1.9586399793624878]', '[0.19497300684452057, 3.2199299335479736]', '[0.19531500339508057, 1.1087299585342407]', '[0.19566500186920166, 2.809999942779541]', '[0.19637000560760498, 3.3097100257873535]', '[0.19736500084400177, 2.7823901176452637]', '[0.19776800274848938, 3.127609968185425]', '[0.19921499490737915, 2.437079906463623]', '[0.1999559998512268, 1.204800009727478]', '[0.20002000033855438, 3.5099799633026123]', '[0.20093199610710144, 1.5241600275039673]', '[0.20123399794101715, 2.7985599040985107]', '[0.2016180008649826, 1.9982800483703613]', '[0.20204399526119232, 0.43121999502182007]', '[0.20214299857616425, 3.0831799507141113]', '[0.20229999721050262, 1.9631400108337402]', '[0.20380699634552002, 3.6203200817108154]', '[0.2038470059633255, 1.9026399850845337]', '[0.20479999482631683, 0.25631898641586304]', '[0.20490899682044983, 2.8747498989105225]', '[0.20523199439048767, 3.0625998973846436]', '[0.20545800030231476, 2.8246800899505615]', '[0.20554499328136444, 0.06843289732933044]', '[0.2074429988861084, 1.9522000551223755]', '[0.20745299756526947, 0.6567450165748596]', '[0.20779000222682953, 1.1416000127792358]', '[0.20822599530220032, 0.7018809914588928]', '[0.2091660052537918, 2.57354998588562]', '[0.21010999381542206, 2.511549949645996]', '[0.21054799854755402, 3.6802399158477783]', '[0.21091000735759735, 2.3427999019622803]', '[0.2110999971628189, 1.59443998336792]', '[0.21249599754810333, 1.497480034828186]', '[0.21300099790096283, 3.008970022201538]', '[0.21411900222301483, 3.0528600215911865]', '[0.21463200449943542, 0.8582689762115479]', '[0.21483099460601807, 2.9154300689697266]', '[0.21504899859428406, -0.02509159967303276]', '[0.21511100232601166, 3.03016996383667]', '[0.21549099683761597, 0.3889389932155609]', '[0.21589800715446472, 3.0746800899505615]', '[0.21626299619674683, 0.48556798696517944]', '[0.21640199422836304, 2.5914900302886963]', '[0.2167699933052063, 0.05565379932522774]', '[0.21818199753761292, 3.5103399753570557]', '[0.2183919996023178, 0.20677199959754944]', '[0.21865199506282806, 1.548699975013733]', '[0.21884000301361084, 0.1050650030374527]', '[0.21908099949359894, 2.8890199661254883]', '[0.22118200361728668, 2.551029920578003]', '[0.22325399518013, 3.0034101009368896]', '[0.22442500293254852, 3.2186501026153564]', '[0.22443999350070953, 0.45013201236724854]', '[0.22444899380207062, 2.3142099380493164]', '[0.22459900379180908, 2.86365008354187]', '[0.22570399940013885, 2.3974599838256836]', '[0.22663000226020813, 2.887809991836548]', '[0.22725899517536163, 2.969320058822632]', '[0.2273789942264557, 0.659546971321106]', '[0.22750000655651093, 3.066879987716675]', '[0.228192999958992, 2.4873900413513184]', '[0.22868099808692932, 2.476069927215576]', '[0.22918400168418884, 1.4368400573730469]', '[0.22940699756145477, 3.200089931488037]', '[0.22961199283599854, 2.5480198860168457]', '[0.23017899692058563, -0.33574700355529785]', '[0.23035700619220734, 0.9133989810943604]', '[0.2311750054359436, 0.5577329993247986]', '[0.23219899833202362, 0.27812498807907104]', '[0.2326579988002777, 0.6998519897460938]', '[0.2328689992427826, 0.5858569741249084]', '[0.23319299519062042, 2.996579885482788]', '[0.23356400430202484, 1.8668400049209595]', '[0.23399899899959564, 2.3853800296783447]', '[0.2347320020198822, 0.17305000126361847]', '[0.23505499958992004, 0.6054080128669739]', '[0.23601000010967255, 0.5075179934501648]', '[0.23616500198841095, 2.7983100414276123]', '[0.23668600618839264, 3.487760066986084]', '[0.2372799962759018, 1.8819400072097778]', '[0.23771199584007263, 2.9063000679016113]', '[0.237869992852211, 1.4166699647903442]', '[0.23795300722122192, 1.4661400318145752]', '[0.2395939975976944, 2.9266700744628906]', '[0.24096600711345673, 3.3544299602508545]', '[0.24130800366401672, 2.9606199264526367]', '[0.2420399934053421, 0.5383070111274719]', '[0.24254600703716278, 0.22945299744606018]', '[0.2429489940404892, 1.10903000831604]', '[0.2434699982404709, 0.1772249937057495]', '[0.24364100396633148, 1.5371500253677368]', '[0.24397000670433044, 2.8018300533294678]', '[0.24438199400901794, -0.07144410163164139]', '[0.2451310008764267, 3.156980037689209]', '[0.2454030066728592, 0.660260021686554]', '[0.24686500430107117, 2.3216099739074707]', '[0.24707500636577606, 2.329129934310913]', '[0.24764800071716309, 1.6945699453353882]', '[0.24773800373077393, 1.7778700590133667]', '[0.24804000556468964, 2.9836199283599854]', '[0.2483299970626831, 0.5574929714202881]', '[0.24845099449157715, 0.9890599846839905]', '[0.2500239908695221, 1.707900047302246]', '[0.25013500452041626, 0.5484610199928284]', '[0.2511169910430908, 0.6882169842720032]', '[0.252469003200531, 2.0244100093841553]', '[0.25298699736595154, 2.51528000831604]', '[0.2536900043487549, 1.8496400117874146]', '[0.25369900465011597, 1.6773799657821655]', '[0.25416699051856995, 0.4991320073604584]', '[0.2541869878768921, 2.654939889907837]', '[0.25429001450538635, 3.136080026626587]', '[0.25465598702430725, 0.7099599838256836]', '[0.255048006772995, 0.5872039794921875]', '[0.2553589940071106, 0.28968098759651184]', '[0.2553830146789551, 0.5452359914779663]', '[0.2563050091266632, 0.42432400584220886]', '[0.2567110061645508, 0.03551020100712776]', '[0.25709500908851624, 1.2028199434280396]', '[0.25764501094818115, 0.3803209960460663]', '[0.2578360140323639, 2.623889923095703]', '[0.26025301218032837, 2.932339906692505]', '[0.2605839967727661, 1.088420033454895]', '[0.26109299063682556, 0.8027139902114868]', '[0.26114600896835327, 2.153140068054199]', '[0.2611899971961975, 3.2690999507904053]', '[0.2616159915924072, 2.8697800636291504]', '[0.26173099875450134, 0.7009389996528625]', '[0.262239009141922, 0.25043800473213196]', '[0.2633489966392517, 1.1896899938583374]', '[0.26364201307296753, 3.2513999938964844]', '[0.263949990272522, 1.294100046157837]', '[0.26553699374198914, 1.52128005027771]', '[0.26557400822639465, 2.16825008392334]', '[0.26568499207496643, 1.6870499849319458]', '[0.2664420008659363, 2.161439895629883]', '[0.2664479911327362, 2.9882400035858154]', '[0.26670199632644653, 1.590019941329956]', '[0.2679019868373871, 0.5252320170402527]', '[0.2681809961795807, 2.8981199264526367]', '[0.26899799704551697, 0.42432901263237]', '[0.2705239951610565, 2.751189947128296]', '[0.2713710069656372, 1.0763800144195557]', '[0.2714940011501312, 0.7220289707183838]', '[0.27176201343536377, 2.799639940261841]', '[0.2719759941101074, 2.7191898822784424]', '[0.27205801010131836, 2.4032399654388428]', '[0.27228400111198425, 1.4890199899673462]', '[0.27232399582862854, 2.7179300785064697]', '[0.2724500000476837, 0.718375027179718]', '[0.2757120132446289, 0.7354580163955688]', '[0.27596500515937805, 3.2197399139404297]', '[0.27653101086616516, 2.901900053024292]', '[0.276964008808136, 0.8955900073051453]', '[0.2770960032939911, 0.25123199820518494]', '[0.27712398767471313, 1.5911999940872192]', '[0.2772960066795349, 2.3250598907470703]', '[0.2774679958820343, -0.0442207008600235]', '[0.27768799662590027, 0.9334310293197632]', '[0.2777960002422333, 0.7074869871139526]', '[0.2780509889125824, 1.9677799940109253]', '[0.27856001257896423, 2.1112499237060547]', '[0.2786119878292084, 0.28912198543548584]', '[0.27897998690605164, 2.5246500968933105]', '[0.27908000349998474, 1.9445899724960327]', '[0.2791540026664734, 3.603760004043579]', '[0.27980300784111023, 0.6222620010375977]', '[0.28076499700546265, 2.1045799255371094]', '[0.2811869978904724, 2.862730026245117]', '[0.2814970016479492, 1.8714900016784668]', '[0.28162598609924316, 2.7416300773620605]', '[0.2817170023918152, -0.04675839841365814]', '[0.28259000182151794, 3.6443300247192383]', '[0.28265801072120667, 2.380539894104004]', '[0.28427499532699585, 2.8278698921203613]', '[0.284292995929718, 0.6856679916381836]', '[0.2843410074710846, 2.5968399047851562]', '[0.2846820056438446, 2.3227999210357666]', '[0.28484898805618286, 0.07471100240945816]', '[0.2854990065097809, 3.778630018234253]', '[0.28570300340652466, 1.4010599851608276]', '[0.2861790060997009, 0.49281299114227295]', '[0.28647300601005554, 0.8794800043106079]', '[0.2882849872112274, 0.6224179863929749]', '[0.28869199752807617, 3.0957698822021484]', '[0.28906500339508057, 2.1098101139068604]', '[0.2890680134296417, 0.8195269703865051]', '[0.2896310091018677, -0.04235289990901947]', '[0.28977200388908386, 0.34434500336647034]', '[0.28977400064468384, 2.7288599014282227]', '[0.2899250090122223, 3.292140007019043]', '[0.29029199481010437, 1.3080400228500366]', '[0.29038500785827637, 3.098050117492676]', '[0.2908029854297638, 2.9272499084472656]', '[0.29124799370765686, 3.0403099060058594]', '[0.2916789948940277, 2.956929922103882]', '[0.29170599579811096, 2.309230089187622]', '[0.2918680012226105, 2.6205201148986816]', '[0.2927339971065521, 2.7965199947357178]', '[0.2934019863605499, 2.6583399772644043]', '[0.29411599040031433, 0.3291209936141968]', '[0.2945060133934021, 2.8767800331115723]', '[0.2946290075778961, 0.3236849904060364]', '[0.2947719991207123, 0.315079003572464]', '[0.2954750061035156, 3.161910057067871]', '[0.29571399092674255, 3.384049892425537]', '[0.29622700810432434, 2.5854899883270264]', '[0.2966359853744507, 2.8361399173736572]', '[0.2967050075531006, 3.313849925994873]', '[0.2968679964542389, 0.6068040132522583]', '[0.2978529930114746, 2.749039888381958]', '[0.2982499897480011, 3.0792899131774902]', '[0.29842400550842285, 0.7764279842376709]', '[0.2985199987888336, 2.9760499000549316]', '[0.2988849878311157, 0.2535490095615387]', '[0.2989790141582489, 2.7588400840759277]', '[0.2993830144405365, 0.19438600540161133]', '[0.29959699511528015, 2.77662992477417]', '[0.2996320128440857, 2.821470022201538]', '[0.29986101388931274, 0.4173150062561035]', '[0.3001059889793396, 2.978940010070801]', '[0.3001280128955841, -0.11917699873447418]', '[0.3002519905567169, 1.8719300031661987]', '[0.30105701088905334, 0.8277419805526733]', '[0.30114901065826416, 2.7300000190734863]', '[0.3012329936027527, 3.0903398990631104]', '[0.3018690049648285, 2.866070032119751]', '[0.3031359910964966, -0.16054199635982513]', '[0.30314499139785767, 3.077440023422241]', '[0.30347099900245667, 1.3234699964523315]', '[0.3040289878845215, 0.5954939723014832]', '[0.3044559955596924, 0.5682119727134705]', '[0.30448099970817566, 1.0090800523757935]', '[0.3047510087490082, 2.996429920196533]', '[0.3054879903793335, 2.3461599349975586]', '[0.3057900071144104, 2.0005600452423096]', '[0.305961012840271, 2.6549899578094482]', '[0.30624300241470337, 2.965630054473877]', '[0.30649200081825256, 1.7785999774932861]', '[0.3074440062046051, 3.4491701126098633]', '[0.3086070120334625, 1.2436000108718872]', '[0.3087320029735565, 1.268030047416687]', '[0.3089509904384613, 3.0188798904418945]', '[0.30940499901771545, 1.9538600444793701]', '[0.3099069893360138, 2.9058399200439453]', '[0.3102380037307739, 0.5902079939842224]', '[0.31035900115966797, 0.2780190110206604]', '[0.3106519877910614, 0.2837730050086975]', '[0.311149001121521, 0.43231400847435]', '[0.31116798520088196, 3.4675099849700928]', '[0.3114579916000366, 2.7531399726867676]', '[0.3118009865283966, 0.25681498646736145]', '[0.3121120035648346, 3.382420063018799]', '[0.3122180104255676, 0.9933800101280212]', '[0.31263700127601624, 0.4574680030345917]', '[0.31292399764060974, 3.0838398933410645]', '[0.31332701444625854, 0.9084460139274597]', '[0.31383898854255676, 1.5420000553131104]', '[0.3139449954032898, 2.205209970474243]', '[0.3140380084514618, 2.342289924621582]', '[0.3141529858112335, 2.8923499584198]', '[0.31438499689102173, 2.269160032272339]', '[0.3148370087146759, 0.6851630210876465]', '[0.31508299708366394, 2.455080032348633]', '[0.31512999534606934, 2.879739999771118]', '[0.3154140114784241, 0.11225699633359909]', '[0.31556200981140137, 0.17045800387859344]', '[0.31564998626708984, 1.46943998336792]', '[0.3157289922237396, 3.597909927368164]', '[0.3170289993286133, 3.132080078125]', '[0.31796199083328247, 0.8814100027084351]', '[0.3191620111465454, 3.2558400630950928]', '[0.31984999775886536, 2.955579996109009]', '[0.3198759853839874, 0.862201988697052]', '[0.31999000906944275, 2.1803300380706787]', '[0.3201180100440979, 3.0035901069641113]', '[0.3201200067996979, 3.065880060195923]', '[0.32035601139068604, 0.7170320153236389]', '[0.320809006690979, 0.6367509961128235]', '[0.32103100419044495, 2.2026000022888184]', '[0.3210740089416504, 3.365499973297119]', '[0.3223179876804352, 3.6826999187469482]', '[0.3223550021648407, 3.2555301189422607]', '[0.3224489986896515, 0.6907740235328674]', '[0.3226799964904785, 0.8038849830627441]', '[0.3230609893798828, 3.30292010307312]', '[0.3233790099620819, 0.9696810245513916]', '[0.32352200150489807, 2.1063599586486816]', '[0.32365500926971436, 0.6359620094299316]', '[0.3238230049610138, 3.197510004043579]', '[0.3241080045700073, 0.23251000046730042]', '[0.324537992477417, 2.6233599185943604]', '[0.32464900612831116, 2.975980043411255]', '[0.3247610032558441, 1.6318700313568115]', '[0.3249100148677826, 3.1103999614715576]', '[0.3250249922275543, 0.6644330024719238]', '[0.3250890076160431, 0.6106340289115906]', '[0.3252849876880646, 0.30681100487709045]', '[0.3252969980239868, 1.2117400169372559]', '[0.3253040015697479, 2.532210111618042]', '[0.3254530131816864, 2.756510019302368]', '[0.32591599225997925, 1.3020600080490112]', '[0.32593798637390137, 0.7771649956703186]', '[0.3260419964790344, 3.255889892578125]', '[0.3263629972934723, 1.0698299407958984]', '[0.327657014131546, 1.7541899681091309]', '[0.3282409906387329, 2.384629964828491]', '[0.32848501205444336, 1.9763599634170532]', '[0.32896700501441956, 1.2750699520111084]', '[0.32918599247932434, 1.4518699645996094]', '[0.32933101058006287, 2.2868800163269043]', '[0.3294450044631958, 0.46256500482559204]', '[0.3295750021934509, 0.7201840281486511]', '[0.3313249945640564, 0.5896940231323242]', '[0.33173200488090515, 2.9685299396514893]', '[0.33178600668907166, 0.44293299317359924]', '[0.3319000005722046, 3.122159957885742]', '[0.3322480022907257, 1.001729965209961]', '[0.3325450122356415, 1.8458900451660156]', '[0.33254700899124146, 1.6499300003051758]', '[0.33264800906181335, 1.4728000164031982]', '[0.3327839970588684, 2.821120023727417]', '[0.3334580063819885, 2.5626800060272217]', '[0.333499014377594, 1.7856800556182861]', '[0.33364200592041016, 1.995270013809204]', '[0.3336699903011322, 2.9115099906921387]', '[0.33382898569107056, 3.3756299018859863]', '[0.33438000082969666, 0.8934080004692078]', '[0.3353019952774048, 3.0297000408172607]', '[0.33546799421310425, 1.5065200328826904]', '[0.33567601442337036, 2.9649100303649902]', '[0.3360320031642914, 1.0100799798965454]', '[0.33711400628089905, 2.542099952697754]', '[0.33778199553489685, 3.7704598903656006]', '[0.338331013917923, 2.9628798961639404]', '[0.3384230136871338, 2.594099998474121]', '[0.3390829861164093, 2.6936299800872803]', '[0.33966800570487976, 2.4683001041412354]', '[0.3398759961128235, 0.37248900532722473]', '[0.3400830030441284, 3.0818800926208496]', '[0.3406200110912323, 3.02485990524292]', '[0.3408370018005371, 0.5816190242767334]', '[0.34118199348449707, 3.3834900856018066]', '[0.3427489995956421, 3.1803600788116455]', '[0.34279298782348633, 0.9857159852981567]', '[0.34312599897384644, 1.1022599935531616]', '[0.3431290090084076, 0.6961169838905334]', '[0.3438650071620941, 0.40964800119400024]', '[0.3442080020904541, 3.648020029067993]', '[0.3444420099258423, 3.1968600749969482]', '[0.34452199935913086, 2.9766900539398193]', '[0.3451719880104065, 2.8392601013183594]', '[0.3456459939479828, 0.2481600046157837]', '[0.3466399908065796, 0.061753299087285995]', '[0.34718000888824463, 2.0987300872802734]', '[0.34804099798202515, 2.0933101177215576]', '[0.3482620120048523, 2.8840699195861816]', '[0.3483960032463074, 0.20547600090503693]', '[0.34847700595855713, 2.348989963531494]', '[0.3508540093898773, 3.0053000450134277]', '[0.3511500060558319, 1.708359956741333]', '[0.35133299231529236, 1.1342899799346924]', '[0.3515770137310028, 3.4773499965667725]', '[0.352167010307312, 0.13749000430107117]', '[0.35255900025367737, 1.7224899530410767]', '[0.3526889979839325, 0.9103279709815979]', '[0.35408300161361694, 0.4372830092906952]', '[0.3542259931564331, 2.0424399375915527]', '[0.3546299934387207, 0.5156099</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr"/>
+      <c r="C532" t="inlineStr"/>
+      <c r="D532" t="inlineStr"/>
+      <c r="E532" t="inlineStr"/>
+      <c r="F532" t="inlineStr"/>
+      <c r="G532" t="inlineStr"/>
+      <c r="H532" t="inlineStr"/>
+      <c r="I532" t="inlineStr"/>
+      <c r="J532" t="inlineStr"/>
+      <c r="K532" t="inlineStr"/>
+      <c r="L532" t="inlineStr"/>
+      <c r="M532" t="inlineStr"/>
+      <c r="N532" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr"/>
+      <c r="C533" t="inlineStr"/>
+      <c r="D533" t="inlineStr"/>
+      <c r="E533" t="inlineStr"/>
+      <c r="F533" t="inlineStr"/>
+      <c r="G533" t="inlineStr"/>
+      <c r="H533" t="inlineStr"/>
+      <c r="I533" t="inlineStr"/>
+      <c r="J533" t="inlineStr"/>
+      <c r="K533" t="inlineStr"/>
+      <c r="L533" t="inlineStr"/>
+      <c r="M533" t="inlineStr"/>
+      <c r="N533" t="inlineStr">
+        <is>
+          <t>[1 1 1 ... 1 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr"/>
+      <c r="C534" t="inlineStr"/>
+      <c r="D534" t="inlineStr"/>
+      <c r="E534" t="inlineStr"/>
+      <c r="F534" t="inlineStr"/>
+      <c r="G534" t="inlineStr"/>
+      <c r="H534" t="inlineStr"/>
+      <c r="I534" t="inlineStr"/>
+      <c r="J534" t="inlineStr"/>
+      <c r="K534" t="inlineStr"/>
+      <c r="L534" t="inlineStr"/>
+      <c r="M534" t="inlineStr"/>
+      <c r="N534" t="inlineStr">
+        <is>
+          <t>[10125]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
some results and stuff
</commit_message>
<xml_diff>
--- a/configs/test_datasets.xlsx
+++ b/configs/test_datasets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N828"/>
+  <dimension ref="A1:N1010"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18796,6 +18796,4236 @@
         </is>
       </c>
     </row>
+    <row r="829">
+      <c r="A829" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr"/>
+      <c r="C829" t="inlineStr"/>
+      <c r="D829" t="inlineStr"/>
+      <c r="E829" t="inlineStr"/>
+      <c r="F829" t="inlineStr"/>
+      <c r="G829" t="inlineStr"/>
+      <c r="H829" t="inlineStr"/>
+      <c r="I829" t="inlineStr"/>
+      <c r="J829" t="inlineStr"/>
+      <c r="K829" t="inlineStr"/>
+      <c r="L829" t="inlineStr"/>
+      <c r="M829" t="inlineStr"/>
+      <c r="N829" t="inlineStr">
+        <is>
+          <t>IMDB-MULTI</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr"/>
+      <c r="C830" t="inlineStr"/>
+      <c r="D830" t="inlineStr"/>
+      <c r="E830" t="inlineStr"/>
+      <c r="F830" t="inlineStr"/>
+      <c r="G830" t="inlineStr"/>
+      <c r="H830" t="inlineStr"/>
+      <c r="I830" t="inlineStr"/>
+      <c r="J830" t="inlineStr"/>
+      <c r="K830" t="inlineStr"/>
+      <c r="L830" t="inlineStr"/>
+      <c r="M830" t="inlineStr"/>
+      <c r="N830" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr"/>
+      <c r="C831" t="inlineStr"/>
+      <c r="D831" t="inlineStr"/>
+      <c r="E831" t="inlineStr"/>
+      <c r="F831" t="inlineStr"/>
+      <c r="G831" t="inlineStr"/>
+      <c r="H831" t="inlineStr"/>
+      <c r="I831" t="inlineStr"/>
+      <c r="J831" t="inlineStr"/>
+      <c r="K831" t="inlineStr"/>
+      <c r="L831" t="inlineStr"/>
+      <c r="M831" t="inlineStr"/>
+      <c r="N831" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr"/>
+      <c r="C832" t="inlineStr"/>
+      <c r="D832" t="inlineStr"/>
+      <c r="E832" t="inlineStr"/>
+      <c r="F832" t="inlineStr"/>
+      <c r="G832" t="inlineStr"/>
+      <c r="H832" t="inlineStr"/>
+      <c r="I832" t="inlineStr"/>
+      <c r="J832" t="inlineStr"/>
+      <c r="K832" t="inlineStr"/>
+      <c r="L832" t="inlineStr"/>
+      <c r="M832" t="inlineStr"/>
+      <c r="N832" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr"/>
+      <c r="C833" t="inlineStr"/>
+      <c r="D833" t="inlineStr"/>
+      <c r="E833" t="inlineStr"/>
+      <c r="F833" t="inlineStr"/>
+      <c r="G833" t="inlineStr"/>
+      <c r="H833" t="inlineStr"/>
+      <c r="I833" t="inlineStr"/>
+      <c r="J833" t="inlineStr"/>
+      <c r="K833" t="inlineStr"/>
+      <c r="L833" t="inlineStr"/>
+      <c r="M833" t="inlineStr"/>
+      <c r="N833" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr"/>
+      <c r="C834" t="inlineStr"/>
+      <c r="D834" t="inlineStr"/>
+      <c r="E834" t="inlineStr"/>
+      <c r="F834" t="inlineStr"/>
+      <c r="G834" t="inlineStr"/>
+      <c r="H834" t="inlineStr"/>
+      <c r="I834" t="inlineStr"/>
+      <c r="J834" t="inlineStr"/>
+      <c r="K834" t="inlineStr"/>
+      <c r="L834" t="inlineStr"/>
+      <c r="M834" t="inlineStr"/>
+      <c r="N834" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr"/>
+      <c r="C835" t="inlineStr"/>
+      <c r="D835" t="inlineStr"/>
+      <c r="E835" t="inlineStr"/>
+      <c r="F835" t="inlineStr"/>
+      <c r="G835" t="inlineStr"/>
+      <c r="H835" t="inlineStr"/>
+      <c r="I835" t="inlineStr"/>
+      <c r="J835" t="inlineStr"/>
+      <c r="K835" t="inlineStr"/>
+      <c r="L835" t="inlineStr"/>
+      <c r="M835" t="inlineStr"/>
+      <c r="N835" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr"/>
+      <c r="C836" t="inlineStr"/>
+      <c r="D836" t="inlineStr"/>
+      <c r="E836" t="inlineStr"/>
+      <c r="F836" t="inlineStr"/>
+      <c r="G836" t="inlineStr"/>
+      <c r="H836" t="inlineStr"/>
+      <c r="I836" t="inlineStr"/>
+      <c r="J836" t="inlineStr"/>
+      <c r="K836" t="inlineStr"/>
+      <c r="L836" t="inlineStr"/>
+      <c r="M836" t="inlineStr"/>
+      <c r="N836" t="n">
+        <v>13.00133333333333</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr"/>
+      <c r="C837" t="inlineStr"/>
+      <c r="D837" t="inlineStr"/>
+      <c r="E837" t="inlineStr"/>
+      <c r="F837" t="inlineStr"/>
+      <c r="G837" t="inlineStr"/>
+      <c r="H837" t="inlineStr"/>
+      <c r="I837" t="inlineStr"/>
+      <c r="J837" t="inlineStr"/>
+      <c r="K837" t="inlineStr"/>
+      <c r="L837" t="inlineStr"/>
+      <c r="M837" t="inlineStr"/>
+      <c r="N837" t="n">
+        <v>65.93533333333333</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr"/>
+      <c r="C838" t="inlineStr"/>
+      <c r="D838" t="inlineStr"/>
+      <c r="E838" t="inlineStr"/>
+      <c r="F838" t="inlineStr"/>
+      <c r="G838" t="inlineStr"/>
+      <c r="H838" t="inlineStr"/>
+      <c r="I838" t="inlineStr"/>
+      <c r="J838" t="inlineStr"/>
+      <c r="K838" t="inlineStr"/>
+      <c r="L838" t="inlineStr"/>
+      <c r="M838" t="inlineStr"/>
+      <c r="N838" t="inlineStr">
+        <is>
+          <t>{1: 0.3333333333333333, 2: 0.3333333333333333, 3: 0.3333333333333333}</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr"/>
+      <c r="C839" t="inlineStr"/>
+      <c r="D839" t="inlineStr"/>
+      <c r="E839" t="inlineStr"/>
+      <c r="F839" t="inlineStr"/>
+      <c r="G839" t="inlineStr"/>
+      <c r="H839" t="inlineStr"/>
+      <c r="I839" t="inlineStr"/>
+      <c r="J839" t="inlineStr"/>
+      <c r="K839" t="inlineStr"/>
+      <c r="L839" t="inlineStr"/>
+      <c r="M839" t="inlineStr"/>
+      <c r="N839" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr"/>
+      <c r="C840" t="inlineStr"/>
+      <c r="D840" t="inlineStr"/>
+      <c r="E840" t="inlineStr"/>
+      <c r="F840" t="inlineStr"/>
+      <c r="G840" t="inlineStr"/>
+      <c r="H840" t="inlineStr"/>
+      <c r="I840" t="inlineStr"/>
+      <c r="J840" t="inlineStr"/>
+      <c r="K840" t="inlineStr"/>
+      <c r="L840" t="inlineStr"/>
+      <c r="M840" t="inlineStr"/>
+      <c r="N840" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr"/>
+      <c r="C841" t="inlineStr"/>
+      <c r="D841" t="inlineStr"/>
+      <c r="E841" t="inlineStr"/>
+      <c r="F841" t="inlineStr"/>
+      <c r="G841" t="inlineStr"/>
+      <c r="H841" t="inlineStr"/>
+      <c r="I841" t="inlineStr"/>
+      <c r="J841" t="inlineStr"/>
+      <c r="K841" t="inlineStr"/>
+      <c r="L841" t="inlineStr"/>
+      <c r="M841" t="inlineStr"/>
+      <c r="N841" t="inlineStr">
+        <is>
+          <t>[19502]</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr"/>
+      <c r="C842" t="inlineStr"/>
+      <c r="D842" t="inlineStr"/>
+      <c r="E842" t="inlineStr"/>
+      <c r="F842" t="inlineStr"/>
+      <c r="G842" t="inlineStr"/>
+      <c r="H842" t="inlineStr"/>
+      <c r="I842" t="inlineStr"/>
+      <c r="J842" t="inlineStr"/>
+      <c r="K842" t="inlineStr"/>
+      <c r="L842" t="inlineStr"/>
+      <c r="M842" t="inlineStr"/>
+      <c r="N842" t="inlineStr">
+        <is>
+          <t>[98903]</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr"/>
+      <c r="C843" t="inlineStr"/>
+      <c r="D843" t="inlineStr"/>
+      <c r="E843" t="inlineStr"/>
+      <c r="F843" t="inlineStr"/>
+      <c r="G843" t="inlineStr"/>
+      <c r="H843" t="inlineStr"/>
+      <c r="I843" t="inlineStr"/>
+      <c r="J843" t="inlineStr"/>
+      <c r="K843" t="inlineStr"/>
+      <c r="L843" t="inlineStr"/>
+      <c r="M843" t="inlineStr"/>
+      <c r="N843" t="inlineStr">
+        <is>
+          <t>IMDB-MULTI</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr"/>
+      <c r="C844" t="inlineStr"/>
+      <c r="D844" t="inlineStr"/>
+      <c r="E844" t="inlineStr"/>
+      <c r="F844" t="inlineStr"/>
+      <c r="G844" t="inlineStr"/>
+      <c r="H844" t="inlineStr"/>
+      <c r="I844" t="inlineStr"/>
+      <c r="J844" t="inlineStr"/>
+      <c r="K844" t="inlineStr"/>
+      <c r="L844" t="inlineStr"/>
+      <c r="M844" t="inlineStr"/>
+      <c r="N844" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr"/>
+      <c r="C845" t="inlineStr"/>
+      <c r="D845" t="inlineStr"/>
+      <c r="E845" t="inlineStr"/>
+      <c r="F845" t="inlineStr"/>
+      <c r="G845" t="inlineStr"/>
+      <c r="H845" t="inlineStr"/>
+      <c r="I845" t="inlineStr"/>
+      <c r="J845" t="inlineStr"/>
+      <c r="K845" t="inlineStr"/>
+      <c r="L845" t="inlineStr"/>
+      <c r="M845" t="inlineStr"/>
+      <c r="N845" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr"/>
+      <c r="C846" t="inlineStr"/>
+      <c r="D846" t="inlineStr"/>
+      <c r="E846" t="inlineStr"/>
+      <c r="F846" t="inlineStr"/>
+      <c r="G846" t="inlineStr"/>
+      <c r="H846" t="inlineStr"/>
+      <c r="I846" t="inlineStr"/>
+      <c r="J846" t="inlineStr"/>
+      <c r="K846" t="inlineStr"/>
+      <c r="L846" t="inlineStr"/>
+      <c r="M846" t="inlineStr"/>
+      <c r="N846" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr"/>
+      <c r="C847" t="inlineStr"/>
+      <c r="D847" t="inlineStr"/>
+      <c r="E847" t="inlineStr"/>
+      <c r="F847" t="inlineStr"/>
+      <c r="G847" t="inlineStr"/>
+      <c r="H847" t="inlineStr"/>
+      <c r="I847" t="inlineStr"/>
+      <c r="J847" t="inlineStr"/>
+      <c r="K847" t="inlineStr"/>
+      <c r="L847" t="inlineStr"/>
+      <c r="M847" t="inlineStr"/>
+      <c r="N847" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr"/>
+      <c r="C848" t="inlineStr"/>
+      <c r="D848" t="inlineStr"/>
+      <c r="E848" t="inlineStr"/>
+      <c r="F848" t="inlineStr"/>
+      <c r="G848" t="inlineStr"/>
+      <c r="H848" t="inlineStr"/>
+      <c r="I848" t="inlineStr"/>
+      <c r="J848" t="inlineStr"/>
+      <c r="K848" t="inlineStr"/>
+      <c r="L848" t="inlineStr"/>
+      <c r="M848" t="inlineStr"/>
+      <c r="N848" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr"/>
+      <c r="C849" t="inlineStr"/>
+      <c r="D849" t="inlineStr"/>
+      <c r="E849" t="inlineStr"/>
+      <c r="F849" t="inlineStr"/>
+      <c r="G849" t="inlineStr"/>
+      <c r="H849" t="inlineStr"/>
+      <c r="I849" t="inlineStr"/>
+      <c r="J849" t="inlineStr"/>
+      <c r="K849" t="inlineStr"/>
+      <c r="L849" t="inlineStr"/>
+      <c r="M849" t="inlineStr"/>
+      <c r="N849" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr"/>
+      <c r="C850" t="inlineStr"/>
+      <c r="D850" t="inlineStr"/>
+      <c r="E850" t="inlineStr"/>
+      <c r="F850" t="inlineStr"/>
+      <c r="G850" t="inlineStr"/>
+      <c r="H850" t="inlineStr"/>
+      <c r="I850" t="inlineStr"/>
+      <c r="J850" t="inlineStr"/>
+      <c r="K850" t="inlineStr"/>
+      <c r="L850" t="inlineStr"/>
+      <c r="M850" t="inlineStr"/>
+      <c r="N850" t="n">
+        <v>13.00133333333333</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr"/>
+      <c r="C851" t="inlineStr"/>
+      <c r="D851" t="inlineStr"/>
+      <c r="E851" t="inlineStr"/>
+      <c r="F851" t="inlineStr"/>
+      <c r="G851" t="inlineStr"/>
+      <c r="H851" t="inlineStr"/>
+      <c r="I851" t="inlineStr"/>
+      <c r="J851" t="inlineStr"/>
+      <c r="K851" t="inlineStr"/>
+      <c r="L851" t="inlineStr"/>
+      <c r="M851" t="inlineStr"/>
+      <c r="N851" t="n">
+        <v>65.93533333333333</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr"/>
+      <c r="C852" t="inlineStr"/>
+      <c r="D852" t="inlineStr"/>
+      <c r="E852" t="inlineStr"/>
+      <c r="F852" t="inlineStr"/>
+      <c r="G852" t="inlineStr"/>
+      <c r="H852" t="inlineStr"/>
+      <c r="I852" t="inlineStr"/>
+      <c r="J852" t="inlineStr"/>
+      <c r="K852" t="inlineStr"/>
+      <c r="L852" t="inlineStr"/>
+      <c r="M852" t="inlineStr"/>
+      <c r="N852" t="inlineStr">
+        <is>
+          <t>{1: 0.3333333333333333, 2: 0.3333333333333333, 3: 0.3333333333333333}</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr"/>
+      <c r="C853" t="inlineStr"/>
+      <c r="D853" t="inlineStr"/>
+      <c r="E853" t="inlineStr"/>
+      <c r="F853" t="inlineStr"/>
+      <c r="G853" t="inlineStr"/>
+      <c r="H853" t="inlineStr"/>
+      <c r="I853" t="inlineStr"/>
+      <c r="J853" t="inlineStr"/>
+      <c r="K853" t="inlineStr"/>
+      <c r="L853" t="inlineStr"/>
+      <c r="M853" t="inlineStr"/>
+      <c r="N853" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr"/>
+      <c r="C854" t="inlineStr"/>
+      <c r="D854" t="inlineStr"/>
+      <c r="E854" t="inlineStr"/>
+      <c r="F854" t="inlineStr"/>
+      <c r="G854" t="inlineStr"/>
+      <c r="H854" t="inlineStr"/>
+      <c r="I854" t="inlineStr"/>
+      <c r="J854" t="inlineStr"/>
+      <c r="K854" t="inlineStr"/>
+      <c r="L854" t="inlineStr"/>
+      <c r="M854" t="inlineStr"/>
+      <c r="N854" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr"/>
+      <c r="C855" t="inlineStr"/>
+      <c r="D855" t="inlineStr"/>
+      <c r="E855" t="inlineStr"/>
+      <c r="F855" t="inlineStr"/>
+      <c r="G855" t="inlineStr"/>
+      <c r="H855" t="inlineStr"/>
+      <c r="I855" t="inlineStr"/>
+      <c r="J855" t="inlineStr"/>
+      <c r="K855" t="inlineStr"/>
+      <c r="L855" t="inlineStr"/>
+      <c r="M855" t="inlineStr"/>
+      <c r="N855" t="inlineStr">
+        <is>
+          <t>[19502]</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr"/>
+      <c r="C856" t="inlineStr"/>
+      <c r="D856" t="inlineStr"/>
+      <c r="E856" t="inlineStr"/>
+      <c r="F856" t="inlineStr"/>
+      <c r="G856" t="inlineStr"/>
+      <c r="H856" t="inlineStr"/>
+      <c r="I856" t="inlineStr"/>
+      <c r="J856" t="inlineStr"/>
+      <c r="K856" t="inlineStr"/>
+      <c r="L856" t="inlineStr"/>
+      <c r="M856" t="inlineStr"/>
+      <c r="N856" t="inlineStr">
+        <is>
+          <t>[98903]</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr"/>
+      <c r="C857" t="inlineStr"/>
+      <c r="D857" t="inlineStr"/>
+      <c r="E857" t="inlineStr"/>
+      <c r="F857" t="inlineStr"/>
+      <c r="G857" t="inlineStr"/>
+      <c r="H857" t="inlineStr"/>
+      <c r="I857" t="inlineStr"/>
+      <c r="J857" t="inlineStr"/>
+      <c r="K857" t="inlineStr"/>
+      <c r="L857" t="inlineStr"/>
+      <c r="M857" t="inlineStr"/>
+      <c r="N857" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr"/>
+      <c r="C858" t="inlineStr"/>
+      <c r="D858" t="inlineStr"/>
+      <c r="E858" t="inlineStr"/>
+      <c r="F858" t="inlineStr"/>
+      <c r="G858" t="inlineStr"/>
+      <c r="H858" t="inlineStr"/>
+      <c r="I858" t="inlineStr"/>
+      <c r="J858" t="inlineStr"/>
+      <c r="K858" t="inlineStr"/>
+      <c r="L858" t="inlineStr"/>
+      <c r="M858" t="inlineStr"/>
+      <c r="N858" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr"/>
+      <c r="C859" t="inlineStr"/>
+      <c r="D859" t="inlineStr"/>
+      <c r="E859" t="inlineStr"/>
+      <c r="F859" t="inlineStr"/>
+      <c r="G859" t="inlineStr"/>
+      <c r="H859" t="inlineStr"/>
+      <c r="I859" t="inlineStr"/>
+      <c r="J859" t="inlineStr"/>
+      <c r="K859" t="inlineStr"/>
+      <c r="L859" t="inlineStr"/>
+      <c r="M859" t="inlineStr"/>
+      <c r="N859" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr"/>
+      <c r="C860" t="inlineStr"/>
+      <c r="D860" t="inlineStr"/>
+      <c r="E860" t="inlineStr"/>
+      <c r="F860" t="inlineStr"/>
+      <c r="G860" t="inlineStr"/>
+      <c r="H860" t="inlineStr"/>
+      <c r="I860" t="inlineStr"/>
+      <c r="J860" t="inlineStr"/>
+      <c r="K860" t="inlineStr"/>
+      <c r="L860" t="inlineStr"/>
+      <c r="M860" t="inlineStr"/>
+      <c r="N860" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr"/>
+      <c r="C861" t="inlineStr"/>
+      <c r="D861" t="inlineStr"/>
+      <c r="E861" t="inlineStr"/>
+      <c r="F861" t="inlineStr"/>
+      <c r="G861" t="inlineStr"/>
+      <c r="H861" t="inlineStr"/>
+      <c r="I861" t="inlineStr"/>
+      <c r="J861" t="inlineStr"/>
+      <c r="K861" t="inlineStr"/>
+      <c r="L861" t="inlineStr"/>
+      <c r="M861" t="inlineStr"/>
+      <c r="N861" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr"/>
+      <c r="C862" t="inlineStr"/>
+      <c r="D862" t="inlineStr"/>
+      <c r="E862" t="inlineStr"/>
+      <c r="F862" t="inlineStr"/>
+      <c r="G862" t="inlineStr"/>
+      <c r="H862" t="inlineStr"/>
+      <c r="I862" t="inlineStr"/>
+      <c r="J862" t="inlineStr"/>
+      <c r="K862" t="inlineStr"/>
+      <c r="L862" t="inlineStr"/>
+      <c r="M862" t="inlineStr"/>
+      <c r="N862" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr"/>
+      <c r="C863" t="inlineStr"/>
+      <c r="D863" t="inlineStr"/>
+      <c r="E863" t="inlineStr"/>
+      <c r="F863" t="inlineStr"/>
+      <c r="G863" t="inlineStr"/>
+      <c r="H863" t="inlineStr"/>
+      <c r="I863" t="inlineStr"/>
+      <c r="J863" t="inlineStr"/>
+      <c r="K863" t="inlineStr"/>
+      <c r="L863" t="inlineStr"/>
+      <c r="M863" t="inlineStr"/>
+      <c r="N863" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr"/>
+      <c r="C864" t="inlineStr"/>
+      <c r="D864" t="inlineStr"/>
+      <c r="E864" t="inlineStr"/>
+      <c r="F864" t="inlineStr"/>
+      <c r="G864" t="inlineStr"/>
+      <c r="H864" t="inlineStr"/>
+      <c r="I864" t="inlineStr"/>
+      <c r="J864" t="inlineStr"/>
+      <c r="K864" t="inlineStr"/>
+      <c r="L864" t="inlineStr"/>
+      <c r="M864" t="inlineStr"/>
+      <c r="N864" t="n">
+        <v>32.63333333333333</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr"/>
+      <c r="C865" t="inlineStr"/>
+      <c r="D865" t="inlineStr"/>
+      <c r="E865" t="inlineStr"/>
+      <c r="F865" t="inlineStr"/>
+      <c r="G865" t="inlineStr"/>
+      <c r="H865" t="inlineStr"/>
+      <c r="I865" t="inlineStr"/>
+      <c r="J865" t="inlineStr"/>
+      <c r="K865" t="inlineStr"/>
+      <c r="L865" t="inlineStr"/>
+      <c r="M865" t="inlineStr"/>
+      <c r="N865" t="n">
+        <v>62.13666666666666</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr"/>
+      <c r="C866" t="inlineStr"/>
+      <c r="D866" t="inlineStr"/>
+      <c r="E866" t="inlineStr"/>
+      <c r="F866" t="inlineStr"/>
+      <c r="G866" t="inlineStr"/>
+      <c r="H866" t="inlineStr"/>
+      <c r="I866" t="inlineStr"/>
+      <c r="J866" t="inlineStr"/>
+      <c r="K866" t="inlineStr"/>
+      <c r="L866" t="inlineStr"/>
+      <c r="M866" t="inlineStr"/>
+      <c r="N866" t="inlineStr">
+        <is>
+          <t>{1: 0.16666666666666666, 2: 0.16666666666666666, 3: 0.16666666666666666, 4: 0.16666666666666666, 5: 0.16666666666666666, 6: 0.16666666666666666}</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr"/>
+      <c r="C867" t="inlineStr"/>
+      <c r="D867" t="inlineStr"/>
+      <c r="E867" t="inlineStr"/>
+      <c r="F867" t="inlineStr"/>
+      <c r="G867" t="inlineStr"/>
+      <c r="H867" t="inlineStr"/>
+      <c r="I867" t="inlineStr"/>
+      <c r="J867" t="inlineStr"/>
+      <c r="K867" t="inlineStr"/>
+      <c r="L867" t="inlineStr"/>
+      <c r="M867" t="inlineStr"/>
+      <c r="N867" t="inlineStr">
+        <is>
+          <t>['1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr"/>
+      <c r="C868" t="inlineStr"/>
+      <c r="D868" t="inlineStr"/>
+      <c r="E868" t="inlineStr"/>
+      <c r="F868" t="inlineStr"/>
+      <c r="G868" t="inlineStr"/>
+      <c r="H868" t="inlineStr"/>
+      <c r="I868" t="inlineStr"/>
+      <c r="J868" t="inlineStr"/>
+      <c r="K868" t="inlineStr"/>
+      <c r="L868" t="inlineStr"/>
+      <c r="M868" t="inlineStr"/>
+      <c r="N868" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr"/>
+      <c r="C869" t="inlineStr"/>
+      <c r="D869" t="inlineStr"/>
+      <c r="E869" t="inlineStr"/>
+      <c r="F869" t="inlineStr"/>
+      <c r="G869" t="inlineStr"/>
+      <c r="H869" t="inlineStr"/>
+      <c r="I869" t="inlineStr"/>
+      <c r="J869" t="inlineStr"/>
+      <c r="K869" t="inlineStr"/>
+      <c r="L869" t="inlineStr"/>
+      <c r="M869" t="inlineStr"/>
+      <c r="N869" t="inlineStr">
+        <is>
+          <t>[9457 9665  458]</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr"/>
+      <c r="C870" t="inlineStr"/>
+      <c r="D870" t="inlineStr"/>
+      <c r="E870" t="inlineStr"/>
+      <c r="F870" t="inlineStr"/>
+      <c r="G870" t="inlineStr"/>
+      <c r="H870" t="inlineStr"/>
+      <c r="I870" t="inlineStr"/>
+      <c r="J870" t="inlineStr"/>
+      <c r="K870" t="inlineStr"/>
+      <c r="L870" t="inlineStr"/>
+      <c r="M870" t="inlineStr"/>
+      <c r="N870" t="inlineStr">
+        <is>
+          <t>[37282]</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr"/>
+      <c r="C871" t="inlineStr"/>
+      <c r="D871" t="inlineStr"/>
+      <c r="E871" t="inlineStr"/>
+      <c r="F871" t="inlineStr"/>
+      <c r="G871" t="inlineStr"/>
+      <c r="H871" t="inlineStr"/>
+      <c r="I871" t="inlineStr"/>
+      <c r="J871" t="inlineStr"/>
+      <c r="K871" t="inlineStr"/>
+      <c r="L871" t="inlineStr"/>
+      <c r="M871" t="inlineStr"/>
+      <c r="N871" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr"/>
+      <c r="C872" t="inlineStr"/>
+      <c r="D872" t="inlineStr"/>
+      <c r="E872" t="inlineStr"/>
+      <c r="F872" t="inlineStr"/>
+      <c r="G872" t="inlineStr"/>
+      <c r="H872" t="inlineStr"/>
+      <c r="I872" t="inlineStr"/>
+      <c r="J872" t="inlineStr"/>
+      <c r="K872" t="inlineStr"/>
+      <c r="L872" t="inlineStr"/>
+      <c r="M872" t="inlineStr"/>
+      <c r="N872" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr"/>
+      <c r="C873" t="inlineStr"/>
+      <c r="D873" t="inlineStr"/>
+      <c r="E873" t="inlineStr"/>
+      <c r="F873" t="inlineStr"/>
+      <c r="G873" t="inlineStr"/>
+      <c r="H873" t="inlineStr"/>
+      <c r="I873" t="inlineStr"/>
+      <c r="J873" t="inlineStr"/>
+      <c r="K873" t="inlineStr"/>
+      <c r="L873" t="inlineStr"/>
+      <c r="M873" t="inlineStr"/>
+      <c r="N873" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr"/>
+      <c r="C874" t="inlineStr"/>
+      <c r="D874" t="inlineStr"/>
+      <c r="E874" t="inlineStr"/>
+      <c r="F874" t="inlineStr"/>
+      <c r="G874" t="inlineStr"/>
+      <c r="H874" t="inlineStr"/>
+      <c r="I874" t="inlineStr"/>
+      <c r="J874" t="inlineStr"/>
+      <c r="K874" t="inlineStr"/>
+      <c r="L874" t="inlineStr"/>
+      <c r="M874" t="inlineStr"/>
+      <c r="N874" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr"/>
+      <c r="C875" t="inlineStr"/>
+      <c r="D875" t="inlineStr"/>
+      <c r="E875" t="inlineStr"/>
+      <c r="F875" t="inlineStr"/>
+      <c r="G875" t="inlineStr"/>
+      <c r="H875" t="inlineStr"/>
+      <c r="I875" t="inlineStr"/>
+      <c r="J875" t="inlineStr"/>
+      <c r="K875" t="inlineStr"/>
+      <c r="L875" t="inlineStr"/>
+      <c r="M875" t="inlineStr"/>
+      <c r="N875" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr"/>
+      <c r="C876" t="inlineStr"/>
+      <c r="D876" t="inlineStr"/>
+      <c r="E876" t="inlineStr"/>
+      <c r="F876" t="inlineStr"/>
+      <c r="G876" t="inlineStr"/>
+      <c r="H876" t="inlineStr"/>
+      <c r="I876" t="inlineStr"/>
+      <c r="J876" t="inlineStr"/>
+      <c r="K876" t="inlineStr"/>
+      <c r="L876" t="inlineStr"/>
+      <c r="M876" t="inlineStr"/>
+      <c r="N876" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr"/>
+      <c r="C877" t="inlineStr"/>
+      <c r="D877" t="inlineStr"/>
+      <c r="E877" t="inlineStr"/>
+      <c r="F877" t="inlineStr"/>
+      <c r="G877" t="inlineStr"/>
+      <c r="H877" t="inlineStr"/>
+      <c r="I877" t="inlineStr"/>
+      <c r="J877" t="inlineStr"/>
+      <c r="K877" t="inlineStr"/>
+      <c r="L877" t="inlineStr"/>
+      <c r="M877" t="inlineStr"/>
+      <c r="N877" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr"/>
+      <c r="C878" t="inlineStr"/>
+      <c r="D878" t="inlineStr"/>
+      <c r="E878" t="inlineStr"/>
+      <c r="F878" t="inlineStr"/>
+      <c r="G878" t="inlineStr"/>
+      <c r="H878" t="inlineStr"/>
+      <c r="I878" t="inlineStr"/>
+      <c r="J878" t="inlineStr"/>
+      <c r="K878" t="inlineStr"/>
+      <c r="L878" t="inlineStr"/>
+      <c r="M878" t="inlineStr"/>
+      <c r="N878" t="n">
+        <v>32.63333333333333</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr"/>
+      <c r="C879" t="inlineStr"/>
+      <c r="D879" t="inlineStr"/>
+      <c r="E879" t="inlineStr"/>
+      <c r="F879" t="inlineStr"/>
+      <c r="G879" t="inlineStr"/>
+      <c r="H879" t="inlineStr"/>
+      <c r="I879" t="inlineStr"/>
+      <c r="J879" t="inlineStr"/>
+      <c r="K879" t="inlineStr"/>
+      <c r="L879" t="inlineStr"/>
+      <c r="M879" t="inlineStr"/>
+      <c r="N879" t="n">
+        <v>62.13666666666666</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr"/>
+      <c r="C880" t="inlineStr"/>
+      <c r="D880" t="inlineStr"/>
+      <c r="E880" t="inlineStr"/>
+      <c r="F880" t="inlineStr"/>
+      <c r="G880" t="inlineStr"/>
+      <c r="H880" t="inlineStr"/>
+      <c r="I880" t="inlineStr"/>
+      <c r="J880" t="inlineStr"/>
+      <c r="K880" t="inlineStr"/>
+      <c r="L880" t="inlineStr"/>
+      <c r="M880" t="inlineStr"/>
+      <c r="N880" t="inlineStr">
+        <is>
+          <t>{1: 0.16666666666666666, 2: 0.16666666666666666, 3: 0.16666666666666666, 4: 0.16666666666666666, 5: 0.16666666666666666, 6: 0.16666666666666666}</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr"/>
+      <c r="C881" t="inlineStr"/>
+      <c r="D881" t="inlineStr"/>
+      <c r="E881" t="inlineStr"/>
+      <c r="F881" t="inlineStr"/>
+      <c r="G881" t="inlineStr"/>
+      <c r="H881" t="inlineStr"/>
+      <c r="I881" t="inlineStr"/>
+      <c r="J881" t="inlineStr"/>
+      <c r="K881" t="inlineStr"/>
+      <c r="L881" t="inlineStr"/>
+      <c r="M881" t="inlineStr"/>
+      <c r="N881" t="inlineStr">
+        <is>
+          <t>['1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr"/>
+      <c r="C882" t="inlineStr"/>
+      <c r="D882" t="inlineStr"/>
+      <c r="E882" t="inlineStr"/>
+      <c r="F882" t="inlineStr"/>
+      <c r="G882" t="inlineStr"/>
+      <c r="H882" t="inlineStr"/>
+      <c r="I882" t="inlineStr"/>
+      <c r="J882" t="inlineStr"/>
+      <c r="K882" t="inlineStr"/>
+      <c r="L882" t="inlineStr"/>
+      <c r="M882" t="inlineStr"/>
+      <c r="N882" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr"/>
+      <c r="C883" t="inlineStr"/>
+      <c r="D883" t="inlineStr"/>
+      <c r="E883" t="inlineStr"/>
+      <c r="F883" t="inlineStr"/>
+      <c r="G883" t="inlineStr"/>
+      <c r="H883" t="inlineStr"/>
+      <c r="I883" t="inlineStr"/>
+      <c r="J883" t="inlineStr"/>
+      <c r="K883" t="inlineStr"/>
+      <c r="L883" t="inlineStr"/>
+      <c r="M883" t="inlineStr"/>
+      <c r="N883" t="inlineStr">
+        <is>
+          <t>[9457 9665  458]</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr"/>
+      <c r="C884" t="inlineStr"/>
+      <c r="D884" t="inlineStr"/>
+      <c r="E884" t="inlineStr"/>
+      <c r="F884" t="inlineStr"/>
+      <c r="G884" t="inlineStr"/>
+      <c r="H884" t="inlineStr"/>
+      <c r="I884" t="inlineStr"/>
+      <c r="J884" t="inlineStr"/>
+      <c r="K884" t="inlineStr"/>
+      <c r="L884" t="inlineStr"/>
+      <c r="M884" t="inlineStr"/>
+      <c r="N884" t="inlineStr">
+        <is>
+          <t>[37282]</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr"/>
+      <c r="C885" t="inlineStr"/>
+      <c r="D885" t="inlineStr"/>
+      <c r="E885" t="inlineStr"/>
+      <c r="F885" t="inlineStr"/>
+      <c r="G885" t="inlineStr"/>
+      <c r="H885" t="inlineStr"/>
+      <c r="I885" t="inlineStr"/>
+      <c r="J885" t="inlineStr"/>
+      <c r="K885" t="inlineStr"/>
+      <c r="L885" t="inlineStr"/>
+      <c r="M885" t="inlineStr"/>
+      <c r="N885" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr"/>
+      <c r="C886" t="inlineStr"/>
+      <c r="D886" t="inlineStr"/>
+      <c r="E886" t="inlineStr"/>
+      <c r="F886" t="inlineStr"/>
+      <c r="G886" t="inlineStr"/>
+      <c r="H886" t="inlineStr"/>
+      <c r="I886" t="inlineStr"/>
+      <c r="J886" t="inlineStr"/>
+      <c r="K886" t="inlineStr"/>
+      <c r="L886" t="inlineStr"/>
+      <c r="M886" t="inlineStr"/>
+      <c r="N886" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr"/>
+      <c r="C887" t="inlineStr"/>
+      <c r="D887" t="inlineStr"/>
+      <c r="E887" t="inlineStr"/>
+      <c r="F887" t="inlineStr"/>
+      <c r="G887" t="inlineStr"/>
+      <c r="H887" t="inlineStr"/>
+      <c r="I887" t="inlineStr"/>
+      <c r="J887" t="inlineStr"/>
+      <c r="K887" t="inlineStr"/>
+      <c r="L887" t="inlineStr"/>
+      <c r="M887" t="inlineStr"/>
+      <c r="N887" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr"/>
+      <c r="C888" t="inlineStr"/>
+      <c r="D888" t="inlineStr"/>
+      <c r="E888" t="inlineStr"/>
+      <c r="F888" t="inlineStr"/>
+      <c r="G888" t="inlineStr"/>
+      <c r="H888" t="inlineStr"/>
+      <c r="I888" t="inlineStr"/>
+      <c r="J888" t="inlineStr"/>
+      <c r="K888" t="inlineStr"/>
+      <c r="L888" t="inlineStr"/>
+      <c r="M888" t="inlineStr"/>
+      <c r="N888" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr"/>
+      <c r="C889" t="inlineStr"/>
+      <c r="D889" t="inlineStr"/>
+      <c r="E889" t="inlineStr"/>
+      <c r="F889" t="inlineStr"/>
+      <c r="G889" t="inlineStr"/>
+      <c r="H889" t="inlineStr"/>
+      <c r="I889" t="inlineStr"/>
+      <c r="J889" t="inlineStr"/>
+      <c r="K889" t="inlineStr"/>
+      <c r="L889" t="inlineStr"/>
+      <c r="M889" t="inlineStr"/>
+      <c r="N889" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr"/>
+      <c r="C890" t="inlineStr"/>
+      <c r="D890" t="inlineStr"/>
+      <c r="E890" t="inlineStr"/>
+      <c r="F890" t="inlineStr"/>
+      <c r="G890" t="inlineStr"/>
+      <c r="H890" t="inlineStr"/>
+      <c r="I890" t="inlineStr"/>
+      <c r="J890" t="inlineStr"/>
+      <c r="K890" t="inlineStr"/>
+      <c r="L890" t="inlineStr"/>
+      <c r="M890" t="inlineStr"/>
+      <c r="N890" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr"/>
+      <c r="C891" t="inlineStr"/>
+      <c r="D891" t="inlineStr"/>
+      <c r="E891" t="inlineStr"/>
+      <c r="F891" t="inlineStr"/>
+      <c r="G891" t="inlineStr"/>
+      <c r="H891" t="inlineStr"/>
+      <c r="I891" t="inlineStr"/>
+      <c r="J891" t="inlineStr"/>
+      <c r="K891" t="inlineStr"/>
+      <c r="L891" t="inlineStr"/>
+      <c r="M891" t="inlineStr"/>
+      <c r="N891" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr"/>
+      <c r="C892" t="inlineStr"/>
+      <c r="D892" t="inlineStr"/>
+      <c r="E892" t="inlineStr"/>
+      <c r="F892" t="inlineStr"/>
+      <c r="G892" t="inlineStr"/>
+      <c r="H892" t="inlineStr"/>
+      <c r="I892" t="inlineStr"/>
+      <c r="J892" t="inlineStr"/>
+      <c r="K892" t="inlineStr"/>
+      <c r="L892" t="inlineStr"/>
+      <c r="M892" t="inlineStr"/>
+      <c r="N892" t="n">
+        <v>32.63333333333333</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr"/>
+      <c r="C893" t="inlineStr"/>
+      <c r="D893" t="inlineStr"/>
+      <c r="E893" t="inlineStr"/>
+      <c r="F893" t="inlineStr"/>
+      <c r="G893" t="inlineStr"/>
+      <c r="H893" t="inlineStr"/>
+      <c r="I893" t="inlineStr"/>
+      <c r="J893" t="inlineStr"/>
+      <c r="K893" t="inlineStr"/>
+      <c r="L893" t="inlineStr"/>
+      <c r="M893" t="inlineStr"/>
+      <c r="N893" t="n">
+        <v>62.13666666666666</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr"/>
+      <c r="C894" t="inlineStr"/>
+      <c r="D894" t="inlineStr"/>
+      <c r="E894" t="inlineStr"/>
+      <c r="F894" t="inlineStr"/>
+      <c r="G894" t="inlineStr"/>
+      <c r="H894" t="inlineStr"/>
+      <c r="I894" t="inlineStr"/>
+      <c r="J894" t="inlineStr"/>
+      <c r="K894" t="inlineStr"/>
+      <c r="L894" t="inlineStr"/>
+      <c r="M894" t="inlineStr"/>
+      <c r="N894" t="inlineStr">
+        <is>
+          <t>{1: 0.16666666666666666, 2: 0.16666666666666666, 3: 0.16666666666666666, 4: 0.16666666666666666, 5: 0.16666666666666666, 6: 0.16666666666666666}</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr"/>
+      <c r="C895" t="inlineStr"/>
+      <c r="D895" t="inlineStr"/>
+      <c r="E895" t="inlineStr"/>
+      <c r="F895" t="inlineStr"/>
+      <c r="G895" t="inlineStr"/>
+      <c r="H895" t="inlineStr"/>
+      <c r="I895" t="inlineStr"/>
+      <c r="J895" t="inlineStr"/>
+      <c r="K895" t="inlineStr"/>
+      <c r="L895" t="inlineStr"/>
+      <c r="M895" t="inlineStr"/>
+      <c r="N895" t="inlineStr">
+        <is>
+          <t>['1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr"/>
+      <c r="C896" t="inlineStr"/>
+      <c r="D896" t="inlineStr"/>
+      <c r="E896" t="inlineStr"/>
+      <c r="F896" t="inlineStr"/>
+      <c r="G896" t="inlineStr"/>
+      <c r="H896" t="inlineStr"/>
+      <c r="I896" t="inlineStr"/>
+      <c r="J896" t="inlineStr"/>
+      <c r="K896" t="inlineStr"/>
+      <c r="L896" t="inlineStr"/>
+      <c r="M896" t="inlineStr"/>
+      <c r="N896" t="inlineStr">
+        <is>
+          <t>['None']</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr"/>
+      <c r="C897" t="inlineStr"/>
+      <c r="D897" t="inlineStr"/>
+      <c r="E897" t="inlineStr"/>
+      <c r="F897" t="inlineStr"/>
+      <c r="G897" t="inlineStr"/>
+      <c r="H897" t="inlineStr"/>
+      <c r="I897" t="inlineStr"/>
+      <c r="J897" t="inlineStr"/>
+      <c r="K897" t="inlineStr"/>
+      <c r="L897" t="inlineStr"/>
+      <c r="M897" t="inlineStr"/>
+      <c r="N897" t="inlineStr">
+        <is>
+          <t>[9457 9665  458]</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr"/>
+      <c r="C898" t="inlineStr"/>
+      <c r="D898" t="inlineStr"/>
+      <c r="E898" t="inlineStr"/>
+      <c r="F898" t="inlineStr"/>
+      <c r="G898" t="inlineStr"/>
+      <c r="H898" t="inlineStr"/>
+      <c r="I898" t="inlineStr"/>
+      <c r="J898" t="inlineStr"/>
+      <c r="K898" t="inlineStr"/>
+      <c r="L898" t="inlineStr"/>
+      <c r="M898" t="inlineStr"/>
+      <c r="N898" t="inlineStr">
+        <is>
+          <t>[37282]</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr"/>
+      <c r="C899" t="inlineStr"/>
+      <c r="D899" t="inlineStr"/>
+      <c r="E899" t="inlineStr"/>
+      <c r="F899" t="inlineStr"/>
+      <c r="G899" t="inlineStr"/>
+      <c r="H899" t="inlineStr"/>
+      <c r="I899" t="inlineStr"/>
+      <c r="J899" t="inlineStr"/>
+      <c r="K899" t="inlineStr"/>
+      <c r="L899" t="inlineStr"/>
+      <c r="M899" t="inlineStr"/>
+      <c r="N899" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr"/>
+      <c r="C900" t="inlineStr"/>
+      <c r="D900" t="inlineStr"/>
+      <c r="E900" t="inlineStr"/>
+      <c r="F900" t="inlineStr"/>
+      <c r="G900" t="inlineStr"/>
+      <c r="H900" t="inlineStr"/>
+      <c r="I900" t="inlineStr"/>
+      <c r="J900" t="inlineStr"/>
+      <c r="K900" t="inlineStr"/>
+      <c r="L900" t="inlineStr"/>
+      <c r="M900" t="inlineStr"/>
+      <c r="N900" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr"/>
+      <c r="C901" t="inlineStr"/>
+      <c r="D901" t="inlineStr"/>
+      <c r="E901" t="inlineStr"/>
+      <c r="F901" t="inlineStr"/>
+      <c r="G901" t="inlineStr"/>
+      <c r="H901" t="inlineStr"/>
+      <c r="I901" t="inlineStr"/>
+      <c r="J901" t="inlineStr"/>
+      <c r="K901" t="inlineStr"/>
+      <c r="L901" t="inlineStr"/>
+      <c r="M901" t="inlineStr"/>
+      <c r="N901" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr"/>
+      <c r="C902" t="inlineStr"/>
+      <c r="D902" t="inlineStr"/>
+      <c r="E902" t="inlineStr"/>
+      <c r="F902" t="inlineStr"/>
+      <c r="G902" t="inlineStr"/>
+      <c r="H902" t="inlineStr"/>
+      <c r="I902" t="inlineStr"/>
+      <c r="J902" t="inlineStr"/>
+      <c r="K902" t="inlineStr"/>
+      <c r="L902" t="inlineStr"/>
+      <c r="M902" t="inlineStr"/>
+      <c r="N902" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr"/>
+      <c r="C903" t="inlineStr"/>
+      <c r="D903" t="inlineStr"/>
+      <c r="E903" t="inlineStr"/>
+      <c r="F903" t="inlineStr"/>
+      <c r="G903" t="inlineStr"/>
+      <c r="H903" t="inlineStr"/>
+      <c r="I903" t="inlineStr"/>
+      <c r="J903" t="inlineStr"/>
+      <c r="K903" t="inlineStr"/>
+      <c r="L903" t="inlineStr"/>
+      <c r="M903" t="inlineStr"/>
+      <c r="N903" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr"/>
+      <c r="C904" t="inlineStr"/>
+      <c r="D904" t="inlineStr"/>
+      <c r="E904" t="inlineStr"/>
+      <c r="F904" t="inlineStr"/>
+      <c r="G904" t="inlineStr"/>
+      <c r="H904" t="inlineStr"/>
+      <c r="I904" t="inlineStr"/>
+      <c r="J904" t="inlineStr"/>
+      <c r="K904" t="inlineStr"/>
+      <c r="L904" t="inlineStr"/>
+      <c r="M904" t="inlineStr"/>
+      <c r="N904" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr"/>
+      <c r="C905" t="inlineStr"/>
+      <c r="D905" t="inlineStr"/>
+      <c r="E905" t="inlineStr"/>
+      <c r="F905" t="inlineStr"/>
+      <c r="G905" t="inlineStr"/>
+      <c r="H905" t="inlineStr"/>
+      <c r="I905" t="inlineStr"/>
+      <c r="J905" t="inlineStr"/>
+      <c r="K905" t="inlineStr"/>
+      <c r="L905" t="inlineStr"/>
+      <c r="M905" t="inlineStr"/>
+      <c r="N905" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr"/>
+      <c r="C906" t="inlineStr"/>
+      <c r="D906" t="inlineStr"/>
+      <c r="E906" t="inlineStr"/>
+      <c r="F906" t="inlineStr"/>
+      <c r="G906" t="inlineStr"/>
+      <c r="H906" t="inlineStr"/>
+      <c r="I906" t="inlineStr"/>
+      <c r="J906" t="inlineStr"/>
+      <c r="K906" t="inlineStr"/>
+      <c r="L906" t="inlineStr"/>
+      <c r="M906" t="inlineStr"/>
+      <c r="N906" t="n">
+        <v>14.55840455840456</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr"/>
+      <c r="C907" t="inlineStr"/>
+      <c r="D907" t="inlineStr"/>
+      <c r="E907" t="inlineStr"/>
+      <c r="F907" t="inlineStr"/>
+      <c r="G907" t="inlineStr"/>
+      <c r="H907" t="inlineStr"/>
+      <c r="I907" t="inlineStr"/>
+      <c r="J907" t="inlineStr"/>
+      <c r="K907" t="inlineStr"/>
+      <c r="L907" t="inlineStr"/>
+      <c r="M907" t="inlineStr"/>
+      <c r="N907" t="n">
+        <v>15.002849002849</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr"/>
+      <c r="C908" t="inlineStr"/>
+      <c r="D908" t="inlineStr"/>
+      <c r="E908" t="inlineStr"/>
+      <c r="F908" t="inlineStr"/>
+      <c r="G908" t="inlineStr"/>
+      <c r="H908" t="inlineStr"/>
+      <c r="I908" t="inlineStr"/>
+      <c r="J908" t="inlineStr"/>
+      <c r="K908" t="inlineStr"/>
+      <c r="L908" t="inlineStr"/>
+      <c r="M908" t="inlineStr"/>
+      <c r="N908" t="inlineStr">
+        <is>
+          <t>{1: 0.34472934472934474, -1: 0.6552706552706553}</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr"/>
+      <c r="C909" t="inlineStr"/>
+      <c r="D909" t="inlineStr"/>
+      <c r="E909" t="inlineStr"/>
+      <c r="F909" t="inlineStr"/>
+      <c r="G909" t="inlineStr"/>
+      <c r="H909" t="inlineStr"/>
+      <c r="I909" t="inlineStr"/>
+      <c r="J909" t="inlineStr"/>
+      <c r="K909" t="inlineStr"/>
+      <c r="L909" t="inlineStr"/>
+      <c r="M909" t="inlineStr"/>
+      <c r="N909" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '2', '3', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr"/>
+      <c r="C910" t="inlineStr"/>
+      <c r="D910" t="inlineStr"/>
+      <c r="E910" t="inlineStr"/>
+      <c r="F910" t="inlineStr"/>
+      <c r="G910" t="inlineStr"/>
+      <c r="H910" t="inlineStr"/>
+      <c r="I910" t="inlineStr"/>
+      <c r="J910" t="inlineStr"/>
+      <c r="K910" t="inlineStr"/>
+      <c r="L910" t="inlineStr"/>
+      <c r="M910" t="inlineStr"/>
+      <c r="N910" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr"/>
+      <c r="C911" t="inlineStr"/>
+      <c r="D911" t="inlineStr"/>
+      <c r="E911" t="inlineStr"/>
+      <c r="F911" t="inlineStr"/>
+      <c r="G911" t="inlineStr"/>
+      <c r="H911" t="inlineStr"/>
+      <c r="I911" t="inlineStr"/>
+      <c r="J911" t="inlineStr"/>
+      <c r="K911" t="inlineStr"/>
+      <c r="L911" t="inlineStr"/>
+      <c r="M911" t="inlineStr"/>
+      <c r="N911" t="inlineStr">
+        <is>
+          <t>[   1   23    1    1    2    1    3    1    1    1    1  721  408   29
+ 3493  269  100   44   10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr"/>
+      <c r="C912" t="inlineStr"/>
+      <c r="D912" t="inlineStr"/>
+      <c r="E912" t="inlineStr"/>
+      <c r="F912" t="inlineStr"/>
+      <c r="G912" t="inlineStr"/>
+      <c r="H912" t="inlineStr"/>
+      <c r="I912" t="inlineStr"/>
+      <c r="J912" t="inlineStr"/>
+      <c r="K912" t="inlineStr"/>
+      <c r="L912" t="inlineStr"/>
+      <c r="M912" t="inlineStr"/>
+      <c r="N912" t="inlineStr">
+        <is>
+          <t>[   7  436 2772 2051]</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr"/>
+      <c r="C913" t="inlineStr"/>
+      <c r="D913" t="inlineStr"/>
+      <c r="E913" t="inlineStr"/>
+      <c r="F913" t="inlineStr"/>
+      <c r="G913" t="inlineStr"/>
+      <c r="H913" t="inlineStr"/>
+      <c r="I913" t="inlineStr"/>
+      <c r="J913" t="inlineStr"/>
+      <c r="K913" t="inlineStr"/>
+      <c r="L913" t="inlineStr"/>
+      <c r="M913" t="inlineStr"/>
+      <c r="N913" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr"/>
+      <c r="C914" t="inlineStr"/>
+      <c r="D914" t="inlineStr"/>
+      <c r="E914" t="inlineStr"/>
+      <c r="F914" t="inlineStr"/>
+      <c r="G914" t="inlineStr"/>
+      <c r="H914" t="inlineStr"/>
+      <c r="I914" t="inlineStr"/>
+      <c r="J914" t="inlineStr"/>
+      <c r="K914" t="inlineStr"/>
+      <c r="L914" t="inlineStr"/>
+      <c r="M914" t="inlineStr"/>
+      <c r="N914" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr"/>
+      <c r="C915" t="inlineStr"/>
+      <c r="D915" t="inlineStr"/>
+      <c r="E915" t="inlineStr"/>
+      <c r="F915" t="inlineStr"/>
+      <c r="G915" t="inlineStr"/>
+      <c r="H915" t="inlineStr"/>
+      <c r="I915" t="inlineStr"/>
+      <c r="J915" t="inlineStr"/>
+      <c r="K915" t="inlineStr"/>
+      <c r="L915" t="inlineStr"/>
+      <c r="M915" t="inlineStr"/>
+      <c r="N915" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr"/>
+      <c r="C916" t="inlineStr"/>
+      <c r="D916" t="inlineStr"/>
+      <c r="E916" t="inlineStr"/>
+      <c r="F916" t="inlineStr"/>
+      <c r="G916" t="inlineStr"/>
+      <c r="H916" t="inlineStr"/>
+      <c r="I916" t="inlineStr"/>
+      <c r="J916" t="inlineStr"/>
+      <c r="K916" t="inlineStr"/>
+      <c r="L916" t="inlineStr"/>
+      <c r="M916" t="inlineStr"/>
+      <c r="N916" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr"/>
+      <c r="C917" t="inlineStr"/>
+      <c r="D917" t="inlineStr"/>
+      <c r="E917" t="inlineStr"/>
+      <c r="F917" t="inlineStr"/>
+      <c r="G917" t="inlineStr"/>
+      <c r="H917" t="inlineStr"/>
+      <c r="I917" t="inlineStr"/>
+      <c r="J917" t="inlineStr"/>
+      <c r="K917" t="inlineStr"/>
+      <c r="L917" t="inlineStr"/>
+      <c r="M917" t="inlineStr"/>
+      <c r="N917" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr"/>
+      <c r="C918" t="inlineStr"/>
+      <c r="D918" t="inlineStr"/>
+      <c r="E918" t="inlineStr"/>
+      <c r="F918" t="inlineStr"/>
+      <c r="G918" t="inlineStr"/>
+      <c r="H918" t="inlineStr"/>
+      <c r="I918" t="inlineStr"/>
+      <c r="J918" t="inlineStr"/>
+      <c r="K918" t="inlineStr"/>
+      <c r="L918" t="inlineStr"/>
+      <c r="M918" t="inlineStr"/>
+      <c r="N918" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr"/>
+      <c r="C919" t="inlineStr"/>
+      <c r="D919" t="inlineStr"/>
+      <c r="E919" t="inlineStr"/>
+      <c r="F919" t="inlineStr"/>
+      <c r="G919" t="inlineStr"/>
+      <c r="H919" t="inlineStr"/>
+      <c r="I919" t="inlineStr"/>
+      <c r="J919" t="inlineStr"/>
+      <c r="K919" t="inlineStr"/>
+      <c r="L919" t="inlineStr"/>
+      <c r="M919" t="inlineStr"/>
+      <c r="N919" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr"/>
+      <c r="C920" t="inlineStr"/>
+      <c r="D920" t="inlineStr"/>
+      <c r="E920" t="inlineStr"/>
+      <c r="F920" t="inlineStr"/>
+      <c r="G920" t="inlineStr"/>
+      <c r="H920" t="inlineStr"/>
+      <c r="I920" t="inlineStr"/>
+      <c r="J920" t="inlineStr"/>
+      <c r="K920" t="inlineStr"/>
+      <c r="L920" t="inlineStr"/>
+      <c r="M920" t="inlineStr"/>
+      <c r="N920" t="n">
+        <v>14.55840455840456</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr"/>
+      <c r="C921" t="inlineStr"/>
+      <c r="D921" t="inlineStr"/>
+      <c r="E921" t="inlineStr"/>
+      <c r="F921" t="inlineStr"/>
+      <c r="G921" t="inlineStr"/>
+      <c r="H921" t="inlineStr"/>
+      <c r="I921" t="inlineStr"/>
+      <c r="J921" t="inlineStr"/>
+      <c r="K921" t="inlineStr"/>
+      <c r="L921" t="inlineStr"/>
+      <c r="M921" t="inlineStr"/>
+      <c r="N921" t="n">
+        <v>15.002849002849</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr"/>
+      <c r="C922" t="inlineStr"/>
+      <c r="D922" t="inlineStr"/>
+      <c r="E922" t="inlineStr"/>
+      <c r="F922" t="inlineStr"/>
+      <c r="G922" t="inlineStr"/>
+      <c r="H922" t="inlineStr"/>
+      <c r="I922" t="inlineStr"/>
+      <c r="J922" t="inlineStr"/>
+      <c r="K922" t="inlineStr"/>
+      <c r="L922" t="inlineStr"/>
+      <c r="M922" t="inlineStr"/>
+      <c r="N922" t="inlineStr">
+        <is>
+          <t>{1: 0.34472934472934474, -1: 0.6552706552706553}</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr"/>
+      <c r="C923" t="inlineStr"/>
+      <c r="D923" t="inlineStr"/>
+      <c r="E923" t="inlineStr"/>
+      <c r="F923" t="inlineStr"/>
+      <c r="G923" t="inlineStr"/>
+      <c r="H923" t="inlineStr"/>
+      <c r="I923" t="inlineStr"/>
+      <c r="J923" t="inlineStr"/>
+      <c r="K923" t="inlineStr"/>
+      <c r="L923" t="inlineStr"/>
+      <c r="M923" t="inlineStr"/>
+      <c r="N923" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '2', '3', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr"/>
+      <c r="C924" t="inlineStr"/>
+      <c r="D924" t="inlineStr"/>
+      <c r="E924" t="inlineStr"/>
+      <c r="F924" t="inlineStr"/>
+      <c r="G924" t="inlineStr"/>
+      <c r="H924" t="inlineStr"/>
+      <c r="I924" t="inlineStr"/>
+      <c r="J924" t="inlineStr"/>
+      <c r="K924" t="inlineStr"/>
+      <c r="L924" t="inlineStr"/>
+      <c r="M924" t="inlineStr"/>
+      <c r="N924" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr"/>
+      <c r="C925" t="inlineStr"/>
+      <c r="D925" t="inlineStr"/>
+      <c r="E925" t="inlineStr"/>
+      <c r="F925" t="inlineStr"/>
+      <c r="G925" t="inlineStr"/>
+      <c r="H925" t="inlineStr"/>
+      <c r="I925" t="inlineStr"/>
+      <c r="J925" t="inlineStr"/>
+      <c r="K925" t="inlineStr"/>
+      <c r="L925" t="inlineStr"/>
+      <c r="M925" t="inlineStr"/>
+      <c r="N925" t="inlineStr">
+        <is>
+          <t>[   1   23    1    1    2    1    3    1    1    1    1  721  408   29
+ 3493  269  100   44   10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr"/>
+      <c r="C926" t="inlineStr"/>
+      <c r="D926" t="inlineStr"/>
+      <c r="E926" t="inlineStr"/>
+      <c r="F926" t="inlineStr"/>
+      <c r="G926" t="inlineStr"/>
+      <c r="H926" t="inlineStr"/>
+      <c r="I926" t="inlineStr"/>
+      <c r="J926" t="inlineStr"/>
+      <c r="K926" t="inlineStr"/>
+      <c r="L926" t="inlineStr"/>
+      <c r="M926" t="inlineStr"/>
+      <c r="N926" t="inlineStr">
+        <is>
+          <t>[   7  436 2772 2051]</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr"/>
+      <c r="C927" t="inlineStr"/>
+      <c r="D927" t="inlineStr"/>
+      <c r="E927" t="inlineStr"/>
+      <c r="F927" t="inlineStr"/>
+      <c r="G927" t="inlineStr"/>
+      <c r="H927" t="inlineStr"/>
+      <c r="I927" t="inlineStr"/>
+      <c r="J927" t="inlineStr"/>
+      <c r="K927" t="inlineStr"/>
+      <c r="L927" t="inlineStr"/>
+      <c r="M927" t="inlineStr"/>
+      <c r="N927" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr"/>
+      <c r="C928" t="inlineStr"/>
+      <c r="D928" t="inlineStr"/>
+      <c r="E928" t="inlineStr"/>
+      <c r="F928" t="inlineStr"/>
+      <c r="G928" t="inlineStr"/>
+      <c r="H928" t="inlineStr"/>
+      <c r="I928" t="inlineStr"/>
+      <c r="J928" t="inlineStr"/>
+      <c r="K928" t="inlineStr"/>
+      <c r="L928" t="inlineStr"/>
+      <c r="M928" t="inlineStr"/>
+      <c r="N928" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr"/>
+      <c r="C929" t="inlineStr"/>
+      <c r="D929" t="inlineStr"/>
+      <c r="E929" t="inlineStr"/>
+      <c r="F929" t="inlineStr"/>
+      <c r="G929" t="inlineStr"/>
+      <c r="H929" t="inlineStr"/>
+      <c r="I929" t="inlineStr"/>
+      <c r="J929" t="inlineStr"/>
+      <c r="K929" t="inlineStr"/>
+      <c r="L929" t="inlineStr"/>
+      <c r="M929" t="inlineStr"/>
+      <c r="N929" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr"/>
+      <c r="C930" t="inlineStr"/>
+      <c r="D930" t="inlineStr"/>
+      <c r="E930" t="inlineStr"/>
+      <c r="F930" t="inlineStr"/>
+      <c r="G930" t="inlineStr"/>
+      <c r="H930" t="inlineStr"/>
+      <c r="I930" t="inlineStr"/>
+      <c r="J930" t="inlineStr"/>
+      <c r="K930" t="inlineStr"/>
+      <c r="L930" t="inlineStr"/>
+      <c r="M930" t="inlineStr"/>
+      <c r="N930" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr"/>
+      <c r="C931" t="inlineStr"/>
+      <c r="D931" t="inlineStr"/>
+      <c r="E931" t="inlineStr"/>
+      <c r="F931" t="inlineStr"/>
+      <c r="G931" t="inlineStr"/>
+      <c r="H931" t="inlineStr"/>
+      <c r="I931" t="inlineStr"/>
+      <c r="J931" t="inlineStr"/>
+      <c r="K931" t="inlineStr"/>
+      <c r="L931" t="inlineStr"/>
+      <c r="M931" t="inlineStr"/>
+      <c r="N931" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr"/>
+      <c r="C932" t="inlineStr"/>
+      <c r="D932" t="inlineStr"/>
+      <c r="E932" t="inlineStr"/>
+      <c r="F932" t="inlineStr"/>
+      <c r="G932" t="inlineStr"/>
+      <c r="H932" t="inlineStr"/>
+      <c r="I932" t="inlineStr"/>
+      <c r="J932" t="inlineStr"/>
+      <c r="K932" t="inlineStr"/>
+      <c r="L932" t="inlineStr"/>
+      <c r="M932" t="inlineStr"/>
+      <c r="N932" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr"/>
+      <c r="C933" t="inlineStr"/>
+      <c r="D933" t="inlineStr"/>
+      <c r="E933" t="inlineStr"/>
+      <c r="F933" t="inlineStr"/>
+      <c r="G933" t="inlineStr"/>
+      <c r="H933" t="inlineStr"/>
+      <c r="I933" t="inlineStr"/>
+      <c r="J933" t="inlineStr"/>
+      <c r="K933" t="inlineStr"/>
+      <c r="L933" t="inlineStr"/>
+      <c r="M933" t="inlineStr"/>
+      <c r="N933" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr"/>
+      <c r="C934" t="inlineStr"/>
+      <c r="D934" t="inlineStr"/>
+      <c r="E934" t="inlineStr"/>
+      <c r="F934" t="inlineStr"/>
+      <c r="G934" t="inlineStr"/>
+      <c r="H934" t="inlineStr"/>
+      <c r="I934" t="inlineStr"/>
+      <c r="J934" t="inlineStr"/>
+      <c r="K934" t="inlineStr"/>
+      <c r="L934" t="inlineStr"/>
+      <c r="M934" t="inlineStr"/>
+      <c r="N934" t="n">
+        <v>14.55840455840456</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr"/>
+      <c r="C935" t="inlineStr"/>
+      <c r="D935" t="inlineStr"/>
+      <c r="E935" t="inlineStr"/>
+      <c r="F935" t="inlineStr"/>
+      <c r="G935" t="inlineStr"/>
+      <c r="H935" t="inlineStr"/>
+      <c r="I935" t="inlineStr"/>
+      <c r="J935" t="inlineStr"/>
+      <c r="K935" t="inlineStr"/>
+      <c r="L935" t="inlineStr"/>
+      <c r="M935" t="inlineStr"/>
+      <c r="N935" t="n">
+        <v>15.002849002849</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr"/>
+      <c r="C936" t="inlineStr"/>
+      <c r="D936" t="inlineStr"/>
+      <c r="E936" t="inlineStr"/>
+      <c r="F936" t="inlineStr"/>
+      <c r="G936" t="inlineStr"/>
+      <c r="H936" t="inlineStr"/>
+      <c r="I936" t="inlineStr"/>
+      <c r="J936" t="inlineStr"/>
+      <c r="K936" t="inlineStr"/>
+      <c r="L936" t="inlineStr"/>
+      <c r="M936" t="inlineStr"/>
+      <c r="N936" t="inlineStr">
+        <is>
+          <t>{1: 0.34472934472934474, -1: 0.6552706552706553}</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr"/>
+      <c r="C937" t="inlineStr"/>
+      <c r="D937" t="inlineStr"/>
+      <c r="E937" t="inlineStr"/>
+      <c r="F937" t="inlineStr"/>
+      <c r="G937" t="inlineStr"/>
+      <c r="H937" t="inlineStr"/>
+      <c r="I937" t="inlineStr"/>
+      <c r="J937" t="inlineStr"/>
+      <c r="K937" t="inlineStr"/>
+      <c r="L937" t="inlineStr"/>
+      <c r="M937" t="inlineStr"/>
+      <c r="N937" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '2', '3', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr"/>
+      <c r="C938" t="inlineStr"/>
+      <c r="D938" t="inlineStr"/>
+      <c r="E938" t="inlineStr"/>
+      <c r="F938" t="inlineStr"/>
+      <c r="G938" t="inlineStr"/>
+      <c r="H938" t="inlineStr"/>
+      <c r="I938" t="inlineStr"/>
+      <c r="J938" t="inlineStr"/>
+      <c r="K938" t="inlineStr"/>
+      <c r="L938" t="inlineStr"/>
+      <c r="M938" t="inlineStr"/>
+      <c r="N938" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr"/>
+      <c r="C939" t="inlineStr"/>
+      <c r="D939" t="inlineStr"/>
+      <c r="E939" t="inlineStr"/>
+      <c r="F939" t="inlineStr"/>
+      <c r="G939" t="inlineStr"/>
+      <c r="H939" t="inlineStr"/>
+      <c r="I939" t="inlineStr"/>
+      <c r="J939" t="inlineStr"/>
+      <c r="K939" t="inlineStr"/>
+      <c r="L939" t="inlineStr"/>
+      <c r="M939" t="inlineStr"/>
+      <c r="N939" t="inlineStr">
+        <is>
+          <t>[   1   23    1    1    2    1    3    1    1    1    1  721  408   29
+ 3493  269  100   44   10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr"/>
+      <c r="C940" t="inlineStr"/>
+      <c r="D940" t="inlineStr"/>
+      <c r="E940" t="inlineStr"/>
+      <c r="F940" t="inlineStr"/>
+      <c r="G940" t="inlineStr"/>
+      <c r="H940" t="inlineStr"/>
+      <c r="I940" t="inlineStr"/>
+      <c r="J940" t="inlineStr"/>
+      <c r="K940" t="inlineStr"/>
+      <c r="L940" t="inlineStr"/>
+      <c r="M940" t="inlineStr"/>
+      <c r="N940" t="inlineStr">
+        <is>
+          <t>[   7  436 2772 2051]</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr"/>
+      <c r="C941" t="inlineStr"/>
+      <c r="D941" t="inlineStr"/>
+      <c r="E941" t="inlineStr"/>
+      <c r="F941" t="inlineStr"/>
+      <c r="G941" t="inlineStr"/>
+      <c r="H941" t="inlineStr"/>
+      <c r="I941" t="inlineStr"/>
+      <c r="J941" t="inlineStr"/>
+      <c r="K941" t="inlineStr"/>
+      <c r="L941" t="inlineStr"/>
+      <c r="M941" t="inlineStr"/>
+      <c r="N941" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr"/>
+      <c r="C942" t="inlineStr"/>
+      <c r="D942" t="inlineStr"/>
+      <c r="E942" t="inlineStr"/>
+      <c r="F942" t="inlineStr"/>
+      <c r="G942" t="inlineStr"/>
+      <c r="H942" t="inlineStr"/>
+      <c r="I942" t="inlineStr"/>
+      <c r="J942" t="inlineStr"/>
+      <c r="K942" t="inlineStr"/>
+      <c r="L942" t="inlineStr"/>
+      <c r="M942" t="inlineStr"/>
+      <c r="N942" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr"/>
+      <c r="C943" t="inlineStr"/>
+      <c r="D943" t="inlineStr"/>
+      <c r="E943" t="inlineStr"/>
+      <c r="F943" t="inlineStr"/>
+      <c r="G943" t="inlineStr"/>
+      <c r="H943" t="inlineStr"/>
+      <c r="I943" t="inlineStr"/>
+      <c r="J943" t="inlineStr"/>
+      <c r="K943" t="inlineStr"/>
+      <c r="L943" t="inlineStr"/>
+      <c r="M943" t="inlineStr"/>
+      <c r="N943" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr"/>
+      <c r="C944" t="inlineStr"/>
+      <c r="D944" t="inlineStr"/>
+      <c r="E944" t="inlineStr"/>
+      <c r="F944" t="inlineStr"/>
+      <c r="G944" t="inlineStr"/>
+      <c r="H944" t="inlineStr"/>
+      <c r="I944" t="inlineStr"/>
+      <c r="J944" t="inlineStr"/>
+      <c r="K944" t="inlineStr"/>
+      <c r="L944" t="inlineStr"/>
+      <c r="M944" t="inlineStr"/>
+      <c r="N944" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr"/>
+      <c r="C945" t="inlineStr"/>
+      <c r="D945" t="inlineStr"/>
+      <c r="E945" t="inlineStr"/>
+      <c r="F945" t="inlineStr"/>
+      <c r="G945" t="inlineStr"/>
+      <c r="H945" t="inlineStr"/>
+      <c r="I945" t="inlineStr"/>
+      <c r="J945" t="inlineStr"/>
+      <c r="K945" t="inlineStr"/>
+      <c r="L945" t="inlineStr"/>
+      <c r="M945" t="inlineStr"/>
+      <c r="N945" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr"/>
+      <c r="C946" t="inlineStr"/>
+      <c r="D946" t="inlineStr"/>
+      <c r="E946" t="inlineStr"/>
+      <c r="F946" t="inlineStr"/>
+      <c r="G946" t="inlineStr"/>
+      <c r="H946" t="inlineStr"/>
+      <c r="I946" t="inlineStr"/>
+      <c r="J946" t="inlineStr"/>
+      <c r="K946" t="inlineStr"/>
+      <c r="L946" t="inlineStr"/>
+      <c r="M946" t="inlineStr"/>
+      <c r="N946" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr"/>
+      <c r="C947" t="inlineStr"/>
+      <c r="D947" t="inlineStr"/>
+      <c r="E947" t="inlineStr"/>
+      <c r="F947" t="inlineStr"/>
+      <c r="G947" t="inlineStr"/>
+      <c r="H947" t="inlineStr"/>
+      <c r="I947" t="inlineStr"/>
+      <c r="J947" t="inlineStr"/>
+      <c r="K947" t="inlineStr"/>
+      <c r="L947" t="inlineStr"/>
+      <c r="M947" t="inlineStr"/>
+      <c r="N947" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr"/>
+      <c r="C948" t="inlineStr"/>
+      <c r="D948" t="inlineStr"/>
+      <c r="E948" t="inlineStr"/>
+      <c r="F948" t="inlineStr"/>
+      <c r="G948" t="inlineStr"/>
+      <c r="H948" t="inlineStr"/>
+      <c r="I948" t="inlineStr"/>
+      <c r="J948" t="inlineStr"/>
+      <c r="K948" t="inlineStr"/>
+      <c r="L948" t="inlineStr"/>
+      <c r="M948" t="inlineStr"/>
+      <c r="N948" t="n">
+        <v>15.6925</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr"/>
+      <c r="C949" t="inlineStr"/>
+      <c r="D949" t="inlineStr"/>
+      <c r="E949" t="inlineStr"/>
+      <c r="F949" t="inlineStr"/>
+      <c r="G949" t="inlineStr"/>
+      <c r="H949" t="inlineStr"/>
+      <c r="I949" t="inlineStr"/>
+      <c r="J949" t="inlineStr"/>
+      <c r="K949" t="inlineStr"/>
+      <c r="L949" t="inlineStr"/>
+      <c r="M949" t="inlineStr"/>
+      <c r="N949" t="n">
+        <v>16.195</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr"/>
+      <c r="C950" t="inlineStr"/>
+      <c r="D950" t="inlineStr"/>
+      <c r="E950" t="inlineStr"/>
+      <c r="F950" t="inlineStr"/>
+      <c r="G950" t="inlineStr"/>
+      <c r="H950" t="inlineStr"/>
+      <c r="I950" t="inlineStr"/>
+      <c r="J950" t="inlineStr"/>
+      <c r="K950" t="inlineStr"/>
+      <c r="L950" t="inlineStr"/>
+      <c r="M950" t="inlineStr"/>
+      <c r="N950" t="inlineStr">
+        <is>
+          <t>{0: 0.2, 1: 0.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr"/>
+      <c r="C951" t="inlineStr"/>
+      <c r="D951" t="inlineStr"/>
+      <c r="E951" t="inlineStr"/>
+      <c r="F951" t="inlineStr"/>
+      <c r="G951" t="inlineStr"/>
+      <c r="H951" t="inlineStr"/>
+      <c r="I951" t="inlineStr"/>
+      <c r="J951" t="inlineStr"/>
+      <c r="K951" t="inlineStr"/>
+      <c r="L951" t="inlineStr"/>
+      <c r="M951" t="inlineStr"/>
+      <c r="N951" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '19', '2', '20', '21', '22', '23', '24', '25', '26', '27', '28', '29', '3', '30', '31', '32', '33', '34', '35', '36', '37', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr"/>
+      <c r="C952" t="inlineStr"/>
+      <c r="D952" t="inlineStr"/>
+      <c r="E952" t="inlineStr"/>
+      <c r="F952" t="inlineStr"/>
+      <c r="G952" t="inlineStr"/>
+      <c r="H952" t="inlineStr"/>
+      <c r="I952" t="inlineStr"/>
+      <c r="J952" t="inlineStr"/>
+      <c r="K952" t="inlineStr"/>
+      <c r="L952" t="inlineStr"/>
+      <c r="M952" t="inlineStr"/>
+      <c r="N952" t="inlineStr">
+        <is>
+          <t>['0', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr"/>
+      <c r="C953" t="inlineStr"/>
+      <c r="D953" t="inlineStr"/>
+      <c r="E953" t="inlineStr"/>
+      <c r="F953" t="inlineStr"/>
+      <c r="G953" t="inlineStr"/>
+      <c r="H953" t="inlineStr"/>
+      <c r="I953" t="inlineStr"/>
+      <c r="J953" t="inlineStr"/>
+      <c r="K953" t="inlineStr"/>
+      <c r="L953" t="inlineStr"/>
+      <c r="M953" t="inlineStr"/>
+      <c r="N953" t="inlineStr">
+        <is>
+          <t>[19564  5492    19   103     4    27     1     5     7    14    13     3
+  4149     6     7     1     4     1     1     3     2     1     1   385
+     1     2     2     3     1     2     2     1    78  1253    16   109
+    60    42]</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr"/>
+      <c r="C954" t="inlineStr"/>
+      <c r="D954" t="inlineStr"/>
+      <c r="E954" t="inlineStr"/>
+      <c r="F954" t="inlineStr"/>
+      <c r="G954" t="inlineStr"/>
+      <c r="H954" t="inlineStr"/>
+      <c r="I954" t="inlineStr"/>
+      <c r="J954" t="inlineStr"/>
+      <c r="K954" t="inlineStr"/>
+      <c r="L954" t="inlineStr"/>
+      <c r="M954" t="inlineStr"/>
+      <c r="N954" t="inlineStr">
+        <is>
+          <t>[23835  8375   180]</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr"/>
+      <c r="C955" t="inlineStr"/>
+      <c r="D955" t="inlineStr"/>
+      <c r="E955" t="inlineStr"/>
+      <c r="F955" t="inlineStr"/>
+      <c r="G955" t="inlineStr"/>
+      <c r="H955" t="inlineStr"/>
+      <c r="I955" t="inlineStr"/>
+      <c r="J955" t="inlineStr"/>
+      <c r="K955" t="inlineStr"/>
+      <c r="L955" t="inlineStr"/>
+      <c r="M955" t="inlineStr"/>
+      <c r="N955" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr"/>
+      <c r="C956" t="inlineStr"/>
+      <c r="D956" t="inlineStr"/>
+      <c r="E956" t="inlineStr"/>
+      <c r="F956" t="inlineStr"/>
+      <c r="G956" t="inlineStr"/>
+      <c r="H956" t="inlineStr"/>
+      <c r="I956" t="inlineStr"/>
+      <c r="J956" t="inlineStr"/>
+      <c r="K956" t="inlineStr"/>
+      <c r="L956" t="inlineStr"/>
+      <c r="M956" t="inlineStr"/>
+      <c r="N956" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr"/>
+      <c r="C957" t="inlineStr"/>
+      <c r="D957" t="inlineStr"/>
+      <c r="E957" t="inlineStr"/>
+      <c r="F957" t="inlineStr"/>
+      <c r="G957" t="inlineStr"/>
+      <c r="H957" t="inlineStr"/>
+      <c r="I957" t="inlineStr"/>
+      <c r="J957" t="inlineStr"/>
+      <c r="K957" t="inlineStr"/>
+      <c r="L957" t="inlineStr"/>
+      <c r="M957" t="inlineStr"/>
+      <c r="N957" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr"/>
+      <c r="C958" t="inlineStr"/>
+      <c r="D958" t="inlineStr"/>
+      <c r="E958" t="inlineStr"/>
+      <c r="F958" t="inlineStr"/>
+      <c r="G958" t="inlineStr"/>
+      <c r="H958" t="inlineStr"/>
+      <c r="I958" t="inlineStr"/>
+      <c r="J958" t="inlineStr"/>
+      <c r="K958" t="inlineStr"/>
+      <c r="L958" t="inlineStr"/>
+      <c r="M958" t="inlineStr"/>
+      <c r="N958" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr"/>
+      <c r="C959" t="inlineStr"/>
+      <c r="D959" t="inlineStr"/>
+      <c r="E959" t="inlineStr"/>
+      <c r="F959" t="inlineStr"/>
+      <c r="G959" t="inlineStr"/>
+      <c r="H959" t="inlineStr"/>
+      <c r="I959" t="inlineStr"/>
+      <c r="J959" t="inlineStr"/>
+      <c r="K959" t="inlineStr"/>
+      <c r="L959" t="inlineStr"/>
+      <c r="M959" t="inlineStr"/>
+      <c r="N959" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr"/>
+      <c r="C960" t="inlineStr"/>
+      <c r="D960" t="inlineStr"/>
+      <c r="E960" t="inlineStr"/>
+      <c r="F960" t="inlineStr"/>
+      <c r="G960" t="inlineStr"/>
+      <c r="H960" t="inlineStr"/>
+      <c r="I960" t="inlineStr"/>
+      <c r="J960" t="inlineStr"/>
+      <c r="K960" t="inlineStr"/>
+      <c r="L960" t="inlineStr"/>
+      <c r="M960" t="inlineStr"/>
+      <c r="N960" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr"/>
+      <c r="C961" t="inlineStr"/>
+      <c r="D961" t="inlineStr"/>
+      <c r="E961" t="inlineStr"/>
+      <c r="F961" t="inlineStr"/>
+      <c r="G961" t="inlineStr"/>
+      <c r="H961" t="inlineStr"/>
+      <c r="I961" t="inlineStr"/>
+      <c r="J961" t="inlineStr"/>
+      <c r="K961" t="inlineStr"/>
+      <c r="L961" t="inlineStr"/>
+      <c r="M961" t="inlineStr"/>
+      <c r="N961" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr"/>
+      <c r="C962" t="inlineStr"/>
+      <c r="D962" t="inlineStr"/>
+      <c r="E962" t="inlineStr"/>
+      <c r="F962" t="inlineStr"/>
+      <c r="G962" t="inlineStr"/>
+      <c r="H962" t="inlineStr"/>
+      <c r="I962" t="inlineStr"/>
+      <c r="J962" t="inlineStr"/>
+      <c r="K962" t="inlineStr"/>
+      <c r="L962" t="inlineStr"/>
+      <c r="M962" t="inlineStr"/>
+      <c r="N962" t="n">
+        <v>15.6925</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr"/>
+      <c r="C963" t="inlineStr"/>
+      <c r="D963" t="inlineStr"/>
+      <c r="E963" t="inlineStr"/>
+      <c r="F963" t="inlineStr"/>
+      <c r="G963" t="inlineStr"/>
+      <c r="H963" t="inlineStr"/>
+      <c r="I963" t="inlineStr"/>
+      <c r="J963" t="inlineStr"/>
+      <c r="K963" t="inlineStr"/>
+      <c r="L963" t="inlineStr"/>
+      <c r="M963" t="inlineStr"/>
+      <c r="N963" t="n">
+        <v>16.195</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr"/>
+      <c r="C964" t="inlineStr"/>
+      <c r="D964" t="inlineStr"/>
+      <c r="E964" t="inlineStr"/>
+      <c r="F964" t="inlineStr"/>
+      <c r="G964" t="inlineStr"/>
+      <c r="H964" t="inlineStr"/>
+      <c r="I964" t="inlineStr"/>
+      <c r="J964" t="inlineStr"/>
+      <c r="K964" t="inlineStr"/>
+      <c r="L964" t="inlineStr"/>
+      <c r="M964" t="inlineStr"/>
+      <c r="N964" t="inlineStr">
+        <is>
+          <t>{0: 0.2, 1: 0.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr"/>
+      <c r="C965" t="inlineStr"/>
+      <c r="D965" t="inlineStr"/>
+      <c r="E965" t="inlineStr"/>
+      <c r="F965" t="inlineStr"/>
+      <c r="G965" t="inlineStr"/>
+      <c r="H965" t="inlineStr"/>
+      <c r="I965" t="inlineStr"/>
+      <c r="J965" t="inlineStr"/>
+      <c r="K965" t="inlineStr"/>
+      <c r="L965" t="inlineStr"/>
+      <c r="M965" t="inlineStr"/>
+      <c r="N965" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '19', '2', '20', '21', '22', '23', '24', '25', '26', '27', '28', '29', '3', '30', '31', '32', '33', '34', '35', '36', '37', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr"/>
+      <c r="C966" t="inlineStr"/>
+      <c r="D966" t="inlineStr"/>
+      <c r="E966" t="inlineStr"/>
+      <c r="F966" t="inlineStr"/>
+      <c r="G966" t="inlineStr"/>
+      <c r="H966" t="inlineStr"/>
+      <c r="I966" t="inlineStr"/>
+      <c r="J966" t="inlineStr"/>
+      <c r="K966" t="inlineStr"/>
+      <c r="L966" t="inlineStr"/>
+      <c r="M966" t="inlineStr"/>
+      <c r="N966" t="inlineStr">
+        <is>
+          <t>['0', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr"/>
+      <c r="C967" t="inlineStr"/>
+      <c r="D967" t="inlineStr"/>
+      <c r="E967" t="inlineStr"/>
+      <c r="F967" t="inlineStr"/>
+      <c r="G967" t="inlineStr"/>
+      <c r="H967" t="inlineStr"/>
+      <c r="I967" t="inlineStr"/>
+      <c r="J967" t="inlineStr"/>
+      <c r="K967" t="inlineStr"/>
+      <c r="L967" t="inlineStr"/>
+      <c r="M967" t="inlineStr"/>
+      <c r="N967" t="inlineStr">
+        <is>
+          <t>[19564  5492    19   103     4    27     1     5     7    14    13     3
+  4149     6     7     1     4     1     1     3     2     1     1   385
+     1     2     2     3     1     2     2     1    78  1253    16   109
+    60    42]</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr"/>
+      <c r="C968" t="inlineStr"/>
+      <c r="D968" t="inlineStr"/>
+      <c r="E968" t="inlineStr"/>
+      <c r="F968" t="inlineStr"/>
+      <c r="G968" t="inlineStr"/>
+      <c r="H968" t="inlineStr"/>
+      <c r="I968" t="inlineStr"/>
+      <c r="J968" t="inlineStr"/>
+      <c r="K968" t="inlineStr"/>
+      <c r="L968" t="inlineStr"/>
+      <c r="M968" t="inlineStr"/>
+      <c r="N968" t="inlineStr">
+        <is>
+          <t>[23835  8375   180]</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr"/>
+      <c r="C969" t="inlineStr"/>
+      <c r="D969" t="inlineStr"/>
+      <c r="E969" t="inlineStr"/>
+      <c r="F969" t="inlineStr"/>
+      <c r="G969" t="inlineStr"/>
+      <c r="H969" t="inlineStr"/>
+      <c r="I969" t="inlineStr"/>
+      <c r="J969" t="inlineStr"/>
+      <c r="K969" t="inlineStr"/>
+      <c r="L969" t="inlineStr"/>
+      <c r="M969" t="inlineStr"/>
+      <c r="N969" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr"/>
+      <c r="C970" t="inlineStr"/>
+      <c r="D970" t="inlineStr"/>
+      <c r="E970" t="inlineStr"/>
+      <c r="F970" t="inlineStr"/>
+      <c r="G970" t="inlineStr"/>
+      <c r="H970" t="inlineStr"/>
+      <c r="I970" t="inlineStr"/>
+      <c r="J970" t="inlineStr"/>
+      <c r="K970" t="inlineStr"/>
+      <c r="L970" t="inlineStr"/>
+      <c r="M970" t="inlineStr"/>
+      <c r="N970" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr"/>
+      <c r="C971" t="inlineStr"/>
+      <c r="D971" t="inlineStr"/>
+      <c r="E971" t="inlineStr"/>
+      <c r="F971" t="inlineStr"/>
+      <c r="G971" t="inlineStr"/>
+      <c r="H971" t="inlineStr"/>
+      <c r="I971" t="inlineStr"/>
+      <c r="J971" t="inlineStr"/>
+      <c r="K971" t="inlineStr"/>
+      <c r="L971" t="inlineStr"/>
+      <c r="M971" t="inlineStr"/>
+      <c r="N971" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr"/>
+      <c r="C972" t="inlineStr"/>
+      <c r="D972" t="inlineStr"/>
+      <c r="E972" t="inlineStr"/>
+      <c r="F972" t="inlineStr"/>
+      <c r="G972" t="inlineStr"/>
+      <c r="H972" t="inlineStr"/>
+      <c r="I972" t="inlineStr"/>
+      <c r="J972" t="inlineStr"/>
+      <c r="K972" t="inlineStr"/>
+      <c r="L972" t="inlineStr"/>
+      <c r="M972" t="inlineStr"/>
+      <c r="N972" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr"/>
+      <c r="C973" t="inlineStr"/>
+      <c r="D973" t="inlineStr"/>
+      <c r="E973" t="inlineStr"/>
+      <c r="F973" t="inlineStr"/>
+      <c r="G973" t="inlineStr"/>
+      <c r="H973" t="inlineStr"/>
+      <c r="I973" t="inlineStr"/>
+      <c r="J973" t="inlineStr"/>
+      <c r="K973" t="inlineStr"/>
+      <c r="L973" t="inlineStr"/>
+      <c r="M973" t="inlineStr"/>
+      <c r="N973" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr"/>
+      <c r="C974" t="inlineStr"/>
+      <c r="D974" t="inlineStr"/>
+      <c r="E974" t="inlineStr"/>
+      <c r="F974" t="inlineStr"/>
+      <c r="G974" t="inlineStr"/>
+      <c r="H974" t="inlineStr"/>
+      <c r="I974" t="inlineStr"/>
+      <c r="J974" t="inlineStr"/>
+      <c r="K974" t="inlineStr"/>
+      <c r="L974" t="inlineStr"/>
+      <c r="M974" t="inlineStr"/>
+      <c r="N974" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr"/>
+      <c r="C975" t="inlineStr"/>
+      <c r="D975" t="inlineStr"/>
+      <c r="E975" t="inlineStr"/>
+      <c r="F975" t="inlineStr"/>
+      <c r="G975" t="inlineStr"/>
+      <c r="H975" t="inlineStr"/>
+      <c r="I975" t="inlineStr"/>
+      <c r="J975" t="inlineStr"/>
+      <c r="K975" t="inlineStr"/>
+      <c r="L975" t="inlineStr"/>
+      <c r="M975" t="inlineStr"/>
+      <c r="N975" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr"/>
+      <c r="C976" t="inlineStr"/>
+      <c r="D976" t="inlineStr"/>
+      <c r="E976" t="inlineStr"/>
+      <c r="F976" t="inlineStr"/>
+      <c r="G976" t="inlineStr"/>
+      <c r="H976" t="inlineStr"/>
+      <c r="I976" t="inlineStr"/>
+      <c r="J976" t="inlineStr"/>
+      <c r="K976" t="inlineStr"/>
+      <c r="L976" t="inlineStr"/>
+      <c r="M976" t="inlineStr"/>
+      <c r="N976" t="n">
+        <v>15.6925</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr"/>
+      <c r="C977" t="inlineStr"/>
+      <c r="D977" t="inlineStr"/>
+      <c r="E977" t="inlineStr"/>
+      <c r="F977" t="inlineStr"/>
+      <c r="G977" t="inlineStr"/>
+      <c r="H977" t="inlineStr"/>
+      <c r="I977" t="inlineStr"/>
+      <c r="J977" t="inlineStr"/>
+      <c r="K977" t="inlineStr"/>
+      <c r="L977" t="inlineStr"/>
+      <c r="M977" t="inlineStr"/>
+      <c r="N977" t="n">
+        <v>16.195</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr"/>
+      <c r="C978" t="inlineStr"/>
+      <c r="D978" t="inlineStr"/>
+      <c r="E978" t="inlineStr"/>
+      <c r="F978" t="inlineStr"/>
+      <c r="G978" t="inlineStr"/>
+      <c r="H978" t="inlineStr"/>
+      <c r="I978" t="inlineStr"/>
+      <c r="J978" t="inlineStr"/>
+      <c r="K978" t="inlineStr"/>
+      <c r="L978" t="inlineStr"/>
+      <c r="M978" t="inlineStr"/>
+      <c r="N978" t="inlineStr">
+        <is>
+          <t>{0: 0.2, 1: 0.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr"/>
+      <c r="C979" t="inlineStr"/>
+      <c r="D979" t="inlineStr"/>
+      <c r="E979" t="inlineStr"/>
+      <c r="F979" t="inlineStr"/>
+      <c r="G979" t="inlineStr"/>
+      <c r="H979" t="inlineStr"/>
+      <c r="I979" t="inlineStr"/>
+      <c r="J979" t="inlineStr"/>
+      <c r="K979" t="inlineStr"/>
+      <c r="L979" t="inlineStr"/>
+      <c r="M979" t="inlineStr"/>
+      <c r="N979" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '19', '2', '20', '21', '22', '23', '24', '25', '26', '27', '28', '29', '3', '30', '31', '32', '33', '34', '35', '36', '37', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr"/>
+      <c r="C980" t="inlineStr"/>
+      <c r="D980" t="inlineStr"/>
+      <c r="E980" t="inlineStr"/>
+      <c r="F980" t="inlineStr"/>
+      <c r="G980" t="inlineStr"/>
+      <c r="H980" t="inlineStr"/>
+      <c r="I980" t="inlineStr"/>
+      <c r="J980" t="inlineStr"/>
+      <c r="K980" t="inlineStr"/>
+      <c r="L980" t="inlineStr"/>
+      <c r="M980" t="inlineStr"/>
+      <c r="N980" t="inlineStr">
+        <is>
+          <t>['0', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr"/>
+      <c r="C981" t="inlineStr"/>
+      <c r="D981" t="inlineStr"/>
+      <c r="E981" t="inlineStr"/>
+      <c r="F981" t="inlineStr"/>
+      <c r="G981" t="inlineStr"/>
+      <c r="H981" t="inlineStr"/>
+      <c r="I981" t="inlineStr"/>
+      <c r="J981" t="inlineStr"/>
+      <c r="K981" t="inlineStr"/>
+      <c r="L981" t="inlineStr"/>
+      <c r="M981" t="inlineStr"/>
+      <c r="N981" t="inlineStr">
+        <is>
+          <t>[19564  5492    19   103     4    27     1     5     7    14    13     3
+  4149     6     7     1     4     1     1     3     2     1     1   385
+     1     2     2     3     1     2     2     1    78  1253    16   109
+    60    42]</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr"/>
+      <c r="C982" t="inlineStr"/>
+      <c r="D982" t="inlineStr"/>
+      <c r="E982" t="inlineStr"/>
+      <c r="F982" t="inlineStr"/>
+      <c r="G982" t="inlineStr"/>
+      <c r="H982" t="inlineStr"/>
+      <c r="I982" t="inlineStr"/>
+      <c r="J982" t="inlineStr"/>
+      <c r="K982" t="inlineStr"/>
+      <c r="L982" t="inlineStr"/>
+      <c r="M982" t="inlineStr"/>
+      <c r="N982" t="inlineStr">
+        <is>
+          <t>[23835  8375   180]</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr"/>
+      <c r="C983" t="inlineStr"/>
+      <c r="D983" t="inlineStr"/>
+      <c r="E983" t="inlineStr"/>
+      <c r="F983" t="inlineStr"/>
+      <c r="G983" t="inlineStr"/>
+      <c r="H983" t="inlineStr"/>
+      <c r="I983" t="inlineStr"/>
+      <c r="J983" t="inlineStr"/>
+      <c r="K983" t="inlineStr"/>
+      <c r="L983" t="inlineStr"/>
+      <c r="M983" t="inlineStr"/>
+      <c r="N983" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr"/>
+      <c r="C984" t="inlineStr"/>
+      <c r="D984" t="inlineStr"/>
+      <c r="E984" t="inlineStr"/>
+      <c r="F984" t="inlineStr"/>
+      <c r="G984" t="inlineStr"/>
+      <c r="H984" t="inlineStr"/>
+      <c r="I984" t="inlineStr"/>
+      <c r="J984" t="inlineStr"/>
+      <c r="K984" t="inlineStr"/>
+      <c r="L984" t="inlineStr"/>
+      <c r="M984" t="inlineStr"/>
+      <c r="N984" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr"/>
+      <c r="C985" t="inlineStr"/>
+      <c r="D985" t="inlineStr"/>
+      <c r="E985" t="inlineStr"/>
+      <c r="F985" t="inlineStr"/>
+      <c r="G985" t="inlineStr"/>
+      <c r="H985" t="inlineStr"/>
+      <c r="I985" t="inlineStr"/>
+      <c r="J985" t="inlineStr"/>
+      <c r="K985" t="inlineStr"/>
+      <c r="L985" t="inlineStr"/>
+      <c r="M985" t="inlineStr"/>
+      <c r="N985" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr"/>
+      <c r="C986" t="inlineStr"/>
+      <c r="D986" t="inlineStr"/>
+      <c r="E986" t="inlineStr"/>
+      <c r="F986" t="inlineStr"/>
+      <c r="G986" t="inlineStr"/>
+      <c r="H986" t="inlineStr"/>
+      <c r="I986" t="inlineStr"/>
+      <c r="J986" t="inlineStr"/>
+      <c r="K986" t="inlineStr"/>
+      <c r="L986" t="inlineStr"/>
+      <c r="M986" t="inlineStr"/>
+      <c r="N986" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr"/>
+      <c r="C987" t="inlineStr"/>
+      <c r="D987" t="inlineStr"/>
+      <c r="E987" t="inlineStr"/>
+      <c r="F987" t="inlineStr"/>
+      <c r="G987" t="inlineStr"/>
+      <c r="H987" t="inlineStr"/>
+      <c r="I987" t="inlineStr"/>
+      <c r="J987" t="inlineStr"/>
+      <c r="K987" t="inlineStr"/>
+      <c r="L987" t="inlineStr"/>
+      <c r="M987" t="inlineStr"/>
+      <c r="N987" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr"/>
+      <c r="C988" t="inlineStr"/>
+      <c r="D988" t="inlineStr"/>
+      <c r="E988" t="inlineStr"/>
+      <c r="F988" t="inlineStr"/>
+      <c r="G988" t="inlineStr"/>
+      <c r="H988" t="inlineStr"/>
+      <c r="I988" t="inlineStr"/>
+      <c r="J988" t="inlineStr"/>
+      <c r="K988" t="inlineStr"/>
+      <c r="L988" t="inlineStr"/>
+      <c r="M988" t="inlineStr"/>
+      <c r="N988" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr"/>
+      <c r="C989" t="inlineStr"/>
+      <c r="D989" t="inlineStr"/>
+      <c r="E989" t="inlineStr"/>
+      <c r="F989" t="inlineStr"/>
+      <c r="G989" t="inlineStr"/>
+      <c r="H989" t="inlineStr"/>
+      <c r="I989" t="inlineStr"/>
+      <c r="J989" t="inlineStr"/>
+      <c r="K989" t="inlineStr"/>
+      <c r="L989" t="inlineStr"/>
+      <c r="M989" t="inlineStr"/>
+      <c r="N989" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr"/>
+      <c r="C990" t="inlineStr"/>
+      <c r="D990" t="inlineStr"/>
+      <c r="E990" t="inlineStr"/>
+      <c r="F990" t="inlineStr"/>
+      <c r="G990" t="inlineStr"/>
+      <c r="H990" t="inlineStr"/>
+      <c r="I990" t="inlineStr"/>
+      <c r="J990" t="inlineStr"/>
+      <c r="K990" t="inlineStr"/>
+      <c r="L990" t="inlineStr"/>
+      <c r="M990" t="inlineStr"/>
+      <c r="N990" t="n">
+        <v>15.6925</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr"/>
+      <c r="C991" t="inlineStr"/>
+      <c r="D991" t="inlineStr"/>
+      <c r="E991" t="inlineStr"/>
+      <c r="F991" t="inlineStr"/>
+      <c r="G991" t="inlineStr"/>
+      <c r="H991" t="inlineStr"/>
+      <c r="I991" t="inlineStr"/>
+      <c r="J991" t="inlineStr"/>
+      <c r="K991" t="inlineStr"/>
+      <c r="L991" t="inlineStr"/>
+      <c r="M991" t="inlineStr"/>
+      <c r="N991" t="n">
+        <v>16.195</v>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr"/>
+      <c r="C992" t="inlineStr"/>
+      <c r="D992" t="inlineStr"/>
+      <c r="E992" t="inlineStr"/>
+      <c r="F992" t="inlineStr"/>
+      <c r="G992" t="inlineStr"/>
+      <c r="H992" t="inlineStr"/>
+      <c r="I992" t="inlineStr"/>
+      <c r="J992" t="inlineStr"/>
+      <c r="K992" t="inlineStr"/>
+      <c r="L992" t="inlineStr"/>
+      <c r="M992" t="inlineStr"/>
+      <c r="N992" t="inlineStr">
+        <is>
+          <t>{0: 0.2, 1: 0.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr"/>
+      <c r="C993" t="inlineStr"/>
+      <c r="D993" t="inlineStr"/>
+      <c r="E993" t="inlineStr"/>
+      <c r="F993" t="inlineStr"/>
+      <c r="G993" t="inlineStr"/>
+      <c r="H993" t="inlineStr"/>
+      <c r="I993" t="inlineStr"/>
+      <c r="J993" t="inlineStr"/>
+      <c r="K993" t="inlineStr"/>
+      <c r="L993" t="inlineStr"/>
+      <c r="M993" t="inlineStr"/>
+      <c r="N993" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '19', '2', '20', '21', '22', '23', '24', '25', '26', '27', '28', '29', '3', '30', '31', '32', '33', '34', '35', '36', '37', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr"/>
+      <c r="C994" t="inlineStr"/>
+      <c r="D994" t="inlineStr"/>
+      <c r="E994" t="inlineStr"/>
+      <c r="F994" t="inlineStr"/>
+      <c r="G994" t="inlineStr"/>
+      <c r="H994" t="inlineStr"/>
+      <c r="I994" t="inlineStr"/>
+      <c r="J994" t="inlineStr"/>
+      <c r="K994" t="inlineStr"/>
+      <c r="L994" t="inlineStr"/>
+      <c r="M994" t="inlineStr"/>
+      <c r="N994" t="inlineStr">
+        <is>
+          <t>['0', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr"/>
+      <c r="C995" t="inlineStr"/>
+      <c r="D995" t="inlineStr"/>
+      <c r="E995" t="inlineStr"/>
+      <c r="F995" t="inlineStr"/>
+      <c r="G995" t="inlineStr"/>
+      <c r="H995" t="inlineStr"/>
+      <c r="I995" t="inlineStr"/>
+      <c r="J995" t="inlineStr"/>
+      <c r="K995" t="inlineStr"/>
+      <c r="L995" t="inlineStr"/>
+      <c r="M995" t="inlineStr"/>
+      <c r="N995" t="inlineStr">
+        <is>
+          <t>[19564  5492    19   103     4    27     1     5     7    14    13     3
+  4149     6     7     1     4     1     1     3     2     1     1   385
+     1     2     2     3     1     2     2     1    78  1253    16   109
+    60    42]</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr"/>
+      <c r="C996" t="inlineStr"/>
+      <c r="D996" t="inlineStr"/>
+      <c r="E996" t="inlineStr"/>
+      <c r="F996" t="inlineStr"/>
+      <c r="G996" t="inlineStr"/>
+      <c r="H996" t="inlineStr"/>
+      <c r="I996" t="inlineStr"/>
+      <c r="J996" t="inlineStr"/>
+      <c r="K996" t="inlineStr"/>
+      <c r="L996" t="inlineStr"/>
+      <c r="M996" t="inlineStr"/>
+      <c r="N996" t="inlineStr">
+        <is>
+          <t>[23835  8375   180]</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr"/>
+      <c r="C997" t="inlineStr"/>
+      <c r="D997" t="inlineStr"/>
+      <c r="E997" t="inlineStr"/>
+      <c r="F997" t="inlineStr"/>
+      <c r="G997" t="inlineStr"/>
+      <c r="H997" t="inlineStr"/>
+      <c r="I997" t="inlineStr"/>
+      <c r="J997" t="inlineStr"/>
+      <c r="K997" t="inlineStr"/>
+      <c r="L997" t="inlineStr"/>
+      <c r="M997" t="inlineStr"/>
+      <c r="N997" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr"/>
+      <c r="C998" t="inlineStr"/>
+      <c r="D998" t="inlineStr"/>
+      <c r="E998" t="inlineStr"/>
+      <c r="F998" t="inlineStr"/>
+      <c r="G998" t="inlineStr"/>
+      <c r="H998" t="inlineStr"/>
+      <c r="I998" t="inlineStr"/>
+      <c r="J998" t="inlineStr"/>
+      <c r="K998" t="inlineStr"/>
+      <c r="L998" t="inlineStr"/>
+      <c r="M998" t="inlineStr"/>
+      <c r="N998" t="inlineStr">
+        <is>
+          <t>TUD</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr"/>
+      <c r="C999" t="inlineStr"/>
+      <c r="D999" t="inlineStr"/>
+      <c r="E999" t="inlineStr"/>
+      <c r="F999" t="inlineStr"/>
+      <c r="G999" t="inlineStr"/>
+      <c r="H999" t="inlineStr"/>
+      <c r="I999" t="inlineStr"/>
+      <c r="J999" t="inlineStr"/>
+      <c r="K999" t="inlineStr"/>
+      <c r="L999" t="inlineStr"/>
+      <c r="M999" t="inlineStr"/>
+      <c r="N999" t="inlineStr">
+        <is>
+          <t>Bioinformatics</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="1" t="inlineStr">
+        <is>
+          <t>num_graphs</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr"/>
+      <c r="C1000" t="inlineStr"/>
+      <c r="D1000" t="inlineStr"/>
+      <c r="E1000" t="inlineStr"/>
+      <c r="F1000" t="inlineStr"/>
+      <c r="G1000" t="inlineStr"/>
+      <c r="H1000" t="inlineStr"/>
+      <c r="I1000" t="inlineStr"/>
+      <c r="J1000" t="inlineStr"/>
+      <c r="K1000" t="inlineStr"/>
+      <c r="L1000" t="inlineStr"/>
+      <c r="M1000" t="inlineStr"/>
+      <c r="N1000" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="1" t="inlineStr">
+        <is>
+          <t>num_classes</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr"/>
+      <c r="C1001" t="inlineStr"/>
+      <c r="D1001" t="inlineStr"/>
+      <c r="E1001" t="inlineStr"/>
+      <c r="F1001" t="inlineStr"/>
+      <c r="G1001" t="inlineStr"/>
+      <c r="H1001" t="inlineStr"/>
+      <c r="I1001" t="inlineStr"/>
+      <c r="J1001" t="inlineStr"/>
+      <c r="K1001" t="inlineStr"/>
+      <c r="L1001" t="inlineStr"/>
+      <c r="M1001" t="inlineStr"/>
+      <c r="N1001" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="1" t="inlineStr">
+        <is>
+          <t>has_node_labels</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr"/>
+      <c r="C1002" t="inlineStr"/>
+      <c r="D1002" t="inlineStr"/>
+      <c r="E1002" t="inlineStr"/>
+      <c r="F1002" t="inlineStr"/>
+      <c r="G1002" t="inlineStr"/>
+      <c r="H1002" t="inlineStr"/>
+      <c r="I1002" t="inlineStr"/>
+      <c r="J1002" t="inlineStr"/>
+      <c r="K1002" t="inlineStr"/>
+      <c r="L1002" t="inlineStr"/>
+      <c r="M1002" t="inlineStr"/>
+      <c r="N1002" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="1" t="inlineStr">
+        <is>
+          <t>has_edge_labels</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr"/>
+      <c r="C1003" t="inlineStr"/>
+      <c r="D1003" t="inlineStr"/>
+      <c r="E1003" t="inlineStr"/>
+      <c r="F1003" t="inlineStr"/>
+      <c r="G1003" t="inlineStr"/>
+      <c r="H1003" t="inlineStr"/>
+      <c r="I1003" t="inlineStr"/>
+      <c r="J1003" t="inlineStr"/>
+      <c r="K1003" t="inlineStr"/>
+      <c r="L1003" t="inlineStr"/>
+      <c r="M1003" t="inlineStr"/>
+      <c r="N1003" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="1" t="inlineStr">
+        <is>
+          <t>mean_nodes</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr"/>
+      <c r="C1004" t="inlineStr"/>
+      <c r="D1004" t="inlineStr"/>
+      <c r="E1004" t="inlineStr"/>
+      <c r="F1004" t="inlineStr"/>
+      <c r="G1004" t="inlineStr"/>
+      <c r="H1004" t="inlineStr"/>
+      <c r="I1004" t="inlineStr"/>
+      <c r="J1004" t="inlineStr"/>
+      <c r="K1004" t="inlineStr"/>
+      <c r="L1004" t="inlineStr"/>
+      <c r="M1004" t="inlineStr"/>
+      <c r="N1004" t="n">
+        <v>15.6925</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="1" t="inlineStr">
+        <is>
+          <t>mean_edges</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr"/>
+      <c r="C1005" t="inlineStr"/>
+      <c r="D1005" t="inlineStr"/>
+      <c r="E1005" t="inlineStr"/>
+      <c r="F1005" t="inlineStr"/>
+      <c r="G1005" t="inlineStr"/>
+      <c r="H1005" t="inlineStr"/>
+      <c r="I1005" t="inlineStr"/>
+      <c r="J1005" t="inlineStr"/>
+      <c r="K1005" t="inlineStr"/>
+      <c r="L1005" t="inlineStr"/>
+      <c r="M1005" t="inlineStr"/>
+      <c r="N1005" t="n">
+        <v>16.195</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="1" t="inlineStr">
+        <is>
+          <t>label_distribution</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr"/>
+      <c r="C1006" t="inlineStr"/>
+      <c r="D1006" t="inlineStr"/>
+      <c r="E1006" t="inlineStr"/>
+      <c r="F1006" t="inlineStr"/>
+      <c r="G1006" t="inlineStr"/>
+      <c r="H1006" t="inlineStr"/>
+      <c r="I1006" t="inlineStr"/>
+      <c r="J1006" t="inlineStr"/>
+      <c r="K1006" t="inlineStr"/>
+      <c r="L1006" t="inlineStr"/>
+      <c r="M1006" t="inlineStr"/>
+      <c r="N1006" t="inlineStr">
+        <is>
+          <t>{0: 0.2, 1: 0.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="1" t="inlineStr">
+        <is>
+          <t>node_labels</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr"/>
+      <c r="C1007" t="inlineStr"/>
+      <c r="D1007" t="inlineStr"/>
+      <c r="E1007" t="inlineStr"/>
+      <c r="F1007" t="inlineStr"/>
+      <c r="G1007" t="inlineStr"/>
+      <c r="H1007" t="inlineStr"/>
+      <c r="I1007" t="inlineStr"/>
+      <c r="J1007" t="inlineStr"/>
+      <c r="K1007" t="inlineStr"/>
+      <c r="L1007" t="inlineStr"/>
+      <c r="M1007" t="inlineStr"/>
+      <c r="N1007" t="inlineStr">
+        <is>
+          <t>['0', '1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '19', '2', '20', '21', '22', '23', '24', '25', '26', '27', '28', '29', '3', '30', '31', '32', '33', '34', '35', '36', '37', '4', '5', '6', '7', '8', '9']</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="1" t="inlineStr">
+        <is>
+          <t>edge_labels</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr"/>
+      <c r="C1008" t="inlineStr"/>
+      <c r="D1008" t="inlineStr"/>
+      <c r="E1008" t="inlineStr"/>
+      <c r="F1008" t="inlineStr"/>
+      <c r="G1008" t="inlineStr"/>
+      <c r="H1008" t="inlineStr"/>
+      <c r="I1008" t="inlineStr"/>
+      <c r="J1008" t="inlineStr"/>
+      <c r="K1008" t="inlineStr"/>
+      <c r="L1008" t="inlineStr"/>
+      <c r="M1008" t="inlineStr"/>
+      <c r="N1008" t="inlineStr">
+        <is>
+          <t>['0', '1', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="1" t="inlineStr">
+        <is>
+          <t>node_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr"/>
+      <c r="C1009" t="inlineStr"/>
+      <c r="D1009" t="inlineStr"/>
+      <c r="E1009" t="inlineStr"/>
+      <c r="F1009" t="inlineStr"/>
+      <c r="G1009" t="inlineStr"/>
+      <c r="H1009" t="inlineStr"/>
+      <c r="I1009" t="inlineStr"/>
+      <c r="J1009" t="inlineStr"/>
+      <c r="K1009" t="inlineStr"/>
+      <c r="L1009" t="inlineStr"/>
+      <c r="M1009" t="inlineStr"/>
+      <c r="N1009" t="inlineStr">
+        <is>
+          <t>[19564  5492    19   103     4    27     1     5     7    14    13     3
+  4149     6     7     1     4     1     1     3     2     1     1   385
+     1     2     2     3     1     2     2     1    78  1253    16   109
+    60    42]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="1" t="inlineStr">
+        <is>
+          <t>edge_histogram_mean</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr"/>
+      <c r="C1010" t="inlineStr"/>
+      <c r="D1010" t="inlineStr"/>
+      <c r="E1010" t="inlineStr"/>
+      <c r="F1010" t="inlineStr"/>
+      <c r="G1010" t="inlineStr"/>
+      <c r="H1010" t="inlineStr"/>
+      <c r="I1010" t="inlineStr"/>
+      <c r="J1010" t="inlineStr"/>
+      <c r="K1010" t="inlineStr"/>
+      <c r="L1010" t="inlineStr"/>
+      <c r="M1010" t="inlineStr"/>
+      <c r="N1010" t="inlineStr">
+        <is>
+          <t>[23835  8375   180]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>